<commit_message>
Database update: context big cards format changed for testing
</commit_message>
<xml_diff>
--- a/data/TP Database.xlsx
+++ b/data/TP Database.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sophiachung/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sophiachung/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2E81815F-62A8-5646-AD14-E84A34E698CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{57683688-78F8-0F44-A953-641DD8AA5A1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13340" yWindow="500" windowWidth="15460" windowHeight="15880" xr2:uid="{F6F91125-3C8A-D047-93DD-1F3A6DE88698}"/>
+    <workbookView xWindow="13340" yWindow="500" windowWidth="15460" windowHeight="15880" activeTab="1" xr2:uid="{F6F91125-3C8A-D047-93DD-1F3A6DE88698}"/>
   </bookViews>
   <sheets>
     <sheet name="Small Cards" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="275">
   <si>
     <t>CardID</t>
   </si>
@@ -446,9 +446,6 @@
     <t>Bluescreen!</t>
   </si>
   <si>
-    <t xml:space="preserve">PLAN doesn't contain Research data management strategy </t>
-  </si>
-  <si>
     <t>Remove any 3 tiles from current section</t>
   </si>
   <si>
@@ -470,9 +467,6 @@
     <t>Tried to do too much?</t>
   </si>
   <si>
-    <t>CONTEXT doesn't contain Refine research questions</t>
-  </si>
-  <si>
     <t>Remove any 2 tiles from current section</t>
   </si>
   <si>
@@ -482,9 +476,6 @@
     <t>Expertise!</t>
   </si>
   <si>
-    <t>CONTEXT contains at least 1 Methodology tile</t>
-  </si>
-  <si>
     <t>Stand in for an Expertise training PLAN tile</t>
   </si>
   <si>
@@ -503,9 +494,6 @@
     <t>Someone has my library book!</t>
   </si>
   <si>
-    <t>PLAN doesn't contain Contingency time</t>
-  </si>
-  <si>
     <t>Remove 1 Relevant or Very relevant article tile from the CONTEXT section</t>
   </si>
   <si>
@@ -515,9 +503,6 @@
     <t>Lit review paradox</t>
   </si>
   <si>
-    <t>CONTEXT doesn't contain Refine research questions OR 2 or more Very relevant article tiles</t>
-  </si>
-  <si>
     <t>Block out 2 spaces in both the IMPLEMENTATION and WRITE-UP sections</t>
   </si>
   <si>
@@ -539,9 +524,6 @@
     <t>Lost enthusiasm</t>
   </si>
   <si>
-    <t>PLAN doesn't contain Holiday time</t>
-  </si>
-  <si>
     <t>Remove any 1 tile from current section</t>
   </si>
   <si>
@@ -572,9 +554,6 @@
     <t>Procrastinate!</t>
   </si>
   <si>
-    <t>PLAN doesn't contain Milestones, else turn over a Milestones tile as your deadlines go sailing by</t>
-  </si>
-  <si>
     <t>event-CONTEXT-shoddynotes.png</t>
   </si>
   <si>
@@ -614,18 +593,12 @@
     <t>Tunnel vision</t>
   </si>
   <si>
-    <t>PLAN doesn't contain Meetings with supervisor AND CONTEXT doesn't contain EITHER Discussion experts OR Refine research questions</t>
-  </si>
-  <si>
     <t>event-CONTEXT-writersblock.png</t>
   </si>
   <si>
     <t>Writer's block</t>
   </si>
   <si>
-    <t>PLAN doesn't contain both Milestones AND Meeting with supervisor</t>
-  </si>
-  <si>
     <t>event-IMP-bluescreen.png</t>
   </si>
   <si>
@@ -861,6 +834,33 @@
   </si>
   <si>
     <t>0,1,0,1</t>
+  </si>
+  <si>
+    <t>!6</t>
+  </si>
+  <si>
+    <t>!13</t>
+  </si>
+  <si>
+    <t>!1</t>
+  </si>
+  <si>
+    <t>!4</t>
+  </si>
+  <si>
+    <t>!5 (else turn over a Milestones tile as your deadlines go sailing by)</t>
+  </si>
+  <si>
+    <t>!7&amp;!9&amp;!13</t>
+  </si>
+  <si>
+    <t>!13&amp;!31:&gt;1</t>
+  </si>
+  <si>
+    <t>!(5&amp;7)</t>
+  </si>
+  <si>
+    <t>(11+12):&gt;=1</t>
   </si>
 </sst>
 </file>
@@ -913,16 +913,16 @@
   </cellStyles>
   <dxfs count="4">
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -941,7 +941,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4A58CFC2-94C3-1B4C-9FA9-2EDE6B381A1D}" name="Table13" displayName="Table13" ref="A1:G59" totalsRowShown="0">
   <autoFilter ref="A1:G59" xr:uid="{4A58CFC2-94C3-1B4C-9FA9-2EDE6B381A1D}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{93B3FC9C-96B8-F541-B39A-A82E1D56BCAA}" name="CardID" dataDxfId="1">
+    <tableColumn id="1" xr3:uid="{93B3FC9C-96B8-F541-B39A-A82E1D56BCAA}" name="CardID" dataDxfId="3">
       <calculatedColumnFormula>ROW() - 1</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="2" xr3:uid="{A33729B5-68D1-CE41-939B-B3B7383FEE9E}" name="Stage"/>
@@ -959,7 +959,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{4E25BA7D-C944-7B48-8D11-C2260663E6FE}" name="Table135" displayName="Table135" ref="A1:I66" totalsRowShown="0">
   <autoFilter ref="A1:I66" xr:uid="{4E25BA7D-C944-7B48-8D11-C2260663E6FE}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{241E3EFA-1556-A24B-8441-368F09FD400E}" name="CardID" dataDxfId="0">
+    <tableColumn id="1" xr3:uid="{241E3EFA-1556-A24B-8441-368F09FD400E}" name="CardID" dataDxfId="2">
       <calculatedColumnFormula>ROW() + 57</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="2" xr3:uid="{4CB802A7-5A14-1843-8D85-057515A93530}" name="Stage"/>
@@ -982,7 +982,7 @@
     <tableColumn id="1" xr3:uid="{9685744F-8B05-1442-9B48-108AE1383418}" name="CardID"/>
     <tableColumn id="2" xr3:uid="{DB16A56D-767D-9F4A-92B0-3F2FF796098B}" name="Stage"/>
     <tableColumn id="3" xr3:uid="{062C43CD-0611-9443-923F-251F6E69C712}" name="Number"/>
-    <tableColumn id="8" xr3:uid="{E7D5FBD8-3951-FF44-897A-D8C691EF33A7}" name="Filename" dataDxfId="3"/>
+    <tableColumn id="8" xr3:uid="{E7D5FBD8-3951-FF44-897A-D8C691EF33A7}" name="Filename" dataDxfId="1"/>
     <tableColumn id="4" xr3:uid="{6339B9FC-2BF1-F94F-9DF5-22F5A6A03A1B}" name="Title"/>
     <tableColumn id="5" xr3:uid="{6C0BBB6B-F2D1-934E-89B9-438520C75EA5}" name="Description"/>
     <tableColumn id="6" xr3:uid="{EC19A1A1-792A-674C-9DF4-EC994909ED61}" name="Placement"/>
@@ -998,7 +998,7 @@
     <tableColumn id="1" xr3:uid="{B781EFFE-21A1-C44F-9762-061D6BE40AE8}" name="CardID"/>
     <tableColumn id="2" xr3:uid="{F86B5EC3-2A3F-A04C-926B-85F4BB4FBD8C}" name="Stage"/>
     <tableColumn id="3" xr3:uid="{B50BAF85-E1F0-394D-BAF7-49DF53A0ADB9}" name="Number"/>
-    <tableColumn id="8" xr3:uid="{951FA9FE-3F95-D44C-96BA-C6860B6AD12B}" name="Filename" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{951FA9FE-3F95-D44C-96BA-C6860B6AD12B}" name="Filename" dataDxfId="0"/>
     <tableColumn id="4" xr3:uid="{F3B3D1F5-9D91-1444-8621-8C3D12AB5900}" name="Title"/>
     <tableColumn id="5" xr3:uid="{86DDE4E7-F385-0742-90D0-8AD93F96551C}" name="Description"/>
     <tableColumn id="6" xr3:uid="{6DBECDC0-D61F-3B47-9969-9D7C4754274A}" name="Left"/>
@@ -1309,7 +1309,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18AE550B-A04F-B142-B067-7E2D879988FA}">
   <dimension ref="A1:H59"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="102" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A39" zoomScale="102" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
@@ -1367,7 +1367,7 @@
         <v>9</v>
       </c>
       <c r="G2" t="s">
-        <v>265</v>
+        <v>256</v>
       </c>
       <c r="H2" t="s">
         <v>36</v>
@@ -1391,7 +1391,7 @@
         <v>44</v>
       </c>
       <c r="G3" t="s">
-        <v>265</v>
+        <v>256</v>
       </c>
       <c r="H3" t="s">
         <v>38</v>
@@ -1415,7 +1415,7 @@
         <v>46</v>
       </c>
       <c r="G4" t="s">
-        <v>265</v>
+        <v>256</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -1436,7 +1436,7 @@
         <v>48</v>
       </c>
       <c r="G5" t="s">
-        <v>265</v>
+        <v>256</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -1457,7 +1457,7 @@
         <v>50</v>
       </c>
       <c r="G6" t="s">
-        <v>265</v>
+        <v>256</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -1478,7 +1478,7 @@
         <v>52</v>
       </c>
       <c r="G7" t="s">
-        <v>265</v>
+        <v>256</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -1499,7 +1499,7 @@
         <v>54</v>
       </c>
       <c r="G8" t="s">
-        <v>265</v>
+        <v>256</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
@@ -1520,7 +1520,7 @@
         <v>12</v>
       </c>
       <c r="G9" t="s">
-        <v>266</v>
+        <v>257</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
@@ -1541,7 +1541,7 @@
         <v>56</v>
       </c>
       <c r="G10" t="s">
-        <v>267</v>
+        <v>258</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
@@ -1562,7 +1562,7 @@
         <v>58</v>
       </c>
       <c r="G11" t="s">
-        <v>268</v>
+        <v>259</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
@@ -1583,7 +1583,7 @@
         <v>60</v>
       </c>
       <c r="G12" t="s">
-        <v>269</v>
+        <v>260</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
@@ -1604,7 +1604,7 @@
         <v>60</v>
       </c>
       <c r="G13" t="s">
-        <v>270</v>
+        <v>261</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
@@ -1625,7 +1625,7 @@
         <v>63</v>
       </c>
       <c r="G14" t="s">
-        <v>267</v>
+        <v>258</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
@@ -1646,7 +1646,7 @@
         <v>65</v>
       </c>
       <c r="G15" t="s">
-        <v>267</v>
+        <v>258</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
@@ -1667,7 +1667,7 @@
         <v>67</v>
       </c>
       <c r="G16" t="s">
-        <v>270</v>
+        <v>261</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
@@ -1688,7 +1688,7 @@
         <v>67</v>
       </c>
       <c r="G17" t="s">
-        <v>269</v>
+        <v>260</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
@@ -1709,7 +1709,7 @@
         <v>70</v>
       </c>
       <c r="G18" t="s">
-        <v>270</v>
+        <v>261</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
@@ -1730,7 +1730,7 @@
         <v>70</v>
       </c>
       <c r="G19" t="s">
-        <v>269</v>
+        <v>260</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
@@ -1751,7 +1751,7 @@
         <v>16</v>
       </c>
       <c r="G20" t="s">
-        <v>270</v>
+        <v>261</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
@@ -1772,7 +1772,7 @@
         <v>16</v>
       </c>
       <c r="G21" t="s">
-        <v>269</v>
+        <v>260</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
@@ -1793,7 +1793,7 @@
         <v>73</v>
       </c>
       <c r="G22" t="s">
-        <v>270</v>
+        <v>261</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
@@ -1814,7 +1814,7 @@
         <v>73</v>
       </c>
       <c r="G23" t="s">
-        <v>269</v>
+        <v>260</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
@@ -1835,7 +1835,7 @@
         <v>76</v>
       </c>
       <c r="G24" t="s">
-        <v>270</v>
+        <v>261</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
@@ -1856,7 +1856,7 @@
         <v>76</v>
       </c>
       <c r="G25" t="s">
-        <v>269</v>
+        <v>260</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
@@ -1877,7 +1877,7 @@
         <v>79</v>
       </c>
       <c r="G26" t="s">
-        <v>270</v>
+        <v>261</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
@@ -1898,7 +1898,7 @@
         <v>79</v>
       </c>
       <c r="G27" t="s">
-        <v>269</v>
+        <v>260</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
@@ -1919,7 +1919,7 @@
         <v>82</v>
       </c>
       <c r="G28" t="s">
-        <v>270</v>
+        <v>261</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
@@ -1940,7 +1940,7 @@
         <v>82</v>
       </c>
       <c r="G29" t="s">
-        <v>269</v>
+        <v>260</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
@@ -1961,7 +1961,7 @@
         <v>85</v>
       </c>
       <c r="G30" t="s">
-        <v>271</v>
+        <v>262</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
@@ -1982,7 +1982,7 @@
         <v>87</v>
       </c>
       <c r="G31" t="s">
-        <v>272</v>
+        <v>263</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
@@ -2003,7 +2003,7 @@
         <v>89</v>
       </c>
       <c r="G32" t="s">
-        <v>267</v>
+        <v>258</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
@@ -2024,7 +2024,7 @@
         <v>91</v>
       </c>
       <c r="G33" t="s">
-        <v>267</v>
+        <v>258</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
@@ -2045,7 +2045,7 @@
         <v>23</v>
       </c>
       <c r="G34" t="s">
-        <v>267</v>
+        <v>258</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
@@ -2066,7 +2066,7 @@
         <v>23</v>
       </c>
       <c r="G35" t="s">
-        <v>268</v>
+        <v>259</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
@@ -2087,7 +2087,7 @@
         <v>23</v>
       </c>
       <c r="G36" t="s">
-        <v>269</v>
+        <v>260</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
@@ -2108,7 +2108,7 @@
         <v>23</v>
       </c>
       <c r="G37" t="s">
-        <v>270</v>
+        <v>261</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
@@ -2129,7 +2129,7 @@
         <v>96</v>
       </c>
       <c r="G38" t="s">
-        <v>267</v>
+        <v>258</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
@@ -2150,7 +2150,7 @@
         <v>96</v>
       </c>
       <c r="G39" t="s">
-        <v>269</v>
+        <v>260</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
@@ -2171,7 +2171,7 @@
         <v>96</v>
       </c>
       <c r="G40" t="s">
-        <v>270</v>
+        <v>261</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
@@ -2192,7 +2192,7 @@
         <v>96</v>
       </c>
       <c r="G41" t="s">
-        <v>268</v>
+        <v>259</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
@@ -2213,7 +2213,7 @@
         <v>101</v>
       </c>
       <c r="G42" t="s">
-        <v>267</v>
+        <v>258</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
@@ -2234,7 +2234,7 @@
         <v>26</v>
       </c>
       <c r="G43" t="s">
-        <v>267</v>
+        <v>258</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
@@ -2255,7 +2255,7 @@
         <v>103</v>
       </c>
       <c r="G44" t="s">
-        <v>269</v>
+        <v>260</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
@@ -2276,7 +2276,7 @@
         <v>103</v>
       </c>
       <c r="G45" t="s">
-        <v>270</v>
+        <v>261</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
@@ -2297,7 +2297,7 @@
         <v>106</v>
       </c>
       <c r="G46" t="s">
-        <v>270</v>
+        <v>261</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
@@ -2318,7 +2318,7 @@
         <v>106</v>
       </c>
       <c r="G47" t="s">
-        <v>269</v>
+        <v>260</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
@@ -2339,7 +2339,7 @@
         <v>109</v>
       </c>
       <c r="G48" t="s">
-        <v>273</v>
+        <v>264</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
@@ -2360,7 +2360,7 @@
         <v>109</v>
       </c>
       <c r="G49" t="s">
-        <v>274</v>
+        <v>265</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
@@ -2381,7 +2381,7 @@
         <v>112</v>
       </c>
       <c r="G50" t="s">
-        <v>268</v>
+        <v>259</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
@@ -2402,7 +2402,7 @@
         <v>32</v>
       </c>
       <c r="G51" t="s">
-        <v>268</v>
+        <v>259</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.2">
@@ -2423,7 +2423,7 @@
         <v>32</v>
       </c>
       <c r="G52" t="s">
-        <v>273</v>
+        <v>264</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
@@ -2444,7 +2444,7 @@
         <v>32</v>
       </c>
       <c r="G53" t="s">
-        <v>274</v>
+        <v>265</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.2">
@@ -2465,7 +2465,7 @@
         <v>116</v>
       </c>
       <c r="G54" t="s">
-        <v>268</v>
+        <v>259</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.2">
@@ -2486,7 +2486,7 @@
         <v>29</v>
       </c>
       <c r="G55" t="s">
-        <v>273</v>
+        <v>264</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.2">
@@ -2507,7 +2507,7 @@
         <v>29</v>
       </c>
       <c r="G56" t="s">
-        <v>274</v>
+        <v>265</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.2">
@@ -2528,7 +2528,7 @@
         <v>119</v>
       </c>
       <c r="G57" t="s">
-        <v>268</v>
+        <v>259</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.2">
@@ -2549,7 +2549,7 @@
         <v>121</v>
       </c>
       <c r="G58" t="s">
-        <v>268</v>
+        <v>259</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.2">
@@ -2570,7 +2570,7 @@
         <v>123</v>
       </c>
       <c r="G59" t="s">
-        <v>268</v>
+        <v>259</v>
       </c>
     </row>
   </sheetData>
@@ -2585,20 +2585,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84DC5E79-A11F-0148-B3A8-F5384824D987}">
   <dimension ref="A1:J66"/>
   <sheetViews>
-    <sheetView zoomScale="99" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" zoomScale="99" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9.1640625" customWidth="1"/>
-    <col min="2" max="2" width="15.1640625" customWidth="1"/>
+    <col min="2" max="2" width="9.5" customWidth="1"/>
     <col min="3" max="3" width="10.6640625" customWidth="1"/>
     <col min="4" max="4" width="25.83203125" customWidth="1"/>
     <col min="5" max="5" width="26" customWidth="1"/>
     <col min="6" max="6" width="14" customWidth="1"/>
-    <col min="7" max="7" width="38.6640625" customWidth="1"/>
-    <col min="8" max="8" width="46.1640625" customWidth="1"/>
+    <col min="7" max="7" width="17" customWidth="1"/>
+    <col min="8" max="8" width="15.83203125" customWidth="1"/>
     <col min="9" max="9" width="88.5" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2636,8 +2636,8 @@
         <f t="shared" ref="A2:A33" si="0">ROW() + 57</f>
         <v>59</v>
       </c>
-      <c r="B2" t="s">
-        <v>14</v>
+      <c r="B2">
+        <v>2</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -2663,8 +2663,8 @@
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
-      <c r="B3" t="s">
-        <v>14</v>
+      <c r="B3">
+        <v>2</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -2690,8 +2690,8 @@
         <f t="shared" si="0"/>
         <v>61</v>
       </c>
-      <c r="B4" t="s">
-        <v>14</v>
+      <c r="B4">
+        <v>2</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -2706,10 +2706,10 @@
         <v>129</v>
       </c>
       <c r="H4" t="s">
+        <v>266</v>
+      </c>
+      <c r="I4" t="s">
         <v>136</v>
-      </c>
-      <c r="I4" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
@@ -2717,17 +2717,17 @@
         <f t="shared" si="0"/>
         <v>62</v>
       </c>
-      <c r="B5" t="s">
-        <v>14</v>
+      <c r="B5">
+        <v>2</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="D5" t="s">
+        <v>137</v>
+      </c>
+      <c r="E5" t="s">
         <v>138</v>
-      </c>
-      <c r="E5" t="s">
-        <v>139</v>
       </c>
       <c r="G5" t="s">
         <v>129</v>
@@ -2736,7 +2736,7 @@
         <v>129</v>
       </c>
       <c r="I5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
@@ -2744,17 +2744,17 @@
         <f t="shared" si="0"/>
         <v>63</v>
       </c>
-      <c r="B6" t="s">
-        <v>14</v>
+      <c r="B6">
+        <v>2</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G6" t="s">
         <v>129</v>
@@ -2763,7 +2763,7 @@
         <v>129</v>
       </c>
       <c r="I6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
@@ -2771,26 +2771,26 @@
         <f t="shared" si="0"/>
         <v>64</v>
       </c>
-      <c r="B7" t="s">
-        <v>14</v>
+      <c r="B7">
+        <v>2</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
       <c r="D7" t="s">
+        <v>141</v>
+      </c>
+      <c r="E7" t="s">
         <v>142</v>
-      </c>
-      <c r="E7" t="s">
-        <v>143</v>
       </c>
       <c r="G7" t="s">
         <v>129</v>
       </c>
       <c r="H7" t="s">
-        <v>144</v>
+        <v>267</v>
       </c>
       <c r="I7" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
@@ -2798,26 +2798,26 @@
         <f t="shared" si="0"/>
         <v>65</v>
       </c>
-      <c r="B8" t="s">
-        <v>14</v>
+      <c r="B8">
+        <v>2</v>
       </c>
       <c r="C8">
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E8" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="G8" t="s">
-        <v>148</v>
+        <v>274</v>
       </c>
       <c r="H8" t="s">
         <v>129</v>
       </c>
       <c r="I8" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
@@ -2825,17 +2825,17 @@
         <f t="shared" si="0"/>
         <v>66</v>
       </c>
-      <c r="B9" t="s">
-        <v>14</v>
+      <c r="B9">
+        <v>2</v>
       </c>
       <c r="C9">
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="E9" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="G9" t="s">
         <v>129</v>
@@ -2844,7 +2844,7 @@
         <v>129</v>
       </c>
       <c r="I9" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
@@ -2852,26 +2852,26 @@
         <f t="shared" si="0"/>
         <v>67</v>
       </c>
-      <c r="B10" t="s">
-        <v>14</v>
+      <c r="B10">
+        <v>2</v>
       </c>
       <c r="C10">
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="E10" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="G10" t="s">
         <v>129</v>
       </c>
       <c r="H10" t="s">
-        <v>155</v>
+        <v>268</v>
       </c>
       <c r="I10" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
@@ -2879,26 +2879,26 @@
         <f t="shared" si="0"/>
         <v>68</v>
       </c>
-      <c r="B11" t="s">
-        <v>14</v>
+      <c r="B11">
+        <v>2</v>
       </c>
       <c r="C11">
         <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="E11" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="G11" t="s">
         <v>129</v>
       </c>
       <c r="H11" t="s">
-        <v>159</v>
+        <v>272</v>
       </c>
       <c r="I11" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
@@ -2906,29 +2906,29 @@
         <f t="shared" si="0"/>
         <v>69</v>
       </c>
-      <c r="B12" t="s">
-        <v>14</v>
+      <c r="B12">
+        <v>2</v>
       </c>
       <c r="C12">
         <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="E12" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="G12" t="s">
         <v>129</v>
       </c>
       <c r="H12" t="s">
-        <v>155</v>
+        <v>268</v>
       </c>
       <c r="I12" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="J12" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
@@ -2936,26 +2936,26 @@
         <f t="shared" si="0"/>
         <v>70</v>
       </c>
-      <c r="B13" t="s">
-        <v>14</v>
+      <c r="B13">
+        <v>2</v>
       </c>
       <c r="C13">
         <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="E13" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="G13" t="s">
         <v>129</v>
       </c>
       <c r="H13" t="s">
-        <v>167</v>
+        <v>269</v>
       </c>
       <c r="I13" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
@@ -2963,17 +2963,17 @@
         <f t="shared" si="0"/>
         <v>71</v>
       </c>
-      <c r="B14" t="s">
-        <v>14</v>
+      <c r="B14">
+        <v>2</v>
       </c>
       <c r="C14">
         <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="E14" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="G14" t="s">
         <v>129</v>
@@ -2982,7 +2982,7 @@
         <v>129</v>
       </c>
       <c r="I14" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
@@ -2990,26 +2990,26 @@
         <f t="shared" si="0"/>
         <v>72</v>
       </c>
-      <c r="B15" t="s">
-        <v>14</v>
+      <c r="B15">
+        <v>2</v>
       </c>
       <c r="C15">
         <v>1</v>
       </c>
       <c r="D15" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="E15" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="G15" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="H15" t="s">
         <v>129</v>
       </c>
       <c r="I15" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
@@ -3017,26 +3017,26 @@
         <f t="shared" si="0"/>
         <v>73</v>
       </c>
-      <c r="B16" t="s">
-        <v>14</v>
+      <c r="B16">
+        <v>2</v>
       </c>
       <c r="C16">
         <v>1</v>
       </c>
       <c r="D16" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="E16" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="G16" t="s">
         <v>129</v>
       </c>
       <c r="H16" t="s">
-        <v>178</v>
+        <v>270</v>
       </c>
       <c r="I16" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
@@ -3044,26 +3044,26 @@
         <f t="shared" si="0"/>
         <v>74</v>
       </c>
-      <c r="B17" t="s">
-        <v>14</v>
+      <c r="B17">
+        <v>2</v>
       </c>
       <c r="C17">
         <v>1</v>
       </c>
       <c r="D17" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="E17" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="G17" t="s">
         <v>129</v>
       </c>
       <c r="H17" t="s">
+        <v>268</v>
+      </c>
+      <c r="I17" t="s">
         <v>155</v>
-      </c>
-      <c r="I17" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
@@ -3071,26 +3071,26 @@
         <f t="shared" si="0"/>
         <v>75</v>
       </c>
-      <c r="B18" t="s">
-        <v>14</v>
+      <c r="B18">
+        <v>2</v>
       </c>
       <c r="C18">
         <v>1</v>
       </c>
       <c r="D18" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="E18" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="G18" t="s">
         <v>129</v>
       </c>
       <c r="H18" t="s">
-        <v>155</v>
+        <v>268</v>
       </c>
       <c r="I18" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
@@ -3098,26 +3098,26 @@
         <f t="shared" si="0"/>
         <v>76</v>
       </c>
-      <c r="B19" t="s">
-        <v>14</v>
+      <c r="B19">
+        <v>2</v>
       </c>
       <c r="C19">
         <v>1</v>
       </c>
       <c r="D19" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="E19" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="G19" t="s">
         <v>129</v>
       </c>
       <c r="H19" t="s">
-        <v>155</v>
+        <v>268</v>
       </c>
       <c r="I19" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
@@ -3125,17 +3125,17 @@
         <f t="shared" si="0"/>
         <v>77</v>
       </c>
-      <c r="B20" t="s">
-        <v>14</v>
+      <c r="B20">
+        <v>2</v>
       </c>
       <c r="C20">
         <v>1</v>
       </c>
       <c r="D20" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="E20" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="G20" t="s">
         <v>129</v>
@@ -3144,7 +3144,7 @@
         <v>129</v>
       </c>
       <c r="I20" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
@@ -3152,17 +3152,17 @@
         <f t="shared" si="0"/>
         <v>78</v>
       </c>
-      <c r="B21" t="s">
-        <v>14</v>
+      <c r="B21">
+        <v>2</v>
       </c>
       <c r="C21">
         <v>1</v>
       </c>
       <c r="D21" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="E21" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="G21" t="s">
         <v>129</v>
@@ -3171,7 +3171,7 @@
         <v>129</v>
       </c>
       <c r="I21" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
@@ -3179,26 +3179,26 @@
         <f t="shared" si="0"/>
         <v>79</v>
       </c>
-      <c r="B22" t="s">
-        <v>14</v>
+      <c r="B22">
+        <v>2</v>
       </c>
       <c r="C22">
         <v>1</v>
       </c>
       <c r="D22" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="E22" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="G22" t="s">
         <v>129</v>
       </c>
       <c r="H22" t="s">
-        <v>192</v>
+        <v>271</v>
       </c>
       <c r="I22" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
@@ -3206,26 +3206,26 @@
         <f t="shared" si="0"/>
         <v>80</v>
       </c>
-      <c r="B23" t="s">
-        <v>14</v>
+      <c r="B23">
+        <v>2</v>
       </c>
       <c r="C23">
         <v>1</v>
       </c>
       <c r="D23" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="E23" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="G23" t="s">
         <v>129</v>
       </c>
       <c r="H23" t="s">
-        <v>195</v>
+        <v>273</v>
       </c>
       <c r="I23" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
@@ -3233,14 +3233,14 @@
         <f t="shared" si="0"/>
         <v>81</v>
       </c>
-      <c r="B24" t="s">
-        <v>21</v>
+      <c r="B24">
+        <v>3</v>
       </c>
       <c r="C24">
         <v>1</v>
       </c>
       <c r="D24" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="E24" t="s">
         <v>135</v>
@@ -3251,17 +3251,17 @@
         <f t="shared" si="0"/>
         <v>82</v>
       </c>
-      <c r="B25" t="s">
-        <v>21</v>
+      <c r="B25">
+        <v>3</v>
       </c>
       <c r="C25">
         <v>1</v>
       </c>
       <c r="D25" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="E25" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
@@ -3269,17 +3269,17 @@
         <f t="shared" si="0"/>
         <v>83</v>
       </c>
-      <c r="B26" t="s">
-        <v>21</v>
+      <c r="B26">
+        <v>3</v>
       </c>
       <c r="C26">
         <v>1</v>
       </c>
       <c r="D26" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="E26" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
@@ -3287,17 +3287,17 @@
         <f t="shared" si="0"/>
         <v>84</v>
       </c>
-      <c r="B27" t="s">
-        <v>21</v>
+      <c r="B27">
+        <v>3</v>
       </c>
       <c r="C27">
         <v>1</v>
       </c>
       <c r="D27" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="E27" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
@@ -3305,17 +3305,17 @@
         <f t="shared" si="0"/>
         <v>85</v>
       </c>
-      <c r="B28" t="s">
-        <v>21</v>
+      <c r="B28">
+        <v>3</v>
       </c>
       <c r="C28">
         <v>1</v>
       </c>
       <c r="D28" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
       <c r="E28" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
@@ -3323,17 +3323,17 @@
         <f t="shared" si="0"/>
         <v>86</v>
       </c>
-      <c r="B29" t="s">
-        <v>21</v>
+      <c r="B29">
+        <v>3</v>
       </c>
       <c r="C29">
         <v>1</v>
       </c>
       <c r="D29" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="E29" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
@@ -3341,17 +3341,17 @@
         <f t="shared" si="0"/>
         <v>87</v>
       </c>
-      <c r="B30" t="s">
-        <v>21</v>
+      <c r="B30">
+        <v>3</v>
       </c>
       <c r="C30">
         <v>1</v>
       </c>
       <c r="D30" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
       <c r="E30" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
@@ -3359,17 +3359,17 @@
         <f t="shared" si="0"/>
         <v>88</v>
       </c>
-      <c r="B31" t="s">
-        <v>21</v>
+      <c r="B31">
+        <v>3</v>
       </c>
       <c r="C31">
         <v>1</v>
       </c>
       <c r="D31" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
       <c r="E31" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
@@ -3377,17 +3377,17 @@
         <f t="shared" si="0"/>
         <v>89</v>
       </c>
-      <c r="B32" t="s">
-        <v>21</v>
+      <c r="B32">
+        <v>3</v>
       </c>
       <c r="C32">
         <v>1</v>
       </c>
       <c r="D32" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="E32" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
@@ -3395,17 +3395,17 @@
         <f t="shared" si="0"/>
         <v>90</v>
       </c>
-      <c r="B33" t="s">
-        <v>21</v>
+      <c r="B33">
+        <v>3</v>
       </c>
       <c r="C33">
         <v>1</v>
       </c>
       <c r="D33" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="E33" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
@@ -3413,17 +3413,17 @@
         <f t="shared" ref="A34:A66" si="1">ROW() + 57</f>
         <v>91</v>
       </c>
-      <c r="B34" t="s">
-        <v>21</v>
+      <c r="B34">
+        <v>3</v>
       </c>
       <c r="C34">
         <v>1</v>
       </c>
       <c r="D34" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="E34" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
@@ -3431,17 +3431,17 @@
         <f t="shared" si="1"/>
         <v>92</v>
       </c>
-      <c r="B35" t="s">
-        <v>21</v>
+      <c r="B35">
+        <v>3</v>
       </c>
       <c r="C35">
         <v>1</v>
       </c>
       <c r="D35" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="E35" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
@@ -3449,17 +3449,17 @@
         <f t="shared" si="1"/>
         <v>93</v>
       </c>
-      <c r="B36" t="s">
-        <v>21</v>
+      <c r="B36">
+        <v>3</v>
       </c>
       <c r="C36">
         <v>1</v>
       </c>
       <c r="D36" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
       <c r="E36" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
@@ -3467,17 +3467,17 @@
         <f t="shared" si="1"/>
         <v>94</v>
       </c>
-      <c r="B37" t="s">
-        <v>21</v>
+      <c r="B37">
+        <v>3</v>
       </c>
       <c r="C37">
         <v>1</v>
       </c>
       <c r="D37" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
       <c r="E37" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
@@ -3485,17 +3485,17 @@
         <f t="shared" si="1"/>
         <v>95</v>
       </c>
-      <c r="B38" t="s">
-        <v>21</v>
+      <c r="B38">
+        <v>3</v>
       </c>
       <c r="C38">
         <v>1</v>
       </c>
       <c r="D38" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="E38" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
@@ -3503,17 +3503,17 @@
         <f t="shared" si="1"/>
         <v>96</v>
       </c>
-      <c r="B39" t="s">
-        <v>21</v>
+      <c r="B39">
+        <v>3</v>
       </c>
       <c r="C39">
         <v>1</v>
       </c>
       <c r="D39" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="E39" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
@@ -3521,17 +3521,17 @@
         <f t="shared" si="1"/>
         <v>97</v>
       </c>
-      <c r="B40" t="s">
-        <v>21</v>
+      <c r="B40">
+        <v>3</v>
       </c>
       <c r="C40">
         <v>1</v>
       </c>
       <c r="D40" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="E40" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
@@ -3539,17 +3539,17 @@
         <f t="shared" si="1"/>
         <v>98</v>
       </c>
-      <c r="B41" t="s">
-        <v>21</v>
+      <c r="B41">
+        <v>3</v>
       </c>
       <c r="C41">
         <v>1</v>
       </c>
       <c r="D41" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="E41" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
@@ -3557,17 +3557,17 @@
         <f t="shared" si="1"/>
         <v>99</v>
       </c>
-      <c r="B42" t="s">
-        <v>21</v>
+      <c r="B42">
+        <v>3</v>
       </c>
       <c r="C42">
         <v>1</v>
       </c>
       <c r="D42" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="E42" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
@@ -3575,17 +3575,17 @@
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
-      <c r="B43" t="s">
-        <v>21</v>
+      <c r="B43">
+        <v>3</v>
       </c>
       <c r="C43">
         <v>1</v>
       </c>
       <c r="D43" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="E43" t="s">
-        <v>228</v>
+        <v>219</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
@@ -3593,17 +3593,17 @@
         <f t="shared" si="1"/>
         <v>101</v>
       </c>
-      <c r="B44" t="s">
-        <v>21</v>
+      <c r="B44">
+        <v>3</v>
       </c>
       <c r="C44">
         <v>1</v>
       </c>
       <c r="D44" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
       <c r="E44" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
@@ -3611,17 +3611,17 @@
         <f t="shared" si="1"/>
         <v>102</v>
       </c>
-      <c r="B45" t="s">
-        <v>27</v>
+      <c r="B45">
+        <v>4</v>
       </c>
       <c r="C45">
         <v>1</v>
       </c>
       <c r="D45" t="s">
-        <v>230</v>
+        <v>221</v>
       </c>
       <c r="E45" t="s">
-        <v>231</v>
+        <v>222</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
@@ -3629,14 +3629,14 @@
         <f t="shared" si="1"/>
         <v>103</v>
       </c>
-      <c r="B46" t="s">
-        <v>27</v>
+      <c r="B46">
+        <v>4</v>
       </c>
       <c r="C46">
         <v>1</v>
       </c>
       <c r="D46" t="s">
-        <v>232</v>
+        <v>223</v>
       </c>
       <c r="E46" t="s">
         <v>135</v>
@@ -3647,17 +3647,17 @@
         <f t="shared" si="1"/>
         <v>104</v>
       </c>
-      <c r="B47" t="s">
-        <v>27</v>
+      <c r="B47">
+        <v>4</v>
       </c>
       <c r="C47">
         <v>1</v>
       </c>
       <c r="D47" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="E47" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
@@ -3665,17 +3665,17 @@
         <f t="shared" si="1"/>
         <v>105</v>
       </c>
-      <c r="B48" t="s">
-        <v>27</v>
+      <c r="B48">
+        <v>4</v>
       </c>
       <c r="C48">
         <v>1</v>
       </c>
       <c r="D48" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="E48" t="s">
-        <v>236</v>
+        <v>227</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
@@ -3683,17 +3683,17 @@
         <f t="shared" si="1"/>
         <v>106</v>
       </c>
-      <c r="B49" t="s">
-        <v>27</v>
+      <c r="B49">
+        <v>4</v>
       </c>
       <c r="C49">
         <v>1</v>
       </c>
       <c r="D49" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
       <c r="E49" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
@@ -3701,17 +3701,17 @@
         <f t="shared" si="1"/>
         <v>107</v>
       </c>
-      <c r="B50" t="s">
-        <v>27</v>
+      <c r="B50">
+        <v>4</v>
       </c>
       <c r="C50">
         <v>1</v>
       </c>
       <c r="D50" t="s">
-        <v>238</v>
+        <v>229</v>
       </c>
       <c r="E50" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
@@ -3719,17 +3719,17 @@
         <f t="shared" si="1"/>
         <v>108</v>
       </c>
-      <c r="B51" t="s">
-        <v>27</v>
+      <c r="B51">
+        <v>4</v>
       </c>
       <c r="C51">
         <v>1</v>
       </c>
       <c r="D51" t="s">
-        <v>239</v>
+        <v>230</v>
       </c>
       <c r="E51" t="s">
-        <v>240</v>
+        <v>231</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
@@ -3737,17 +3737,17 @@
         <f t="shared" si="1"/>
         <v>109</v>
       </c>
-      <c r="B52" t="s">
-        <v>27</v>
+      <c r="B52">
+        <v>4</v>
       </c>
       <c r="C52">
         <v>1</v>
       </c>
       <c r="D52" t="s">
-        <v>241</v>
+        <v>232</v>
       </c>
       <c r="E52" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
@@ -3755,17 +3755,17 @@
         <f t="shared" si="1"/>
         <v>110</v>
       </c>
-      <c r="B53" t="s">
-        <v>27</v>
+      <c r="B53">
+        <v>4</v>
       </c>
       <c r="C53">
         <v>1</v>
       </c>
       <c r="D53" t="s">
-        <v>242</v>
+        <v>233</v>
       </c>
       <c r="E53" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
@@ -3773,17 +3773,17 @@
         <f t="shared" si="1"/>
         <v>111</v>
       </c>
-      <c r="B54" t="s">
-        <v>27</v>
+      <c r="B54">
+        <v>4</v>
       </c>
       <c r="C54">
         <v>1</v>
       </c>
       <c r="D54" t="s">
-        <v>243</v>
+        <v>234</v>
       </c>
       <c r="E54" t="s">
-        <v>244</v>
+        <v>235</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
@@ -3791,17 +3791,17 @@
         <f t="shared" si="1"/>
         <v>112</v>
       </c>
-      <c r="B55" t="s">
-        <v>27</v>
+      <c r="B55">
+        <v>4</v>
       </c>
       <c r="C55">
         <v>1</v>
       </c>
       <c r="D55" t="s">
-        <v>245</v>
+        <v>236</v>
       </c>
       <c r="E55" t="s">
-        <v>246</v>
+        <v>237</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
@@ -3809,17 +3809,17 @@
         <f t="shared" si="1"/>
         <v>113</v>
       </c>
-      <c r="B56" t="s">
-        <v>27</v>
+      <c r="B56">
+        <v>4</v>
       </c>
       <c r="C56">
         <v>1</v>
       </c>
       <c r="D56" t="s">
-        <v>247</v>
+        <v>238</v>
       </c>
       <c r="E56" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
@@ -3827,17 +3827,17 @@
         <f t="shared" si="1"/>
         <v>114</v>
       </c>
-      <c r="B57" t="s">
-        <v>27</v>
+      <c r="B57">
+        <v>4</v>
       </c>
       <c r="C57">
         <v>1</v>
       </c>
       <c r="D57" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
       <c r="E57" t="s">
-        <v>249</v>
+        <v>240</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
@@ -3845,17 +3845,17 @@
         <f t="shared" si="1"/>
         <v>115</v>
       </c>
-      <c r="B58" t="s">
-        <v>27</v>
+      <c r="B58">
+        <v>4</v>
       </c>
       <c r="C58">
         <v>1</v>
       </c>
       <c r="D58" t="s">
-        <v>250</v>
+        <v>241</v>
       </c>
       <c r="E58" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
@@ -3863,17 +3863,17 @@
         <f t="shared" si="1"/>
         <v>116</v>
       </c>
-      <c r="B59" t="s">
-        <v>27</v>
+      <c r="B59">
+        <v>4</v>
       </c>
       <c r="C59">
         <v>1</v>
       </c>
       <c r="D59" t="s">
-        <v>251</v>
+        <v>242</v>
       </c>
       <c r="E59" t="s">
-        <v>252</v>
+        <v>243</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
@@ -3881,17 +3881,17 @@
         <f t="shared" si="1"/>
         <v>117</v>
       </c>
-      <c r="B60" t="s">
-        <v>27</v>
+      <c r="B60">
+        <v>4</v>
       </c>
       <c r="C60">
         <v>1</v>
       </c>
       <c r="D60" t="s">
-        <v>253</v>
+        <v>244</v>
       </c>
       <c r="E60" t="s">
-        <v>254</v>
+        <v>245</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
@@ -3899,17 +3899,17 @@
         <f t="shared" si="1"/>
         <v>118</v>
       </c>
-      <c r="B61" t="s">
-        <v>27</v>
+      <c r="B61">
+        <v>4</v>
       </c>
       <c r="C61">
         <v>1</v>
       </c>
       <c r="D61" t="s">
-        <v>255</v>
+        <v>246</v>
       </c>
       <c r="E61" t="s">
-        <v>256</v>
+        <v>247</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
@@ -3917,17 +3917,17 @@
         <f t="shared" si="1"/>
         <v>119</v>
       </c>
-      <c r="B62" t="s">
-        <v>27</v>
+      <c r="B62">
+        <v>4</v>
       </c>
       <c r="C62">
         <v>1</v>
       </c>
       <c r="D62" t="s">
-        <v>257</v>
+        <v>248</v>
       </c>
       <c r="E62" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
@@ -3935,17 +3935,17 @@
         <f t="shared" si="1"/>
         <v>120</v>
       </c>
-      <c r="B63" t="s">
-        <v>27</v>
+      <c r="B63">
+        <v>4</v>
       </c>
       <c r="C63">
         <v>1</v>
       </c>
       <c r="D63" t="s">
-        <v>258</v>
+        <v>249</v>
       </c>
       <c r="E63" t="s">
-        <v>259</v>
+        <v>250</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
@@ -3953,17 +3953,17 @@
         <f t="shared" si="1"/>
         <v>121</v>
       </c>
-      <c r="B64" t="s">
-        <v>27</v>
+      <c r="B64">
+        <v>4</v>
       </c>
       <c r="C64">
         <v>1</v>
       </c>
       <c r="D64" t="s">
-        <v>260</v>
+        <v>251</v>
       </c>
       <c r="E64" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
@@ -3971,17 +3971,17 @@
         <f t="shared" si="1"/>
         <v>122</v>
       </c>
-      <c r="B65" t="s">
-        <v>27</v>
+      <c r="B65">
+        <v>4</v>
       </c>
       <c r="C65">
         <v>1</v>
       </c>
       <c r="D65" t="s">
-        <v>261</v>
+        <v>252</v>
       </c>
       <c r="E65" t="s">
-        <v>262</v>
+        <v>253</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
@@ -3989,17 +3989,17 @@
         <f t="shared" si="1"/>
         <v>123</v>
       </c>
-      <c r="B66" t="s">
-        <v>27</v>
+      <c r="B66">
+        <v>4</v>
       </c>
       <c r="C66">
         <v>1</v>
       </c>
       <c r="D66" t="s">
-        <v>263</v>
+        <v>254</v>
       </c>
       <c r="E66" t="s">
-        <v>264</v>
+        <v>255</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated format of CONTEXT effect column in big cards
</commit_message>
<xml_diff>
--- a/data/TP Database.xlsx
+++ b/data/TP Database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sophiachung/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{57683688-78F8-0F44-A953-641DD8AA5A1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{48AA0B1A-9287-6046-9E1E-D7401F1A0566}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13340" yWindow="500" windowWidth="15460" windowHeight="15880" activeTab="1" xr2:uid="{F6F91125-3C8A-D047-93DD-1F3A6DE88698}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="280">
   <si>
     <t>CardID</t>
   </si>
@@ -428,36 +428,24 @@
     <t>Null</t>
   </si>
   <si>
-    <t>You may search through the PLAN deck and (if possible) add an Ethical clearance tile to your PLAN section</t>
-  </si>
-  <si>
     <t>event-CONTEXT-advicespecialist.png</t>
   </si>
   <si>
     <t>Advice from specialist</t>
   </si>
   <si>
-    <t>You may remove 1 Useless article tile from the CONTEXT section</t>
-  </si>
-  <si>
     <t>event-CONTEXT-bluescreen.png</t>
   </si>
   <si>
     <t>Bluescreen!</t>
   </si>
   <si>
-    <t>Remove any 3 tiles from current section</t>
-  </si>
-  <si>
     <t>event-CONTEXT-distraction.png</t>
   </si>
   <si>
     <t>Distraction!</t>
   </si>
   <si>
-    <t>Remove any 2 tiles from current section. If PLAN contains Milestones only remove 1 tile</t>
-  </si>
-  <si>
     <t>event-CONTEXT-distraction2.png</t>
   </si>
   <si>
@@ -467,36 +455,24 @@
     <t>Tried to do too much?</t>
   </si>
   <si>
-    <t>Remove any 2 tiles from current section</t>
-  </si>
-  <si>
     <t>event-CONTEXT-expertise.png</t>
   </si>
   <si>
     <t>Expertise!</t>
   </si>
   <si>
-    <t>Stand in for an Expertise training PLAN tile</t>
-  </si>
-  <si>
     <t>event-CONTEXT-greatresource.png</t>
   </si>
   <si>
     <t>Great resource!</t>
   </si>
   <si>
-    <t>Search through the IMPLEMENTATION deck and take a Great resources tile. Next round you may play this tile in your IMPLEMENTATION section</t>
-  </si>
-  <si>
     <t>event-CONTEXT-hasmybook.png</t>
   </si>
   <si>
     <t>Someone has my library book!</t>
   </si>
   <si>
-    <t>Remove 1 Relevant or Very relevant article tile from the CONTEXT section</t>
-  </si>
-  <si>
     <t>event-CONTEXT-litreviewparadox.png</t>
   </si>
   <si>
@@ -512,9 +488,6 @@
     <t>Interlibrary loan delay</t>
   </si>
   <si>
-    <t>Remove 1 relevant or Very relevant article tile from the current section</t>
-  </si>
-  <si>
     <t>* typo in this image (aticle)</t>
   </si>
   <si>
@@ -524,18 +497,12 @@
     <t>Lost enthusiasm</t>
   </si>
   <si>
-    <t>Remove any 1 tile from current section</t>
-  </si>
-  <si>
     <t>event-CONTEXT-mentorleaves.png</t>
   </si>
   <si>
     <t>Mentor leaves</t>
   </si>
   <si>
-    <t>Remove all Meetings with supervisor tiles from the PLAN section</t>
-  </si>
-  <si>
     <t>event-CONTEXT-multiperspective.png</t>
   </si>
   <si>
@@ -545,9 +512,6 @@
     <t>CONTEXT contains more than one type of Resource tile (e.g. Lab/Archive)</t>
   </si>
   <si>
-    <t>Ignore the effects of a Tunnel vision card</t>
-  </si>
-  <si>
     <t>event-CONTEXT-procrastinate.png</t>
   </si>
   <si>
@@ -584,9 +548,6 @@
     <t>Evaluation of sources: win!</t>
   </si>
   <si>
-    <t>You may search through the CONTEXT deck and (if possible) add a Very relevant article tile to the current section</t>
-  </si>
-  <si>
     <t>event-CONTEXT-tunnelvision.png</t>
   </si>
   <si>
@@ -861,6 +822,60 @@
   </si>
   <si>
     <t>(11+12):&gt;=1</t>
+  </si>
+  <si>
+    <t>n0:3:2</t>
+  </si>
+  <si>
+    <t>n0:2:2 (If PLAN contains Milestones only remove 1 tile)</t>
+  </si>
+  <si>
+    <t>n0:2:2</t>
+  </si>
+  <si>
+    <t>n0:1:2</t>
+  </si>
+  <si>
+    <t>i(79/101/121):1:(2/3/4)</t>
+  </si>
+  <si>
+    <t>b0:2:(3&amp;4)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">remove one relevant or very relevant article tile </t>
+  </si>
+  <si>
+    <t>ignore effects of a Tunnel vision card at any point</t>
+  </si>
+  <si>
+    <t>use at any point to stand in for an Expertise training PLAN tile</t>
+  </si>
+  <si>
+    <t>s3:1:(2/3/4)</t>
+  </si>
+  <si>
+    <t>p2:1</t>
+  </si>
+  <si>
+    <t>n30:1</t>
+  </si>
+  <si>
+    <t>p41:1</t>
+  </si>
+  <si>
+    <t>n(15/16/31):1</t>
+  </si>
+  <si>
+    <t>n0:1</t>
+  </si>
+  <si>
+    <t>n7:&lt;=9</t>
+  </si>
+  <si>
+    <t>p31:1</t>
+  </si>
+  <si>
+    <t>o0:2:(3&amp;4)</t>
   </si>
 </sst>
 </file>
@@ -890,7 +905,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -898,15 +913,29 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1367,7 +1396,7 @@
         <v>9</v>
       </c>
       <c r="G2" t="s">
-        <v>256</v>
+        <v>243</v>
       </c>
       <c r="H2" t="s">
         <v>36</v>
@@ -1391,7 +1420,7 @@
         <v>44</v>
       </c>
       <c r="G3" t="s">
-        <v>256</v>
+        <v>243</v>
       </c>
       <c r="H3" t="s">
         <v>38</v>
@@ -1415,7 +1444,7 @@
         <v>46</v>
       </c>
       <c r="G4" t="s">
-        <v>256</v>
+        <v>243</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -1436,7 +1465,7 @@
         <v>48</v>
       </c>
       <c r="G5" t="s">
-        <v>256</v>
+        <v>243</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -1457,7 +1486,7 @@
         <v>50</v>
       </c>
       <c r="G6" t="s">
-        <v>256</v>
+        <v>243</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -1478,7 +1507,7 @@
         <v>52</v>
       </c>
       <c r="G7" t="s">
-        <v>256</v>
+        <v>243</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -1499,7 +1528,7 @@
         <v>54</v>
       </c>
       <c r="G8" t="s">
-        <v>256</v>
+        <v>243</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
@@ -1520,7 +1549,7 @@
         <v>12</v>
       </c>
       <c r="G9" t="s">
-        <v>257</v>
+        <v>244</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
@@ -1541,7 +1570,7 @@
         <v>56</v>
       </c>
       <c r="G10" t="s">
-        <v>258</v>
+        <v>245</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
@@ -1562,7 +1591,7 @@
         <v>58</v>
       </c>
       <c r="G11" t="s">
-        <v>259</v>
+        <v>246</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
@@ -1583,7 +1612,7 @@
         <v>60</v>
       </c>
       <c r="G12" t="s">
-        <v>260</v>
+        <v>247</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
@@ -1604,7 +1633,7 @@
         <v>60</v>
       </c>
       <c r="G13" t="s">
-        <v>261</v>
+        <v>248</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
@@ -1625,7 +1654,7 @@
         <v>63</v>
       </c>
       <c r="G14" t="s">
-        <v>258</v>
+        <v>245</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
@@ -1646,7 +1675,7 @@
         <v>65</v>
       </c>
       <c r="G15" t="s">
-        <v>258</v>
+        <v>245</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
@@ -1667,7 +1696,7 @@
         <v>67</v>
       </c>
       <c r="G16" t="s">
-        <v>261</v>
+        <v>248</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
@@ -1688,7 +1717,7 @@
         <v>67</v>
       </c>
       <c r="G17" t="s">
-        <v>260</v>
+        <v>247</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
@@ -1709,7 +1738,7 @@
         <v>70</v>
       </c>
       <c r="G18" t="s">
-        <v>261</v>
+        <v>248</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
@@ -1730,7 +1759,7 @@
         <v>70</v>
       </c>
       <c r="G19" t="s">
-        <v>260</v>
+        <v>247</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
@@ -1751,7 +1780,7 @@
         <v>16</v>
       </c>
       <c r="G20" t="s">
-        <v>261</v>
+        <v>248</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
@@ -1772,7 +1801,7 @@
         <v>16</v>
       </c>
       <c r="G21" t="s">
-        <v>260</v>
+        <v>247</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
@@ -1793,7 +1822,7 @@
         <v>73</v>
       </c>
       <c r="G22" t="s">
-        <v>261</v>
+        <v>248</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
@@ -1814,7 +1843,7 @@
         <v>73</v>
       </c>
       <c r="G23" t="s">
-        <v>260</v>
+        <v>247</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
@@ -1835,7 +1864,7 @@
         <v>76</v>
       </c>
       <c r="G24" t="s">
-        <v>261</v>
+        <v>248</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
@@ -1856,7 +1885,7 @@
         <v>76</v>
       </c>
       <c r="G25" t="s">
-        <v>260</v>
+        <v>247</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
@@ -1877,7 +1906,7 @@
         <v>79</v>
       </c>
       <c r="G26" t="s">
-        <v>261</v>
+        <v>248</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
@@ -1898,7 +1927,7 @@
         <v>79</v>
       </c>
       <c r="G27" t="s">
-        <v>260</v>
+        <v>247</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
@@ -1919,7 +1948,7 @@
         <v>82</v>
       </c>
       <c r="G28" t="s">
-        <v>261</v>
+        <v>248</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
@@ -1940,7 +1969,7 @@
         <v>82</v>
       </c>
       <c r="G29" t="s">
-        <v>260</v>
+        <v>247</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
@@ -1961,7 +1990,7 @@
         <v>85</v>
       </c>
       <c r="G30" t="s">
-        <v>262</v>
+        <v>249</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
@@ -1982,7 +2011,7 @@
         <v>87</v>
       </c>
       <c r="G31" t="s">
-        <v>263</v>
+        <v>250</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
@@ -2003,7 +2032,7 @@
         <v>89</v>
       </c>
       <c r="G32" t="s">
-        <v>258</v>
+        <v>245</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
@@ -2024,7 +2053,7 @@
         <v>91</v>
       </c>
       <c r="G33" t="s">
-        <v>258</v>
+        <v>245</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
@@ -2045,7 +2074,7 @@
         <v>23</v>
       </c>
       <c r="G34" t="s">
-        <v>258</v>
+        <v>245</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
@@ -2066,7 +2095,7 @@
         <v>23</v>
       </c>
       <c r="G35" t="s">
-        <v>259</v>
+        <v>246</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
@@ -2087,7 +2116,7 @@
         <v>23</v>
       </c>
       <c r="G36" t="s">
-        <v>260</v>
+        <v>247</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
@@ -2108,7 +2137,7 @@
         <v>23</v>
       </c>
       <c r="G37" t="s">
-        <v>261</v>
+        <v>248</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
@@ -2129,7 +2158,7 @@
         <v>96</v>
       </c>
       <c r="G38" t="s">
-        <v>258</v>
+        <v>245</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
@@ -2150,7 +2179,7 @@
         <v>96</v>
       </c>
       <c r="G39" t="s">
-        <v>260</v>
+        <v>247</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
@@ -2171,7 +2200,7 @@
         <v>96</v>
       </c>
       <c r="G40" t="s">
-        <v>261</v>
+        <v>248</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
@@ -2192,7 +2221,7 @@
         <v>96</v>
       </c>
       <c r="G41" t="s">
-        <v>259</v>
+        <v>246</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
@@ -2213,7 +2242,7 @@
         <v>101</v>
       </c>
       <c r="G42" t="s">
-        <v>258</v>
+        <v>245</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
@@ -2234,7 +2263,7 @@
         <v>26</v>
       </c>
       <c r="G43" t="s">
-        <v>258</v>
+        <v>245</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
@@ -2255,7 +2284,7 @@
         <v>103</v>
       </c>
       <c r="G44" t="s">
-        <v>260</v>
+        <v>247</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
@@ -2276,7 +2305,7 @@
         <v>103</v>
       </c>
       <c r="G45" t="s">
-        <v>261</v>
+        <v>248</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
@@ -2297,7 +2326,7 @@
         <v>106</v>
       </c>
       <c r="G46" t="s">
-        <v>261</v>
+        <v>248</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
@@ -2318,7 +2347,7 @@
         <v>106</v>
       </c>
       <c r="G47" t="s">
-        <v>260</v>
+        <v>247</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
@@ -2339,7 +2368,7 @@
         <v>109</v>
       </c>
       <c r="G48" t="s">
-        <v>264</v>
+        <v>251</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
@@ -2360,7 +2389,7 @@
         <v>109</v>
       </c>
       <c r="G49" t="s">
-        <v>265</v>
+        <v>252</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
@@ -2381,7 +2410,7 @@
         <v>112</v>
       </c>
       <c r="G50" t="s">
-        <v>259</v>
+        <v>246</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
@@ -2402,7 +2431,7 @@
         <v>32</v>
       </c>
       <c r="G51" t="s">
-        <v>259</v>
+        <v>246</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.2">
@@ -2423,7 +2452,7 @@
         <v>32</v>
       </c>
       <c r="G52" t="s">
-        <v>264</v>
+        <v>251</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
@@ -2444,7 +2473,7 @@
         <v>32</v>
       </c>
       <c r="G53" t="s">
-        <v>265</v>
+        <v>252</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.2">
@@ -2465,7 +2494,7 @@
         <v>116</v>
       </c>
       <c r="G54" t="s">
-        <v>259</v>
+        <v>246</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.2">
@@ -2486,7 +2515,7 @@
         <v>29</v>
       </c>
       <c r="G55" t="s">
-        <v>264</v>
+        <v>251</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.2">
@@ -2507,7 +2536,7 @@
         <v>29</v>
       </c>
       <c r="G56" t="s">
-        <v>265</v>
+        <v>252</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.2">
@@ -2528,7 +2557,7 @@
         <v>119</v>
       </c>
       <c r="G57" t="s">
-        <v>259</v>
+        <v>246</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.2">
@@ -2549,7 +2578,7 @@
         <v>121</v>
       </c>
       <c r="G58" t="s">
-        <v>259</v>
+        <v>246</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.2">
@@ -2570,7 +2599,7 @@
         <v>123</v>
       </c>
       <c r="G59" t="s">
-        <v>259</v>
+        <v>246</v>
       </c>
     </row>
   </sheetData>
@@ -2585,8 +2614,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84DC5E79-A11F-0148-B3A8-F5384824D987}">
   <dimension ref="A1:J66"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="99" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="99" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2599,7 +2628,7 @@
     <col min="6" max="6" width="14" customWidth="1"/>
     <col min="7" max="7" width="17" customWidth="1"/>
     <col min="8" max="8" width="15.83203125" customWidth="1"/>
-    <col min="9" max="9" width="88.5" customWidth="1"/>
+    <col min="9" max="9" width="45.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
@@ -2655,7 +2684,7 @@
         <v>129</v>
       </c>
       <c r="I2" t="s">
-        <v>130</v>
+        <v>272</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
@@ -2670,10 +2699,10 @@
         <v>1</v>
       </c>
       <c r="D3" t="s">
+        <v>130</v>
+      </c>
+      <c r="E3" t="s">
         <v>131</v>
-      </c>
-      <c r="E3" t="s">
-        <v>132</v>
       </c>
       <c r="G3" t="s">
         <v>129</v>
@@ -2682,7 +2711,7 @@
         <v>129</v>
       </c>
       <c r="I3" t="s">
-        <v>133</v>
+        <v>273</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
@@ -2697,19 +2726,19 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E4" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="G4" t="s">
         <v>129</v>
       </c>
       <c r="H4" t="s">
-        <v>266</v>
+        <v>253</v>
       </c>
       <c r="I4" t="s">
-        <v>136</v>
+        <v>262</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
@@ -2724,10 +2753,10 @@
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="E5" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="G5" t="s">
         <v>129</v>
@@ -2736,7 +2765,7 @@
         <v>129</v>
       </c>
       <c r="I5" t="s">
-        <v>139</v>
+        <v>263</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
@@ -2751,10 +2780,10 @@
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="E6" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="G6" t="s">
         <v>129</v>
@@ -2763,7 +2792,7 @@
         <v>129</v>
       </c>
       <c r="I6" t="s">
-        <v>139</v>
+        <v>263</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
@@ -2778,19 +2807,19 @@
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="E7" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="G7" t="s">
         <v>129</v>
       </c>
       <c r="H7" t="s">
-        <v>267</v>
+        <v>254</v>
       </c>
       <c r="I7" t="s">
-        <v>143</v>
+        <v>264</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
@@ -2805,19 +2834,22 @@
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="E8" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="G8" t="s">
-        <v>274</v>
+        <v>261</v>
       </c>
       <c r="H8" t="s">
         <v>129</v>
       </c>
       <c r="I8" t="s">
-        <v>146</v>
+        <v>271</v>
+      </c>
+      <c r="J8" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
@@ -2832,10 +2864,10 @@
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="E9" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="G9" t="s">
         <v>129</v>
@@ -2844,7 +2876,7 @@
         <v>129</v>
       </c>
       <c r="I9" t="s">
-        <v>149</v>
+        <v>274</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
@@ -2859,19 +2891,22 @@
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="E10" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="G10" t="s">
         <v>129</v>
       </c>
       <c r="H10" t="s">
+        <v>255</v>
+      </c>
+      <c r="I10" t="s">
+        <v>275</v>
+      </c>
+      <c r="J10" t="s">
         <v>268</v>
-      </c>
-      <c r="I10" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
@@ -2886,19 +2921,22 @@
         <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="E11" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="G11" t="s">
         <v>129</v>
       </c>
       <c r="H11" t="s">
-        <v>272</v>
+        <v>259</v>
       </c>
       <c r="I11" t="s">
-        <v>155</v>
+        <v>279</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
@@ -2913,22 +2951,22 @@
         <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="E12" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="G12" t="s">
         <v>129</v>
       </c>
       <c r="H12" t="s">
-        <v>268</v>
+        <v>255</v>
       </c>
       <c r="I12" t="s">
-        <v>158</v>
+        <v>275</v>
       </c>
       <c r="J12" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
@@ -2943,19 +2981,19 @@
         <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="E13" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="G13" t="s">
         <v>129</v>
       </c>
       <c r="H13" t="s">
-        <v>269</v>
+        <v>256</v>
       </c>
       <c r="I13" t="s">
-        <v>162</v>
+        <v>276</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
@@ -2970,10 +3008,10 @@
         <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="E14" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="G14" t="s">
         <v>129</v>
@@ -2982,7 +3020,7 @@
         <v>129</v>
       </c>
       <c r="I14" t="s">
-        <v>165</v>
+        <v>277</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
@@ -2997,19 +3035,22 @@
         <v>1</v>
       </c>
       <c r="D15" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
       <c r="E15" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="G15" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
       <c r="H15" t="s">
         <v>129</v>
       </c>
       <c r="I15" t="s">
-        <v>169</v>
+        <v>266</v>
+      </c>
+      <c r="J15" t="s">
+        <v>269</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
@@ -3024,19 +3065,19 @@
         <v>1</v>
       </c>
       <c r="D16" t="s">
-        <v>170</v>
+        <v>158</v>
       </c>
       <c r="E16" t="s">
-        <v>171</v>
+        <v>159</v>
       </c>
       <c r="G16" t="s">
         <v>129</v>
       </c>
       <c r="H16" t="s">
-        <v>270</v>
+        <v>257</v>
       </c>
       <c r="I16" t="s">
-        <v>136</v>
+        <v>262</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
@@ -3051,19 +3092,19 @@
         <v>1</v>
       </c>
       <c r="D17" t="s">
-        <v>172</v>
+        <v>160</v>
       </c>
       <c r="E17" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
       <c r="G17" t="s">
         <v>129</v>
       </c>
       <c r="H17" t="s">
-        <v>268</v>
+        <v>255</v>
       </c>
       <c r="I17" t="s">
-        <v>155</v>
+        <v>267</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
@@ -3078,19 +3119,19 @@
         <v>1</v>
       </c>
       <c r="D18" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
       <c r="E18" t="s">
-        <v>175</v>
+        <v>163</v>
       </c>
       <c r="G18" t="s">
         <v>129</v>
       </c>
       <c r="H18" t="s">
-        <v>268</v>
+        <v>255</v>
       </c>
       <c r="I18" t="s">
-        <v>143</v>
+        <v>264</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
@@ -3105,19 +3146,19 @@
         <v>1</v>
       </c>
       <c r="D19" t="s">
-        <v>176</v>
+        <v>164</v>
       </c>
       <c r="E19" t="s">
-        <v>177</v>
+        <v>165</v>
       </c>
       <c r="G19" t="s">
         <v>129</v>
       </c>
       <c r="H19" t="s">
-        <v>268</v>
+        <v>255</v>
       </c>
       <c r="I19" t="s">
-        <v>162</v>
+        <v>265</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
@@ -3132,10 +3173,10 @@
         <v>1</v>
       </c>
       <c r="D20" t="s">
-        <v>178</v>
+        <v>166</v>
       </c>
       <c r="E20" t="s">
-        <v>179</v>
+        <v>167</v>
       </c>
       <c r="G20" t="s">
         <v>129</v>
@@ -3144,7 +3185,7 @@
         <v>129</v>
       </c>
       <c r="I20" t="s">
-        <v>143</v>
+        <v>264</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
@@ -3159,10 +3200,10 @@
         <v>1</v>
       </c>
       <c r="D21" t="s">
-        <v>180</v>
+        <v>168</v>
       </c>
       <c r="E21" t="s">
-        <v>181</v>
+        <v>169</v>
       </c>
       <c r="G21" t="s">
         <v>129</v>
@@ -3171,7 +3212,7 @@
         <v>129</v>
       </c>
       <c r="I21" t="s">
-        <v>182</v>
+        <v>278</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
@@ -3186,19 +3227,19 @@
         <v>1</v>
       </c>
       <c r="D22" t="s">
-        <v>183</v>
+        <v>170</v>
       </c>
       <c r="E22" t="s">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="G22" t="s">
         <v>129</v>
       </c>
       <c r="H22" t="s">
-        <v>271</v>
+        <v>258</v>
       </c>
       <c r="I22" t="s">
-        <v>162</v>
+        <v>265</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
@@ -3213,19 +3254,19 @@
         <v>1</v>
       </c>
       <c r="D23" t="s">
-        <v>185</v>
+        <v>172</v>
       </c>
       <c r="E23" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
       <c r="G23" t="s">
         <v>129</v>
       </c>
       <c r="H23" t="s">
-        <v>273</v>
+        <v>260</v>
       </c>
       <c r="I23" t="s">
-        <v>155</v>
+        <v>279</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
@@ -3240,10 +3281,10 @@
         <v>1</v>
       </c>
       <c r="D24" t="s">
-        <v>187</v>
+        <v>174</v>
       </c>
       <c r="E24" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
@@ -3258,10 +3299,10 @@
         <v>1</v>
       </c>
       <c r="D25" t="s">
-        <v>188</v>
+        <v>175</v>
       </c>
       <c r="E25" t="s">
-        <v>189</v>
+        <v>176</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
@@ -3276,10 +3317,10 @@
         <v>1</v>
       </c>
       <c r="D26" t="s">
-        <v>190</v>
+        <v>177</v>
       </c>
       <c r="E26" t="s">
-        <v>191</v>
+        <v>178</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
@@ -3294,10 +3335,10 @@
         <v>1</v>
       </c>
       <c r="D27" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="E27" t="s">
-        <v>193</v>
+        <v>180</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
@@ -3312,10 +3353,10 @@
         <v>1</v>
       </c>
       <c r="D28" t="s">
-        <v>194</v>
+        <v>181</v>
       </c>
       <c r="E28" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
@@ -3330,10 +3371,10 @@
         <v>1</v>
       </c>
       <c r="D29" t="s">
-        <v>195</v>
+        <v>182</v>
       </c>
       <c r="E29" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
@@ -3348,10 +3389,10 @@
         <v>1</v>
       </c>
       <c r="D30" t="s">
-        <v>196</v>
+        <v>183</v>
       </c>
       <c r="E30" t="s">
-        <v>197</v>
+        <v>184</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
@@ -3366,10 +3407,10 @@
         <v>1</v>
       </c>
       <c r="D31" t="s">
-        <v>198</v>
+        <v>185</v>
       </c>
       <c r="E31" t="s">
-        <v>199</v>
+        <v>186</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
@@ -3384,10 +3425,10 @@
         <v>1</v>
       </c>
       <c r="D32" t="s">
-        <v>200</v>
+        <v>187</v>
       </c>
       <c r="E32" t="s">
-        <v>201</v>
+        <v>188</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
@@ -3402,10 +3443,10 @@
         <v>1</v>
       </c>
       <c r="D33" t="s">
-        <v>202</v>
+        <v>189</v>
       </c>
       <c r="E33" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
@@ -3420,10 +3461,10 @@
         <v>1</v>
       </c>
       <c r="D34" t="s">
-        <v>203</v>
+        <v>190</v>
       </c>
       <c r="E34" t="s">
-        <v>204</v>
+        <v>191</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
@@ -3438,10 +3479,10 @@
         <v>1</v>
       </c>
       <c r="D35" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
       <c r="E35" t="s">
-        <v>206</v>
+        <v>193</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
@@ -3456,10 +3497,10 @@
         <v>1</v>
       </c>
       <c r="D36" t="s">
-        <v>207</v>
+        <v>194</v>
       </c>
       <c r="E36" t="s">
-        <v>171</v>
+        <v>159</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
@@ -3474,10 +3515,10 @@
         <v>1</v>
       </c>
       <c r="D37" t="s">
-        <v>208</v>
+        <v>195</v>
       </c>
       <c r="E37" t="s">
-        <v>209</v>
+        <v>196</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
@@ -3492,10 +3533,10 @@
         <v>1</v>
       </c>
       <c r="D38" t="s">
-        <v>210</v>
+        <v>197</v>
       </c>
       <c r="E38" t="s">
-        <v>211</v>
+        <v>198</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
@@ -3510,10 +3551,10 @@
         <v>1</v>
       </c>
       <c r="D39" t="s">
-        <v>212</v>
+        <v>199</v>
       </c>
       <c r="E39" t="s">
-        <v>175</v>
+        <v>163</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
@@ -3528,10 +3569,10 @@
         <v>1</v>
       </c>
       <c r="D40" t="s">
-        <v>213</v>
+        <v>200</v>
       </c>
       <c r="E40" t="s">
-        <v>177</v>
+        <v>165</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
@@ -3546,10 +3587,10 @@
         <v>1</v>
       </c>
       <c r="D41" t="s">
-        <v>214</v>
+        <v>201</v>
       </c>
       <c r="E41" t="s">
-        <v>215</v>
+        <v>202</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
@@ -3564,10 +3605,10 @@
         <v>1</v>
       </c>
       <c r="D42" t="s">
-        <v>216</v>
+        <v>203</v>
       </c>
       <c r="E42" t="s">
-        <v>217</v>
+        <v>204</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
@@ -3582,10 +3623,10 @@
         <v>1</v>
       </c>
       <c r="D43" t="s">
-        <v>218</v>
+        <v>205</v>
       </c>
       <c r="E43" t="s">
-        <v>219</v>
+        <v>206</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
@@ -3600,10 +3641,10 @@
         <v>1</v>
       </c>
       <c r="D44" t="s">
-        <v>220</v>
+        <v>207</v>
       </c>
       <c r="E44" t="s">
-        <v>184</v>
+        <v>171</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
@@ -3618,10 +3659,10 @@
         <v>1</v>
       </c>
       <c r="D45" t="s">
-        <v>221</v>
+        <v>208</v>
       </c>
       <c r="E45" t="s">
-        <v>222</v>
+        <v>209</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
@@ -3636,10 +3677,10 @@
         <v>1</v>
       </c>
       <c r="D46" t="s">
-        <v>223</v>
+        <v>210</v>
       </c>
       <c r="E46" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
@@ -3654,10 +3695,10 @@
         <v>1</v>
       </c>
       <c r="D47" t="s">
-        <v>224</v>
+        <v>211</v>
       </c>
       <c r="E47" t="s">
-        <v>225</v>
+        <v>212</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
@@ -3672,10 +3713,10 @@
         <v>1</v>
       </c>
       <c r="D48" t="s">
-        <v>226</v>
+        <v>213</v>
       </c>
       <c r="E48" t="s">
-        <v>227</v>
+        <v>214</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
@@ -3690,10 +3731,10 @@
         <v>1</v>
       </c>
       <c r="D49" t="s">
-        <v>228</v>
+        <v>215</v>
       </c>
       <c r="E49" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
@@ -3708,10 +3749,10 @@
         <v>1</v>
       </c>
       <c r="D50" t="s">
-        <v>229</v>
+        <v>216</v>
       </c>
       <c r="E50" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
@@ -3726,10 +3767,10 @@
         <v>1</v>
       </c>
       <c r="D51" t="s">
-        <v>230</v>
+        <v>217</v>
       </c>
       <c r="E51" t="s">
-        <v>231</v>
+        <v>218</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
@@ -3744,10 +3785,10 @@
         <v>1</v>
       </c>
       <c r="D52" t="s">
-        <v>232</v>
+        <v>219</v>
       </c>
       <c r="E52" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
@@ -3762,10 +3803,10 @@
         <v>1</v>
       </c>
       <c r="D53" t="s">
-        <v>233</v>
+        <v>220</v>
       </c>
       <c r="E53" t="s">
-        <v>197</v>
+        <v>184</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
@@ -3780,10 +3821,10 @@
         <v>1</v>
       </c>
       <c r="D54" t="s">
-        <v>234</v>
+        <v>221</v>
       </c>
       <c r="E54" t="s">
-        <v>235</v>
+        <v>222</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
@@ -3798,10 +3839,10 @@
         <v>1</v>
       </c>
       <c r="D55" t="s">
-        <v>236</v>
+        <v>223</v>
       </c>
       <c r="E55" t="s">
-        <v>237</v>
+        <v>224</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
@@ -3816,10 +3857,10 @@
         <v>1</v>
       </c>
       <c r="D56" t="s">
-        <v>238</v>
+        <v>225</v>
       </c>
       <c r="E56" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
@@ -3834,10 +3875,10 @@
         <v>1</v>
       </c>
       <c r="D57" t="s">
-        <v>239</v>
+        <v>226</v>
       </c>
       <c r="E57" t="s">
-        <v>240</v>
+        <v>227</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
@@ -3852,10 +3893,10 @@
         <v>1</v>
       </c>
       <c r="D58" t="s">
-        <v>241</v>
+        <v>228</v>
       </c>
       <c r="E58" t="s">
-        <v>171</v>
+        <v>159</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
@@ -3870,10 +3911,10 @@
         <v>1</v>
       </c>
       <c r="D59" t="s">
-        <v>242</v>
+        <v>229</v>
       </c>
       <c r="E59" t="s">
-        <v>243</v>
+        <v>230</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
@@ -3888,10 +3929,10 @@
         <v>1</v>
       </c>
       <c r="D60" t="s">
-        <v>244</v>
+        <v>231</v>
       </c>
       <c r="E60" t="s">
-        <v>245</v>
+        <v>232</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
@@ -3906,10 +3947,10 @@
         <v>1</v>
       </c>
       <c r="D61" t="s">
-        <v>246</v>
+        <v>233</v>
       </c>
       <c r="E61" t="s">
-        <v>247</v>
+        <v>234</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
@@ -3924,10 +3965,10 @@
         <v>1</v>
       </c>
       <c r="D62" t="s">
-        <v>248</v>
+        <v>235</v>
       </c>
       <c r="E62" t="s">
-        <v>175</v>
+        <v>163</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
@@ -3942,10 +3983,10 @@
         <v>1</v>
       </c>
       <c r="D63" t="s">
-        <v>249</v>
+        <v>236</v>
       </c>
       <c r="E63" t="s">
-        <v>250</v>
+        <v>237</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
@@ -3960,10 +4001,10 @@
         <v>1</v>
       </c>
       <c r="D64" t="s">
-        <v>251</v>
+        <v>238</v>
       </c>
       <c r="E64" t="s">
-        <v>184</v>
+        <v>171</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
@@ -3978,10 +4019,10 @@
         <v>1</v>
       </c>
       <c r="D65" t="s">
-        <v>252</v>
+        <v>239</v>
       </c>
       <c r="E65" t="s">
-        <v>253</v>
+        <v>240</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
@@ -3996,10 +4037,10 @@
         <v>1</v>
       </c>
       <c r="D66" t="s">
-        <v>254</v>
+        <v>241</v>
       </c>
       <c r="E66" t="s">
-        <v>255</v>
+        <v>242</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Issue #70 - Put activities card data into database
- Changed the id in the Big Cards table in `TP Database.xlsx` to begin 
at 1
- Converted the Big Cards table in the `TP Database.xlsx` file to 
`Events.csv`
- Changed id fields in both tables to **not** be autoincrementing, since 
the number of entries will never change, and it will ensure that 
referencing the IDs will always be consistent if for whatever reason the 
order the cards are added changes.
- Deleted the number field in the Events table and in Big Cards table in 
`TP Database.xlsx` because all the cards only appear once
- Added code to insert data from `Events.csv` into `Cards.db` in 
`card_database_setup.py`
- Updated README.md in the `data` folder to show the new fields in 
Cards.db

Closed [Issue 
#70](https://stgit.dcs.gla.ac.uk/team-project-h/2021/cs01/cs01-main/-/issues/70)
</commit_message>
<xml_diff>
--- a/data/TP Database.xlsx
+++ b/data/TP Database.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sophiachung/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_My Files\_Uni\Year 3\Term 1\3 - Team Project\_TP Code\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{48AA0B1A-9287-6046-9E1E-D7401F1A0566}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A694393-3198-423B-AD9D-079C58C70633}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13340" yWindow="500" windowWidth="15460" windowHeight="15880" activeTab="1" xr2:uid="{F6F91125-3C8A-D047-93DD-1F3A6DE88698}"/>
+    <workbookView xWindow="28680" yWindow="-1290" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{F6F91125-3C8A-D047-93DD-1F3A6DE88698}"/>
   </bookViews>
   <sheets>
     <sheet name="Small Cards" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="281">
   <si>
     <t>CardID</t>
   </si>
@@ -876,6 +876,9 @@
   </si>
   <si>
     <t>o0:2:(3&amp;4)</t>
+  </si>
+  <si>
+    <t>Column1</t>
   </si>
 </sst>
 </file>
@@ -989,16 +992,16 @@
   <autoFilter ref="A1:I66" xr:uid="{4E25BA7D-C944-7B48-8D11-C2260663E6FE}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{241E3EFA-1556-A24B-8441-368F09FD400E}" name="CardID" dataDxfId="2">
-      <calculatedColumnFormula>ROW() + 57</calculatedColumnFormula>
+      <calculatedColumnFormula>ROW() - 1</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="2" xr3:uid="{4CB802A7-5A14-1843-8D85-057515A93530}" name="Stage"/>
-    <tableColumn id="3" xr3:uid="{45AAD7C9-BD08-B241-A106-B2FFC2B22B18}" name="Number"/>
-    <tableColumn id="8" xr3:uid="{98D9D00E-0FDA-C645-9758-69E917F00870}" name="Filename"/>
-    <tableColumn id="4" xr3:uid="{1F7BF006-71BD-D542-96ED-747B93E53C9C}" name="Title"/>
-    <tableColumn id="5" xr3:uid="{5BD78171-150E-AB4C-80DC-D8A061F5BF5E}" name="Description"/>
-    <tableColumn id="9" xr3:uid="{318B7552-B230-384E-9C27-A0F990859B0F}" name="Save_condition"/>
-    <tableColumn id="6" xr3:uid="{FCFA78C0-6299-A941-AD36-DE9122010D1F}" name="Requirement"/>
-    <tableColumn id="7" xr3:uid="{6E4CEF28-DC4C-D54A-9279-428FA0FAB941}" name="Effect"/>
+    <tableColumn id="3" xr3:uid="{45AAD7C9-BD08-B241-A106-B2FFC2B22B18}" name="Filename"/>
+    <tableColumn id="8" xr3:uid="{98D9D00E-0FDA-C645-9758-69E917F00870}" name="Title"/>
+    <tableColumn id="4" xr3:uid="{1F7BF006-71BD-D542-96ED-747B93E53C9C}" name="Description"/>
+    <tableColumn id="5" xr3:uid="{5BD78171-150E-AB4C-80DC-D8A061F5BF5E}" name="Save_condition"/>
+    <tableColumn id="9" xr3:uid="{318B7552-B230-384E-9C27-A0F990859B0F}" name="Requirement"/>
+    <tableColumn id="6" xr3:uid="{FCFA78C0-6299-A941-AD36-DE9122010D1F}" name="Effect"/>
+    <tableColumn id="7" xr3:uid="{6E4CEF28-DC4C-D54A-9279-428FA0FAB941}" name="Column1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1338,21 +1341,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18AE550B-A04F-B142-B067-7E2D879988FA}">
   <dimension ref="A1:H59"/>
   <sheetViews>
-    <sheetView topLeftCell="A39" zoomScale="102" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView zoomScale="102" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H41" sqref="H41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.6640625" customWidth="1"/>
-    <col min="2" max="2" width="15.1640625" customWidth="1"/>
-    <col min="3" max="3" width="10.33203125" customWidth="1"/>
-    <col min="4" max="4" width="25.1640625" customWidth="1"/>
+    <col min="1" max="1" width="9.625" customWidth="1"/>
+    <col min="2" max="2" width="15.125" customWidth="1"/>
+    <col min="3" max="3" width="10.375" customWidth="1"/>
+    <col min="4" max="4" width="25.125" customWidth="1"/>
     <col min="5" max="6" width="17.5" customWidth="1"/>
     <col min="7" max="7" width="9.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1378,7 +1381,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <f t="shared" ref="A2:A33" si="0">ROW() - 1</f>
         <v>1</v>
@@ -1402,7 +1405,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -1426,7 +1429,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -1447,7 +1450,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1468,7 +1471,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1489,7 +1492,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1510,7 +1513,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1531,7 +1534,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1552,7 +1555,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1573,7 +1576,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1594,7 +1597,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1615,7 +1618,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1636,7 +1639,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1657,7 +1660,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1678,7 +1681,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1699,7 +1702,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1720,7 +1723,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1741,7 +1744,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -1762,7 +1765,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -1783,7 +1786,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -1804,7 +1807,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -1825,7 +1828,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -1846,7 +1849,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -1867,7 +1870,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -1888,7 +1891,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -1909,7 +1912,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -1930,7 +1933,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -1951,7 +1954,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -1972,7 +1975,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -1993,7 +1996,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -2014,7 +2017,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -2035,7 +2038,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -2056,7 +2059,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34">
         <f t="shared" ref="A34:A59" si="1">ROW() - 1</f>
         <v>33</v>
@@ -2077,7 +2080,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35">
         <f t="shared" si="1"/>
         <v>34</v>
@@ -2098,7 +2101,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36">
         <f t="shared" si="1"/>
         <v>35</v>
@@ -2119,7 +2122,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37">
         <f t="shared" si="1"/>
         <v>36</v>
@@ -2140,7 +2143,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38">
         <f t="shared" si="1"/>
         <v>37</v>
@@ -2161,7 +2164,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39">
         <f t="shared" si="1"/>
         <v>38</v>
@@ -2182,7 +2185,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40">
         <f t="shared" si="1"/>
         <v>39</v>
@@ -2203,7 +2206,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41">
         <f t="shared" si="1"/>
         <v>40</v>
@@ -2224,7 +2227,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42">
         <f t="shared" si="1"/>
         <v>41</v>
@@ -2245,7 +2248,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43">
         <f t="shared" si="1"/>
         <v>42</v>
@@ -2266,7 +2269,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44">
         <f t="shared" si="1"/>
         <v>43</v>
@@ -2287,7 +2290,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45">
         <f t="shared" si="1"/>
         <v>44</v>
@@ -2308,7 +2311,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46">
         <f t="shared" si="1"/>
         <v>45</v>
@@ -2329,7 +2332,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47">
         <f t="shared" si="1"/>
         <v>46</v>
@@ -2350,7 +2353,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48">
         <f t="shared" si="1"/>
         <v>47</v>
@@ -2371,7 +2374,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49">
         <f t="shared" si="1"/>
         <v>48</v>
@@ -2392,7 +2395,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50">
         <f t="shared" si="1"/>
         <v>49</v>
@@ -2413,7 +2416,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51">
         <f t="shared" si="1"/>
         <v>50</v>
@@ -2434,7 +2437,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52">
         <f t="shared" si="1"/>
         <v>51</v>
@@ -2455,7 +2458,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53">
         <f t="shared" si="1"/>
         <v>52</v>
@@ -2476,7 +2479,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54">
         <f t="shared" si="1"/>
         <v>53</v>
@@ -2497,7 +2500,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55">
         <f t="shared" si="1"/>
         <v>54</v>
@@ -2518,7 +2521,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56">
         <f t="shared" si="1"/>
         <v>55</v>
@@ -2539,7 +2542,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57">
         <f t="shared" si="1"/>
         <v>56</v>
@@ -2560,7 +2563,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58">
         <f t="shared" si="1"/>
         <v>57</v>
@@ -2581,7 +2584,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59">
         <f t="shared" si="1"/>
         <v>58</v>
@@ -2612,26 +2615,26 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84DC5E79-A11F-0148-B3A8-F5384824D987}">
-  <dimension ref="A1:J66"/>
+  <dimension ref="A1:I66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="99" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" zoomScale="99" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.1640625" customWidth="1"/>
+    <col min="1" max="1" width="9.125" customWidth="1"/>
     <col min="2" max="2" width="9.5" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" customWidth="1"/>
-    <col min="4" max="4" width="25.83203125" customWidth="1"/>
-    <col min="5" max="5" width="26" customWidth="1"/>
+    <col min="3" max="3" width="33" customWidth="1"/>
+    <col min="4" max="4" width="25.875" customWidth="1"/>
+    <col min="5" max="5" width="12.125" customWidth="1"/>
     <col min="6" max="6" width="14" customWidth="1"/>
     <col min="7" max="7" width="17" customWidth="1"/>
-    <col min="8" max="8" width="15.83203125" customWidth="1"/>
-    <col min="9" max="9" width="45.83203125" customWidth="1"/>
+    <col min="8" max="8" width="52.125" customWidth="1"/>
+    <col min="9" max="9" width="45.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2639,1407 +2642,1212 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F1" t="s">
-        <v>5</v>
+        <v>124</v>
       </c>
       <c r="G1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="H1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="I1" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
-        <f t="shared" ref="A2:A33" si="0">ROW() + 57</f>
-        <v>59</v>
+        <f t="shared" ref="A2:A33" si="0">ROW() - 1</f>
+        <v>1</v>
       </c>
       <c r="B2">
         <v>2</v>
       </c>
-      <c r="C2">
-        <v>1</v>
+      <c r="C2" t="s">
+        <v>127</v>
       </c>
       <c r="D2" t="s">
-        <v>127</v>
-      </c>
-      <c r="E2" t="s">
         <v>128</v>
+      </c>
+      <c r="F2" t="s">
+        <v>129</v>
       </c>
       <c r="G2" t="s">
         <v>129</v>
       </c>
       <c r="H2" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>130</v>
+      </c>
+      <c r="D3" t="s">
+        <v>131</v>
+      </c>
+      <c r="F3" t="s">
         <v>129</v>
-      </c>
-      <c r="I2" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <f t="shared" si="0"/>
-        <v>60</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3" t="s">
-        <v>130</v>
-      </c>
-      <c r="E3" t="s">
-        <v>131</v>
       </c>
       <c r="G3" t="s">
         <v>129</v>
       </c>
       <c r="H3" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>132</v>
+      </c>
+      <c r="D4" t="s">
+        <v>133</v>
+      </c>
+      <c r="F4" t="s">
         <v>129</v>
       </c>
-      <c r="I3" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <f t="shared" si="0"/>
-        <v>61</v>
-      </c>
-      <c r="B4">
-        <v>2</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4" t="s">
-        <v>132</v>
-      </c>
-      <c r="E4" t="s">
-        <v>133</v>
-      </c>
       <c r="G4" t="s">
+        <v>253</v>
+      </c>
+      <c r="H4" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>134</v>
+      </c>
+      <c r="D5" t="s">
+        <v>135</v>
+      </c>
+      <c r="F5" t="s">
         <v>129</v>
-      </c>
-      <c r="H4" t="s">
-        <v>253</v>
-      </c>
-      <c r="I4" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <f t="shared" si="0"/>
-        <v>62</v>
-      </c>
-      <c r="B5">
-        <v>2</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5" t="s">
-        <v>134</v>
-      </c>
-      <c r="E5" t="s">
-        <v>135</v>
       </c>
       <c r="G5" t="s">
         <v>129</v>
       </c>
       <c r="H5" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>136</v>
+      </c>
+      <c r="D6" t="s">
+        <v>135</v>
+      </c>
+      <c r="F6" t="s">
         <v>129</v>
-      </c>
-      <c r="I5" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <f t="shared" si="0"/>
-        <v>63</v>
-      </c>
-      <c r="B6">
-        <v>2</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="D6" t="s">
-        <v>136</v>
-      </c>
-      <c r="E6" t="s">
-        <v>135</v>
       </c>
       <c r="G6" t="s">
         <v>129</v>
       </c>
       <c r="H6" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>137</v>
+      </c>
+      <c r="D7" t="s">
+        <v>138</v>
+      </c>
+      <c r="F7" t="s">
         <v>129</v>
       </c>
-      <c r="I6" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <f t="shared" si="0"/>
-        <v>64</v>
-      </c>
-      <c r="B7">
-        <v>2</v>
-      </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7" t="s">
-        <v>137</v>
-      </c>
-      <c r="E7" t="s">
-        <v>138</v>
-      </c>
       <c r="G7" t="s">
+        <v>254</v>
+      </c>
+      <c r="H7" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8" t="s">
+        <v>139</v>
+      </c>
+      <c r="D8" t="s">
+        <v>140</v>
+      </c>
+      <c r="F8" t="s">
+        <v>261</v>
+      </c>
+      <c r="G8" t="s">
         <v>129</v>
       </c>
-      <c r="H7" t="s">
-        <v>254</v>
-      </c>
-      <c r="I7" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <f t="shared" si="0"/>
-        <v>65</v>
-      </c>
-      <c r="B8">
-        <v>2</v>
-      </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-      <c r="D8" t="s">
-        <v>139</v>
-      </c>
-      <c r="E8" t="s">
-        <v>140</v>
-      </c>
-      <c r="G8" t="s">
-        <v>261</v>
-      </c>
       <c r="H8" t="s">
+        <v>271</v>
+      </c>
+      <c r="I8" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9" t="s">
+        <v>141</v>
+      </c>
+      <c r="D9" t="s">
+        <v>142</v>
+      </c>
+      <c r="F9" t="s">
         <v>129</v>
-      </c>
-      <c r="I8" t="s">
-        <v>271</v>
-      </c>
-      <c r="J8" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <f t="shared" si="0"/>
-        <v>66</v>
-      </c>
-      <c r="B9">
-        <v>2</v>
-      </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="D9" t="s">
-        <v>141</v>
-      </c>
-      <c r="E9" t="s">
-        <v>142</v>
       </c>
       <c r="G9" t="s">
         <v>129</v>
       </c>
       <c r="H9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10" t="s">
+        <v>143</v>
+      </c>
+      <c r="D10" t="s">
+        <v>144</v>
+      </c>
+      <c r="F10" t="s">
         <v>129</v>
       </c>
-      <c r="I9" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <f t="shared" si="0"/>
-        <v>67</v>
-      </c>
-      <c r="B10">
-        <v>2</v>
-      </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="D10" t="s">
-        <v>143</v>
-      </c>
-      <c r="E10" t="s">
-        <v>144</v>
-      </c>
       <c r="G10" t="s">
+        <v>255</v>
+      </c>
+      <c r="H10" t="s">
+        <v>275</v>
+      </c>
+      <c r="I10" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11" t="s">
+        <v>145</v>
+      </c>
+      <c r="D11" t="s">
+        <v>146</v>
+      </c>
+      <c r="F11" t="s">
         <v>129</v>
       </c>
-      <c r="H10" t="s">
+      <c r="G11" t="s">
+        <v>259</v>
+      </c>
+      <c r="H11" t="s">
+        <v>279</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12" t="s">
+        <v>148</v>
+      </c>
+      <c r="D12" t="s">
+        <v>149</v>
+      </c>
+      <c r="F12" t="s">
+        <v>129</v>
+      </c>
+      <c r="G12" t="s">
         <v>255</v>
       </c>
-      <c r="I10" t="s">
+      <c r="H12" t="s">
         <v>275</v>
       </c>
-      <c r="J10" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <f t="shared" si="0"/>
-        <v>68</v>
-      </c>
-      <c r="B11">
-        <v>2</v>
-      </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="D11" t="s">
-        <v>145</v>
-      </c>
-      <c r="E11" t="s">
-        <v>146</v>
-      </c>
-      <c r="G11" t="s">
+      <c r="I12" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13" t="s">
+        <v>151</v>
+      </c>
+      <c r="D13" t="s">
+        <v>152</v>
+      </c>
+      <c r="F13" t="s">
         <v>129</v>
       </c>
-      <c r="H11" t="s">
-        <v>259</v>
-      </c>
-      <c r="I11" t="s">
-        <v>279</v>
-      </c>
-      <c r="J11" s="2" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <f t="shared" si="0"/>
-        <v>69</v>
-      </c>
-      <c r="B12">
-        <v>2</v>
-      </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-      <c r="D12" t="s">
-        <v>148</v>
-      </c>
-      <c r="E12" t="s">
-        <v>149</v>
-      </c>
-      <c r="G12" t="s">
+      <c r="G13" t="s">
+        <v>256</v>
+      </c>
+      <c r="H13" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14" t="s">
+        <v>153</v>
+      </c>
+      <c r="D14" t="s">
+        <v>154</v>
+      </c>
+      <c r="F14" t="s">
         <v>129</v>
-      </c>
-      <c r="H12" t="s">
-        <v>255</v>
-      </c>
-      <c r="I12" t="s">
-        <v>275</v>
-      </c>
-      <c r="J12" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <f t="shared" si="0"/>
-        <v>70</v>
-      </c>
-      <c r="B13">
-        <v>2</v>
-      </c>
-      <c r="C13">
-        <v>1</v>
-      </c>
-      <c r="D13" t="s">
-        <v>151</v>
-      </c>
-      <c r="E13" t="s">
-        <v>152</v>
-      </c>
-      <c r="G13" t="s">
-        <v>129</v>
-      </c>
-      <c r="H13" t="s">
-        <v>256</v>
-      </c>
-      <c r="I13" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A14">
-        <f t="shared" si="0"/>
-        <v>71</v>
-      </c>
-      <c r="B14">
-        <v>2</v>
-      </c>
-      <c r="C14">
-        <v>1</v>
-      </c>
-      <c r="D14" t="s">
-        <v>153</v>
-      </c>
-      <c r="E14" t="s">
-        <v>154</v>
       </c>
       <c r="G14" t="s">
         <v>129</v>
       </c>
       <c r="H14" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15" t="s">
+        <v>155</v>
+      </c>
+      <c r="D15" t="s">
+        <v>156</v>
+      </c>
+      <c r="F15" t="s">
+        <v>157</v>
+      </c>
+      <c r="G15" t="s">
         <v>129</v>
       </c>
-      <c r="I14" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A15">
-        <f t="shared" si="0"/>
-        <v>72</v>
-      </c>
-      <c r="B15">
-        <v>2</v>
-      </c>
-      <c r="C15">
-        <v>1</v>
-      </c>
-      <c r="D15" t="s">
-        <v>155</v>
-      </c>
-      <c r="E15" t="s">
-        <v>156</v>
-      </c>
-      <c r="G15" t="s">
-        <v>157</v>
-      </c>
       <c r="H15" t="s">
+        <v>266</v>
+      </c>
+      <c r="I15" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16" t="s">
+        <v>158</v>
+      </c>
+      <c r="D16" t="s">
+        <v>159</v>
+      </c>
+      <c r="F16" t="s">
         <v>129</v>
       </c>
-      <c r="I15" t="s">
-        <v>266</v>
-      </c>
-      <c r="J15" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A16">
-        <f t="shared" si="0"/>
-        <v>73</v>
-      </c>
-      <c r="B16">
-        <v>2</v>
-      </c>
-      <c r="C16">
-        <v>1</v>
-      </c>
-      <c r="D16" t="s">
-        <v>158</v>
-      </c>
-      <c r="E16" t="s">
-        <v>159</v>
-      </c>
       <c r="G16" t="s">
+        <v>257</v>
+      </c>
+      <c r="H16" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>2</v>
+      </c>
+      <c r="C17" t="s">
+        <v>160</v>
+      </c>
+      <c r="D17" t="s">
+        <v>161</v>
+      </c>
+      <c r="F17" t="s">
         <v>129</v>
       </c>
-      <c r="H16" t="s">
-        <v>257</v>
-      </c>
-      <c r="I16" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17">
-        <f t="shared" si="0"/>
-        <v>74</v>
-      </c>
-      <c r="B17">
-        <v>2</v>
-      </c>
-      <c r="C17">
-        <v>1</v>
-      </c>
-      <c r="D17" t="s">
-        <v>160</v>
-      </c>
-      <c r="E17" t="s">
-        <v>161</v>
-      </c>
       <c r="G17" t="s">
+        <v>255</v>
+      </c>
+      <c r="H17" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>2</v>
+      </c>
+      <c r="C18" t="s">
+        <v>162</v>
+      </c>
+      <c r="D18" t="s">
+        <v>163</v>
+      </c>
+      <c r="F18" t="s">
         <v>129</v>
       </c>
-      <c r="H17" t="s">
+      <c r="G18" t="s">
         <v>255</v>
       </c>
-      <c r="I17" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A18">
-        <f t="shared" si="0"/>
-        <v>75</v>
-      </c>
-      <c r="B18">
-        <v>2</v>
-      </c>
-      <c r="C18">
-        <v>1</v>
-      </c>
-      <c r="D18" t="s">
-        <v>162</v>
-      </c>
-      <c r="E18" t="s">
-        <v>163</v>
-      </c>
-      <c r="G18" t="s">
+      <c r="H18" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>2</v>
+      </c>
+      <c r="C19" t="s">
+        <v>164</v>
+      </c>
+      <c r="D19" t="s">
+        <v>165</v>
+      </c>
+      <c r="F19" t="s">
         <v>129</v>
       </c>
-      <c r="H18" t="s">
+      <c r="G19" t="s">
         <v>255</v>
       </c>
-      <c r="I18" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A19">
-        <f t="shared" si="0"/>
-        <v>76</v>
-      </c>
-      <c r="B19">
-        <v>2</v>
-      </c>
-      <c r="C19">
-        <v>1</v>
-      </c>
-      <c r="D19" t="s">
-        <v>164</v>
-      </c>
-      <c r="E19" t="s">
-        <v>165</v>
-      </c>
-      <c r="G19" t="s">
+      <c r="H19" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>2</v>
+      </c>
+      <c r="C20" t="s">
+        <v>166</v>
+      </c>
+      <c r="D20" t="s">
+        <v>167</v>
+      </c>
+      <c r="F20" t="s">
         <v>129</v>
-      </c>
-      <c r="H19" t="s">
-        <v>255</v>
-      </c>
-      <c r="I19" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A20">
-        <f t="shared" si="0"/>
-        <v>77</v>
-      </c>
-      <c r="B20">
-        <v>2</v>
-      </c>
-      <c r="C20">
-        <v>1</v>
-      </c>
-      <c r="D20" t="s">
-        <v>166</v>
-      </c>
-      <c r="E20" t="s">
-        <v>167</v>
       </c>
       <c r="G20" t="s">
         <v>129</v>
       </c>
       <c r="H20" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>2</v>
+      </c>
+      <c r="C21" t="s">
+        <v>168</v>
+      </c>
+      <c r="D21" t="s">
+        <v>169</v>
+      </c>
+      <c r="F21" t="s">
         <v>129</v>
-      </c>
-      <c r="I20" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A21">
-        <f t="shared" si="0"/>
-        <v>78</v>
-      </c>
-      <c r="B21">
-        <v>2</v>
-      </c>
-      <c r="C21">
-        <v>1</v>
-      </c>
-      <c r="D21" t="s">
-        <v>168</v>
-      </c>
-      <c r="E21" t="s">
-        <v>169</v>
       </c>
       <c r="G21" t="s">
         <v>129</v>
       </c>
       <c r="H21" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>2</v>
+      </c>
+      <c r="C22" t="s">
+        <v>170</v>
+      </c>
+      <c r="D22" t="s">
+        <v>171</v>
+      </c>
+      <c r="F22" t="s">
         <v>129</v>
       </c>
-      <c r="I21" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A22">
-        <f t="shared" si="0"/>
-        <v>79</v>
-      </c>
-      <c r="B22">
-        <v>2</v>
-      </c>
-      <c r="C22">
-        <v>1</v>
-      </c>
-      <c r="D22" t="s">
-        <v>170</v>
-      </c>
-      <c r="E22" t="s">
+      <c r="G22" t="s">
+        <v>258</v>
+      </c>
+      <c r="H22" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>2</v>
+      </c>
+      <c r="C23" t="s">
+        <v>172</v>
+      </c>
+      <c r="D23" t="s">
+        <v>173</v>
+      </c>
+      <c r="F23" t="s">
+        <v>129</v>
+      </c>
+      <c r="G23" t="s">
+        <v>260</v>
+      </c>
+      <c r="H23" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <v>3</v>
+      </c>
+      <c r="C24" t="s">
+        <v>174</v>
+      </c>
+      <c r="D24" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <v>3</v>
+      </c>
+      <c r="C25" t="s">
+        <v>175</v>
+      </c>
+      <c r="D25" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <v>3</v>
+      </c>
+      <c r="C26" t="s">
+        <v>177</v>
+      </c>
+      <c r="D26" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="B27">
+        <v>3</v>
+      </c>
+      <c r="C27" t="s">
+        <v>179</v>
+      </c>
+      <c r="D27" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="B28">
+        <v>3</v>
+      </c>
+      <c r="C28" t="s">
+        <v>181</v>
+      </c>
+      <c r="D28" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="B29">
+        <v>3</v>
+      </c>
+      <c r="C29" t="s">
+        <v>182</v>
+      </c>
+      <c r="D29" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="B30">
+        <v>3</v>
+      </c>
+      <c r="C30" t="s">
+        <v>183</v>
+      </c>
+      <c r="D30" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="B31">
+        <v>3</v>
+      </c>
+      <c r="C31" t="s">
+        <v>185</v>
+      </c>
+      <c r="D31" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="B32">
+        <v>3</v>
+      </c>
+      <c r="C32" t="s">
+        <v>187</v>
+      </c>
+      <c r="D32" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="B33">
+        <v>3</v>
+      </c>
+      <c r="C33" t="s">
+        <v>189</v>
+      </c>
+      <c r="D33" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <f t="shared" ref="A34:A66" si="1">ROW() - 1</f>
+        <v>33</v>
+      </c>
+      <c r="B34">
+        <v>3</v>
+      </c>
+      <c r="C34" t="s">
+        <v>190</v>
+      </c>
+      <c r="D34" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <f t="shared" si="1"/>
+        <v>34</v>
+      </c>
+      <c r="B35">
+        <v>3</v>
+      </c>
+      <c r="C35" t="s">
+        <v>192</v>
+      </c>
+      <c r="D35" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <f t="shared" si="1"/>
+        <v>35</v>
+      </c>
+      <c r="B36">
+        <v>3</v>
+      </c>
+      <c r="C36" t="s">
+        <v>194</v>
+      </c>
+      <c r="D36" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+      <c r="B37">
+        <v>3</v>
+      </c>
+      <c r="C37" t="s">
+        <v>195</v>
+      </c>
+      <c r="D37" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <f t="shared" si="1"/>
+        <v>37</v>
+      </c>
+      <c r="B38">
+        <v>3</v>
+      </c>
+      <c r="C38" t="s">
+        <v>197</v>
+      </c>
+      <c r="D38" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <f t="shared" si="1"/>
+        <v>38</v>
+      </c>
+      <c r="B39">
+        <v>3</v>
+      </c>
+      <c r="C39" t="s">
+        <v>199</v>
+      </c>
+      <c r="D39" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <f t="shared" si="1"/>
+        <v>39</v>
+      </c>
+      <c r="B40">
+        <v>3</v>
+      </c>
+      <c r="C40" t="s">
+        <v>200</v>
+      </c>
+      <c r="D40" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="B41">
+        <v>3</v>
+      </c>
+      <c r="C41" t="s">
+        <v>201</v>
+      </c>
+      <c r="D41" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <f t="shared" si="1"/>
+        <v>41</v>
+      </c>
+      <c r="B42">
+        <v>3</v>
+      </c>
+      <c r="C42" t="s">
+        <v>203</v>
+      </c>
+      <c r="D42" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <f t="shared" si="1"/>
+        <v>42</v>
+      </c>
+      <c r="B43">
+        <v>3</v>
+      </c>
+      <c r="C43" t="s">
+        <v>205</v>
+      </c>
+      <c r="D43" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <f t="shared" si="1"/>
+        <v>43</v>
+      </c>
+      <c r="B44">
+        <v>3</v>
+      </c>
+      <c r="C44" t="s">
+        <v>207</v>
+      </c>
+      <c r="D44" t="s">
         <v>171</v>
       </c>
-      <c r="G22" t="s">
-        <v>129</v>
-      </c>
-      <c r="H22" t="s">
-        <v>258</v>
-      </c>
-      <c r="I22" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A23">
-        <f t="shared" si="0"/>
-        <v>80</v>
-      </c>
-      <c r="B23">
-        <v>2</v>
-      </c>
-      <c r="C23">
-        <v>1</v>
-      </c>
-      <c r="D23" t="s">
-        <v>172</v>
-      </c>
-      <c r="E23" t="s">
-        <v>173</v>
-      </c>
-      <c r="G23" t="s">
-        <v>129</v>
-      </c>
-      <c r="H23" t="s">
-        <v>260</v>
-      </c>
-      <c r="I23" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A24">
-        <f t="shared" si="0"/>
-        <v>81</v>
-      </c>
-      <c r="B24">
-        <v>3</v>
-      </c>
-      <c r="C24">
-        <v>1</v>
-      </c>
-      <c r="D24" t="s">
-        <v>174</v>
-      </c>
-      <c r="E24" t="s">
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <f t="shared" si="1"/>
+        <v>44</v>
+      </c>
+      <c r="B45">
+        <v>4</v>
+      </c>
+      <c r="C45" t="s">
+        <v>208</v>
+      </c>
+      <c r="D45" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <f t="shared" si="1"/>
+        <v>45</v>
+      </c>
+      <c r="B46">
+        <v>4</v>
+      </c>
+      <c r="C46" t="s">
+        <v>210</v>
+      </c>
+      <c r="D46" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A25">
-        <f t="shared" si="0"/>
-        <v>82</v>
-      </c>
-      <c r="B25">
-        <v>3</v>
-      </c>
-      <c r="C25">
-        <v>1</v>
-      </c>
-      <c r="D25" t="s">
-        <v>175</v>
-      </c>
-      <c r="E25" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A26">
-        <f t="shared" si="0"/>
-        <v>83</v>
-      </c>
-      <c r="B26">
-        <v>3</v>
-      </c>
-      <c r="C26">
-        <v>1</v>
-      </c>
-      <c r="D26" t="s">
-        <v>177</v>
-      </c>
-      <c r="E26" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A27">
-        <f t="shared" si="0"/>
-        <v>84</v>
-      </c>
-      <c r="B27">
-        <v>3</v>
-      </c>
-      <c r="C27">
-        <v>1</v>
-      </c>
-      <c r="D27" t="s">
-        <v>179</v>
-      </c>
-      <c r="E27" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A28">
-        <f t="shared" si="0"/>
-        <v>85</v>
-      </c>
-      <c r="B28">
-        <v>3</v>
-      </c>
-      <c r="C28">
-        <v>1</v>
-      </c>
-      <c r="D28" t="s">
-        <v>181</v>
-      </c>
-      <c r="E28" t="s">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <f t="shared" si="1"/>
+        <v>46</v>
+      </c>
+      <c r="B47">
+        <v>4</v>
+      </c>
+      <c r="C47" t="s">
+        <v>211</v>
+      </c>
+      <c r="D47" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <f t="shared" si="1"/>
+        <v>47</v>
+      </c>
+      <c r="B48">
+        <v>4</v>
+      </c>
+      <c r="C48" t="s">
+        <v>213</v>
+      </c>
+      <c r="D48" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <f t="shared" si="1"/>
+        <v>48</v>
+      </c>
+      <c r="B49">
+        <v>4</v>
+      </c>
+      <c r="C49" t="s">
+        <v>215</v>
+      </c>
+      <c r="D49" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A29">
-        <f t="shared" si="0"/>
-        <v>86</v>
-      </c>
-      <c r="B29">
-        <v>3</v>
-      </c>
-      <c r="C29">
-        <v>1</v>
-      </c>
-      <c r="D29" t="s">
-        <v>182</v>
-      </c>
-      <c r="E29" t="s">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <f t="shared" si="1"/>
+        <v>49</v>
+      </c>
+      <c r="B50">
+        <v>4</v>
+      </c>
+      <c r="C50" t="s">
+        <v>216</v>
+      </c>
+      <c r="D50" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="B51">
+        <v>4</v>
+      </c>
+      <c r="C51" t="s">
+        <v>217</v>
+      </c>
+      <c r="D51" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <f t="shared" si="1"/>
+        <v>51</v>
+      </c>
+      <c r="B52">
+        <v>4</v>
+      </c>
+      <c r="C52" t="s">
+        <v>219</v>
+      </c>
+      <c r="D52" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A30">
-        <f t="shared" si="0"/>
-        <v>87</v>
-      </c>
-      <c r="B30">
-        <v>3</v>
-      </c>
-      <c r="C30">
-        <v>1</v>
-      </c>
-      <c r="D30" t="s">
-        <v>183</v>
-      </c>
-      <c r="E30" t="s">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <f t="shared" si="1"/>
+        <v>52</v>
+      </c>
+      <c r="B53">
+        <v>4</v>
+      </c>
+      <c r="C53" t="s">
+        <v>220</v>
+      </c>
+      <c r="D53" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A31">
-        <f t="shared" si="0"/>
-        <v>88</v>
-      </c>
-      <c r="B31">
-        <v>3</v>
-      </c>
-      <c r="C31">
-        <v>1</v>
-      </c>
-      <c r="D31" t="s">
-        <v>185</v>
-      </c>
-      <c r="E31" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A32">
-        <f t="shared" si="0"/>
-        <v>89</v>
-      </c>
-      <c r="B32">
-        <v>3</v>
-      </c>
-      <c r="C32">
-        <v>1</v>
-      </c>
-      <c r="D32" t="s">
-        <v>187</v>
-      </c>
-      <c r="E32" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A33">
-        <f t="shared" si="0"/>
-        <v>90</v>
-      </c>
-      <c r="B33">
-        <v>3</v>
-      </c>
-      <c r="C33">
-        <v>1</v>
-      </c>
-      <c r="D33" t="s">
-        <v>189</v>
-      </c>
-      <c r="E33" t="s">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <f t="shared" si="1"/>
+        <v>53</v>
+      </c>
+      <c r="B54">
+        <v>4</v>
+      </c>
+      <c r="C54" t="s">
+        <v>221</v>
+      </c>
+      <c r="D54" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <f t="shared" si="1"/>
+        <v>54</v>
+      </c>
+      <c r="B55">
+        <v>4</v>
+      </c>
+      <c r="C55" t="s">
+        <v>223</v>
+      </c>
+      <c r="D55" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <f t="shared" si="1"/>
+        <v>55</v>
+      </c>
+      <c r="B56">
+        <v>4</v>
+      </c>
+      <c r="C56" t="s">
+        <v>225</v>
+      </c>
+      <c r="D56" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A34">
-        <f t="shared" ref="A34:A66" si="1">ROW() + 57</f>
-        <v>91</v>
-      </c>
-      <c r="B34">
-        <v>3</v>
-      </c>
-      <c r="C34">
-        <v>1</v>
-      </c>
-      <c r="D34" t="s">
-        <v>190</v>
-      </c>
-      <c r="E34" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A35">
-        <f t="shared" si="1"/>
-        <v>92</v>
-      </c>
-      <c r="B35">
-        <v>3</v>
-      </c>
-      <c r="C35">
-        <v>1</v>
-      </c>
-      <c r="D35" t="s">
-        <v>192</v>
-      </c>
-      <c r="E35" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A36">
-        <f t="shared" si="1"/>
-        <v>93</v>
-      </c>
-      <c r="B36">
-        <v>3</v>
-      </c>
-      <c r="C36">
-        <v>1</v>
-      </c>
-      <c r="D36" t="s">
-        <v>194</v>
-      </c>
-      <c r="E36" t="s">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <f t="shared" si="1"/>
+        <v>56</v>
+      </c>
+      <c r="B57">
+        <v>4</v>
+      </c>
+      <c r="C57" t="s">
+        <v>226</v>
+      </c>
+      <c r="D57" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <f t="shared" si="1"/>
+        <v>57</v>
+      </c>
+      <c r="B58">
+        <v>4</v>
+      </c>
+      <c r="C58" t="s">
+        <v>228</v>
+      </c>
+      <c r="D58" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A37">
-        <f t="shared" si="1"/>
-        <v>94</v>
-      </c>
-      <c r="B37">
-        <v>3</v>
-      </c>
-      <c r="C37">
-        <v>1</v>
-      </c>
-      <c r="D37" t="s">
-        <v>195</v>
-      </c>
-      <c r="E37" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A38">
-        <f t="shared" si="1"/>
-        <v>95</v>
-      </c>
-      <c r="B38">
-        <v>3</v>
-      </c>
-      <c r="C38">
-        <v>1</v>
-      </c>
-      <c r="D38" t="s">
-        <v>197</v>
-      </c>
-      <c r="E38" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A39">
-        <f t="shared" si="1"/>
-        <v>96</v>
-      </c>
-      <c r="B39">
-        <v>3</v>
-      </c>
-      <c r="C39">
-        <v>1</v>
-      </c>
-      <c r="D39" t="s">
-        <v>199</v>
-      </c>
-      <c r="E39" t="s">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <f t="shared" si="1"/>
+        <v>58</v>
+      </c>
+      <c r="B59">
+        <v>4</v>
+      </c>
+      <c r="C59" t="s">
+        <v>229</v>
+      </c>
+      <c r="D59" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <f t="shared" si="1"/>
+        <v>59</v>
+      </c>
+      <c r="B60">
+        <v>4</v>
+      </c>
+      <c r="C60" t="s">
+        <v>231</v>
+      </c>
+      <c r="D60" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+      <c r="B61">
+        <v>4</v>
+      </c>
+      <c r="C61" t="s">
+        <v>233</v>
+      </c>
+      <c r="D61" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <f t="shared" si="1"/>
+        <v>61</v>
+      </c>
+      <c r="B62">
+        <v>4</v>
+      </c>
+      <c r="C62" t="s">
+        <v>235</v>
+      </c>
+      <c r="D62" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A40">
-        <f t="shared" si="1"/>
-        <v>97</v>
-      </c>
-      <c r="B40">
-        <v>3</v>
-      </c>
-      <c r="C40">
-        <v>1</v>
-      </c>
-      <c r="D40" t="s">
-        <v>200</v>
-      </c>
-      <c r="E40" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A41">
-        <f t="shared" si="1"/>
-        <v>98</v>
-      </c>
-      <c r="B41">
-        <v>3</v>
-      </c>
-      <c r="C41">
-        <v>1</v>
-      </c>
-      <c r="D41" t="s">
-        <v>201</v>
-      </c>
-      <c r="E41" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A42">
-        <f t="shared" si="1"/>
-        <v>99</v>
-      </c>
-      <c r="B42">
-        <v>3</v>
-      </c>
-      <c r="C42">
-        <v>1</v>
-      </c>
-      <c r="D42" t="s">
-        <v>203</v>
-      </c>
-      <c r="E42" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A43">
-        <f t="shared" si="1"/>
-        <v>100</v>
-      </c>
-      <c r="B43">
-        <v>3</v>
-      </c>
-      <c r="C43">
-        <v>1</v>
-      </c>
-      <c r="D43" t="s">
-        <v>205</v>
-      </c>
-      <c r="E43" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A44">
-        <f t="shared" si="1"/>
-        <v>101</v>
-      </c>
-      <c r="B44">
-        <v>3</v>
-      </c>
-      <c r="C44">
-        <v>1</v>
-      </c>
-      <c r="D44" t="s">
-        <v>207</v>
-      </c>
-      <c r="E44" t="s">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <f t="shared" si="1"/>
+        <v>62</v>
+      </c>
+      <c r="B63">
+        <v>4</v>
+      </c>
+      <c r="C63" t="s">
+        <v>236</v>
+      </c>
+      <c r="D63" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <f t="shared" si="1"/>
+        <v>63</v>
+      </c>
+      <c r="B64">
+        <v>4</v>
+      </c>
+      <c r="C64" t="s">
+        <v>238</v>
+      </c>
+      <c r="D64" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A45">
-        <f t="shared" si="1"/>
-        <v>102</v>
-      </c>
-      <c r="B45">
-        <v>4</v>
-      </c>
-      <c r="C45">
-        <v>1</v>
-      </c>
-      <c r="D45" t="s">
-        <v>208</v>
-      </c>
-      <c r="E45" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A46">
-        <f t="shared" si="1"/>
-        <v>103</v>
-      </c>
-      <c r="B46">
-        <v>4</v>
-      </c>
-      <c r="C46">
-        <v>1</v>
-      </c>
-      <c r="D46" t="s">
-        <v>210</v>
-      </c>
-      <c r="E46" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A47">
-        <f t="shared" si="1"/>
-        <v>104</v>
-      </c>
-      <c r="B47">
-        <v>4</v>
-      </c>
-      <c r="C47">
-        <v>1</v>
-      </c>
-      <c r="D47" t="s">
-        <v>211</v>
-      </c>
-      <c r="E47" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A48">
-        <f t="shared" si="1"/>
-        <v>105</v>
-      </c>
-      <c r="B48">
-        <v>4</v>
-      </c>
-      <c r="C48">
-        <v>1</v>
-      </c>
-      <c r="D48" t="s">
-        <v>213</v>
-      </c>
-      <c r="E48" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A49">
-        <f t="shared" si="1"/>
-        <v>106</v>
-      </c>
-      <c r="B49">
-        <v>4</v>
-      </c>
-      <c r="C49">
-        <v>1</v>
-      </c>
-      <c r="D49" t="s">
-        <v>215</v>
-      </c>
-      <c r="E49" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A50">
-        <f t="shared" si="1"/>
-        <v>107</v>
-      </c>
-      <c r="B50">
-        <v>4</v>
-      </c>
-      <c r="C50">
-        <v>1</v>
-      </c>
-      <c r="D50" t="s">
-        <v>216</v>
-      </c>
-      <c r="E50" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A51">
-        <f t="shared" si="1"/>
-        <v>108</v>
-      </c>
-      <c r="B51">
-        <v>4</v>
-      </c>
-      <c r="C51">
-        <v>1</v>
-      </c>
-      <c r="D51" t="s">
-        <v>217</v>
-      </c>
-      <c r="E51" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A52">
-        <f t="shared" si="1"/>
-        <v>109</v>
-      </c>
-      <c r="B52">
-        <v>4</v>
-      </c>
-      <c r="C52">
-        <v>1</v>
-      </c>
-      <c r="D52" t="s">
-        <v>219</v>
-      </c>
-      <c r="E52" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A53">
-        <f t="shared" si="1"/>
-        <v>110</v>
-      </c>
-      <c r="B53">
-        <v>4</v>
-      </c>
-      <c r="C53">
-        <v>1</v>
-      </c>
-      <c r="D53" t="s">
-        <v>220</v>
-      </c>
-      <c r="E53" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A54">
-        <f t="shared" si="1"/>
-        <v>111</v>
-      </c>
-      <c r="B54">
-        <v>4</v>
-      </c>
-      <c r="C54">
-        <v>1</v>
-      </c>
-      <c r="D54" t="s">
-        <v>221</v>
-      </c>
-      <c r="E54" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A55">
-        <f t="shared" si="1"/>
-        <v>112</v>
-      </c>
-      <c r="B55">
-        <v>4</v>
-      </c>
-      <c r="C55">
-        <v>1</v>
-      </c>
-      <c r="D55" t="s">
-        <v>223</v>
-      </c>
-      <c r="E55" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A56">
-        <f t="shared" si="1"/>
-        <v>113</v>
-      </c>
-      <c r="B56">
-        <v>4</v>
-      </c>
-      <c r="C56">
-        <v>1</v>
-      </c>
-      <c r="D56" t="s">
-        <v>225</v>
-      </c>
-      <c r="E56" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A57">
-        <f t="shared" si="1"/>
-        <v>114</v>
-      </c>
-      <c r="B57">
-        <v>4</v>
-      </c>
-      <c r="C57">
-        <v>1</v>
-      </c>
-      <c r="D57" t="s">
-        <v>226</v>
-      </c>
-      <c r="E57" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A58">
-        <f t="shared" si="1"/>
-        <v>115</v>
-      </c>
-      <c r="B58">
-        <v>4</v>
-      </c>
-      <c r="C58">
-        <v>1</v>
-      </c>
-      <c r="D58" t="s">
-        <v>228</v>
-      </c>
-      <c r="E58" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A59">
-        <f t="shared" si="1"/>
-        <v>116</v>
-      </c>
-      <c r="B59">
-        <v>4</v>
-      </c>
-      <c r="C59">
-        <v>1</v>
-      </c>
-      <c r="D59" t="s">
-        <v>229</v>
-      </c>
-      <c r="E59" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A60">
-        <f t="shared" si="1"/>
-        <v>117</v>
-      </c>
-      <c r="B60">
-        <v>4</v>
-      </c>
-      <c r="C60">
-        <v>1</v>
-      </c>
-      <c r="D60" t="s">
-        <v>231</v>
-      </c>
-      <c r="E60" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A61">
-        <f t="shared" si="1"/>
-        <v>118</v>
-      </c>
-      <c r="B61">
-        <v>4</v>
-      </c>
-      <c r="C61">
-        <v>1</v>
-      </c>
-      <c r="D61" t="s">
-        <v>233</v>
-      </c>
-      <c r="E61" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A62">
-        <f t="shared" si="1"/>
-        <v>119</v>
-      </c>
-      <c r="B62">
-        <v>4</v>
-      </c>
-      <c r="C62">
-        <v>1</v>
-      </c>
-      <c r="D62" t="s">
-        <v>235</v>
-      </c>
-      <c r="E62" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A63">
-        <f t="shared" si="1"/>
-        <v>120</v>
-      </c>
-      <c r="B63">
-        <v>4</v>
-      </c>
-      <c r="C63">
-        <v>1</v>
-      </c>
-      <c r="D63" t="s">
-        <v>236</v>
-      </c>
-      <c r="E63" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A64">
-        <f t="shared" si="1"/>
-        <v>121</v>
-      </c>
-      <c r="B64">
-        <v>4</v>
-      </c>
-      <c r="C64">
-        <v>1</v>
-      </c>
-      <c r="D64" t="s">
-        <v>238</v>
-      </c>
-      <c r="E64" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65">
         <f t="shared" si="1"/>
-        <v>122</v>
+        <v>64</v>
       </c>
       <c r="B65">
         <v>4</v>
       </c>
-      <c r="C65">
-        <v>1</v>
+      <c r="C65" t="s">
+        <v>239</v>
       </c>
       <c r="D65" t="s">
-        <v>239</v>
-      </c>
-      <c r="E65" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66">
         <f t="shared" si="1"/>
-        <v>123</v>
+        <v>65</v>
       </c>
       <c r="B66">
         <v>4</v>
       </c>
-      <c r="C66">
-        <v>1</v>
+      <c r="C66" t="s">
+        <v>241</v>
       </c>
       <c r="D66" t="s">
-        <v>241</v>
-      </c>
-      <c r="E66" t="s">
         <v>242</v>
       </c>
     </row>
@@ -4059,14 +3867,14 @@
       <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="18.83203125" customWidth="1"/>
-    <col min="4" max="4" width="18.83203125" style="1" customWidth="1"/>
-    <col min="5" max="10" width="18.83203125" customWidth="1"/>
+    <col min="1" max="3" width="18.875" customWidth="1"/>
+    <col min="4" max="4" width="18.875" style="1" customWidth="1"/>
+    <col min="5" max="10" width="18.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4089,7 +3897,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -4109,7 +3917,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -4129,7 +3937,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -4152,7 +3960,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -4172,7 +3980,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -4192,7 +4000,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -4212,7 +4020,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -4232,7 +4040,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -4252,7 +4060,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>34</v>
       </c>
@@ -4260,7 +4068,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>36</v>
       </c>
@@ -4268,12 +4076,12 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -4305,7 +4113,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1</v>
       </c>
@@ -4334,7 +4142,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2</v>
       </c>
@@ -4363,7 +4171,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>3</v>
       </c>
@@ -4392,7 +4200,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>4</v>
       </c>
@@ -4421,7 +4229,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>5</v>
       </c>
@@ -4450,7 +4258,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>6</v>
       </c>
@@ -4479,7 +4287,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>7</v>
       </c>
@@ -4508,7 +4316,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>8</v>
       </c>
@@ -4537,7 +4345,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D24"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated database: complete excel table for big cards
</commit_message>
<xml_diff>
--- a/data/TP Database.xlsx
+++ b/data/TP Database.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_My Files\_Uni\Year 3\Term 1\3 - Team Project\_TP Code\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sophiachung/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A694393-3198-423B-AD9D-079C58C70633}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{74A9764C-AA4B-034B-AD6E-5334636B3DBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-1290" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{F6F91125-3C8A-D047-93DD-1F3A6DE88698}"/>
+    <workbookView xWindow="13340" yWindow="500" windowWidth="15460" windowHeight="15880" activeTab="1" xr2:uid="{F6F91125-3C8A-D047-93DD-1F3A6DE88698}"/>
   </bookViews>
   <sheets>
     <sheet name="Small Cards" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="333">
   <si>
     <t>CardID</t>
   </si>
@@ -509,9 +509,6 @@
     <t>Multiple perspectives</t>
   </si>
   <si>
-    <t>CONTEXT contains more than one type of Resource tile (e.g. Lab/Archive)</t>
-  </si>
-  <si>
     <t>event-CONTEXT-procrastinate.png</t>
   </si>
   <si>
@@ -878,7 +875,166 @@
     <t>o0:2:(3&amp;4)</t>
   </si>
   <si>
-    <t>Column1</t>
+    <t>n0:3:3</t>
+  </si>
+  <si>
+    <t>n(37/38/39/40/42/45/46):3</t>
+  </si>
+  <si>
+    <t>!3</t>
+  </si>
+  <si>
+    <t>remove one great resources tile from IMPLEMENTATION section AND one Resource (any) tile from CONTEXT section</t>
+  </si>
+  <si>
+    <t>!41</t>
+  </si>
+  <si>
+    <t>n(42/45/46):1</t>
+  </si>
+  <si>
+    <t>n0:2:3 (If PLAN contains Milestones only remove 1 tile)</t>
+  </si>
+  <si>
+    <t>n0:2:3</t>
+  </si>
+  <si>
+    <t>!2</t>
+  </si>
+  <si>
+    <t>n0:4:3</t>
+  </si>
+  <si>
+    <t>n(33/34/35/36/37/38/39/40/43/44/45/46):3</t>
+  </si>
+  <si>
+    <t>n0:1:3</t>
+  </si>
+  <si>
+    <t>n41:1, , n(42/45/46):2</t>
+  </si>
+  <si>
+    <t>n(43/44):2</t>
+  </si>
+  <si>
+    <t>!5</t>
+  </si>
+  <si>
+    <t>27/28</t>
+  </si>
+  <si>
+    <t>p(43/44):1</t>
+  </si>
+  <si>
+    <t>!9</t>
+  </si>
+  <si>
+    <t>n(17/18/19/20/21/22/23/24/25/26/27/28):1</t>
+  </si>
+  <si>
+    <t>n(33/34/35/36):1, n(45/46):1</t>
+  </si>
+  <si>
+    <t>b0:2:4</t>
+  </si>
+  <si>
+    <t>n(33/34/35/36/43/44):2</t>
+  </si>
+  <si>
+    <t>(17+18+19+20+21+22+23+24+25+26+27+28):&gt;1</t>
+  </si>
+  <si>
+    <t>!14</t>
+  </si>
+  <si>
+    <t>n(47/48/49/54/55/57):1</t>
+  </si>
+  <si>
+    <t>remove any 3 non-adjacent tiles from current section</t>
+  </si>
+  <si>
+    <t>!(31&amp;32)</t>
+  </si>
+  <si>
+    <t>n(47/48/57):2</t>
+  </si>
+  <si>
+    <t>!5 (else remove only 1)</t>
+  </si>
+  <si>
+    <t>remove 2 non-adjacent thesis tiles from current section</t>
+  </si>
+  <si>
+    <t>n-0:3:4</t>
+  </si>
+  <si>
+    <t>n-(47/48/49/54/55/57):2</t>
+  </si>
+  <si>
+    <t>!53</t>
+  </si>
+  <si>
+    <t>n0:3:4</t>
+  </si>
+  <si>
+    <t>!13&amp;!56</t>
+  </si>
+  <si>
+    <t>n0:4:4</t>
+  </si>
+  <si>
+    <t>n-(54/55):2</t>
+  </si>
+  <si>
+    <t>!58</t>
+  </si>
+  <si>
+    <t>!58&amp;!116</t>
+  </si>
+  <si>
+    <t>n0:2:4</t>
+  </si>
+  <si>
+    <t>!(15/16/31):&gt;2</t>
+  </si>
+  <si>
+    <t>!7&amp;!(43/44):&gt;1</t>
+  </si>
+  <si>
+    <t>!(43/44):&gt;1</t>
+  </si>
+  <si>
+    <t>n-(49/54/55):2</t>
+  </si>
+  <si>
+    <t>!(11/12/32):&gt;1</t>
+  </si>
+  <si>
+    <t>n41:1&amp;n(17/18/19/20/21/22/23/24/25/26/27/28):1</t>
+  </si>
+  <si>
+    <t>n(45/46):1&amp;n(43/44):1</t>
+  </si>
+  <si>
+    <t>keep this card to protect against any future Jargon events</t>
+  </si>
+  <si>
+    <t>p(54/55):1&amp;i112:1</t>
+  </si>
+  <si>
+    <t>!(33/34/35/36):&gt;2</t>
+  </si>
+  <si>
+    <t>n-(47/48/49/54/55/57):3</t>
+  </si>
+  <si>
+    <t>!31:&gt;1</t>
+  </si>
+  <si>
+    <t>!56</t>
+  </si>
+  <si>
+    <t>n49:2</t>
   </si>
 </sst>
 </file>
@@ -992,16 +1148,16 @@
   <autoFilter ref="A1:I66" xr:uid="{4E25BA7D-C944-7B48-8D11-C2260663E6FE}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{241E3EFA-1556-A24B-8441-368F09FD400E}" name="CardID" dataDxfId="2">
-      <calculatedColumnFormula>ROW() - 1</calculatedColumnFormula>
+      <calculatedColumnFormula>ROW() + 57</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="2" xr3:uid="{4CB802A7-5A14-1843-8D85-057515A93530}" name="Stage"/>
-    <tableColumn id="3" xr3:uid="{45AAD7C9-BD08-B241-A106-B2FFC2B22B18}" name="Filename"/>
-    <tableColumn id="8" xr3:uid="{98D9D00E-0FDA-C645-9758-69E917F00870}" name="Title"/>
-    <tableColumn id="4" xr3:uid="{1F7BF006-71BD-D542-96ED-747B93E53C9C}" name="Description"/>
-    <tableColumn id="5" xr3:uid="{5BD78171-150E-AB4C-80DC-D8A061F5BF5E}" name="Save_condition"/>
-    <tableColumn id="9" xr3:uid="{318B7552-B230-384E-9C27-A0F990859B0F}" name="Requirement"/>
-    <tableColumn id="6" xr3:uid="{FCFA78C0-6299-A941-AD36-DE9122010D1F}" name="Effect"/>
-    <tableColumn id="7" xr3:uid="{6E4CEF28-DC4C-D54A-9279-428FA0FAB941}" name="Column1"/>
+    <tableColumn id="3" xr3:uid="{45AAD7C9-BD08-B241-A106-B2FFC2B22B18}" name="Number"/>
+    <tableColumn id="8" xr3:uid="{98D9D00E-0FDA-C645-9758-69E917F00870}" name="Filename"/>
+    <tableColumn id="4" xr3:uid="{1F7BF006-71BD-D542-96ED-747B93E53C9C}" name="Title"/>
+    <tableColumn id="5" xr3:uid="{5BD78171-150E-AB4C-80DC-D8A061F5BF5E}" name="Description"/>
+    <tableColumn id="9" xr3:uid="{318B7552-B230-384E-9C27-A0F990859B0F}" name="Save_condition"/>
+    <tableColumn id="6" xr3:uid="{FCFA78C0-6299-A941-AD36-DE9122010D1F}" name="Requirement"/>
+    <tableColumn id="7" xr3:uid="{6E4CEF28-DC4C-D54A-9279-428FA0FAB941}" name="Effect"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1341,21 +1497,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18AE550B-A04F-B142-B067-7E2D879988FA}">
   <dimension ref="A1:H59"/>
   <sheetViews>
-    <sheetView zoomScale="102" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H41" sqref="H41"/>
+    <sheetView topLeftCell="A39" zoomScale="102" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.625" customWidth="1"/>
-    <col min="2" max="2" width="15.125" customWidth="1"/>
-    <col min="3" max="3" width="10.375" customWidth="1"/>
-    <col min="4" max="4" width="25.125" customWidth="1"/>
+    <col min="1" max="1" width="9.6640625" customWidth="1"/>
+    <col min="2" max="2" width="15.1640625" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" customWidth="1"/>
+    <col min="4" max="4" width="25.1640625" customWidth="1"/>
     <col min="5" max="6" width="17.5" customWidth="1"/>
     <col min="7" max="7" width="9.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1381,7 +1537,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2">
         <f t="shared" ref="A2:A33" si="0">ROW() - 1</f>
         <v>1</v>
@@ -1399,13 +1555,13 @@
         <v>9</v>
       </c>
       <c r="G2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="H2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -1423,13 +1579,13 @@
         <v>44</v>
       </c>
       <c r="G3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="H3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -1447,10 +1603,10 @@
         <v>46</v>
       </c>
       <c r="G4" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1468,10 +1624,10 @@
         <v>48</v>
       </c>
       <c r="G5" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1489,10 +1645,10 @@
         <v>50</v>
       </c>
       <c r="G6" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1510,10 +1666,10 @@
         <v>52</v>
       </c>
       <c r="G7" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1531,10 +1687,10 @@
         <v>54</v>
       </c>
       <c r="G8" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1552,10 +1708,10 @@
         <v>12</v>
       </c>
       <c r="G9" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1573,10 +1729,10 @@
         <v>56</v>
       </c>
       <c r="G10" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1594,10 +1750,10 @@
         <v>58</v>
       </c>
       <c r="G11" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1615,10 +1771,10 @@
         <v>60</v>
       </c>
       <c r="G12" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1636,10 +1792,10 @@
         <v>60</v>
       </c>
       <c r="G13" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1657,10 +1813,10 @@
         <v>63</v>
       </c>
       <c r="G14" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1678,10 +1834,10 @@
         <v>65</v>
       </c>
       <c r="G15" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1699,10 +1855,10 @@
         <v>67</v>
       </c>
       <c r="G16" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1720,10 +1876,10 @@
         <v>67</v>
       </c>
       <c r="G17" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1741,10 +1897,10 @@
         <v>70</v>
       </c>
       <c r="G18" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -1762,10 +1918,10 @@
         <v>70</v>
       </c>
       <c r="G19" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -1783,10 +1939,10 @@
         <v>16</v>
       </c>
       <c r="G20" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -1804,10 +1960,10 @@
         <v>16</v>
       </c>
       <c r="G21" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -1825,10 +1981,10 @@
         <v>73</v>
       </c>
       <c r="G22" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -1846,10 +2002,10 @@
         <v>73</v>
       </c>
       <c r="G23" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -1867,10 +2023,10 @@
         <v>76</v>
       </c>
       <c r="G24" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -1888,10 +2044,10 @@
         <v>76</v>
       </c>
       <c r="G25" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -1909,10 +2065,10 @@
         <v>79</v>
       </c>
       <c r="G26" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -1930,10 +2086,10 @@
         <v>79</v>
       </c>
       <c r="G27" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -1951,10 +2107,10 @@
         <v>82</v>
       </c>
       <c r="G28" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -1972,10 +2128,10 @@
         <v>82</v>
       </c>
       <c r="G29" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -1993,10 +2149,10 @@
         <v>85</v>
       </c>
       <c r="G30" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -2014,10 +2170,10 @@
         <v>87</v>
       </c>
       <c r="G31" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -2035,10 +2191,10 @@
         <v>89</v>
       </c>
       <c r="G32" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -2056,10 +2212,10 @@
         <v>91</v>
       </c>
       <c r="G33" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34">
         <f t="shared" ref="A34:A59" si="1">ROW() - 1</f>
         <v>33</v>
@@ -2077,10 +2233,10 @@
         <v>23</v>
       </c>
       <c r="G34" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35">
         <f t="shared" si="1"/>
         <v>34</v>
@@ -2098,10 +2254,10 @@
         <v>23</v>
       </c>
       <c r="G35" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36">
         <f t="shared" si="1"/>
         <v>35</v>
@@ -2119,10 +2275,10 @@
         <v>23</v>
       </c>
       <c r="G36" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37">
         <f t="shared" si="1"/>
         <v>36</v>
@@ -2140,10 +2296,10 @@
         <v>23</v>
       </c>
       <c r="G37" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38">
         <f t="shared" si="1"/>
         <v>37</v>
@@ -2161,10 +2317,10 @@
         <v>96</v>
       </c>
       <c r="G38" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39">
         <f t="shared" si="1"/>
         <v>38</v>
@@ -2182,10 +2338,10 @@
         <v>96</v>
       </c>
       <c r="G39" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40">
         <f t="shared" si="1"/>
         <v>39</v>
@@ -2203,10 +2359,10 @@
         <v>96</v>
       </c>
       <c r="G40" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41">
         <f t="shared" si="1"/>
         <v>40</v>
@@ -2224,10 +2380,10 @@
         <v>96</v>
       </c>
       <c r="G41" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42">
         <f t="shared" si="1"/>
         <v>41</v>
@@ -2245,10 +2401,10 @@
         <v>101</v>
       </c>
       <c r="G42" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43">
         <f t="shared" si="1"/>
         <v>42</v>
@@ -2266,10 +2422,10 @@
         <v>26</v>
       </c>
       <c r="G43" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44">
         <f t="shared" si="1"/>
         <v>43</v>
@@ -2287,10 +2443,10 @@
         <v>103</v>
       </c>
       <c r="G44" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45">
         <f t="shared" si="1"/>
         <v>44</v>
@@ -2308,10 +2464,10 @@
         <v>103</v>
       </c>
       <c r="G45" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46">
         <f t="shared" si="1"/>
         <v>45</v>
@@ -2329,10 +2485,10 @@
         <v>106</v>
       </c>
       <c r="G46" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47">
         <f t="shared" si="1"/>
         <v>46</v>
@@ -2350,10 +2506,10 @@
         <v>106</v>
       </c>
       <c r="G47" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48">
         <f t="shared" si="1"/>
         <v>47</v>
@@ -2371,10 +2527,10 @@
         <v>109</v>
       </c>
       <c r="G48" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49">
         <f t="shared" si="1"/>
         <v>48</v>
@@ -2392,10 +2548,10 @@
         <v>109</v>
       </c>
       <c r="G49" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50">
         <f t="shared" si="1"/>
         <v>49</v>
@@ -2413,10 +2569,10 @@
         <v>112</v>
       </c>
       <c r="G50" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51">
         <f t="shared" si="1"/>
         <v>50</v>
@@ -2434,10 +2590,10 @@
         <v>32</v>
       </c>
       <c r="G51" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52">
         <f t="shared" si="1"/>
         <v>51</v>
@@ -2455,10 +2611,10 @@
         <v>32</v>
       </c>
       <c r="G52" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53">
         <f t="shared" si="1"/>
         <v>52</v>
@@ -2476,10 +2632,10 @@
         <v>32</v>
       </c>
       <c r="G53" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54">
         <f t="shared" si="1"/>
         <v>53</v>
@@ -2497,10 +2653,10 @@
         <v>116</v>
       </c>
       <c r="G54" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55">
         <f t="shared" si="1"/>
         <v>54</v>
@@ -2518,10 +2674,10 @@
         <v>29</v>
       </c>
       <c r="G55" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56">
         <f t="shared" si="1"/>
         <v>55</v>
@@ -2539,10 +2695,10 @@
         <v>29</v>
       </c>
       <c r="G56" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57">
         <f t="shared" si="1"/>
         <v>56</v>
@@ -2560,10 +2716,10 @@
         <v>119</v>
       </c>
       <c r="G57" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58">
         <f t="shared" si="1"/>
         <v>57</v>
@@ -2581,10 +2737,10 @@
         <v>121</v>
       </c>
       <c r="G58" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59">
         <f t="shared" si="1"/>
         <v>58</v>
@@ -2602,7 +2758,7 @@
         <v>123</v>
       </c>
       <c r="G59" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
   </sheetData>
@@ -2615,26 +2771,26 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84DC5E79-A11F-0148-B3A8-F5384824D987}">
-  <dimension ref="A1:I66"/>
+  <dimension ref="A1:J66"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="99" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" topLeftCell="D34" zoomScale="99" workbookViewId="0">
+      <selection activeCell="I67" sqref="I67"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.125" customWidth="1"/>
+    <col min="1" max="1" width="9.1640625" customWidth="1"/>
     <col min="2" max="2" width="9.5" customWidth="1"/>
-    <col min="3" max="3" width="33" customWidth="1"/>
-    <col min="4" max="4" width="25.875" customWidth="1"/>
-    <col min="5" max="5" width="12.125" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" customWidth="1"/>
+    <col min="4" max="4" width="25.83203125" customWidth="1"/>
+    <col min="5" max="5" width="26" customWidth="1"/>
     <col min="6" max="6" width="14" customWidth="1"/>
     <col min="7" max="7" width="17" customWidth="1"/>
-    <col min="8" max="8" width="52.125" customWidth="1"/>
-    <col min="9" max="9" width="45.875" customWidth="1"/>
+    <col min="8" max="8" width="15.83203125" customWidth="1"/>
+    <col min="9" max="9" width="45.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2642,1213 +2798,1807 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
-        <v>4</v>
-      </c>
       <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>124</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>125</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>126</v>
       </c>
-      <c r="I1" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2">
-        <f t="shared" ref="A2:A33" si="0">ROW() - 1</f>
-        <v>1</v>
+        <f t="shared" ref="A2:A33" si="0">ROW() + 57</f>
+        <v>59</v>
       </c>
       <c r="B2">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
         <v>127</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>128</v>
       </c>
-      <c r="F2" t="s">
-        <v>129</v>
-      </c>
       <c r="G2" t="s">
         <v>129</v>
       </c>
       <c r="H2" t="s">
+        <v>129</v>
+      </c>
+      <c r="I2" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>130</v>
+      </c>
+      <c r="E3" t="s">
+        <v>131</v>
+      </c>
+      <c r="G3" t="s">
+        <v>129</v>
+      </c>
+      <c r="H3" t="s">
+        <v>129</v>
+      </c>
+      <c r="I3" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3" t="s">
-        <v>130</v>
-      </c>
-      <c r="D3" t="s">
-        <v>131</v>
-      </c>
-      <c r="F3" t="s">
-        <v>129</v>
-      </c>
-      <c r="G3" t="s">
-        <v>129</v>
-      </c>
-      <c r="H3" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>61</v>
       </c>
       <c r="B4">
         <v>2</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
         <v>132</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>133</v>
       </c>
-      <c r="F4" t="s">
-        <v>129</v>
-      </c>
       <c r="G4" t="s">
+        <v>129</v>
+      </c>
+      <c r="H4" t="s">
+        <v>252</v>
+      </c>
+      <c r="I4" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <f t="shared" si="0"/>
+        <v>62</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>134</v>
+      </c>
+      <c r="E5" t="s">
+        <v>135</v>
+      </c>
+      <c r="G5" t="s">
+        <v>129</v>
+      </c>
+      <c r="H5" t="s">
+        <v>129</v>
+      </c>
+      <c r="I5" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <f t="shared" si="0"/>
+        <v>63</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>136</v>
+      </c>
+      <c r="E6" t="s">
+        <v>135</v>
+      </c>
+      <c r="G6" t="s">
+        <v>129</v>
+      </c>
+      <c r="H6" t="s">
+        <v>129</v>
+      </c>
+      <c r="I6" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7" t="s">
+        <v>137</v>
+      </c>
+      <c r="E7" t="s">
+        <v>138</v>
+      </c>
+      <c r="G7" t="s">
+        <v>129</v>
+      </c>
+      <c r="H7" t="s">
         <v>253</v>
       </c>
-      <c r="H4" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>2</v>
-      </c>
-      <c r="C5" t="s">
-        <v>134</v>
-      </c>
-      <c r="D5" t="s">
-        <v>135</v>
-      </c>
-      <c r="F5" t="s">
-        <v>129</v>
-      </c>
-      <c r="G5" t="s">
-        <v>129</v>
-      </c>
-      <c r="H5" t="s">
+      <c r="I7" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="B6">
-        <v>2</v>
-      </c>
-      <c r="C6" t="s">
-        <v>136</v>
-      </c>
-      <c r="D6" t="s">
-        <v>135</v>
-      </c>
-      <c r="F6" t="s">
-        <v>129</v>
-      </c>
-      <c r="G6" t="s">
-        <v>129</v>
-      </c>
-      <c r="H6" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="B7">
-        <v>2</v>
-      </c>
-      <c r="C7" t="s">
-        <v>137</v>
-      </c>
-      <c r="D7" t="s">
-        <v>138</v>
-      </c>
-      <c r="F7" t="s">
-        <v>129</v>
-      </c>
-      <c r="G7" t="s">
-        <v>254</v>
-      </c>
-      <c r="H7" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>65</v>
       </c>
       <c r="B8">
         <v>2</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8" t="s">
         <v>139</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>140</v>
       </c>
-      <c r="F8" t="s">
-        <v>261</v>
-      </c>
       <c r="G8" t="s">
-        <v>129</v>
+        <v>260</v>
       </c>
       <c r="H8" t="s">
-        <v>271</v>
+        <v>129</v>
       </c>
       <c r="I8" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J8" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>66</v>
       </c>
       <c r="B9">
         <v>2</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9" t="s">
         <v>141</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>142</v>
       </c>
-      <c r="F9" t="s">
-        <v>129</v>
-      </c>
       <c r="G9" t="s">
         <v>129</v>
       </c>
       <c r="H9" t="s">
+        <v>129</v>
+      </c>
+      <c r="I9" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <f t="shared" si="0"/>
+        <v>67</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10" t="s">
+        <v>143</v>
+      </c>
+      <c r="E10" t="s">
+        <v>144</v>
+      </c>
+      <c r="G10" t="s">
+        <v>129</v>
+      </c>
+      <c r="H10" t="s">
+        <v>254</v>
+      </c>
+      <c r="I10" t="s">
         <v>274</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="B10">
-        <v>2</v>
-      </c>
-      <c r="C10" t="s">
-        <v>143</v>
-      </c>
-      <c r="D10" t="s">
-        <v>144</v>
-      </c>
-      <c r="F10" t="s">
-        <v>129</v>
-      </c>
-      <c r="G10" t="s">
+      <c r="J10" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <f t="shared" si="0"/>
+        <v>68</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11" t="s">
+        <v>145</v>
+      </c>
+      <c r="E11" t="s">
+        <v>146</v>
+      </c>
+      <c r="G11" t="s">
+        <v>129</v>
+      </c>
+      <c r="H11" t="s">
+        <v>258</v>
+      </c>
+      <c r="I11" t="s">
+        <v>278</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <f t="shared" si="0"/>
+        <v>69</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12" t="s">
+        <v>148</v>
+      </c>
+      <c r="E12" t="s">
+        <v>149</v>
+      </c>
+      <c r="G12" t="s">
+        <v>129</v>
+      </c>
+      <c r="H12" t="s">
+        <v>254</v>
+      </c>
+      <c r="I12" t="s">
+        <v>274</v>
+      </c>
+      <c r="J12" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <f t="shared" si="0"/>
+        <v>70</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13" t="s">
+        <v>151</v>
+      </c>
+      <c r="E13" t="s">
+        <v>152</v>
+      </c>
+      <c r="G13" t="s">
+        <v>129</v>
+      </c>
+      <c r="H13" t="s">
         <v>255</v>
       </c>
-      <c r="H10" t="s">
+      <c r="I13" t="s">
         <v>275</v>
       </c>
-      <c r="I10" t="s">
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <f t="shared" si="0"/>
+        <v>71</v>
+      </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14" t="s">
+        <v>153</v>
+      </c>
+      <c r="E14" t="s">
+        <v>154</v>
+      </c>
+      <c r="G14" t="s">
+        <v>129</v>
+      </c>
+      <c r="H14" t="s">
+        <v>129</v>
+      </c>
+      <c r="I14" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <f t="shared" si="0"/>
+        <v>72</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15" t="s">
+        <v>155</v>
+      </c>
+      <c r="E15" t="s">
+        <v>156</v>
+      </c>
+      <c r="G15" t="s">
+        <v>301</v>
+      </c>
+      <c r="H15" t="s">
+        <v>129</v>
+      </c>
+      <c r="I15" t="s">
+        <v>265</v>
+      </c>
+      <c r="J15" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="B11">
-        <v>2</v>
-      </c>
-      <c r="C11" t="s">
-        <v>145</v>
-      </c>
-      <c r="D11" t="s">
-        <v>146</v>
-      </c>
-      <c r="F11" t="s">
-        <v>129</v>
-      </c>
-      <c r="G11" t="s">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <f t="shared" si="0"/>
+        <v>73</v>
+      </c>
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16" t="s">
+        <v>157</v>
+      </c>
+      <c r="E16" t="s">
+        <v>158</v>
+      </c>
+      <c r="G16" t="s">
+        <v>129</v>
+      </c>
+      <c r="H16" t="s">
+        <v>256</v>
+      </c>
+      <c r="I16" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <f t="shared" si="0"/>
+        <v>74</v>
+      </c>
+      <c r="B17">
+        <v>2</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17" t="s">
+        <v>159</v>
+      </c>
+      <c r="E17" t="s">
+        <v>160</v>
+      </c>
+      <c r="G17" t="s">
+        <v>129</v>
+      </c>
+      <c r="H17" t="s">
+        <v>254</v>
+      </c>
+      <c r="I17" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <f t="shared" si="0"/>
+        <v>75</v>
+      </c>
+      <c r="B18">
+        <v>2</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18" t="s">
+        <v>161</v>
+      </c>
+      <c r="E18" t="s">
+        <v>162</v>
+      </c>
+      <c r="G18" t="s">
+        <v>129</v>
+      </c>
+      <c r="H18" t="s">
+        <v>254</v>
+      </c>
+      <c r="I18" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <f t="shared" si="0"/>
+        <v>76</v>
+      </c>
+      <c r="B19">
+        <v>2</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19" t="s">
+        <v>163</v>
+      </c>
+      <c r="E19" t="s">
+        <v>164</v>
+      </c>
+      <c r="G19" t="s">
+        <v>129</v>
+      </c>
+      <c r="H19" t="s">
+        <v>254</v>
+      </c>
+      <c r="I19" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <f t="shared" si="0"/>
+        <v>77</v>
+      </c>
+      <c r="B20">
+        <v>2</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20" t="s">
+        <v>165</v>
+      </c>
+      <c r="E20" t="s">
+        <v>166</v>
+      </c>
+      <c r="G20" t="s">
+        <v>129</v>
+      </c>
+      <c r="H20" t="s">
+        <v>129</v>
+      </c>
+      <c r="I20" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <f t="shared" si="0"/>
+        <v>78</v>
+      </c>
+      <c r="B21">
+        <v>2</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21" t="s">
+        <v>167</v>
+      </c>
+      <c r="E21" t="s">
+        <v>168</v>
+      </c>
+      <c r="G21" t="s">
+        <v>129</v>
+      </c>
+      <c r="H21" t="s">
+        <v>129</v>
+      </c>
+      <c r="I21" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <f t="shared" si="0"/>
+        <v>79</v>
+      </c>
+      <c r="B22">
+        <v>2</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22" t="s">
+        <v>169</v>
+      </c>
+      <c r="E22" t="s">
+        <v>170</v>
+      </c>
+      <c r="G22" t="s">
+        <v>129</v>
+      </c>
+      <c r="H22" t="s">
+        <v>257</v>
+      </c>
+      <c r="I22" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <f t="shared" si="0"/>
+        <v>80</v>
+      </c>
+      <c r="B23">
+        <v>2</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23" t="s">
+        <v>171</v>
+      </c>
+      <c r="E23" t="s">
+        <v>172</v>
+      </c>
+      <c r="G23" t="s">
+        <v>129</v>
+      </c>
+      <c r="H23" t="s">
         <v>259</v>
       </c>
-      <c r="H11" t="s">
-        <v>279</v>
-      </c>
-      <c r="I11" s="2" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="B12">
-        <v>2</v>
-      </c>
-      <c r="C12" t="s">
-        <v>148</v>
-      </c>
-      <c r="D12" t="s">
-        <v>149</v>
-      </c>
-      <c r="F12" t="s">
-        <v>129</v>
-      </c>
-      <c r="G12" t="s">
-        <v>255</v>
-      </c>
-      <c r="H12" t="s">
-        <v>275</v>
-      </c>
-      <c r="I12" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="B13">
-        <v>2</v>
-      </c>
-      <c r="C13" t="s">
-        <v>151</v>
-      </c>
-      <c r="D13" t="s">
-        <v>152</v>
-      </c>
-      <c r="F13" t="s">
-        <v>129</v>
-      </c>
-      <c r="G13" t="s">
-        <v>256</v>
-      </c>
-      <c r="H13" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-      <c r="B14">
-        <v>2</v>
-      </c>
-      <c r="C14" t="s">
-        <v>153</v>
-      </c>
-      <c r="D14" t="s">
-        <v>154</v>
-      </c>
-      <c r="F14" t="s">
-        <v>129</v>
-      </c>
-      <c r="G14" t="s">
-        <v>129</v>
-      </c>
-      <c r="H14" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="B15">
-        <v>2</v>
-      </c>
-      <c r="C15" t="s">
-        <v>155</v>
-      </c>
-      <c r="D15" t="s">
-        <v>156</v>
-      </c>
-      <c r="F15" t="s">
-        <v>157</v>
-      </c>
-      <c r="G15" t="s">
-        <v>129</v>
-      </c>
-      <c r="H15" t="s">
-        <v>266</v>
-      </c>
-      <c r="I15" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="B16">
-        <v>2</v>
-      </c>
-      <c r="C16" t="s">
-        <v>158</v>
-      </c>
-      <c r="D16" t="s">
-        <v>159</v>
-      </c>
-      <c r="F16" t="s">
-        <v>129</v>
-      </c>
-      <c r="G16" t="s">
-        <v>257</v>
-      </c>
-      <c r="H16" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="B17">
-        <v>2</v>
-      </c>
-      <c r="C17" t="s">
-        <v>160</v>
-      </c>
-      <c r="D17" t="s">
-        <v>161</v>
-      </c>
-      <c r="F17" t="s">
-        <v>129</v>
-      </c>
-      <c r="G17" t="s">
-        <v>255</v>
-      </c>
-      <c r="H17" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <f t="shared" si="0"/>
-        <v>17</v>
-      </c>
-      <c r="B18">
-        <v>2</v>
-      </c>
-      <c r="C18" t="s">
-        <v>162</v>
-      </c>
-      <c r="D18" t="s">
-        <v>163</v>
-      </c>
-      <c r="F18" t="s">
-        <v>129</v>
-      </c>
-      <c r="G18" t="s">
-        <v>255</v>
-      </c>
-      <c r="H18" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-      <c r="B19">
-        <v>2</v>
-      </c>
-      <c r="C19" t="s">
-        <v>164</v>
-      </c>
-      <c r="D19" t="s">
-        <v>165</v>
-      </c>
-      <c r="F19" t="s">
-        <v>129</v>
-      </c>
-      <c r="G19" t="s">
-        <v>255</v>
-      </c>
-      <c r="H19" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <f t="shared" si="0"/>
-        <v>19</v>
-      </c>
-      <c r="B20">
-        <v>2</v>
-      </c>
-      <c r="C20" t="s">
-        <v>166</v>
-      </c>
-      <c r="D20" t="s">
-        <v>167</v>
-      </c>
-      <c r="F20" t="s">
-        <v>129</v>
-      </c>
-      <c r="G20" t="s">
-        <v>129</v>
-      </c>
-      <c r="H20" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="B21">
-        <v>2</v>
-      </c>
-      <c r="C21" t="s">
-        <v>168</v>
-      </c>
-      <c r="D21" t="s">
-        <v>169</v>
-      </c>
-      <c r="F21" t="s">
-        <v>129</v>
-      </c>
-      <c r="G21" t="s">
-        <v>129</v>
-      </c>
-      <c r="H21" t="s">
+      <c r="I23" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <f t="shared" si="0"/>
-        <v>21</v>
-      </c>
-      <c r="B22">
-        <v>2</v>
-      </c>
-      <c r="C22" t="s">
-        <v>170</v>
-      </c>
-      <c r="D22" t="s">
-        <v>171</v>
-      </c>
-      <c r="F22" t="s">
-        <v>129</v>
-      </c>
-      <c r="G22" t="s">
-        <v>258</v>
-      </c>
-      <c r="H22" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <f t="shared" si="0"/>
-        <v>22</v>
-      </c>
-      <c r="B23">
-        <v>2</v>
-      </c>
-      <c r="C23" t="s">
-        <v>172</v>
-      </c>
-      <c r="D23" t="s">
-        <v>173</v>
-      </c>
-      <c r="F23" t="s">
-        <v>129</v>
-      </c>
-      <c r="G23" t="s">
-        <v>260</v>
-      </c>
-      <c r="H23" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24">
         <f t="shared" si="0"/>
-        <v>23</v>
+        <v>81</v>
       </c>
       <c r="B24">
         <v>3</v>
       </c>
-      <c r="C24" t="s">
-        <v>174</v>
+      <c r="C24">
+        <v>1</v>
       </c>
       <c r="D24" t="s">
+        <v>173</v>
+      </c>
+      <c r="E24" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G24" t="s">
+        <v>129</v>
+      </c>
+      <c r="H24" t="s">
+        <v>252</v>
+      </c>
+      <c r="I24" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25">
         <f t="shared" si="0"/>
-        <v>24</v>
+        <v>82</v>
       </c>
       <c r="B25">
         <v>3</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25" t="s">
+        <v>174</v>
+      </c>
+      <c r="E25" t="s">
         <v>175</v>
       </c>
-      <c r="D25" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G25" t="s">
+        <v>129</v>
+      </c>
+      <c r="H25" t="s">
+        <v>129</v>
+      </c>
+      <c r="I25" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26">
         <f t="shared" si="0"/>
-        <v>25</v>
+        <v>83</v>
       </c>
       <c r="B26">
         <v>3</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26" t="s">
+        <v>176</v>
+      </c>
+      <c r="E26" t="s">
         <v>177</v>
       </c>
-      <c r="D26" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G26" t="s">
+        <v>129</v>
+      </c>
+      <c r="H26" t="s">
+        <v>281</v>
+      </c>
+      <c r="I26" t="s">
+        <v>324</v>
+      </c>
+      <c r="J26" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27">
         <f t="shared" si="0"/>
-        <v>26</v>
+        <v>84</v>
       </c>
       <c r="B27">
         <v>3</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27" t="s">
+        <v>178</v>
+      </c>
+      <c r="E27" t="s">
         <v>179</v>
       </c>
-      <c r="D27" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G27" t="s">
+        <v>129</v>
+      </c>
+      <c r="H27" t="s">
+        <v>283</v>
+      </c>
+      <c r="I27" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28">
         <f t="shared" si="0"/>
-        <v>27</v>
+        <v>85</v>
       </c>
       <c r="B28">
         <v>3</v>
       </c>
-      <c r="C28" t="s">
-        <v>181</v>
+      <c r="C28">
+        <v>1</v>
       </c>
       <c r="D28" t="s">
+        <v>180</v>
+      </c>
+      <c r="E28" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G28" t="s">
+        <v>129</v>
+      </c>
+      <c r="H28" t="s">
+        <v>129</v>
+      </c>
+      <c r="I28" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29">
         <f t="shared" si="0"/>
-        <v>28</v>
+        <v>86</v>
       </c>
       <c r="B29">
         <v>3</v>
       </c>
-      <c r="C29" t="s">
-        <v>182</v>
+      <c r="C29">
+        <v>1</v>
       </c>
       <c r="D29" t="s">
+        <v>181</v>
+      </c>
+      <c r="E29" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G29" t="s">
+        <v>129</v>
+      </c>
+      <c r="H29" t="s">
+        <v>253</v>
+      </c>
+      <c r="I29" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30">
         <f t="shared" si="0"/>
-        <v>29</v>
+        <v>87</v>
       </c>
       <c r="B30">
         <v>3</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="D30" t="s">
+        <v>182</v>
+      </c>
+      <c r="E30" t="s">
         <v>183</v>
       </c>
-      <c r="D30" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G30" t="s">
+        <v>129</v>
+      </c>
+      <c r="H30" t="s">
+        <v>287</v>
+      </c>
+      <c r="I30" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>88</v>
       </c>
       <c r="B31">
         <v>3</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31">
+        <v>1</v>
+      </c>
+      <c r="D31" t="s">
+        <v>184</v>
+      </c>
+      <c r="E31" t="s">
         <v>185</v>
       </c>
-      <c r="D31" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G31" t="s">
+        <v>129</v>
+      </c>
+      <c r="H31" t="s">
+        <v>129</v>
+      </c>
+      <c r="I31" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32">
         <f t="shared" si="0"/>
-        <v>31</v>
+        <v>89</v>
       </c>
       <c r="B32">
         <v>3</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="D32" t="s">
+        <v>186</v>
+      </c>
+      <c r="E32" t="s">
         <v>187</v>
       </c>
-      <c r="D32" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G32" t="s">
+        <v>129</v>
+      </c>
+      <c r="H32" t="s">
+        <v>129</v>
+      </c>
+      <c r="I32" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33">
         <f t="shared" si="0"/>
-        <v>32</v>
+        <v>90</v>
       </c>
       <c r="B33">
         <v>3</v>
       </c>
-      <c r="C33" t="s">
-        <v>189</v>
+      <c r="C33">
+        <v>1</v>
       </c>
       <c r="D33" t="s">
+        <v>188</v>
+      </c>
+      <c r="E33" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G33" t="s">
+        <v>129</v>
+      </c>
+      <c r="H33" t="s">
+        <v>255</v>
+      </c>
+      <c r="I33" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34">
-        <f t="shared" ref="A34:A66" si="1">ROW() - 1</f>
-        <v>33</v>
+        <f t="shared" ref="A34:A66" si="1">ROW() + 57</f>
+        <v>91</v>
       </c>
       <c r="B34">
         <v>3</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34">
+        <v>1</v>
+      </c>
+      <c r="D34" t="s">
+        <v>189</v>
+      </c>
+      <c r="E34" t="s">
         <v>190</v>
       </c>
-      <c r="D34" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G34" t="s">
+        <v>129</v>
+      </c>
+      <c r="H34" t="s">
+        <v>252</v>
+      </c>
+      <c r="I34" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35">
         <f t="shared" si="1"/>
-        <v>34</v>
+        <v>92</v>
       </c>
       <c r="B35">
         <v>3</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C35">
+        <v>1</v>
+      </c>
+      <c r="D35" t="s">
+        <v>191</v>
+      </c>
+      <c r="E35" t="s">
         <v>192</v>
       </c>
-      <c r="D35" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G35" t="s">
+        <v>129</v>
+      </c>
+      <c r="H35" t="s">
+        <v>281</v>
+      </c>
+      <c r="I35" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36">
         <f t="shared" si="1"/>
-        <v>35</v>
+        <v>93</v>
       </c>
       <c r="B36">
         <v>3</v>
       </c>
-      <c r="C36" t="s">
-        <v>194</v>
+      <c r="C36">
+        <v>1</v>
       </c>
       <c r="D36" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+        <v>193</v>
+      </c>
+      <c r="E36" t="s">
+        <v>158</v>
+      </c>
+      <c r="G36" t="s">
+        <v>129</v>
+      </c>
+      <c r="H36" t="s">
+        <v>256</v>
+      </c>
+      <c r="I36" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37">
         <f t="shared" si="1"/>
-        <v>36</v>
+        <v>94</v>
       </c>
       <c r="B37">
         <v>3</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C37">
+        <v>1</v>
+      </c>
+      <c r="D37" t="s">
+        <v>194</v>
+      </c>
+      <c r="E37" t="s">
         <v>195</v>
       </c>
-      <c r="D37" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G37" t="s">
+        <v>129</v>
+      </c>
+      <c r="H37" t="s">
+        <v>294</v>
+      </c>
+      <c r="I37" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38">
         <f t="shared" si="1"/>
-        <v>37</v>
+        <v>95</v>
       </c>
       <c r="B38">
         <v>3</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C38">
+        <v>1</v>
+      </c>
+      <c r="D38" t="s">
+        <v>196</v>
+      </c>
+      <c r="E38" t="s">
         <v>197</v>
       </c>
-      <c r="D38" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G38" t="s">
+        <v>129</v>
+      </c>
+      <c r="H38" t="s">
+        <v>296</v>
+      </c>
+      <c r="I38" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39">
         <f t="shared" si="1"/>
-        <v>38</v>
+        <v>96</v>
       </c>
       <c r="B39">
         <v>3</v>
       </c>
-      <c r="C39" t="s">
-        <v>199</v>
+      <c r="C39">
+        <v>1</v>
       </c>
       <c r="D39" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+        <v>198</v>
+      </c>
+      <c r="E39" t="s">
+        <v>162</v>
+      </c>
+      <c r="G39" t="s">
+        <v>129</v>
+      </c>
+      <c r="H39" t="s">
+        <v>254</v>
+      </c>
+      <c r="I39" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40">
         <f t="shared" si="1"/>
-        <v>39</v>
+        <v>97</v>
       </c>
       <c r="B40">
         <v>3</v>
       </c>
-      <c r="C40" t="s">
-        <v>200</v>
+      <c r="C40">
+        <v>1</v>
       </c>
       <c r="D40" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+        <v>199</v>
+      </c>
+      <c r="E40" t="s">
+        <v>164</v>
+      </c>
+      <c r="G40" t="s">
+        <v>129</v>
+      </c>
+      <c r="H40" t="s">
+        <v>254</v>
+      </c>
+      <c r="I40" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41">
         <f t="shared" si="1"/>
-        <v>40</v>
+        <v>98</v>
       </c>
       <c r="B41">
         <v>3</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C41">
+        <v>1</v>
+      </c>
+      <c r="D41" t="s">
+        <v>200</v>
+      </c>
+      <c r="E41" t="s">
         <v>201</v>
       </c>
-      <c r="D41" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G41" t="s">
+        <v>129</v>
+      </c>
+      <c r="H41" t="s">
+        <v>281</v>
+      </c>
+      <c r="I41" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42">
         <f t="shared" si="1"/>
-        <v>41</v>
+        <v>99</v>
       </c>
       <c r="B42">
         <v>3</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C42">
+        <v>1</v>
+      </c>
+      <c r="D42" t="s">
+        <v>202</v>
+      </c>
+      <c r="E42" t="s">
         <v>203</v>
       </c>
-      <c r="D42" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G42" t="s">
+        <v>129</v>
+      </c>
+      <c r="H42" t="s">
+        <v>293</v>
+      </c>
+      <c r="I42" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43">
         <f t="shared" si="1"/>
-        <v>42</v>
+        <v>100</v>
       </c>
       <c r="B43">
         <v>3</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C43">
+        <v>1</v>
+      </c>
+      <c r="D43" t="s">
+        <v>204</v>
+      </c>
+      <c r="E43" t="s">
         <v>205</v>
       </c>
-      <c r="D43" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G43" t="s">
+        <v>129</v>
+      </c>
+      <c r="H43" t="s">
+        <v>319</v>
+      </c>
+      <c r="I43" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44">
         <f t="shared" si="1"/>
-        <v>43</v>
+        <v>101</v>
       </c>
       <c r="B44">
         <v>3</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C44">
+        <v>1</v>
+      </c>
+      <c r="D44" t="s">
+        <v>206</v>
+      </c>
+      <c r="E44" t="s">
+        <v>170</v>
+      </c>
+      <c r="G44" t="s">
+        <v>129</v>
+      </c>
+      <c r="H44" t="s">
+        <v>320</v>
+      </c>
+      <c r="I44" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <f t="shared" si="1"/>
+        <v>102</v>
+      </c>
+      <c r="B45">
+        <v>4</v>
+      </c>
+      <c r="C45">
+        <v>1</v>
+      </c>
+      <c r="D45" t="s">
         <v>207</v>
       </c>
-      <c r="D44" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45">
-        <f t="shared" si="1"/>
-        <v>44</v>
-      </c>
-      <c r="B45">
-        <v>4</v>
-      </c>
-      <c r="C45" t="s">
+      <c r="E45" t="s">
         <v>208</v>
       </c>
-      <c r="D45" t="s">
+      <c r="G45" t="s">
+        <v>129</v>
+      </c>
+      <c r="H45" t="s">
+        <v>302</v>
+      </c>
+      <c r="I45" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <f t="shared" si="1"/>
+        <v>103</v>
+      </c>
+      <c r="B46">
+        <v>4</v>
+      </c>
+      <c r="C46">
+        <v>1</v>
+      </c>
+      <c r="D46" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46">
-        <f t="shared" si="1"/>
-        <v>45</v>
-      </c>
-      <c r="B46">
-        <v>4</v>
-      </c>
-      <c r="C46" t="s">
+      <c r="E46" t="s">
+        <v>133</v>
+      </c>
+      <c r="G46" t="s">
+        <v>129</v>
+      </c>
+      <c r="H46" t="s">
+        <v>252</v>
+      </c>
+      <c r="I46" t="s">
+        <v>309</v>
+      </c>
+      <c r="J46" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <f t="shared" si="1"/>
+        <v>104</v>
+      </c>
+      <c r="B47">
+        <v>4</v>
+      </c>
+      <c r="C47">
+        <v>1</v>
+      </c>
+      <c r="D47" t="s">
         <v>210</v>
       </c>
-      <c r="D46" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47">
-        <f t="shared" si="1"/>
-        <v>46</v>
-      </c>
-      <c r="B47">
-        <v>4</v>
-      </c>
-      <c r="C47" t="s">
+      <c r="E47" t="s">
         <v>211</v>
       </c>
-      <c r="D47" t="s">
+      <c r="G47" t="s">
+        <v>129</v>
+      </c>
+      <c r="H47" t="s">
+        <v>254</v>
+      </c>
+      <c r="I47" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <f t="shared" si="1"/>
+        <v>105</v>
+      </c>
+      <c r="B48">
+        <v>4</v>
+      </c>
+      <c r="C48">
+        <v>1</v>
+      </c>
+      <c r="D48" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48">
-        <f t="shared" si="1"/>
-        <v>47</v>
-      </c>
-      <c r="B48">
-        <v>4</v>
-      </c>
-      <c r="C48" t="s">
+      <c r="E48" t="s">
         <v>213</v>
       </c>
-      <c r="D48" t="s">
+      <c r="G48" t="s">
+        <v>129</v>
+      </c>
+      <c r="H48" t="s">
+        <v>305</v>
+      </c>
+      <c r="I48" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <f t="shared" si="1"/>
+        <v>106</v>
+      </c>
+      <c r="B49">
+        <v>4</v>
+      </c>
+      <c r="C49">
+        <v>1</v>
+      </c>
+      <c r="D49" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49">
-        <f t="shared" si="1"/>
-        <v>48</v>
-      </c>
-      <c r="B49">
-        <v>4</v>
-      </c>
-      <c r="C49" t="s">
+      <c r="E49" t="s">
+        <v>135</v>
+      </c>
+      <c r="G49" t="s">
+        <v>129</v>
+      </c>
+      <c r="H49" t="s">
+        <v>307</v>
+      </c>
+      <c r="I49" t="s">
+        <v>310</v>
+      </c>
+      <c r="J49" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <f t="shared" si="1"/>
+        <v>107</v>
+      </c>
+      <c r="B50">
+        <v>4</v>
+      </c>
+      <c r="C50">
+        <v>1</v>
+      </c>
+      <c r="D50" t="s">
         <v>215</v>
       </c>
-      <c r="D49" t="s">
+      <c r="E50" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50">
-        <f t="shared" si="1"/>
-        <v>49</v>
-      </c>
-      <c r="B50">
-        <v>4</v>
-      </c>
-      <c r="C50" t="s">
+      <c r="G50" t="s">
+        <v>129</v>
+      </c>
+      <c r="H50" t="s">
+        <v>307</v>
+      </c>
+      <c r="I50" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <f t="shared" si="1"/>
+        <v>108</v>
+      </c>
+      <c r="B51">
+        <v>4</v>
+      </c>
+      <c r="C51">
+        <v>1</v>
+      </c>
+      <c r="D51" t="s">
         <v>216</v>
       </c>
-      <c r="D50" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51">
-        <f t="shared" si="1"/>
-        <v>50</v>
-      </c>
-      <c r="B51">
-        <v>4</v>
-      </c>
-      <c r="C51" t="s">
+      <c r="E51" t="s">
         <v>217</v>
       </c>
-      <c r="D51" t="s">
+      <c r="G51" t="s">
+        <v>129</v>
+      </c>
+      <c r="H51" t="s">
+        <v>311</v>
+      </c>
+      <c r="I51" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <f t="shared" si="1"/>
+        <v>109</v>
+      </c>
+      <c r="B52">
+        <v>4</v>
+      </c>
+      <c r="C52">
+        <v>1</v>
+      </c>
+      <c r="D52" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52">
-        <f t="shared" si="1"/>
-        <v>51</v>
-      </c>
-      <c r="B52">
-        <v>4</v>
-      </c>
-      <c r="C52" t="s">
+      <c r="E52" t="s">
+        <v>138</v>
+      </c>
+      <c r="G52" t="s">
+        <v>129</v>
+      </c>
+      <c r="H52" t="s">
+        <v>313</v>
+      </c>
+      <c r="I52" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <f t="shared" si="1"/>
+        <v>110</v>
+      </c>
+      <c r="B53">
+        <v>4</v>
+      </c>
+      <c r="C53">
+        <v>1</v>
+      </c>
+      <c r="D53" t="s">
         <v>219</v>
       </c>
-      <c r="D52" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53">
-        <f t="shared" si="1"/>
-        <v>52</v>
-      </c>
-      <c r="B53">
-        <v>4</v>
-      </c>
-      <c r="C53" t="s">
+      <c r="E53" t="s">
+        <v>183</v>
+      </c>
+      <c r="G53" t="s">
+        <v>129</v>
+      </c>
+      <c r="H53" t="s">
+        <v>287</v>
+      </c>
+      <c r="I53" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <f t="shared" si="1"/>
+        <v>111</v>
+      </c>
+      <c r="B54">
+        <v>4</v>
+      </c>
+      <c r="C54">
+        <v>1</v>
+      </c>
+      <c r="D54" t="s">
         <v>220</v>
       </c>
-      <c r="D53" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54">
-        <f t="shared" si="1"/>
-        <v>53</v>
-      </c>
-      <c r="B54">
-        <v>4</v>
-      </c>
-      <c r="C54" t="s">
+      <c r="E54" t="s">
         <v>221</v>
       </c>
-      <c r="D54" t="s">
+      <c r="G54" t="s">
+        <v>129</v>
+      </c>
+      <c r="H54" t="s">
+        <v>323</v>
+      </c>
+      <c r="I54" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <f t="shared" si="1"/>
+        <v>112</v>
+      </c>
+      <c r="B55">
+        <v>4</v>
+      </c>
+      <c r="C55">
+        <v>1</v>
+      </c>
+      <c r="D55" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55">
-        <f t="shared" si="1"/>
-        <v>54</v>
-      </c>
-      <c r="B55">
-        <v>4</v>
-      </c>
-      <c r="C55" t="s">
+      <c r="E55" t="s">
         <v>223</v>
       </c>
-      <c r="D55" t="s">
+      <c r="G55" t="s">
+        <v>129</v>
+      </c>
+      <c r="H55" t="s">
+        <v>317</v>
+      </c>
+      <c r="I55" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <f t="shared" si="1"/>
+        <v>113</v>
+      </c>
+      <c r="B56">
+        <v>4</v>
+      </c>
+      <c r="C56">
+        <v>1</v>
+      </c>
+      <c r="D56" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56">
-        <f t="shared" si="1"/>
-        <v>55</v>
-      </c>
-      <c r="B56">
-        <v>4</v>
-      </c>
-      <c r="C56" t="s">
+      <c r="E56" t="s">
+        <v>152</v>
+      </c>
+      <c r="G56" t="s">
+        <v>129</v>
+      </c>
+      <c r="H56" t="s">
+        <v>316</v>
+      </c>
+      <c r="I56" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <f t="shared" si="1"/>
+        <v>114</v>
+      </c>
+      <c r="B57">
+        <v>4</v>
+      </c>
+      <c r="C57">
+        <v>1</v>
+      </c>
+      <c r="D57" t="s">
         <v>225</v>
       </c>
-      <c r="D56" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57">
-        <f t="shared" si="1"/>
-        <v>56</v>
-      </c>
-      <c r="B57">
-        <v>4</v>
-      </c>
-      <c r="C57" t="s">
+      <c r="E57" t="s">
         <v>226</v>
       </c>
-      <c r="D57" t="s">
+      <c r="G57" t="s">
+        <v>129</v>
+      </c>
+      <c r="H57" t="s">
+        <v>321</v>
+      </c>
+      <c r="I57" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <f t="shared" si="1"/>
+        <v>115</v>
+      </c>
+      <c r="B58">
+        <v>4</v>
+      </c>
+      <c r="C58">
+        <v>1</v>
+      </c>
+      <c r="D58" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58">
-        <f t="shared" si="1"/>
-        <v>57</v>
-      </c>
-      <c r="B58">
-        <v>4</v>
-      </c>
-      <c r="C58" t="s">
+      <c r="E58" t="s">
+        <v>158</v>
+      </c>
+      <c r="G58" t="s">
+        <v>129</v>
+      </c>
+      <c r="H58" t="s">
+        <v>256</v>
+      </c>
+      <c r="I58" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <f t="shared" si="1"/>
+        <v>116</v>
+      </c>
+      <c r="B59">
+        <v>4</v>
+      </c>
+      <c r="C59">
+        <v>1</v>
+      </c>
+      <c r="D59" t="s">
         <v>228</v>
       </c>
-      <c r="D58" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59">
-        <f t="shared" si="1"/>
-        <v>58</v>
-      </c>
-      <c r="B59">
-        <v>4</v>
-      </c>
-      <c r="C59" t="s">
+      <c r="E59" t="s">
         <v>229</v>
       </c>
-      <c r="D59" t="s">
+      <c r="G59" t="b">
+        <v>1</v>
+      </c>
+      <c r="H59" t="s">
+        <v>129</v>
+      </c>
+      <c r="I59" t="s">
+        <v>327</v>
+      </c>
+      <c r="J59" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <f t="shared" si="1"/>
+        <v>117</v>
+      </c>
+      <c r="B60">
+        <v>4</v>
+      </c>
+      <c r="C60">
+        <v>1</v>
+      </c>
+      <c r="D60" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60">
-        <f t="shared" si="1"/>
-        <v>59</v>
-      </c>
-      <c r="B60">
-        <v>4</v>
-      </c>
-      <c r="C60" t="s">
+      <c r="E60" t="s">
         <v>231</v>
       </c>
-      <c r="D60" t="s">
+      <c r="G60" t="s">
+        <v>129</v>
+      </c>
+      <c r="H60" t="s">
+        <v>302</v>
+      </c>
+      <c r="I60" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <f t="shared" si="1"/>
+        <v>118</v>
+      </c>
+      <c r="B61">
+        <v>4</v>
+      </c>
+      <c r="C61">
+        <v>1</v>
+      </c>
+      <c r="D61" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61">
-        <f t="shared" si="1"/>
-        <v>60</v>
-      </c>
-      <c r="B61">
-        <v>4</v>
-      </c>
-      <c r="C61" t="s">
+      <c r="E61" t="s">
         <v>233</v>
       </c>
-      <c r="D61" t="s">
+      <c r="G61" t="s">
+        <v>129</v>
+      </c>
+      <c r="H61" t="s">
+        <v>328</v>
+      </c>
+      <c r="I61" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <f t="shared" si="1"/>
+        <v>119</v>
+      </c>
+      <c r="B62">
+        <v>4</v>
+      </c>
+      <c r="C62">
+        <v>1</v>
+      </c>
+      <c r="D62" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62">
-        <f t="shared" si="1"/>
-        <v>61</v>
-      </c>
-      <c r="B62">
-        <v>4</v>
-      </c>
-      <c r="C62" t="s">
+      <c r="E62" t="s">
+        <v>162</v>
+      </c>
+      <c r="G62" t="s">
+        <v>129</v>
+      </c>
+      <c r="H62" t="s">
+        <v>254</v>
+      </c>
+      <c r="I62" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <f t="shared" si="1"/>
+        <v>120</v>
+      </c>
+      <c r="B63">
+        <v>4</v>
+      </c>
+      <c r="C63">
+        <v>1</v>
+      </c>
+      <c r="D63" t="s">
         <v>235</v>
       </c>
-      <c r="D62" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63">
-        <f t="shared" si="1"/>
-        <v>62</v>
-      </c>
-      <c r="B63">
-        <v>4</v>
-      </c>
-      <c r="C63" t="s">
+      <c r="E63" t="s">
         <v>236</v>
       </c>
-      <c r="D63" t="s">
+      <c r="G63" t="s">
+        <v>129</v>
+      </c>
+      <c r="H63" t="s">
+        <v>330</v>
+      </c>
+      <c r="I63" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A64">
+        <f t="shared" si="1"/>
+        <v>121</v>
+      </c>
+      <c r="B64">
+        <v>4</v>
+      </c>
+      <c r="C64">
+        <v>1</v>
+      </c>
+      <c r="D64" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64">
-        <f t="shared" si="1"/>
-        <v>63</v>
-      </c>
-      <c r="B64">
-        <v>4</v>
-      </c>
-      <c r="C64" t="s">
+      <c r="E64" t="s">
+        <v>170</v>
+      </c>
+      <c r="G64" t="s">
+        <v>129</v>
+      </c>
+      <c r="H64" t="s">
+        <v>331</v>
+      </c>
+      <c r="I64" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A65">
+        <f t="shared" si="1"/>
+        <v>122</v>
+      </c>
+      <c r="B65">
+        <v>4</v>
+      </c>
+      <c r="C65">
+        <v>1</v>
+      </c>
+      <c r="D65" t="s">
         <v>238</v>
       </c>
-      <c r="D64" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65">
-        <f t="shared" si="1"/>
-        <v>64</v>
-      </c>
-      <c r="B65">
-        <v>4</v>
-      </c>
-      <c r="C65" t="s">
+      <c r="E65" t="s">
         <v>239</v>
       </c>
-      <c r="D65" t="s">
+      <c r="G65" t="s">
+        <v>129</v>
+      </c>
+      <c r="H65" t="s">
+        <v>319</v>
+      </c>
+      <c r="I65" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A66">
+        <f t="shared" si="1"/>
+        <v>123</v>
+      </c>
+      <c r="B66">
+        <v>4</v>
+      </c>
+      <c r="C66">
+        <v>1</v>
+      </c>
+      <c r="D66" t="s">
         <v>240</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66">
-        <f t="shared" si="1"/>
-        <v>65</v>
-      </c>
-      <c r="B66">
-        <v>4</v>
-      </c>
-      <c r="C66" t="s">
+      <c r="E66" t="s">
         <v>241</v>
       </c>
-      <c r="D66" t="s">
-        <v>242</v>
+      <c r="G66" t="s">
+        <v>129</v>
+      </c>
+      <c r="H66" t="s">
+        <v>129</v>
+      </c>
+      <c r="I66" t="s">
+        <v>332</v>
       </c>
     </row>
   </sheetData>
@@ -3867,14 +4617,14 @@
       <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="3" width="18.875" customWidth="1"/>
-    <col min="4" max="4" width="18.875" style="1" customWidth="1"/>
-    <col min="5" max="10" width="18.875" customWidth="1"/>
+    <col min="1" max="3" width="18.83203125" customWidth="1"/>
+    <col min="4" max="4" width="18.83203125" style="1" customWidth="1"/>
+    <col min="5" max="10" width="18.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3897,7 +4647,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3917,7 +4667,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3937,7 +4687,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -3960,7 +4710,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -3980,7 +4730,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -4000,7 +4750,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -4020,7 +4770,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -4040,7 +4790,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -4060,7 +4810,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>34</v>
       </c>
@@ -4068,7 +4818,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>36</v>
       </c>
@@ -4076,12 +4826,12 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -4113,7 +4863,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>1</v>
       </c>
@@ -4142,7 +4892,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>2</v>
       </c>
@@ -4171,7 +4921,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>3</v>
       </c>
@@ -4200,7 +4950,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>4</v>
       </c>
@@ -4229,7 +4979,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>5</v>
       </c>
@@ -4258,7 +5008,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>6</v>
       </c>
@@ -4287,7 +5037,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>7</v>
       </c>
@@ -4316,7 +5066,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>8</v>
       </c>
@@ -4345,7 +5095,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="D24"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated databse: corrected errors
</commit_message>
<xml_diff>
--- a/data/TP Database.xlsx
+++ b/data/TP Database.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sophiachung/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sophiachung/cs01-main/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{74A9764C-AA4B-034B-AD6E-5334636B3DBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B51C7AB-3926-104C-B7E0-A9AB133A3B24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13340" yWindow="500" windowWidth="15460" windowHeight="15880" activeTab="1" xr2:uid="{F6F91125-3C8A-D047-93DD-1F3A6DE88698}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="333">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="332">
   <si>
     <t>CardID</t>
   </si>
@@ -836,9 +836,6 @@
     <t>i(79/101/121):1:(2/3/4)</t>
   </si>
   <si>
-    <t>b0:2:(3&amp;4)</t>
-  </si>
-  <si>
     <t xml:space="preserve">remove one relevant or very relevant article tile </t>
   </si>
   <si>
@@ -935,9 +932,6 @@
     <t>n(33/34/35/36):1, n(45/46):1</t>
   </si>
   <si>
-    <t>b0:2:4</t>
-  </si>
-  <si>
     <t>n(33/34/35/36/43/44):2</t>
   </si>
   <si>
@@ -1035,6 +1029,9 @@
   </si>
   <si>
     <t>n49:2</t>
+  </si>
+  <si>
+    <t>o0:2:4</t>
   </si>
 </sst>
 </file>
@@ -2773,8 +2770,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84DC5E79-A11F-0148-B3A8-F5384824D987}">
   <dimension ref="A1:J66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D34" zoomScale="99" workbookViewId="0">
-      <selection activeCell="I67" sqref="I67"/>
+    <sheetView tabSelected="1" topLeftCell="E7" zoomScale="99" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2843,7 +2840,7 @@
         <v>129</v>
       </c>
       <c r="I2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
@@ -2870,7 +2867,7 @@
         <v>129</v>
       </c>
       <c r="I3" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
@@ -3005,10 +3002,10 @@
         <v>129</v>
       </c>
       <c r="I8" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="J8" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
@@ -3035,7 +3032,7 @@
         <v>129</v>
       </c>
       <c r="I9" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
@@ -3062,10 +3059,10 @@
         <v>254</v>
       </c>
       <c r="I10" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="J10" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
@@ -3092,7 +3089,7 @@
         <v>258</v>
       </c>
       <c r="I11" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="J11" s="2" t="s">
         <v>147</v>
@@ -3122,7 +3119,7 @@
         <v>254</v>
       </c>
       <c r="I12" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="J12" t="s">
         <v>150</v>
@@ -3152,7 +3149,7 @@
         <v>255</v>
       </c>
       <c r="I13" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
@@ -3179,7 +3176,7 @@
         <v>129</v>
       </c>
       <c r="I14" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
@@ -3200,7 +3197,7 @@
         <v>156</v>
       </c>
       <c r="G15" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="H15" t="s">
         <v>129</v>
@@ -3209,7 +3206,7 @@
         <v>265</v>
       </c>
       <c r="J15" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
@@ -3263,7 +3260,7 @@
         <v>254</v>
       </c>
       <c r="I17" t="s">
-        <v>266</v>
+        <v>277</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
@@ -3371,7 +3368,7 @@
         <v>129</v>
       </c>
       <c r="I21" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
@@ -3425,7 +3422,7 @@
         <v>259</v>
       </c>
       <c r="I23" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
@@ -3452,7 +3449,7 @@
         <v>252</v>
       </c>
       <c r="I24" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
@@ -3479,7 +3476,7 @@
         <v>129</v>
       </c>
       <c r="I25" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
@@ -3503,13 +3500,13 @@
         <v>129</v>
       </c>
       <c r="H26" t="s">
+        <v>280</v>
+      </c>
+      <c r="I26" t="s">
+        <v>322</v>
+      </c>
+      <c r="J26" t="s">
         <v>281</v>
-      </c>
-      <c r="I26" t="s">
-        <v>324</v>
-      </c>
-      <c r="J26" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.2">
@@ -3533,10 +3530,10 @@
         <v>129</v>
       </c>
       <c r="H27" t="s">
+        <v>282</v>
+      </c>
+      <c r="I27" t="s">
         <v>283</v>
-      </c>
-      <c r="I27" t="s">
-        <v>284</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.2">
@@ -3563,7 +3560,7 @@
         <v>129</v>
       </c>
       <c r="I28" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.2">
@@ -3590,7 +3587,7 @@
         <v>253</v>
       </c>
       <c r="I29" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.2">
@@ -3614,10 +3611,10 @@
         <v>129</v>
       </c>
       <c r="H30" t="s">
+        <v>286</v>
+      </c>
+      <c r="I30" t="s">
         <v>287</v>
-      </c>
-      <c r="I30" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.2">
@@ -3644,7 +3641,7 @@
         <v>129</v>
       </c>
       <c r="I31" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.2">
@@ -3671,7 +3668,7 @@
         <v>129</v>
       </c>
       <c r="I32" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.2">
@@ -3698,7 +3695,7 @@
         <v>255</v>
       </c>
       <c r="I33" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.2">
@@ -3725,7 +3722,7 @@
         <v>252</v>
       </c>
       <c r="I34" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.2">
@@ -3749,10 +3746,10 @@
         <v>129</v>
       </c>
       <c r="H35" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="I35" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.2">
@@ -3779,7 +3776,7 @@
         <v>256</v>
       </c>
       <c r="I36" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.2">
@@ -3803,10 +3800,10 @@
         <v>129</v>
       </c>
       <c r="H37" t="s">
+        <v>293</v>
+      </c>
+      <c r="I37" t="s">
         <v>294</v>
-      </c>
-      <c r="I37" t="s">
-        <v>295</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.2">
@@ -3830,10 +3827,10 @@
         <v>129</v>
       </c>
       <c r="H38" t="s">
+        <v>295</v>
+      </c>
+      <c r="I38" t="s">
         <v>296</v>
-      </c>
-      <c r="I38" t="s">
-        <v>297</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.2">
@@ -3860,7 +3857,7 @@
         <v>254</v>
       </c>
       <c r="I39" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.2">
@@ -3887,7 +3884,7 @@
         <v>254</v>
       </c>
       <c r="I40" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.2">
@@ -3911,10 +3908,10 @@
         <v>129</v>
       </c>
       <c r="H41" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="I41" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.2">
@@ -3938,10 +3935,10 @@
         <v>129</v>
       </c>
       <c r="H42" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="I42" t="s">
-        <v>299</v>
+        <v>331</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.2">
@@ -3965,10 +3962,10 @@
         <v>129</v>
       </c>
       <c r="H43" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="I43" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.2">
@@ -3992,10 +3989,10 @@
         <v>129</v>
       </c>
       <c r="H44" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="I44" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.2">
@@ -4019,10 +4016,10 @@
         <v>129</v>
       </c>
       <c r="H45" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="I45" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.2">
@@ -4049,10 +4046,10 @@
         <v>252</v>
       </c>
       <c r="I46" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="J46" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.2">
@@ -4079,7 +4076,7 @@
         <v>254</v>
       </c>
       <c r="I47" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.2">
@@ -4103,10 +4100,10 @@
         <v>129</v>
       </c>
       <c r="H48" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="I48" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.2">
@@ -4130,13 +4127,13 @@
         <v>129</v>
       </c>
       <c r="H49" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="I49" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="J49" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.2">
@@ -4160,10 +4157,10 @@
         <v>129</v>
       </c>
       <c r="H50" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="I50" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.2">
@@ -4187,10 +4184,10 @@
         <v>129</v>
       </c>
       <c r="H51" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="I51" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.2">
@@ -4214,10 +4211,10 @@
         <v>129</v>
       </c>
       <c r="H52" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="I52" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.2">
@@ -4241,10 +4238,10 @@
         <v>129</v>
       </c>
       <c r="H53" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I53" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.2">
@@ -4268,10 +4265,10 @@
         <v>129</v>
       </c>
       <c r="H54" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="I54" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.2">
@@ -4295,10 +4292,10 @@
         <v>129</v>
       </c>
       <c r="H55" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="I55" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.2">
@@ -4322,10 +4319,10 @@
         <v>129</v>
       </c>
       <c r="H56" t="s">
+        <v>314</v>
+      </c>
+      <c r="I56" t="s">
         <v>316</v>
-      </c>
-      <c r="I56" t="s">
-        <v>318</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.2">
@@ -4349,10 +4346,10 @@
         <v>129</v>
       </c>
       <c r="H57" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="I57" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.2">
@@ -4379,7 +4376,7 @@
         <v>256</v>
       </c>
       <c r="I58" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.2">
@@ -4406,10 +4403,10 @@
         <v>129</v>
       </c>
       <c r="I59" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="J59" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.2">
@@ -4433,10 +4430,10 @@
         <v>129</v>
       </c>
       <c r="H60" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="I60" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.2">
@@ -4460,10 +4457,10 @@
         <v>129</v>
       </c>
       <c r="H61" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="I61" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.2">
@@ -4490,7 +4487,7 @@
         <v>254</v>
       </c>
       <c r="I62" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.2">
@@ -4514,10 +4511,10 @@
         <v>129</v>
       </c>
       <c r="H63" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="I63" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.2">
@@ -4541,10 +4538,10 @@
         <v>129</v>
       </c>
       <c r="H64" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="I64" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.2">
@@ -4568,10 +4565,10 @@
         <v>129</v>
       </c>
       <c r="H65" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="I65" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.2">
@@ -4598,7 +4595,7 @@
         <v>129</v>
       </c>
       <c r="I66" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update database: correct errors
</commit_message>
<xml_diff>
--- a/data/TP Database.xlsx
+++ b/data/TP Database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sophiachung/cs01-main/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B51C7AB-3926-104C-B7E0-A9AB133A3B24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ED460C1-C0F1-7946-9B66-5674DDD2B7E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13340" yWindow="500" windowWidth="15460" windowHeight="15880" activeTab="1" xr2:uid="{F6F91125-3C8A-D047-93DD-1F3A6DE88698}"/>
   </bookViews>
@@ -908,9 +908,6 @@
     <t>n0:1:3</t>
   </si>
   <si>
-    <t>n41:1, , n(42/45/46):2</t>
-  </si>
-  <si>
     <t>n(43/44):2</t>
   </si>
   <si>
@@ -1032,6 +1029,9 @@
   </si>
   <si>
     <t>o0:2:4</t>
+  </si>
+  <si>
+    <t>n41:1&amp;n(42/45/46):2</t>
   </si>
 </sst>
 </file>
@@ -2770,8 +2770,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84DC5E79-A11F-0148-B3A8-F5384824D987}">
   <dimension ref="A1:J66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E7" zoomScale="99" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView tabSelected="1" topLeftCell="E20" zoomScale="99" workbookViewId="0">
+      <selection activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3197,7 +3197,7 @@
         <v>156</v>
       </c>
       <c r="G15" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="H15" t="s">
         <v>129</v>
@@ -3503,7 +3503,7 @@
         <v>280</v>
       </c>
       <c r="I26" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="J26" t="s">
         <v>281</v>
@@ -3668,7 +3668,7 @@
         <v>129</v>
       </c>
       <c r="I32" t="s">
-        <v>290</v>
+        <v>331</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.2">
@@ -3722,7 +3722,7 @@
         <v>252</v>
       </c>
       <c r="I34" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.2">
@@ -3749,7 +3749,7 @@
         <v>280</v>
       </c>
       <c r="I35" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.2">
@@ -3800,10 +3800,10 @@
         <v>129</v>
       </c>
       <c r="H37" t="s">
+        <v>292</v>
+      </c>
+      <c r="I37" t="s">
         <v>293</v>
-      </c>
-      <c r="I37" t="s">
-        <v>294</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.2">
@@ -3827,10 +3827,10 @@
         <v>129</v>
       </c>
       <c r="H38" t="s">
+        <v>294</v>
+      </c>
+      <c r="I38" t="s">
         <v>295</v>
-      </c>
-      <c r="I38" t="s">
-        <v>296</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.2">
@@ -3911,7 +3911,7 @@
         <v>280</v>
       </c>
       <c r="I41" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.2">
@@ -3935,10 +3935,10 @@
         <v>129</v>
       </c>
       <c r="H42" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="I42" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.2">
@@ -3962,10 +3962,10 @@
         <v>129</v>
       </c>
       <c r="H43" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="I43" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.2">
@@ -3989,7 +3989,7 @@
         <v>129</v>
       </c>
       <c r="H44" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="I44" t="s">
         <v>289</v>
@@ -4016,10 +4016,10 @@
         <v>129</v>
       </c>
       <c r="H45" t="s">
+        <v>299</v>
+      </c>
+      <c r="I45" t="s">
         <v>300</v>
-      </c>
-      <c r="I45" t="s">
-        <v>301</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.2">
@@ -4046,10 +4046,10 @@
         <v>252</v>
       </c>
       <c r="I46" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="J46" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.2">
@@ -4076,7 +4076,7 @@
         <v>254</v>
       </c>
       <c r="I47" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.2">
@@ -4100,10 +4100,10 @@
         <v>129</v>
       </c>
       <c r="H48" t="s">
+        <v>302</v>
+      </c>
+      <c r="I48" t="s">
         <v>303</v>
-      </c>
-      <c r="I48" t="s">
-        <v>304</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.2">
@@ -4127,13 +4127,13 @@
         <v>129</v>
       </c>
       <c r="H49" t="s">
+        <v>304</v>
+      </c>
+      <c r="I49" t="s">
+        <v>307</v>
+      </c>
+      <c r="J49" t="s">
         <v>305</v>
-      </c>
-      <c r="I49" t="s">
-        <v>308</v>
-      </c>
-      <c r="J49" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.2">
@@ -4157,10 +4157,10 @@
         <v>129</v>
       </c>
       <c r="H50" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="I50" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.2">
@@ -4184,10 +4184,10 @@
         <v>129</v>
       </c>
       <c r="H51" t="s">
+        <v>308</v>
+      </c>
+      <c r="I51" t="s">
         <v>309</v>
-      </c>
-      <c r="I51" t="s">
-        <v>310</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.2">
@@ -4211,10 +4211,10 @@
         <v>129</v>
       </c>
       <c r="H52" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="I52" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.2">
@@ -4241,7 +4241,7 @@
         <v>286</v>
       </c>
       <c r="I53" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.2">
@@ -4265,10 +4265,10 @@
         <v>129</v>
       </c>
       <c r="H54" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="I54" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.2">
@@ -4292,10 +4292,10 @@
         <v>129</v>
       </c>
       <c r="H55" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="I55" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.2">
@@ -4319,10 +4319,10 @@
         <v>129</v>
       </c>
       <c r="H56" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="I56" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.2">
@@ -4346,10 +4346,10 @@
         <v>129</v>
       </c>
       <c r="H57" t="s">
+        <v>318</v>
+      </c>
+      <c r="I57" t="s">
         <v>319</v>
-      </c>
-      <c r="I57" t="s">
-        <v>320</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.2">
@@ -4376,7 +4376,7 @@
         <v>256</v>
       </c>
       <c r="I58" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.2">
@@ -4403,10 +4403,10 @@
         <v>129</v>
       </c>
       <c r="I59" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="J59" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.2">
@@ -4430,10 +4430,10 @@
         <v>129</v>
       </c>
       <c r="H60" t="s">
+        <v>299</v>
+      </c>
+      <c r="I60" t="s">
         <v>300</v>
-      </c>
-      <c r="I60" t="s">
-        <v>301</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.2">
@@ -4457,10 +4457,10 @@
         <v>129</v>
       </c>
       <c r="H61" t="s">
+        <v>325</v>
+      </c>
+      <c r="I61" t="s">
         <v>326</v>
-      </c>
-      <c r="I61" t="s">
-        <v>327</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.2">
@@ -4487,7 +4487,7 @@
         <v>254</v>
       </c>
       <c r="I62" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.2">
@@ -4511,10 +4511,10 @@
         <v>129</v>
       </c>
       <c r="H63" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="I63" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.2">
@@ -4538,10 +4538,10 @@
         <v>129</v>
       </c>
       <c r="H64" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="I64" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.2">
@@ -4565,10 +4565,10 @@
         <v>129</v>
       </c>
       <c r="H65" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="I65" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.2">
@@ -4595,7 +4595,7 @@
         <v>129</v>
       </c>
       <c r="I66" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated database: added an Else column to big cards
</commit_message>
<xml_diff>
--- a/data/TP Database.xlsx
+++ b/data/TP Database.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sophiachung/cs01-main/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sophiachung/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63024F02-109E-3544-8EB6-90AD74D0C595}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{68D784CF-B910-7845-B38A-B5F62C215C94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-1400" yWindow="680" windowWidth="15460" windowHeight="15880" activeTab="1" xr2:uid="{F6F91125-3C8A-D047-93DD-1F3A6DE88698}"/>
+    <workbookView xWindow="13340" yWindow="500" windowWidth="15460" windowHeight="15880" activeTab="1" xr2:uid="{F6F91125-3C8A-D047-93DD-1F3A6DE88698}"/>
   </bookViews>
   <sheets>
     <sheet name="Small Cards" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="332">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="671" uniqueCount="331">
   <si>
     <t>CardID</t>
   </si>
@@ -806,9 +806,6 @@
     <t>!4</t>
   </si>
   <si>
-    <t>!5 (else turn over a Milestones tile as your deadlines go sailing by)</t>
-  </si>
-  <si>
     <t>!7&amp;!9&amp;!13</t>
   </si>
   <si>
@@ -824,9 +821,6 @@
     <t>n0:3:2</t>
   </si>
   <si>
-    <t>n0:2:2 (If PLAN contains Milestones only remove 1 tile)</t>
-  </si>
-  <si>
     <t>n0:2:2</t>
   </si>
   <si>
@@ -836,6 +830,9 @@
     <t>i(79/101/121):1:(2/3/4)</t>
   </si>
   <si>
+    <t>b0:2:(3&amp;4)</t>
+  </si>
+  <si>
     <t xml:space="preserve">remove one relevant or very relevant article tile </t>
   </si>
   <si>
@@ -890,9 +887,6 @@
     <t>n(42/45/46):1</t>
   </si>
   <si>
-    <t>n0:2:3 (If PLAN contains Milestones only remove 1 tile)</t>
-  </si>
-  <si>
     <t>n0:2:3</t>
   </si>
   <si>
@@ -908,6 +902,9 @@
     <t>n0:1:3</t>
   </si>
   <si>
+    <t>n41:1, , n(42/45/46):2</t>
+  </si>
+  <si>
     <t>n(43/44):2</t>
   </si>
   <si>
@@ -926,6 +923,12 @@
     <t>n(17/18/19/20/21/22/23/24/25/26/27/28):1</t>
   </si>
   <si>
+    <t>n(33/34/35/36):1, n(45/46):1</t>
+  </si>
+  <si>
+    <t>b0:2:4</t>
+  </si>
+  <si>
     <t>n(33/34/35/36/43/44):2</t>
   </si>
   <si>
@@ -947,9 +950,6 @@
     <t>n(47/48/57):2</t>
   </si>
   <si>
-    <t>!5 (else remove only 1)</t>
-  </si>
-  <si>
     <t>remove 2 non-adjacent thesis tiles from current section</t>
   </si>
   <si>
@@ -1025,13 +1025,10 @@
     <t>n49:2</t>
   </si>
   <si>
-    <t>o0:2:4</t>
-  </si>
-  <si>
-    <t>n41:1&amp;n(42/45/46):2</t>
-  </si>
-  <si>
-    <t>n(33/34/35/36):1&amp;n(45/46):1</t>
+    <t>Else</t>
+  </si>
+  <si>
+    <t>f5:1</t>
   </si>
 </sst>
 </file>
@@ -1141,9 +1138,9 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{4E25BA7D-C944-7B48-8D11-C2260663E6FE}" name="Table135" displayName="Table135" ref="A1:I66" totalsRowShown="0">
-  <autoFilter ref="A1:I66" xr:uid="{4E25BA7D-C944-7B48-8D11-C2260663E6FE}"/>
-  <tableColumns count="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{4E25BA7D-C944-7B48-8D11-C2260663E6FE}" name="Table135" displayName="Table135" ref="A1:J66" totalsRowShown="0">
+  <autoFilter ref="A1:J66" xr:uid="{4E25BA7D-C944-7B48-8D11-C2260663E6FE}"/>
+  <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{241E3EFA-1556-A24B-8441-368F09FD400E}" name="CardID" dataDxfId="2">
       <calculatedColumnFormula>ROW() + 57</calculatedColumnFormula>
     </tableColumn>
@@ -1154,7 +1151,8 @@
     <tableColumn id="5" xr3:uid="{5BD78171-150E-AB4C-80DC-D8A061F5BF5E}" name="Description"/>
     <tableColumn id="9" xr3:uid="{318B7552-B230-384E-9C27-A0F990859B0F}" name="Save_condition"/>
     <tableColumn id="6" xr3:uid="{FCFA78C0-6299-A941-AD36-DE9122010D1F}" name="Requirement"/>
-    <tableColumn id="7" xr3:uid="{6E4CEF28-DC4C-D54A-9279-428FA0FAB941}" name="Effect"/>
+    <tableColumn id="11" xr3:uid="{5A0104B9-2CD4-4B40-BB25-1654C8CD91EA}" name="Effect"/>
+    <tableColumn id="7" xr3:uid="{6E4CEF28-DC4C-D54A-9279-428FA0FAB941}" name="Else"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1494,8 +1492,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18AE550B-A04F-B142-B067-7E2D879988FA}">
   <dimension ref="A1:H59"/>
   <sheetViews>
-    <sheetView topLeftCell="A39" zoomScale="102" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView zoomScale="102" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2768,10 +2766,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84DC5E79-A11F-0148-B3A8-F5384824D987}">
-  <dimension ref="A1:J66"/>
+  <dimension ref="A1:K66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E34" zoomScale="99" workbookViewId="0">
-      <selection activeCell="I41" sqref="I41"/>
+    <sheetView tabSelected="1" topLeftCell="G30" zoomScale="99" zoomScaleNormal="99" workbookViewId="0">
+      <selection activeCell="H55" sqref="H55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2784,10 +2782,11 @@
     <col min="6" max="6" width="14" customWidth="1"/>
     <col min="7" max="7" width="17" customWidth="1"/>
     <col min="8" max="8" width="15.83203125" customWidth="1"/>
-    <col min="9" max="9" width="45.83203125" customWidth="1"/>
+    <col min="9" max="9" width="46" customWidth="1"/>
+    <col min="10" max="10" width="22.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2815,8 +2814,11 @@
       <c r="I1" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J1" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2">
         <f t="shared" ref="A2:A33" si="0">ROW() + 57</f>
         <v>59</v>
@@ -2840,10 +2842,13 @@
         <v>129</v>
       </c>
       <c r="I2" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+        <v>269</v>
+      </c>
+      <c r="J2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3">
         <f t="shared" si="0"/>
         <v>60</v>
@@ -2867,10 +2872,13 @@
         <v>129</v>
       </c>
       <c r="I3" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+        <v>270</v>
+      </c>
+      <c r="J3" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4">
         <f t="shared" si="0"/>
         <v>61</v>
@@ -2894,10 +2902,13 @@
         <v>252</v>
       </c>
       <c r="I4" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+        <v>260</v>
+      </c>
+      <c r="J4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>62</v>
@@ -2918,13 +2929,16 @@
         <v>129</v>
       </c>
       <c r="H5" t="s">
-        <v>129</v>
+        <v>290</v>
       </c>
       <c r="I5" t="s">
+        <v>261</v>
+      </c>
+      <c r="J5" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>63</v>
@@ -2945,13 +2959,16 @@
         <v>129</v>
       </c>
       <c r="H6" t="s">
-        <v>129</v>
+        <v>290</v>
       </c>
       <c r="I6" t="s">
+        <v>261</v>
+      </c>
+      <c r="J6" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>64</v>
@@ -2975,10 +2992,13 @@
         <v>253</v>
       </c>
       <c r="I7" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+        <v>261</v>
+      </c>
+      <c r="J7" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>65</v>
@@ -2996,19 +3016,22 @@
         <v>140</v>
       </c>
       <c r="G8" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="H8" t="s">
         <v>129</v>
       </c>
       <c r="I8" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="J8" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+        <v>129</v>
+      </c>
+      <c r="K8" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>66</v>
@@ -3032,10 +3055,13 @@
         <v>129</v>
       </c>
       <c r="I9" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+        <v>271</v>
+      </c>
+      <c r="J9" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>67</v>
@@ -3059,13 +3085,16 @@
         <v>254</v>
       </c>
       <c r="I10" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="J10" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+        <v>129</v>
+      </c>
+      <c r="K10" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>68</v>
@@ -3086,16 +3115,19 @@
         <v>129</v>
       </c>
       <c r="H11" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="I11" t="s">
-        <v>277</v>
-      </c>
-      <c r="J11" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="J11" t="s">
+        <v>129</v>
+      </c>
+      <c r="K11" s="2" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>69</v>
@@ -3119,13 +3151,16 @@
         <v>254</v>
       </c>
       <c r="I12" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="J12" t="s">
+        <v>129</v>
+      </c>
+      <c r="K12" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>70</v>
@@ -3149,10 +3184,13 @@
         <v>255</v>
       </c>
       <c r="I13" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+        <v>273</v>
+      </c>
+      <c r="J13" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>71</v>
@@ -3176,10 +3214,13 @@
         <v>129</v>
       </c>
       <c r="I14" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+        <v>274</v>
+      </c>
+      <c r="J14" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>72</v>
@@ -3197,19 +3238,22 @@
         <v>156</v>
       </c>
       <c r="G15" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="H15" t="s">
         <v>129</v>
       </c>
       <c r="I15" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="J15" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+        <v>129</v>
+      </c>
+      <c r="K15" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>73</v>
@@ -3230,13 +3274,16 @@
         <v>129</v>
       </c>
       <c r="H16" t="s">
-        <v>256</v>
+        <v>290</v>
       </c>
       <c r="I16" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+        <v>260</v>
+      </c>
+      <c r="J16" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>74</v>
@@ -3260,10 +3307,13 @@
         <v>254</v>
       </c>
       <c r="I17" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+        <v>264</v>
+      </c>
+      <c r="J17" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>75</v>
@@ -3287,10 +3337,13 @@
         <v>254</v>
       </c>
       <c r="I18" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+        <v>261</v>
+      </c>
+      <c r="J18" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>76</v>
@@ -3314,10 +3367,13 @@
         <v>254</v>
       </c>
       <c r="I19" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+        <v>262</v>
+      </c>
+      <c r="J19" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>77</v>
@@ -3341,10 +3397,13 @@
         <v>129</v>
       </c>
       <c r="I20" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+        <v>261</v>
+      </c>
+      <c r="J20" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>78</v>
@@ -3368,10 +3427,13 @@
         <v>129</v>
       </c>
       <c r="I21" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+        <v>275</v>
+      </c>
+      <c r="J21" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22">
         <f t="shared" si="0"/>
         <v>79</v>
@@ -3392,13 +3454,16 @@
         <v>129</v>
       </c>
       <c r="H22" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="I22" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+        <v>262</v>
+      </c>
+      <c r="J22" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23">
         <f t="shared" si="0"/>
         <v>80</v>
@@ -3419,13 +3484,16 @@
         <v>129</v>
       </c>
       <c r="H23" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="I23" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+        <v>276</v>
+      </c>
+      <c r="J23" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24">
         <f t="shared" si="0"/>
         <v>81</v>
@@ -3449,10 +3517,13 @@
         <v>252</v>
       </c>
       <c r="I24" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+        <v>277</v>
+      </c>
+      <c r="J24" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25">
         <f t="shared" si="0"/>
         <v>82</v>
@@ -3476,10 +3547,13 @@
         <v>129</v>
       </c>
       <c r="I25" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+        <v>278</v>
+      </c>
+      <c r="J25" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26">
         <f t="shared" si="0"/>
         <v>83</v>
@@ -3500,16 +3574,19 @@
         <v>129</v>
       </c>
       <c r="H26" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="I26" t="s">
         <v>320</v>
       </c>
       <c r="J26" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+        <v>129</v>
+      </c>
+      <c r="K26" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27">
         <f t="shared" si="0"/>
         <v>84</v>
@@ -3530,13 +3607,16 @@
         <v>129</v>
       </c>
       <c r="H27" t="s">
+        <v>281</v>
+      </c>
+      <c r="I27" t="s">
         <v>282</v>
       </c>
-      <c r="I27" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J27" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28">
         <f t="shared" si="0"/>
         <v>85</v>
@@ -3557,13 +3637,16 @@
         <v>129</v>
       </c>
       <c r="H28" t="s">
-        <v>129</v>
+        <v>290</v>
       </c>
       <c r="I28" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+        <v>283</v>
+      </c>
+      <c r="J28" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29">
         <f t="shared" si="0"/>
         <v>86</v>
@@ -3587,10 +3670,13 @@
         <v>253</v>
       </c>
       <c r="I29" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+        <v>283</v>
+      </c>
+      <c r="J29" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30">
         <f t="shared" si="0"/>
         <v>87</v>
@@ -3611,13 +3697,16 @@
         <v>129</v>
       </c>
       <c r="H30" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="I30" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+        <v>285</v>
+      </c>
+      <c r="J30" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31">
         <f t="shared" si="0"/>
         <v>88</v>
@@ -3641,10 +3730,13 @@
         <v>129</v>
       </c>
       <c r="I31" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+        <v>286</v>
+      </c>
+      <c r="J31" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32">
         <f t="shared" si="0"/>
         <v>89</v>
@@ -3668,10 +3760,13 @@
         <v>129</v>
       </c>
       <c r="I32" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+        <v>288</v>
+      </c>
+      <c r="J32" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33">
         <f t="shared" si="0"/>
         <v>90</v>
@@ -3695,10 +3790,13 @@
         <v>255</v>
       </c>
       <c r="I33" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+        <v>287</v>
+      </c>
+      <c r="J33" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34">
         <f t="shared" ref="A34:A66" si="1">ROW() + 57</f>
         <v>91</v>
@@ -3722,10 +3820,13 @@
         <v>252</v>
       </c>
       <c r="I34" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+        <v>289</v>
+      </c>
+      <c r="J34" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35">
         <f t="shared" si="1"/>
         <v>92</v>
@@ -3746,13 +3847,16 @@
         <v>129</v>
       </c>
       <c r="H35" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="I35" t="s">
         <v>321</v>
       </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J35" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36">
         <f t="shared" si="1"/>
         <v>93</v>
@@ -3773,13 +3877,16 @@
         <v>129</v>
       </c>
       <c r="H36" t="s">
-        <v>256</v>
+        <v>290</v>
       </c>
       <c r="I36" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+        <v>277</v>
+      </c>
+      <c r="J36" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37">
         <f t="shared" si="1"/>
         <v>94</v>
@@ -3800,13 +3907,16 @@
         <v>129</v>
       </c>
       <c r="H37" t="s">
+        <v>291</v>
+      </c>
+      <c r="I37" t="s">
         <v>292</v>
       </c>
-      <c r="I37" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J37" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38">
         <f t="shared" si="1"/>
         <v>95</v>
@@ -3827,13 +3937,16 @@
         <v>129</v>
       </c>
       <c r="H38" t="s">
+        <v>293</v>
+      </c>
+      <c r="I38" t="s">
         <v>294</v>
       </c>
-      <c r="I38" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J38" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39">
         <f t="shared" si="1"/>
         <v>96</v>
@@ -3857,10 +3970,13 @@
         <v>254</v>
       </c>
       <c r="I39" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+        <v>283</v>
+      </c>
+      <c r="J39" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40">
         <f t="shared" si="1"/>
         <v>97</v>
@@ -3884,10 +4000,13 @@
         <v>254</v>
       </c>
       <c r="I40" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+        <v>287</v>
+      </c>
+      <c r="J40" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41">
         <f t="shared" si="1"/>
         <v>98</v>
@@ -3908,13 +4027,16 @@
         <v>129</v>
       </c>
       <c r="H41" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="I41" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+        <v>295</v>
+      </c>
+      <c r="J41" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42">
         <f t="shared" si="1"/>
         <v>99</v>
@@ -3935,13 +4057,16 @@
         <v>129</v>
       </c>
       <c r="H42" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="I42" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+        <v>296</v>
+      </c>
+      <c r="J42" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -3965,10 +4090,13 @@
         <v>315</v>
       </c>
       <c r="I43" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+        <v>297</v>
+      </c>
+      <c r="J43" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44">
         <f t="shared" si="1"/>
         <v>101</v>
@@ -3992,10 +4120,13 @@
         <v>316</v>
       </c>
       <c r="I44" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+        <v>287</v>
+      </c>
+      <c r="J44" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45">
         <f t="shared" si="1"/>
         <v>102</v>
@@ -4016,13 +4147,16 @@
         <v>129</v>
       </c>
       <c r="H45" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="I45" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+        <v>300</v>
+      </c>
+      <c r="J45" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46">
         <f t="shared" si="1"/>
         <v>103</v>
@@ -4049,10 +4183,13 @@
         <v>305</v>
       </c>
       <c r="J46" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+        <v>129</v>
+      </c>
+      <c r="K46" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47">
         <f t="shared" si="1"/>
         <v>104</v>
@@ -4076,10 +4213,13 @@
         <v>254</v>
       </c>
       <c r="I47" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+        <v>300</v>
+      </c>
+      <c r="J47" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48">
         <f t="shared" si="1"/>
         <v>105</v>
@@ -4100,13 +4240,16 @@
         <v>129</v>
       </c>
       <c r="H48" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="I48" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
+        <v>303</v>
+      </c>
+      <c r="J48" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49">
         <f t="shared" si="1"/>
         <v>106</v>
@@ -4127,16 +4270,19 @@
         <v>129</v>
       </c>
       <c r="H49" t="s">
-        <v>303</v>
+        <v>290</v>
       </c>
       <c r="I49" t="s">
         <v>306</v>
       </c>
       <c r="J49" t="s">
+        <v>300</v>
+      </c>
+      <c r="K49" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A50">
         <f t="shared" si="1"/>
         <v>107</v>
@@ -4157,13 +4303,16 @@
         <v>129</v>
       </c>
       <c r="H50" t="s">
-        <v>303</v>
+        <v>290</v>
       </c>
       <c r="I50" t="s">
         <v>306</v>
       </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J50" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A51">
         <f t="shared" si="1"/>
         <v>108</v>
@@ -4189,8 +4338,11 @@
       <c r="I51" t="s">
         <v>308</v>
       </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J51" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A52">
         <f t="shared" si="1"/>
         <v>109</v>
@@ -4216,8 +4368,11 @@
       <c r="I52" t="s">
         <v>306</v>
       </c>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J52" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A53">
         <f t="shared" si="1"/>
         <v>110</v>
@@ -4238,13 +4393,16 @@
         <v>129</v>
       </c>
       <c r="H53" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="I53" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J53" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A54">
         <f t="shared" si="1"/>
         <v>111</v>
@@ -4270,8 +4428,11 @@
       <c r="I54" t="s">
         <v>306</v>
       </c>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J54" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A55">
         <f t="shared" si="1"/>
         <v>112</v>
@@ -4297,8 +4458,11 @@
       <c r="I55" t="s">
         <v>311</v>
       </c>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J55" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A56">
         <f t="shared" si="1"/>
         <v>113</v>
@@ -4324,8 +4488,11 @@
       <c r="I56" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J56" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A57">
         <f t="shared" si="1"/>
         <v>114</v>
@@ -4351,8 +4518,11 @@
       <c r="I57" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J57" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A58">
         <f t="shared" si="1"/>
         <v>115</v>
@@ -4373,13 +4543,16 @@
         <v>129</v>
       </c>
       <c r="H58" t="s">
-        <v>256</v>
+        <v>290</v>
       </c>
       <c r="I58" t="s">
         <v>306</v>
       </c>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J58" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A59">
         <f t="shared" si="1"/>
         <v>116</v>
@@ -4406,10 +4579,13 @@
         <v>323</v>
       </c>
       <c r="J59" t="s">
+        <v>129</v>
+      </c>
+      <c r="K59" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A60">
         <f t="shared" si="1"/>
         <v>117</v>
@@ -4430,13 +4606,16 @@
         <v>129</v>
       </c>
       <c r="H60" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="I60" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
+        <v>300</v>
+      </c>
+      <c r="J60" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A61">
         <f t="shared" si="1"/>
         <v>118</v>
@@ -4462,8 +4641,11 @@
       <c r="I61" t="s">
         <v>325</v>
       </c>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J61" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A62">
         <f t="shared" si="1"/>
         <v>119</v>
@@ -4489,8 +4671,11 @@
       <c r="I62" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J62" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A63">
         <f t="shared" si="1"/>
         <v>120</v>
@@ -4516,8 +4701,11 @@
       <c r="I63" t="s">
         <v>306</v>
       </c>
-    </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J63" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A64">
         <f t="shared" si="1"/>
         <v>121</v>
@@ -4541,10 +4729,13 @@
         <v>327</v>
       </c>
       <c r="I64" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
+        <v>300</v>
+      </c>
+      <c r="J64" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A65">
         <f t="shared" si="1"/>
         <v>122</v>
@@ -4570,8 +4761,11 @@
       <c r="I65" t="s">
         <v>306</v>
       </c>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J65" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A66">
         <f t="shared" si="1"/>
         <v>123</v>
@@ -4596,6 +4790,9 @@
       </c>
       <c r="I66" t="s">
         <v>328</v>
+      </c>
+      <c r="J66" t="s">
+        <v>129</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Issue #73 - Added all cards to database
## Changes Made
- Removed number column from Big Cards table since there is only 1 of 
each event card
- Renamed the tables in the excel to Activites and Events to match the 
tables in the database
- Converted data in excel file to csv files
- Loaded data from csv files into the database
- Updated the readme to match the new columns in the database

Closed Issue #73
</commit_message>
<xml_diff>
--- a/data/TP Database.xlsx
+++ b/data/TP Database.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sophiachung/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_My Files\_Uni\Year 3\Term 1\3 - Team Project\_TP Code\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{68D784CF-B910-7845-B38A-B5F62C215C94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41FD4BA5-A2DD-4BD3-81F9-144B5265B7FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13340" yWindow="500" windowWidth="15460" windowHeight="15880" activeTab="1" xr2:uid="{F6F91125-3C8A-D047-93DD-1F3A6DE88698}"/>
+    <workbookView xWindow="28680" yWindow="-1290" windowWidth="29040" windowHeight="15840" xr2:uid="{F6F91125-3C8A-D047-93DD-1F3A6DE88698}"/>
   </bookViews>
   <sheets>
-    <sheet name="Small Cards" sheetId="2" r:id="rId1"/>
-    <sheet name="Big Cards" sheetId="3" r:id="rId2"/>
+    <sheet name="Activities" sheetId="2" r:id="rId1"/>
+    <sheet name="Events" sheetId="3" r:id="rId2"/>
     <sheet name="Small cards sample" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191028"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="671" uniqueCount="331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="670" uniqueCount="331">
   <si>
     <t>CardID</t>
   </si>
@@ -1138,21 +1138,20 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{4E25BA7D-C944-7B48-8D11-C2260663E6FE}" name="Table135" displayName="Table135" ref="A1:J66" totalsRowShown="0">
-  <autoFilter ref="A1:J66" xr:uid="{4E25BA7D-C944-7B48-8D11-C2260663E6FE}"/>
-  <tableColumns count="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{4E25BA7D-C944-7B48-8D11-C2260663E6FE}" name="Table135" displayName="Table135" ref="A1:I66" totalsRowShown="0">
+  <autoFilter ref="A1:I66" xr:uid="{4E25BA7D-C944-7B48-8D11-C2260663E6FE}"/>
+  <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{241E3EFA-1556-A24B-8441-368F09FD400E}" name="CardID" dataDxfId="2">
       <calculatedColumnFormula>ROW() + 57</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="2" xr3:uid="{4CB802A7-5A14-1843-8D85-057515A93530}" name="Stage"/>
-    <tableColumn id="3" xr3:uid="{45AAD7C9-BD08-B241-A106-B2FFC2B22B18}" name="Number"/>
-    <tableColumn id="8" xr3:uid="{98D9D00E-0FDA-C645-9758-69E917F00870}" name="Filename"/>
-    <tableColumn id="4" xr3:uid="{1F7BF006-71BD-D542-96ED-747B93E53C9C}" name="Title"/>
-    <tableColumn id="5" xr3:uid="{5BD78171-150E-AB4C-80DC-D8A061F5BF5E}" name="Description"/>
-    <tableColumn id="9" xr3:uid="{318B7552-B230-384E-9C27-A0F990859B0F}" name="Save_condition"/>
-    <tableColumn id="6" xr3:uid="{FCFA78C0-6299-A941-AD36-DE9122010D1F}" name="Requirement"/>
-    <tableColumn id="11" xr3:uid="{5A0104B9-2CD4-4B40-BB25-1654C8CD91EA}" name="Effect"/>
-    <tableColumn id="7" xr3:uid="{6E4CEF28-DC4C-D54A-9279-428FA0FAB941}" name="Else"/>
+    <tableColumn id="3" xr3:uid="{45AAD7C9-BD08-B241-A106-B2FFC2B22B18}" name="Filename"/>
+    <tableColumn id="8" xr3:uid="{98D9D00E-0FDA-C645-9758-69E917F00870}" name="Title"/>
+    <tableColumn id="4" xr3:uid="{1F7BF006-71BD-D542-96ED-747B93E53C9C}" name="Description"/>
+    <tableColumn id="5" xr3:uid="{5BD78171-150E-AB4C-80DC-D8A061F5BF5E}" name="Save_condition"/>
+    <tableColumn id="9" xr3:uid="{318B7552-B230-384E-9C27-A0F990859B0F}" name="Requirement"/>
+    <tableColumn id="6" xr3:uid="{FCFA78C0-6299-A941-AD36-DE9122010D1F}" name="Effect"/>
+    <tableColumn id="11" xr3:uid="{5A0104B9-2CD4-4B40-BB25-1654C8CD91EA}" name="Else"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1492,21 +1491,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18AE550B-A04F-B142-B067-7E2D879988FA}">
   <dimension ref="A1:H59"/>
   <sheetViews>
-    <sheetView zoomScale="102" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="102" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.6640625" customWidth="1"/>
-    <col min="2" max="2" width="15.1640625" customWidth="1"/>
-    <col min="3" max="3" width="10.33203125" customWidth="1"/>
-    <col min="4" max="4" width="25.1640625" customWidth="1"/>
+    <col min="1" max="1" width="9.625" customWidth="1"/>
+    <col min="2" max="2" width="15.125" customWidth="1"/>
+    <col min="3" max="3" width="10.375" customWidth="1"/>
+    <col min="4" max="4" width="25.125" customWidth="1"/>
     <col min="5" max="6" width="17.5" customWidth="1"/>
     <col min="7" max="7" width="9.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1532,7 +1531,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <f t="shared" ref="A2:A33" si="0">ROW() - 1</f>
         <v>1</v>
@@ -1556,7 +1555,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -1580,7 +1579,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -1601,7 +1600,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1622,7 +1621,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1643,7 +1642,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1664,7 +1663,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1685,7 +1684,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1706,7 +1705,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1727,7 +1726,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1748,7 +1747,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1769,7 +1768,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1790,7 +1789,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1811,7 +1810,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1832,7 +1831,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1853,7 +1852,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1874,7 +1873,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1895,7 +1894,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -1916,7 +1915,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -1937,7 +1936,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -1958,7 +1957,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -1979,7 +1978,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -2000,7 +1999,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -2021,7 +2020,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -2042,7 +2041,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -2063,7 +2062,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -2084,7 +2083,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -2105,7 +2104,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -2126,7 +2125,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -2147,7 +2146,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -2168,7 +2167,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -2189,7 +2188,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -2210,7 +2209,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34">
         <f t="shared" ref="A34:A59" si="1">ROW() - 1</f>
         <v>33</v>
@@ -2231,7 +2230,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35">
         <f t="shared" si="1"/>
         <v>34</v>
@@ -2252,7 +2251,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36">
         <f t="shared" si="1"/>
         <v>35</v>
@@ -2273,7 +2272,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37">
         <f t="shared" si="1"/>
         <v>36</v>
@@ -2294,7 +2293,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38">
         <f t="shared" si="1"/>
         <v>37</v>
@@ -2315,7 +2314,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39">
         <f t="shared" si="1"/>
         <v>38</v>
@@ -2336,7 +2335,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40">
         <f t="shared" si="1"/>
         <v>39</v>
@@ -2357,7 +2356,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41">
         <f t="shared" si="1"/>
         <v>40</v>
@@ -2378,7 +2377,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42">
         <f t="shared" si="1"/>
         <v>41</v>
@@ -2399,7 +2398,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43">
         <f t="shared" si="1"/>
         <v>42</v>
@@ -2420,7 +2419,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44">
         <f t="shared" si="1"/>
         <v>43</v>
@@ -2441,7 +2440,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45">
         <f t="shared" si="1"/>
         <v>44</v>
@@ -2462,7 +2461,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46">
         <f t="shared" si="1"/>
         <v>45</v>
@@ -2483,7 +2482,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47">
         <f t="shared" si="1"/>
         <v>46</v>
@@ -2504,7 +2503,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48">
         <f t="shared" si="1"/>
         <v>47</v>
@@ -2525,7 +2524,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49">
         <f t="shared" si="1"/>
         <v>48</v>
@@ -2546,7 +2545,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50">
         <f t="shared" si="1"/>
         <v>49</v>
@@ -2567,7 +2566,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51">
         <f t="shared" si="1"/>
         <v>50</v>
@@ -2588,7 +2587,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52">
         <f t="shared" si="1"/>
         <v>51</v>
@@ -2609,7 +2608,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53">
         <f t="shared" si="1"/>
         <v>52</v>
@@ -2630,7 +2629,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54">
         <f t="shared" si="1"/>
         <v>53</v>
@@ -2651,7 +2650,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55">
         <f t="shared" si="1"/>
         <v>54</v>
@@ -2672,7 +2671,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56">
         <f t="shared" si="1"/>
         <v>55</v>
@@ -2693,7 +2692,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57">
         <f t="shared" si="1"/>
         <v>56</v>
@@ -2714,7 +2713,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58">
         <f t="shared" si="1"/>
         <v>57</v>
@@ -2735,7 +2734,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59">
         <f t="shared" si="1"/>
         <v>58</v>
@@ -2766,27 +2765,26 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84DC5E79-A11F-0148-B3A8-F5384824D987}">
-  <dimension ref="A1:K66"/>
+  <dimension ref="A1:J66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G30" zoomScale="99" zoomScaleNormal="99" workbookViewId="0">
-      <selection activeCell="H55" sqref="H55"/>
+    <sheetView zoomScale="99" zoomScaleNormal="99" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.1640625" customWidth="1"/>
+    <col min="1" max="1" width="9.125" customWidth="1"/>
     <col min="2" max="2" width="9.5" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" customWidth="1"/>
-    <col min="4" max="4" width="25.83203125" customWidth="1"/>
+    <col min="3" max="3" width="10.625" customWidth="1"/>
+    <col min="4" max="4" width="25.875" customWidth="1"/>
     <col min="5" max="5" width="26" customWidth="1"/>
     <col min="6" max="6" width="14" customWidth="1"/>
     <col min="7" max="7" width="17" customWidth="1"/>
-    <col min="8" max="8" width="15.83203125" customWidth="1"/>
-    <col min="9" max="9" width="46" customWidth="1"/>
-    <col min="10" max="10" width="22.83203125" customWidth="1"/>
+    <col min="8" max="8" width="15.875" customWidth="1"/>
+    <col min="9" max="9" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2794,31 +2792,28 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F1" t="s">
-        <v>5</v>
+        <v>124</v>
       </c>
       <c r="G1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="H1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="I1" t="s">
-        <v>126</v>
-      </c>
-      <c r="J1" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <f t="shared" ref="A2:A33" si="0">ROW() + 57</f>
         <v>59</v>
@@ -2826,29 +2821,26 @@
       <c r="B2">
         <v>2</v>
       </c>
-      <c r="C2">
-        <v>1</v>
+      <c r="C2" t="s">
+        <v>127</v>
       </c>
       <c r="D2" t="s">
-        <v>127</v>
-      </c>
-      <c r="E2" t="s">
         <v>128</v>
       </c>
+      <c r="F2" t="s">
+        <v>129</v>
+      </c>
       <c r="G2" t="s">
         <v>129</v>
       </c>
       <c r="H2" t="s">
-        <v>129</v>
+        <v>269</v>
       </c>
       <c r="I2" t="s">
-        <v>269</v>
-      </c>
-      <c r="J2" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <f t="shared" si="0"/>
         <v>60</v>
@@ -2856,29 +2848,26 @@
       <c r="B3">
         <v>2</v>
       </c>
-      <c r="C3">
-        <v>1</v>
+      <c r="C3" t="s">
+        <v>130</v>
       </c>
       <c r="D3" t="s">
-        <v>130</v>
-      </c>
-      <c r="E3" t="s">
         <v>131</v>
       </c>
+      <c r="F3" t="s">
+        <v>129</v>
+      </c>
       <c r="G3" t="s">
         <v>129</v>
       </c>
       <c r="H3" t="s">
-        <v>129</v>
+        <v>270</v>
       </c>
       <c r="I3" t="s">
-        <v>270</v>
-      </c>
-      <c r="J3" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <f t="shared" si="0"/>
         <v>61</v>
@@ -2886,614 +2875,554 @@
       <c r="B4">
         <v>2</v>
       </c>
-      <c r="C4">
-        <v>1</v>
+      <c r="C4" t="s">
+        <v>132</v>
       </c>
       <c r="D4" t="s">
-        <v>132</v>
-      </c>
-      <c r="E4" t="s">
         <v>133</v>
       </c>
+      <c r="F4" t="s">
+        <v>129</v>
+      </c>
       <c r="G4" t="s">
-        <v>129</v>
+        <v>252</v>
       </c>
       <c r="H4" t="s">
-        <v>252</v>
+        <v>260</v>
       </c>
       <c r="I4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <f t="shared" si="0"/>
+        <v>62</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>134</v>
+      </c>
+      <c r="D5" t="s">
+        <v>135</v>
+      </c>
+      <c r="F5" t="s">
+        <v>129</v>
+      </c>
+      <c r="G5" t="s">
+        <v>290</v>
+      </c>
+      <c r="H5" t="s">
+        <v>261</v>
+      </c>
+      <c r="I5" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <f t="shared" si="0"/>
+        <v>63</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>136</v>
+      </c>
+      <c r="D6" t="s">
+        <v>135</v>
+      </c>
+      <c r="F6" t="s">
+        <v>129</v>
+      </c>
+      <c r="G6" t="s">
+        <v>290</v>
+      </c>
+      <c r="H6" t="s">
+        <v>261</v>
+      </c>
+      <c r="I6" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>137</v>
+      </c>
+      <c r="D7" t="s">
+        <v>138</v>
+      </c>
+      <c r="F7" t="s">
+        <v>129</v>
+      </c>
+      <c r="G7" t="s">
+        <v>253</v>
+      </c>
+      <c r="H7" t="s">
+        <v>261</v>
+      </c>
+      <c r="I7" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <f t="shared" si="0"/>
+        <v>65</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8" t="s">
+        <v>139</v>
+      </c>
+      <c r="D8" t="s">
+        <v>140</v>
+      </c>
+      <c r="F8" t="s">
+        <v>259</v>
+      </c>
+      <c r="G8" t="s">
+        <v>129</v>
+      </c>
+      <c r="H8" t="s">
+        <v>268</v>
+      </c>
+      <c r="I8" t="s">
+        <v>129</v>
+      </c>
+      <c r="J8" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <f t="shared" si="0"/>
+        <v>66</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9" t="s">
+        <v>141</v>
+      </c>
+      <c r="D9" t="s">
+        <v>142</v>
+      </c>
+      <c r="F9" t="s">
+        <v>129</v>
+      </c>
+      <c r="G9" t="s">
+        <v>129</v>
+      </c>
+      <c r="H9" t="s">
+        <v>271</v>
+      </c>
+      <c r="I9" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <f t="shared" si="0"/>
+        <v>67</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10" t="s">
+        <v>143</v>
+      </c>
+      <c r="D10" t="s">
+        <v>144</v>
+      </c>
+      <c r="F10" t="s">
+        <v>129</v>
+      </c>
+      <c r="G10" t="s">
+        <v>254</v>
+      </c>
+      <c r="H10" t="s">
+        <v>272</v>
+      </c>
+      <c r="I10" t="s">
+        <v>129</v>
+      </c>
+      <c r="J10" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <f t="shared" si="0"/>
+        <v>68</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11" t="s">
+        <v>145</v>
+      </c>
+      <c r="D11" t="s">
+        <v>146</v>
+      </c>
+      <c r="F11" t="s">
+        <v>129</v>
+      </c>
+      <c r="G11" t="s">
+        <v>257</v>
+      </c>
+      <c r="H11" t="s">
+        <v>276</v>
+      </c>
+      <c r="I11" t="s">
+        <v>129</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <f t="shared" si="0"/>
+        <v>69</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12" t="s">
+        <v>148</v>
+      </c>
+      <c r="D12" t="s">
+        <v>149</v>
+      </c>
+      <c r="F12" t="s">
+        <v>129</v>
+      </c>
+      <c r="G12" t="s">
+        <v>254</v>
+      </c>
+      <c r="H12" t="s">
+        <v>272</v>
+      </c>
+      <c r="I12" t="s">
+        <v>129</v>
+      </c>
+      <c r="J12" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <f t="shared" si="0"/>
+        <v>70</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13" t="s">
+        <v>151</v>
+      </c>
+      <c r="D13" t="s">
+        <v>152</v>
+      </c>
+      <c r="F13" t="s">
+        <v>129</v>
+      </c>
+      <c r="G13" t="s">
+        <v>255</v>
+      </c>
+      <c r="H13" t="s">
+        <v>273</v>
+      </c>
+      <c r="I13" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <f t="shared" si="0"/>
+        <v>71</v>
+      </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14" t="s">
+        <v>153</v>
+      </c>
+      <c r="D14" t="s">
+        <v>154</v>
+      </c>
+      <c r="F14" t="s">
+        <v>129</v>
+      </c>
+      <c r="G14" t="s">
+        <v>129</v>
+      </c>
+      <c r="H14" t="s">
+        <v>274</v>
+      </c>
+      <c r="I14" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <f t="shared" si="0"/>
+        <v>72</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15" t="s">
+        <v>155</v>
+      </c>
+      <c r="D15" t="s">
+        <v>156</v>
+      </c>
+      <c r="F15" t="s">
+        <v>298</v>
+      </c>
+      <c r="G15" t="s">
+        <v>129</v>
+      </c>
+      <c r="H15" t="s">
+        <v>263</v>
+      </c>
+      <c r="I15" t="s">
+        <v>129</v>
+      </c>
+      <c r="J15" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <f t="shared" si="0"/>
+        <v>73</v>
+      </c>
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16" t="s">
+        <v>157</v>
+      </c>
+      <c r="D16" t="s">
+        <v>158</v>
+      </c>
+      <c r="F16" t="s">
+        <v>129</v>
+      </c>
+      <c r="G16" t="s">
+        <v>290</v>
+      </c>
+      <c r="H16" t="s">
         <v>260</v>
       </c>
-      <c r="J4" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <f t="shared" si="0"/>
-        <v>62</v>
-      </c>
-      <c r="B5">
-        <v>2</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5" t="s">
-        <v>134</v>
-      </c>
-      <c r="E5" t="s">
-        <v>135</v>
-      </c>
-      <c r="G5" t="s">
-        <v>129</v>
-      </c>
-      <c r="H5" t="s">
-        <v>290</v>
-      </c>
-      <c r="I5" t="s">
+      <c r="I16" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <f t="shared" si="0"/>
+        <v>74</v>
+      </c>
+      <c r="B17">
+        <v>2</v>
+      </c>
+      <c r="C17" t="s">
+        <v>159</v>
+      </c>
+      <c r="D17" t="s">
+        <v>160</v>
+      </c>
+      <c r="F17" t="s">
+        <v>129</v>
+      </c>
+      <c r="G17" t="s">
+        <v>254</v>
+      </c>
+      <c r="H17" t="s">
+        <v>264</v>
+      </c>
+      <c r="I17" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <f t="shared" si="0"/>
+        <v>75</v>
+      </c>
+      <c r="B18">
+        <v>2</v>
+      </c>
+      <c r="C18" t="s">
+        <v>161</v>
+      </c>
+      <c r="D18" t="s">
+        <v>162</v>
+      </c>
+      <c r="F18" t="s">
+        <v>129</v>
+      </c>
+      <c r="G18" t="s">
+        <v>254</v>
+      </c>
+      <c r="H18" t="s">
         <v>261</v>
       </c>
-      <c r="J5" t="s">
+      <c r="I18" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <f t="shared" si="0"/>
+        <v>76</v>
+      </c>
+      <c r="B19">
+        <v>2</v>
+      </c>
+      <c r="C19" t="s">
+        <v>163</v>
+      </c>
+      <c r="D19" t="s">
+        <v>164</v>
+      </c>
+      <c r="F19" t="s">
+        <v>129</v>
+      </c>
+      <c r="G19" t="s">
+        <v>254</v>
+      </c>
+      <c r="H19" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <f t="shared" si="0"/>
-        <v>63</v>
-      </c>
-      <c r="B6">
-        <v>2</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="D6" t="s">
-        <v>136</v>
-      </c>
-      <c r="E6" t="s">
-        <v>135</v>
-      </c>
-      <c r="G6" t="s">
-        <v>129</v>
-      </c>
-      <c r="H6" t="s">
-        <v>290</v>
-      </c>
-      <c r="I6" t="s">
+      <c r="I19" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <f t="shared" si="0"/>
+        <v>77</v>
+      </c>
+      <c r="B20">
+        <v>2</v>
+      </c>
+      <c r="C20" t="s">
+        <v>165</v>
+      </c>
+      <c r="D20" t="s">
+        <v>166</v>
+      </c>
+      <c r="F20" t="s">
+        <v>129</v>
+      </c>
+      <c r="G20" t="s">
+        <v>129</v>
+      </c>
+      <c r="H20" t="s">
         <v>261</v>
       </c>
-      <c r="J6" t="s">
+      <c r="I20" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <f t="shared" si="0"/>
+        <v>78</v>
+      </c>
+      <c r="B21">
+        <v>2</v>
+      </c>
+      <c r="C21" t="s">
+        <v>167</v>
+      </c>
+      <c r="D21" t="s">
+        <v>168</v>
+      </c>
+      <c r="F21" t="s">
+        <v>129</v>
+      </c>
+      <c r="G21" t="s">
+        <v>129</v>
+      </c>
+      <c r="H21" t="s">
+        <v>275</v>
+      </c>
+      <c r="I21" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <f t="shared" si="0"/>
+        <v>79</v>
+      </c>
+      <c r="B22">
+        <v>2</v>
+      </c>
+      <c r="C22" t="s">
+        <v>169</v>
+      </c>
+      <c r="D22" t="s">
+        <v>170</v>
+      </c>
+      <c r="F22" t="s">
+        <v>129</v>
+      </c>
+      <c r="G22" t="s">
+        <v>256</v>
+      </c>
+      <c r="H22" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <f t="shared" si="0"/>
-        <v>64</v>
-      </c>
-      <c r="B7">
-        <v>2</v>
-      </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7" t="s">
-        <v>137</v>
-      </c>
-      <c r="E7" t="s">
-        <v>138</v>
-      </c>
-      <c r="G7" t="s">
-        <v>129</v>
-      </c>
-      <c r="H7" t="s">
-        <v>253</v>
-      </c>
-      <c r="I7" t="s">
-        <v>261</v>
-      </c>
-      <c r="J7" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <f t="shared" si="0"/>
-        <v>65</v>
-      </c>
-      <c r="B8">
-        <v>2</v>
-      </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-      <c r="D8" t="s">
-        <v>139</v>
-      </c>
-      <c r="E8" t="s">
-        <v>140</v>
-      </c>
-      <c r="G8" t="s">
-        <v>259</v>
-      </c>
-      <c r="H8" t="s">
-        <v>129</v>
-      </c>
-      <c r="I8" t="s">
-        <v>268</v>
-      </c>
-      <c r="J8" t="s">
-        <v>129</v>
-      </c>
-      <c r="K8" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <f t="shared" si="0"/>
-        <v>66</v>
-      </c>
-      <c r="B9">
-        <v>2</v>
-      </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="D9" t="s">
-        <v>141</v>
-      </c>
-      <c r="E9" t="s">
-        <v>142</v>
-      </c>
-      <c r="G9" t="s">
-        <v>129</v>
-      </c>
-      <c r="H9" t="s">
-        <v>129</v>
-      </c>
-      <c r="I9" t="s">
-        <v>271</v>
-      </c>
-      <c r="J9" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <f t="shared" si="0"/>
-        <v>67</v>
-      </c>
-      <c r="B10">
-        <v>2</v>
-      </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="D10" t="s">
-        <v>143</v>
-      </c>
-      <c r="E10" t="s">
-        <v>144</v>
-      </c>
-      <c r="G10" t="s">
-        <v>129</v>
-      </c>
-      <c r="H10" t="s">
-        <v>254</v>
-      </c>
-      <c r="I10" t="s">
-        <v>272</v>
-      </c>
-      <c r="J10" t="s">
-        <v>129</v>
-      </c>
-      <c r="K10" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <f t="shared" si="0"/>
-        <v>68</v>
-      </c>
-      <c r="B11">
-        <v>2</v>
-      </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="D11" t="s">
-        <v>145</v>
-      </c>
-      <c r="E11" t="s">
-        <v>146</v>
-      </c>
-      <c r="G11" t="s">
-        <v>129</v>
-      </c>
-      <c r="H11" t="s">
-        <v>257</v>
-      </c>
-      <c r="I11" t="s">
+      <c r="I22" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <f t="shared" si="0"/>
+        <v>80</v>
+      </c>
+      <c r="B23">
+        <v>2</v>
+      </c>
+      <c r="C23" t="s">
+        <v>171</v>
+      </c>
+      <c r="D23" t="s">
+        <v>172</v>
+      </c>
+      <c r="F23" t="s">
+        <v>129</v>
+      </c>
+      <c r="G23" t="s">
+        <v>258</v>
+      </c>
+      <c r="H23" t="s">
         <v>276</v>
       </c>
-      <c r="J11" t="s">
-        <v>129</v>
-      </c>
-      <c r="K11" s="2" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <f t="shared" si="0"/>
-        <v>69</v>
-      </c>
-      <c r="B12">
-        <v>2</v>
-      </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-      <c r="D12" t="s">
-        <v>148</v>
-      </c>
-      <c r="E12" t="s">
-        <v>149</v>
-      </c>
-      <c r="G12" t="s">
-        <v>129</v>
-      </c>
-      <c r="H12" t="s">
-        <v>254</v>
-      </c>
-      <c r="I12" t="s">
-        <v>272</v>
-      </c>
-      <c r="J12" t="s">
-        <v>129</v>
-      </c>
-      <c r="K12" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <f t="shared" si="0"/>
-        <v>70</v>
-      </c>
-      <c r="B13">
-        <v>2</v>
-      </c>
-      <c r="C13">
-        <v>1</v>
-      </c>
-      <c r="D13" t="s">
-        <v>151</v>
-      </c>
-      <c r="E13" t="s">
-        <v>152</v>
-      </c>
-      <c r="G13" t="s">
-        <v>129</v>
-      </c>
-      <c r="H13" t="s">
-        <v>255</v>
-      </c>
-      <c r="I13" t="s">
-        <v>273</v>
-      </c>
-      <c r="J13" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A14">
-        <f t="shared" si="0"/>
-        <v>71</v>
-      </c>
-      <c r="B14">
-        <v>2</v>
-      </c>
-      <c r="C14">
-        <v>1</v>
-      </c>
-      <c r="D14" t="s">
-        <v>153</v>
-      </c>
-      <c r="E14" t="s">
-        <v>154</v>
-      </c>
-      <c r="G14" t="s">
-        <v>129</v>
-      </c>
-      <c r="H14" t="s">
-        <v>129</v>
-      </c>
-      <c r="I14" t="s">
-        <v>274</v>
-      </c>
-      <c r="J14" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A15">
-        <f t="shared" si="0"/>
-        <v>72</v>
-      </c>
-      <c r="B15">
-        <v>2</v>
-      </c>
-      <c r="C15">
-        <v>1</v>
-      </c>
-      <c r="D15" t="s">
-        <v>155</v>
-      </c>
-      <c r="E15" t="s">
-        <v>156</v>
-      </c>
-      <c r="G15" t="s">
-        <v>298</v>
-      </c>
-      <c r="H15" t="s">
-        <v>129</v>
-      </c>
-      <c r="I15" t="s">
-        <v>263</v>
-      </c>
-      <c r="J15" t="s">
-        <v>129</v>
-      </c>
-      <c r="K15" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A16">
-        <f t="shared" si="0"/>
-        <v>73</v>
-      </c>
-      <c r="B16">
-        <v>2</v>
-      </c>
-      <c r="C16">
-        <v>1</v>
-      </c>
-      <c r="D16" t="s">
-        <v>157</v>
-      </c>
-      <c r="E16" t="s">
-        <v>158</v>
-      </c>
-      <c r="G16" t="s">
-        <v>129</v>
-      </c>
-      <c r="H16" t="s">
-        <v>290</v>
-      </c>
-      <c r="I16" t="s">
-        <v>260</v>
-      </c>
-      <c r="J16" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A17">
-        <f t="shared" si="0"/>
-        <v>74</v>
-      </c>
-      <c r="B17">
-        <v>2</v>
-      </c>
-      <c r="C17">
-        <v>1</v>
-      </c>
-      <c r="D17" t="s">
-        <v>159</v>
-      </c>
-      <c r="E17" t="s">
-        <v>160</v>
-      </c>
-      <c r="G17" t="s">
-        <v>129</v>
-      </c>
-      <c r="H17" t="s">
-        <v>254</v>
-      </c>
-      <c r="I17" t="s">
-        <v>264</v>
-      </c>
-      <c r="J17" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A18">
-        <f t="shared" si="0"/>
-        <v>75</v>
-      </c>
-      <c r="B18">
-        <v>2</v>
-      </c>
-      <c r="C18">
-        <v>1</v>
-      </c>
-      <c r="D18" t="s">
-        <v>161</v>
-      </c>
-      <c r="E18" t="s">
-        <v>162</v>
-      </c>
-      <c r="G18" t="s">
-        <v>129</v>
-      </c>
-      <c r="H18" t="s">
-        <v>254</v>
-      </c>
-      <c r="I18" t="s">
-        <v>261</v>
-      </c>
-      <c r="J18" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A19">
-        <f t="shared" si="0"/>
-        <v>76</v>
-      </c>
-      <c r="B19">
-        <v>2</v>
-      </c>
-      <c r="C19">
-        <v>1</v>
-      </c>
-      <c r="D19" t="s">
-        <v>163</v>
-      </c>
-      <c r="E19" t="s">
-        <v>164</v>
-      </c>
-      <c r="G19" t="s">
-        <v>129</v>
-      </c>
-      <c r="H19" t="s">
-        <v>254</v>
-      </c>
-      <c r="I19" t="s">
-        <v>262</v>
-      </c>
-      <c r="J19" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A20">
-        <f t="shared" si="0"/>
-        <v>77</v>
-      </c>
-      <c r="B20">
-        <v>2</v>
-      </c>
-      <c r="C20">
-        <v>1</v>
-      </c>
-      <c r="D20" t="s">
-        <v>165</v>
-      </c>
-      <c r="E20" t="s">
-        <v>166</v>
-      </c>
-      <c r="G20" t="s">
-        <v>129</v>
-      </c>
-      <c r="H20" t="s">
-        <v>129</v>
-      </c>
-      <c r="I20" t="s">
-        <v>261</v>
-      </c>
-      <c r="J20" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A21">
-        <f t="shared" si="0"/>
-        <v>78</v>
-      </c>
-      <c r="B21">
-        <v>2</v>
-      </c>
-      <c r="C21">
-        <v>1</v>
-      </c>
-      <c r="D21" t="s">
-        <v>167</v>
-      </c>
-      <c r="E21" t="s">
-        <v>168</v>
-      </c>
-      <c r="G21" t="s">
-        <v>129</v>
-      </c>
-      <c r="H21" t="s">
-        <v>129</v>
-      </c>
-      <c r="I21" t="s">
-        <v>275</v>
-      </c>
-      <c r="J21" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A22">
-        <f t="shared" si="0"/>
-        <v>79</v>
-      </c>
-      <c r="B22">
-        <v>2</v>
-      </c>
-      <c r="C22">
-        <v>1</v>
-      </c>
-      <c r="D22" t="s">
-        <v>169</v>
-      </c>
-      <c r="E22" t="s">
-        <v>170</v>
-      </c>
-      <c r="G22" t="s">
-        <v>129</v>
-      </c>
-      <c r="H22" t="s">
-        <v>256</v>
-      </c>
-      <c r="I22" t="s">
-        <v>262</v>
-      </c>
-      <c r="J22" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A23">
-        <f t="shared" si="0"/>
-        <v>80</v>
-      </c>
-      <c r="B23">
-        <v>2</v>
-      </c>
-      <c r="C23">
-        <v>1</v>
-      </c>
-      <c r="D23" t="s">
-        <v>171</v>
-      </c>
-      <c r="E23" t="s">
-        <v>172</v>
-      </c>
-      <c r="G23" t="s">
-        <v>129</v>
-      </c>
-      <c r="H23" t="s">
-        <v>258</v>
-      </c>
       <c r="I23" t="s">
-        <v>276</v>
-      </c>
-      <c r="J23" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24">
         <f t="shared" si="0"/>
         <v>81</v>
@@ -3501,29 +3430,26 @@
       <c r="B24">
         <v>3</v>
       </c>
-      <c r="C24">
-        <v>1</v>
+      <c r="C24" t="s">
+        <v>173</v>
       </c>
       <c r="D24" t="s">
-        <v>173</v>
-      </c>
-      <c r="E24" t="s">
         <v>133</v>
       </c>
+      <c r="F24" t="s">
+        <v>129</v>
+      </c>
       <c r="G24" t="s">
-        <v>129</v>
+        <v>252</v>
       </c>
       <c r="H24" t="s">
-        <v>252</v>
+        <v>277</v>
       </c>
       <c r="I24" t="s">
-        <v>277</v>
-      </c>
-      <c r="J24" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25">
         <f t="shared" si="0"/>
         <v>82</v>
@@ -3531,29 +3457,26 @@
       <c r="B25">
         <v>3</v>
       </c>
-      <c r="C25">
-        <v>1</v>
+      <c r="C25" t="s">
+        <v>174</v>
       </c>
       <c r="D25" t="s">
-        <v>174</v>
-      </c>
-      <c r="E25" t="s">
         <v>175</v>
       </c>
+      <c r="F25" t="s">
+        <v>129</v>
+      </c>
       <c r="G25" t="s">
         <v>129</v>
       </c>
       <c r="H25" t="s">
-        <v>129</v>
+        <v>278</v>
       </c>
       <c r="I25" t="s">
-        <v>278</v>
-      </c>
-      <c r="J25" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26">
         <f t="shared" si="0"/>
         <v>83</v>
@@ -3561,32 +3484,29 @@
       <c r="B26">
         <v>3</v>
       </c>
-      <c r="C26">
-        <v>1</v>
+      <c r="C26" t="s">
+        <v>176</v>
       </c>
       <c r="D26" t="s">
-        <v>176</v>
-      </c>
-      <c r="E26" t="s">
         <v>177</v>
       </c>
+      <c r="F26" t="s">
+        <v>129</v>
+      </c>
       <c r="G26" t="s">
-        <v>129</v>
+        <v>279</v>
       </c>
       <c r="H26" t="s">
-        <v>279</v>
+        <v>320</v>
       </c>
       <c r="I26" t="s">
-        <v>320</v>
+        <v>129</v>
       </c>
       <c r="J26" t="s">
-        <v>129</v>
-      </c>
-      <c r="K26" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27">
         <f t="shared" si="0"/>
         <v>84</v>
@@ -3594,29 +3514,26 @@
       <c r="B27">
         <v>3</v>
       </c>
-      <c r="C27">
-        <v>1</v>
+      <c r="C27" t="s">
+        <v>178</v>
       </c>
       <c r="D27" t="s">
-        <v>178</v>
-      </c>
-      <c r="E27" t="s">
         <v>179</v>
       </c>
+      <c r="F27" t="s">
+        <v>129</v>
+      </c>
       <c r="G27" t="s">
-        <v>129</v>
+        <v>281</v>
       </c>
       <c r="H27" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="I27" t="s">
-        <v>282</v>
-      </c>
-      <c r="J27" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28">
         <f t="shared" si="0"/>
         <v>85</v>
@@ -3624,29 +3541,26 @@
       <c r="B28">
         <v>3</v>
       </c>
-      <c r="C28">
-        <v>1</v>
+      <c r="C28" t="s">
+        <v>180</v>
       </c>
       <c r="D28" t="s">
-        <v>180</v>
-      </c>
-      <c r="E28" t="s">
         <v>135</v>
       </c>
+      <c r="F28" t="s">
+        <v>129</v>
+      </c>
       <c r="G28" t="s">
-        <v>129</v>
+        <v>290</v>
       </c>
       <c r="H28" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="I28" t="s">
-        <v>283</v>
-      </c>
-      <c r="J28" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29">
         <f t="shared" si="0"/>
         <v>86</v>
@@ -3654,29 +3568,26 @@
       <c r="B29">
         <v>3</v>
       </c>
-      <c r="C29">
-        <v>1</v>
+      <c r="C29" t="s">
+        <v>181</v>
       </c>
       <c r="D29" t="s">
-        <v>181</v>
-      </c>
-      <c r="E29" t="s">
         <v>138</v>
       </c>
+      <c r="F29" t="s">
+        <v>129</v>
+      </c>
       <c r="G29" t="s">
-        <v>129</v>
+        <v>253</v>
       </c>
       <c r="H29" t="s">
-        <v>253</v>
+        <v>283</v>
       </c>
       <c r="I29" t="s">
-        <v>283</v>
-      </c>
-      <c r="J29" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30">
         <f t="shared" si="0"/>
         <v>87</v>
@@ -3684,29 +3595,26 @@
       <c r="B30">
         <v>3</v>
       </c>
-      <c r="C30">
-        <v>1</v>
+      <c r="C30" t="s">
+        <v>182</v>
       </c>
       <c r="D30" t="s">
-        <v>182</v>
-      </c>
-      <c r="E30" t="s">
         <v>183</v>
       </c>
+      <c r="F30" t="s">
+        <v>129</v>
+      </c>
       <c r="G30" t="s">
-        <v>129</v>
+        <v>284</v>
       </c>
       <c r="H30" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="I30" t="s">
-        <v>285</v>
-      </c>
-      <c r="J30" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31">
         <f t="shared" si="0"/>
         <v>88</v>
@@ -3714,29 +3622,26 @@
       <c r="B31">
         <v>3</v>
       </c>
-      <c r="C31">
-        <v>1</v>
+      <c r="C31" t="s">
+        <v>184</v>
       </c>
       <c r="D31" t="s">
-        <v>184</v>
-      </c>
-      <c r="E31" t="s">
         <v>185</v>
       </c>
+      <c r="F31" t="s">
+        <v>129</v>
+      </c>
       <c r="G31" t="s">
         <v>129</v>
       </c>
       <c r="H31" t="s">
-        <v>129</v>
+        <v>286</v>
       </c>
       <c r="I31" t="s">
-        <v>286</v>
-      </c>
-      <c r="J31" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32">
         <f t="shared" si="0"/>
         <v>89</v>
@@ -3744,29 +3649,26 @@
       <c r="B32">
         <v>3</v>
       </c>
-      <c r="C32">
-        <v>1</v>
+      <c r="C32" t="s">
+        <v>186</v>
       </c>
       <c r="D32" t="s">
-        <v>186</v>
-      </c>
-      <c r="E32" t="s">
         <v>187</v>
       </c>
+      <c r="F32" t="s">
+        <v>129</v>
+      </c>
       <c r="G32" t="s">
         <v>129</v>
       </c>
       <c r="H32" t="s">
-        <v>129</v>
+        <v>288</v>
       </c>
       <c r="I32" t="s">
-        <v>288</v>
-      </c>
-      <c r="J32" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33">
         <f t="shared" si="0"/>
         <v>90</v>
@@ -3774,29 +3676,26 @@
       <c r="B33">
         <v>3</v>
       </c>
-      <c r="C33">
-        <v>1</v>
+      <c r="C33" t="s">
+        <v>188</v>
       </c>
       <c r="D33" t="s">
-        <v>188</v>
-      </c>
-      <c r="E33" t="s">
         <v>152</v>
       </c>
+      <c r="F33" t="s">
+        <v>129</v>
+      </c>
       <c r="G33" t="s">
-        <v>129</v>
+        <v>255</v>
       </c>
       <c r="H33" t="s">
-        <v>255</v>
+        <v>287</v>
       </c>
       <c r="I33" t="s">
-        <v>287</v>
-      </c>
-      <c r="J33" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34">
         <f t="shared" ref="A34:A66" si="1">ROW() + 57</f>
         <v>91</v>
@@ -3804,29 +3703,26 @@
       <c r="B34">
         <v>3</v>
       </c>
-      <c r="C34">
-        <v>1</v>
+      <c r="C34" t="s">
+        <v>189</v>
       </c>
       <c r="D34" t="s">
-        <v>189</v>
-      </c>
-      <c r="E34" t="s">
         <v>190</v>
       </c>
+      <c r="F34" t="s">
+        <v>129</v>
+      </c>
       <c r="G34" t="s">
-        <v>129</v>
+        <v>252</v>
       </c>
       <c r="H34" t="s">
-        <v>252</v>
+        <v>289</v>
       </c>
       <c r="I34" t="s">
-        <v>289</v>
-      </c>
-      <c r="J34" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35">
         <f t="shared" si="1"/>
         <v>92</v>
@@ -3834,29 +3730,26 @@
       <c r="B35">
         <v>3</v>
       </c>
-      <c r="C35">
-        <v>1</v>
+      <c r="C35" t="s">
+        <v>191</v>
       </c>
       <c r="D35" t="s">
-        <v>191</v>
-      </c>
-      <c r="E35" t="s">
         <v>192</v>
       </c>
+      <c r="F35" t="s">
+        <v>129</v>
+      </c>
       <c r="G35" t="s">
-        <v>129</v>
+        <v>279</v>
       </c>
       <c r="H35" t="s">
-        <v>279</v>
+        <v>321</v>
       </c>
       <c r="I35" t="s">
-        <v>321</v>
-      </c>
-      <c r="J35" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36">
         <f t="shared" si="1"/>
         <v>93</v>
@@ -3864,29 +3757,26 @@
       <c r="B36">
         <v>3</v>
       </c>
-      <c r="C36">
-        <v>1</v>
+      <c r="C36" t="s">
+        <v>193</v>
       </c>
       <c r="D36" t="s">
-        <v>193</v>
-      </c>
-      <c r="E36" t="s">
         <v>158</v>
       </c>
+      <c r="F36" t="s">
+        <v>129</v>
+      </c>
       <c r="G36" t="s">
-        <v>129</v>
+        <v>290</v>
       </c>
       <c r="H36" t="s">
-        <v>290</v>
+        <v>277</v>
       </c>
       <c r="I36" t="s">
-        <v>277</v>
-      </c>
-      <c r="J36" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37">
         <f t="shared" si="1"/>
         <v>94</v>
@@ -3894,29 +3784,26 @@
       <c r="B37">
         <v>3</v>
       </c>
-      <c r="C37">
-        <v>1</v>
+      <c r="C37" t="s">
+        <v>194</v>
       </c>
       <c r="D37" t="s">
-        <v>194</v>
-      </c>
-      <c r="E37" t="s">
         <v>195</v>
       </c>
+      <c r="F37" t="s">
+        <v>129</v>
+      </c>
       <c r="G37" t="s">
-        <v>129</v>
+        <v>291</v>
       </c>
       <c r="H37" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="I37" t="s">
-        <v>292</v>
-      </c>
-      <c r="J37" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38">
         <f t="shared" si="1"/>
         <v>95</v>
@@ -3924,29 +3811,26 @@
       <c r="B38">
         <v>3</v>
       </c>
-      <c r="C38">
-        <v>1</v>
+      <c r="C38" t="s">
+        <v>196</v>
       </c>
       <c r="D38" t="s">
-        <v>196</v>
-      </c>
-      <c r="E38" t="s">
         <v>197</v>
       </c>
+      <c r="F38" t="s">
+        <v>129</v>
+      </c>
       <c r="G38" t="s">
-        <v>129</v>
+        <v>293</v>
       </c>
       <c r="H38" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="I38" t="s">
-        <v>294</v>
-      </c>
-      <c r="J38" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39">
         <f t="shared" si="1"/>
         <v>96</v>
@@ -3954,29 +3838,26 @@
       <c r="B39">
         <v>3</v>
       </c>
-      <c r="C39">
-        <v>1</v>
+      <c r="C39" t="s">
+        <v>198</v>
       </c>
       <c r="D39" t="s">
-        <v>198</v>
-      </c>
-      <c r="E39" t="s">
         <v>162</v>
       </c>
+      <c r="F39" t="s">
+        <v>129</v>
+      </c>
       <c r="G39" t="s">
-        <v>129</v>
+        <v>254</v>
       </c>
       <c r="H39" t="s">
-        <v>254</v>
+        <v>283</v>
       </c>
       <c r="I39" t="s">
-        <v>283</v>
-      </c>
-      <c r="J39" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40">
         <f t="shared" si="1"/>
         <v>97</v>
@@ -3984,29 +3865,26 @@
       <c r="B40">
         <v>3</v>
       </c>
-      <c r="C40">
-        <v>1</v>
+      <c r="C40" t="s">
+        <v>199</v>
       </c>
       <c r="D40" t="s">
-        <v>199</v>
-      </c>
-      <c r="E40" t="s">
         <v>164</v>
       </c>
+      <c r="F40" t="s">
+        <v>129</v>
+      </c>
       <c r="G40" t="s">
-        <v>129</v>
+        <v>254</v>
       </c>
       <c r="H40" t="s">
-        <v>254</v>
+        <v>287</v>
       </c>
       <c r="I40" t="s">
-        <v>287</v>
-      </c>
-      <c r="J40" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41">
         <f t="shared" si="1"/>
         <v>98</v>
@@ -4014,29 +3892,26 @@
       <c r="B41">
         <v>3</v>
       </c>
-      <c r="C41">
-        <v>1</v>
+      <c r="C41" t="s">
+        <v>200</v>
       </c>
       <c r="D41" t="s">
-        <v>200</v>
-      </c>
-      <c r="E41" t="s">
         <v>201</v>
       </c>
+      <c r="F41" t="s">
+        <v>129</v>
+      </c>
       <c r="G41" t="s">
-        <v>129</v>
+        <v>279</v>
       </c>
       <c r="H41" t="s">
-        <v>279</v>
+        <v>295</v>
       </c>
       <c r="I41" t="s">
-        <v>295</v>
-      </c>
-      <c r="J41" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42">
         <f t="shared" si="1"/>
         <v>99</v>
@@ -4044,29 +3919,26 @@
       <c r="B42">
         <v>3</v>
       </c>
-      <c r="C42">
-        <v>1</v>
+      <c r="C42" t="s">
+        <v>202</v>
       </c>
       <c r="D42" t="s">
-        <v>202</v>
-      </c>
-      <c r="E42" t="s">
         <v>203</v>
       </c>
+      <c r="F42" t="s">
+        <v>129</v>
+      </c>
       <c r="G42" t="s">
-        <v>129</v>
+        <v>290</v>
       </c>
       <c r="H42" t="s">
-        <v>290</v>
+        <v>296</v>
       </c>
       <c r="I42" t="s">
-        <v>296</v>
-      </c>
-      <c r="J42" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4074,29 +3946,26 @@
       <c r="B43">
         <v>3</v>
       </c>
-      <c r="C43">
-        <v>1</v>
+      <c r="C43" t="s">
+        <v>204</v>
       </c>
       <c r="D43" t="s">
-        <v>204</v>
-      </c>
-      <c r="E43" t="s">
         <v>205</v>
       </c>
+      <c r="F43" t="s">
+        <v>129</v>
+      </c>
       <c r="G43" t="s">
-        <v>129</v>
+        <v>315</v>
       </c>
       <c r="H43" t="s">
-        <v>315</v>
+        <v>297</v>
       </c>
       <c r="I43" t="s">
-        <v>297</v>
-      </c>
-      <c r="J43" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44">
         <f t="shared" si="1"/>
         <v>101</v>
@@ -4104,668 +3973,602 @@
       <c r="B44">
         <v>3</v>
       </c>
-      <c r="C44">
+      <c r="C44" t="s">
+        <v>206</v>
+      </c>
+      <c r="D44" t="s">
+        <v>170</v>
+      </c>
+      <c r="F44" t="s">
+        <v>129</v>
+      </c>
+      <c r="G44" t="s">
+        <v>316</v>
+      </c>
+      <c r="H44" t="s">
+        <v>287</v>
+      </c>
+      <c r="I44" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <f t="shared" si="1"/>
+        <v>102</v>
+      </c>
+      <c r="B45">
+        <v>4</v>
+      </c>
+      <c r="C45" t="s">
+        <v>207</v>
+      </c>
+      <c r="D45" t="s">
+        <v>208</v>
+      </c>
+      <c r="F45" t="s">
+        <v>129</v>
+      </c>
+      <c r="G45" t="s">
+        <v>299</v>
+      </c>
+      <c r="H45" t="s">
+        <v>300</v>
+      </c>
+      <c r="I45" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <f t="shared" si="1"/>
+        <v>103</v>
+      </c>
+      <c r="B46">
+        <v>4</v>
+      </c>
+      <c r="C46" t="s">
+        <v>209</v>
+      </c>
+      <c r="D46" t="s">
+        <v>133</v>
+      </c>
+      <c r="F46" t="s">
+        <v>129</v>
+      </c>
+      <c r="G46" t="s">
+        <v>252</v>
+      </c>
+      <c r="H46" t="s">
+        <v>305</v>
+      </c>
+      <c r="I46" t="s">
+        <v>129</v>
+      </c>
+      <c r="J46" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <f t="shared" si="1"/>
+        <v>104</v>
+      </c>
+      <c r="B47">
+        <v>4</v>
+      </c>
+      <c r="C47" t="s">
+        <v>210</v>
+      </c>
+      <c r="D47" t="s">
+        <v>211</v>
+      </c>
+      <c r="F47" t="s">
+        <v>129</v>
+      </c>
+      <c r="G47" t="s">
+        <v>254</v>
+      </c>
+      <c r="H47" t="s">
+        <v>300</v>
+      </c>
+      <c r="I47" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <f t="shared" si="1"/>
+        <v>105</v>
+      </c>
+      <c r="B48">
+        <v>4</v>
+      </c>
+      <c r="C48" t="s">
+        <v>212</v>
+      </c>
+      <c r="D48" t="s">
+        <v>213</v>
+      </c>
+      <c r="F48" t="s">
+        <v>129</v>
+      </c>
+      <c r="G48" t="s">
+        <v>302</v>
+      </c>
+      <c r="H48" t="s">
+        <v>303</v>
+      </c>
+      <c r="I48" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <f t="shared" si="1"/>
+        <v>106</v>
+      </c>
+      <c r="B49">
+        <v>4</v>
+      </c>
+      <c r="C49" t="s">
+        <v>214</v>
+      </c>
+      <c r="D49" t="s">
+        <v>135</v>
+      </c>
+      <c r="F49" t="s">
+        <v>129</v>
+      </c>
+      <c r="G49" t="s">
+        <v>290</v>
+      </c>
+      <c r="H49" t="s">
+        <v>306</v>
+      </c>
+      <c r="I49" t="s">
+        <v>300</v>
+      </c>
+      <c r="J49" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <f t="shared" si="1"/>
+        <v>107</v>
+      </c>
+      <c r="B50">
+        <v>4</v>
+      </c>
+      <c r="C50" t="s">
+        <v>215</v>
+      </c>
+      <c r="D50" t="s">
+        <v>135</v>
+      </c>
+      <c r="F50" t="s">
+        <v>129</v>
+      </c>
+      <c r="G50" t="s">
+        <v>290</v>
+      </c>
+      <c r="H50" t="s">
+        <v>306</v>
+      </c>
+      <c r="I50" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <f t="shared" si="1"/>
+        <v>108</v>
+      </c>
+      <c r="B51">
+        <v>4</v>
+      </c>
+      <c r="C51" t="s">
+        <v>216</v>
+      </c>
+      <c r="D51" t="s">
+        <v>217</v>
+      </c>
+      <c r="F51" t="s">
+        <v>129</v>
+      </c>
+      <c r="G51" t="s">
+        <v>307</v>
+      </c>
+      <c r="H51" t="s">
+        <v>308</v>
+      </c>
+      <c r="I51" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <f t="shared" si="1"/>
+        <v>109</v>
+      </c>
+      <c r="B52">
+        <v>4</v>
+      </c>
+      <c r="C52" t="s">
+        <v>218</v>
+      </c>
+      <c r="D52" t="s">
+        <v>138</v>
+      </c>
+      <c r="F52" t="s">
+        <v>129</v>
+      </c>
+      <c r="G52" t="s">
+        <v>309</v>
+      </c>
+      <c r="H52" t="s">
+        <v>306</v>
+      </c>
+      <c r="I52" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <f t="shared" si="1"/>
+        <v>110</v>
+      </c>
+      <c r="B53">
+        <v>4</v>
+      </c>
+      <c r="C53" t="s">
+        <v>219</v>
+      </c>
+      <c r="D53" t="s">
+        <v>183</v>
+      </c>
+      <c r="F53" t="s">
+        <v>129</v>
+      </c>
+      <c r="G53" t="s">
+        <v>284</v>
+      </c>
+      <c r="H53" t="s">
+        <v>310</v>
+      </c>
+      <c r="I53" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <f t="shared" si="1"/>
+        <v>111</v>
+      </c>
+      <c r="B54">
+        <v>4</v>
+      </c>
+      <c r="C54" t="s">
+        <v>220</v>
+      </c>
+      <c r="D54" t="s">
+        <v>221</v>
+      </c>
+      <c r="F54" t="s">
+        <v>129</v>
+      </c>
+      <c r="G54" t="s">
+        <v>319</v>
+      </c>
+      <c r="H54" t="s">
+        <v>306</v>
+      </c>
+      <c r="I54" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <f t="shared" si="1"/>
+        <v>112</v>
+      </c>
+      <c r="B55">
+        <v>4</v>
+      </c>
+      <c r="C55" t="s">
+        <v>222</v>
+      </c>
+      <c r="D55" t="s">
+        <v>223</v>
+      </c>
+      <c r="F55" t="s">
+        <v>129</v>
+      </c>
+      <c r="G55" t="s">
+        <v>313</v>
+      </c>
+      <c r="H55" t="s">
+        <v>311</v>
+      </c>
+      <c r="I55" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <f t="shared" si="1"/>
+        <v>113</v>
+      </c>
+      <c r="B56">
+        <v>4</v>
+      </c>
+      <c r="C56" t="s">
+        <v>224</v>
+      </c>
+      <c r="D56" t="s">
+        <v>152</v>
+      </c>
+      <c r="F56" t="s">
+        <v>129</v>
+      </c>
+      <c r="G56" t="s">
+        <v>312</v>
+      </c>
+      <c r="H56" t="s">
+        <v>314</v>
+      </c>
+      <c r="I56" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <f t="shared" si="1"/>
+        <v>114</v>
+      </c>
+      <c r="B57">
+        <v>4</v>
+      </c>
+      <c r="C57" t="s">
+        <v>225</v>
+      </c>
+      <c r="D57" t="s">
+        <v>226</v>
+      </c>
+      <c r="F57" t="s">
+        <v>129</v>
+      </c>
+      <c r="G57" t="s">
+        <v>317</v>
+      </c>
+      <c r="H57" t="s">
+        <v>318</v>
+      </c>
+      <c r="I57" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <f t="shared" si="1"/>
+        <v>115</v>
+      </c>
+      <c r="B58">
+        <v>4</v>
+      </c>
+      <c r="C58" t="s">
+        <v>227</v>
+      </c>
+      <c r="D58" t="s">
+        <v>158</v>
+      </c>
+      <c r="F58" t="s">
+        <v>129</v>
+      </c>
+      <c r="G58" t="s">
+        <v>290</v>
+      </c>
+      <c r="H58" t="s">
+        <v>306</v>
+      </c>
+      <c r="I58" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <f t="shared" si="1"/>
+        <v>116</v>
+      </c>
+      <c r="B59">
+        <v>4</v>
+      </c>
+      <c r="C59" t="s">
+        <v>228</v>
+      </c>
+      <c r="D59" t="s">
+        <v>229</v>
+      </c>
+      <c r="F59" t="b">
         <v>1</v>
       </c>
-      <c r="D44" t="s">
-        <v>206</v>
-      </c>
-      <c r="E44" t="s">
+      <c r="G59" t="s">
+        <v>129</v>
+      </c>
+      <c r="H59" t="s">
+        <v>323</v>
+      </c>
+      <c r="I59" t="s">
+        <v>129</v>
+      </c>
+      <c r="J59" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <f t="shared" si="1"/>
+        <v>117</v>
+      </c>
+      <c r="B60">
+        <v>4</v>
+      </c>
+      <c r="C60" t="s">
+        <v>230</v>
+      </c>
+      <c r="D60" t="s">
+        <v>231</v>
+      </c>
+      <c r="F60" t="s">
+        <v>129</v>
+      </c>
+      <c r="G60" t="s">
+        <v>299</v>
+      </c>
+      <c r="H60" t="s">
+        <v>300</v>
+      </c>
+      <c r="I60" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <f t="shared" si="1"/>
+        <v>118</v>
+      </c>
+      <c r="B61">
+        <v>4</v>
+      </c>
+      <c r="C61" t="s">
+        <v>232</v>
+      </c>
+      <c r="D61" t="s">
+        <v>233</v>
+      </c>
+      <c r="F61" t="s">
+        <v>129</v>
+      </c>
+      <c r="G61" t="s">
+        <v>324</v>
+      </c>
+      <c r="H61" t="s">
+        <v>325</v>
+      </c>
+      <c r="I61" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <f t="shared" si="1"/>
+        <v>119</v>
+      </c>
+      <c r="B62">
+        <v>4</v>
+      </c>
+      <c r="C62" t="s">
+        <v>234</v>
+      </c>
+      <c r="D62" t="s">
+        <v>162</v>
+      </c>
+      <c r="F62" t="s">
+        <v>129</v>
+      </c>
+      <c r="G62" t="s">
+        <v>254</v>
+      </c>
+      <c r="H62" t="s">
+        <v>314</v>
+      </c>
+      <c r="I62" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <f t="shared" si="1"/>
+        <v>120</v>
+      </c>
+      <c r="B63">
+        <v>4</v>
+      </c>
+      <c r="C63" t="s">
+        <v>235</v>
+      </c>
+      <c r="D63" t="s">
+        <v>236</v>
+      </c>
+      <c r="F63" t="s">
+        <v>129</v>
+      </c>
+      <c r="G63" t="s">
+        <v>326</v>
+      </c>
+      <c r="H63" t="s">
+        <v>306</v>
+      </c>
+      <c r="I63" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <f t="shared" si="1"/>
+        <v>121</v>
+      </c>
+      <c r="B64">
+        <v>4</v>
+      </c>
+      <c r="C64" t="s">
+        <v>237</v>
+      </c>
+      <c r="D64" t="s">
         <v>170</v>
       </c>
-      <c r="G44" t="s">
-        <v>129</v>
-      </c>
-      <c r="H44" t="s">
-        <v>316</v>
-      </c>
-      <c r="I44" t="s">
-        <v>287</v>
-      </c>
-      <c r="J44" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A45">
-        <f t="shared" si="1"/>
-        <v>102</v>
-      </c>
-      <c r="B45">
-        <v>4</v>
-      </c>
-      <c r="C45">
-        <v>1</v>
-      </c>
-      <c r="D45" t="s">
-        <v>207</v>
-      </c>
-      <c r="E45" t="s">
-        <v>208</v>
-      </c>
-      <c r="G45" t="s">
-        <v>129</v>
-      </c>
-      <c r="H45" t="s">
-        <v>299</v>
-      </c>
-      <c r="I45" t="s">
+      <c r="F64" t="s">
+        <v>129</v>
+      </c>
+      <c r="G64" t="s">
+        <v>327</v>
+      </c>
+      <c r="H64" t="s">
         <v>300</v>
       </c>
-      <c r="J45" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A46">
-        <f t="shared" si="1"/>
-        <v>103</v>
-      </c>
-      <c r="B46">
-        <v>4</v>
-      </c>
-      <c r="C46">
-        <v>1</v>
-      </c>
-      <c r="D46" t="s">
-        <v>209</v>
-      </c>
-      <c r="E46" t="s">
-        <v>133</v>
-      </c>
-      <c r="G46" t="s">
-        <v>129</v>
-      </c>
-      <c r="H46" t="s">
-        <v>252</v>
-      </c>
-      <c r="I46" t="s">
-        <v>305</v>
-      </c>
-      <c r="J46" t="s">
-        <v>129</v>
-      </c>
-      <c r="K46" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A47">
-        <f t="shared" si="1"/>
-        <v>104</v>
-      </c>
-      <c r="B47">
-        <v>4</v>
-      </c>
-      <c r="C47">
-        <v>1</v>
-      </c>
-      <c r="D47" t="s">
-        <v>210</v>
-      </c>
-      <c r="E47" t="s">
-        <v>211</v>
-      </c>
-      <c r="G47" t="s">
-        <v>129</v>
-      </c>
-      <c r="H47" t="s">
-        <v>254</v>
-      </c>
-      <c r="I47" t="s">
-        <v>300</v>
-      </c>
-      <c r="J47" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A48">
-        <f t="shared" si="1"/>
-        <v>105</v>
-      </c>
-      <c r="B48">
-        <v>4</v>
-      </c>
-      <c r="C48">
-        <v>1</v>
-      </c>
-      <c r="D48" t="s">
-        <v>212</v>
-      </c>
-      <c r="E48" t="s">
-        <v>213</v>
-      </c>
-      <c r="G48" t="s">
-        <v>129</v>
-      </c>
-      <c r="H48" t="s">
-        <v>302</v>
-      </c>
-      <c r="I48" t="s">
-        <v>303</v>
-      </c>
-      <c r="J48" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A49">
-        <f t="shared" si="1"/>
-        <v>106</v>
-      </c>
-      <c r="B49">
-        <v>4</v>
-      </c>
-      <c r="C49">
-        <v>1</v>
-      </c>
-      <c r="D49" t="s">
-        <v>214</v>
-      </c>
-      <c r="E49" t="s">
-        <v>135</v>
-      </c>
-      <c r="G49" t="s">
-        <v>129</v>
-      </c>
-      <c r="H49" t="s">
-        <v>290</v>
-      </c>
-      <c r="I49" t="s">
+      <c r="I64" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <f t="shared" si="1"/>
+        <v>122</v>
+      </c>
+      <c r="B65">
+        <v>4</v>
+      </c>
+      <c r="C65" t="s">
+        <v>238</v>
+      </c>
+      <c r="D65" t="s">
+        <v>239</v>
+      </c>
+      <c r="F65" t="s">
+        <v>129</v>
+      </c>
+      <c r="G65" t="s">
+        <v>315</v>
+      </c>
+      <c r="H65" t="s">
         <v>306</v>
       </c>
-      <c r="J49" t="s">
-        <v>300</v>
-      </c>
-      <c r="K49" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A50">
-        <f t="shared" si="1"/>
-        <v>107</v>
-      </c>
-      <c r="B50">
-        <v>4</v>
-      </c>
-      <c r="C50">
-        <v>1</v>
-      </c>
-      <c r="D50" t="s">
-        <v>215</v>
-      </c>
-      <c r="E50" t="s">
-        <v>135</v>
-      </c>
-      <c r="G50" t="s">
-        <v>129</v>
-      </c>
-      <c r="H50" t="s">
-        <v>290</v>
-      </c>
-      <c r="I50" t="s">
-        <v>306</v>
-      </c>
-      <c r="J50" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A51">
-        <f t="shared" si="1"/>
-        <v>108</v>
-      </c>
-      <c r="B51">
-        <v>4</v>
-      </c>
-      <c r="C51">
-        <v>1</v>
-      </c>
-      <c r="D51" t="s">
-        <v>216</v>
-      </c>
-      <c r="E51" t="s">
-        <v>217</v>
-      </c>
-      <c r="G51" t="s">
-        <v>129</v>
-      </c>
-      <c r="H51" t="s">
-        <v>307</v>
-      </c>
-      <c r="I51" t="s">
-        <v>308</v>
-      </c>
-      <c r="J51" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A52">
-        <f t="shared" si="1"/>
-        <v>109</v>
-      </c>
-      <c r="B52">
-        <v>4</v>
-      </c>
-      <c r="C52">
-        <v>1</v>
-      </c>
-      <c r="D52" t="s">
-        <v>218</v>
-      </c>
-      <c r="E52" t="s">
-        <v>138</v>
-      </c>
-      <c r="G52" t="s">
-        <v>129</v>
-      </c>
-      <c r="H52" t="s">
-        <v>309</v>
-      </c>
-      <c r="I52" t="s">
-        <v>306</v>
-      </c>
-      <c r="J52" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A53">
-        <f t="shared" si="1"/>
-        <v>110</v>
-      </c>
-      <c r="B53">
-        <v>4</v>
-      </c>
-      <c r="C53">
-        <v>1</v>
-      </c>
-      <c r="D53" t="s">
-        <v>219</v>
-      </c>
-      <c r="E53" t="s">
-        <v>183</v>
-      </c>
-      <c r="G53" t="s">
-        <v>129</v>
-      </c>
-      <c r="H53" t="s">
-        <v>284</v>
-      </c>
-      <c r="I53" t="s">
-        <v>310</v>
-      </c>
-      <c r="J53" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A54">
-        <f t="shared" si="1"/>
-        <v>111</v>
-      </c>
-      <c r="B54">
-        <v>4</v>
-      </c>
-      <c r="C54">
-        <v>1</v>
-      </c>
-      <c r="D54" t="s">
-        <v>220</v>
-      </c>
-      <c r="E54" t="s">
-        <v>221</v>
-      </c>
-      <c r="G54" t="s">
-        <v>129</v>
-      </c>
-      <c r="H54" t="s">
-        <v>319</v>
-      </c>
-      <c r="I54" t="s">
-        <v>306</v>
-      </c>
-      <c r="J54" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A55">
-        <f t="shared" si="1"/>
-        <v>112</v>
-      </c>
-      <c r="B55">
-        <v>4</v>
-      </c>
-      <c r="C55">
-        <v>1</v>
-      </c>
-      <c r="D55" t="s">
-        <v>222</v>
-      </c>
-      <c r="E55" t="s">
-        <v>223</v>
-      </c>
-      <c r="G55" t="s">
-        <v>129</v>
-      </c>
-      <c r="H55" t="s">
-        <v>313</v>
-      </c>
-      <c r="I55" t="s">
-        <v>311</v>
-      </c>
-      <c r="J55" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A56">
-        <f t="shared" si="1"/>
-        <v>113</v>
-      </c>
-      <c r="B56">
-        <v>4</v>
-      </c>
-      <c r="C56">
-        <v>1</v>
-      </c>
-      <c r="D56" t="s">
-        <v>224</v>
-      </c>
-      <c r="E56" t="s">
-        <v>152</v>
-      </c>
-      <c r="G56" t="s">
-        <v>129</v>
-      </c>
-      <c r="H56" t="s">
-        <v>312</v>
-      </c>
-      <c r="I56" t="s">
-        <v>314</v>
-      </c>
-      <c r="J56" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A57">
-        <f t="shared" si="1"/>
-        <v>114</v>
-      </c>
-      <c r="B57">
-        <v>4</v>
-      </c>
-      <c r="C57">
-        <v>1</v>
-      </c>
-      <c r="D57" t="s">
-        <v>225</v>
-      </c>
-      <c r="E57" t="s">
-        <v>226</v>
-      </c>
-      <c r="G57" t="s">
-        <v>129</v>
-      </c>
-      <c r="H57" t="s">
-        <v>317</v>
-      </c>
-      <c r="I57" t="s">
-        <v>318</v>
-      </c>
-      <c r="J57" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A58">
-        <f t="shared" si="1"/>
-        <v>115</v>
-      </c>
-      <c r="B58">
-        <v>4</v>
-      </c>
-      <c r="C58">
-        <v>1</v>
-      </c>
-      <c r="D58" t="s">
-        <v>227</v>
-      </c>
-      <c r="E58" t="s">
-        <v>158</v>
-      </c>
-      <c r="G58" t="s">
-        <v>129</v>
-      </c>
-      <c r="H58" t="s">
-        <v>290</v>
-      </c>
-      <c r="I58" t="s">
-        <v>306</v>
-      </c>
-      <c r="J58" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A59">
-        <f t="shared" si="1"/>
-        <v>116</v>
-      </c>
-      <c r="B59">
-        <v>4</v>
-      </c>
-      <c r="C59">
-        <v>1</v>
-      </c>
-      <c r="D59" t="s">
-        <v>228</v>
-      </c>
-      <c r="E59" t="s">
-        <v>229</v>
-      </c>
-      <c r="G59" t="b">
-        <v>1</v>
-      </c>
-      <c r="H59" t="s">
-        <v>129</v>
-      </c>
-      <c r="I59" t="s">
-        <v>323</v>
-      </c>
-      <c r="J59" t="s">
-        <v>129</v>
-      </c>
-      <c r="K59" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A60">
-        <f t="shared" si="1"/>
-        <v>117</v>
-      </c>
-      <c r="B60">
-        <v>4</v>
-      </c>
-      <c r="C60">
-        <v>1</v>
-      </c>
-      <c r="D60" t="s">
-        <v>230</v>
-      </c>
-      <c r="E60" t="s">
-        <v>231</v>
-      </c>
-      <c r="G60" t="s">
-        <v>129</v>
-      </c>
-      <c r="H60" t="s">
-        <v>299</v>
-      </c>
-      <c r="I60" t="s">
-        <v>300</v>
-      </c>
-      <c r="J60" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A61">
-        <f t="shared" si="1"/>
-        <v>118</v>
-      </c>
-      <c r="B61">
-        <v>4</v>
-      </c>
-      <c r="C61">
-        <v>1</v>
-      </c>
-      <c r="D61" t="s">
-        <v>232</v>
-      </c>
-      <c r="E61" t="s">
-        <v>233</v>
-      </c>
-      <c r="G61" t="s">
-        <v>129</v>
-      </c>
-      <c r="H61" t="s">
-        <v>324</v>
-      </c>
-      <c r="I61" t="s">
-        <v>325</v>
-      </c>
-      <c r="J61" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A62">
-        <f t="shared" si="1"/>
-        <v>119</v>
-      </c>
-      <c r="B62">
-        <v>4</v>
-      </c>
-      <c r="C62">
-        <v>1</v>
-      </c>
-      <c r="D62" t="s">
-        <v>234</v>
-      </c>
-      <c r="E62" t="s">
-        <v>162</v>
-      </c>
-      <c r="G62" t="s">
-        <v>129</v>
-      </c>
-      <c r="H62" t="s">
-        <v>254</v>
-      </c>
-      <c r="I62" t="s">
-        <v>314</v>
-      </c>
-      <c r="J62" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A63">
-        <f t="shared" si="1"/>
-        <v>120</v>
-      </c>
-      <c r="B63">
-        <v>4</v>
-      </c>
-      <c r="C63">
-        <v>1</v>
-      </c>
-      <c r="D63" t="s">
-        <v>235</v>
-      </c>
-      <c r="E63" t="s">
-        <v>236</v>
-      </c>
-      <c r="G63" t="s">
-        <v>129</v>
-      </c>
-      <c r="H63" t="s">
-        <v>326</v>
-      </c>
-      <c r="I63" t="s">
-        <v>306</v>
-      </c>
-      <c r="J63" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A64">
-        <f t="shared" si="1"/>
-        <v>121</v>
-      </c>
-      <c r="B64">
-        <v>4</v>
-      </c>
-      <c r="C64">
-        <v>1</v>
-      </c>
-      <c r="D64" t="s">
-        <v>237</v>
-      </c>
-      <c r="E64" t="s">
-        <v>170</v>
-      </c>
-      <c r="G64" t="s">
-        <v>129</v>
-      </c>
-      <c r="H64" t="s">
-        <v>327</v>
-      </c>
-      <c r="I64" t="s">
-        <v>300</v>
-      </c>
-      <c r="J64" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A65">
-        <f t="shared" si="1"/>
-        <v>122</v>
-      </c>
-      <c r="B65">
-        <v>4</v>
-      </c>
-      <c r="C65">
-        <v>1</v>
-      </c>
-      <c r="D65" t="s">
-        <v>238</v>
-      </c>
-      <c r="E65" t="s">
-        <v>239</v>
-      </c>
-      <c r="G65" t="s">
-        <v>129</v>
-      </c>
-      <c r="H65" t="s">
-        <v>315</v>
-      </c>
       <c r="I65" t="s">
-        <v>306</v>
-      </c>
-      <c r="J65" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66">
         <f t="shared" si="1"/>
         <v>123</v>
@@ -4773,32 +4576,30 @@
       <c r="B66">
         <v>4</v>
       </c>
-      <c r="C66">
-        <v>1</v>
+      <c r="C66" t="s">
+        <v>240</v>
       </c>
       <c r="D66" t="s">
-        <v>240</v>
-      </c>
-      <c r="E66" t="s">
         <v>241</v>
       </c>
+      <c r="F66" t="s">
+        <v>129</v>
+      </c>
       <c r="G66" t="s">
         <v>129</v>
       </c>
       <c r="H66" t="s">
-        <v>129</v>
+        <v>328</v>
       </c>
       <c r="I66" t="s">
-        <v>328</v>
-      </c>
-      <c r="J66" t="s">
         <v>129</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -4811,14 +4612,14 @@
       <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="18.83203125" customWidth="1"/>
-    <col min="4" max="4" width="18.83203125" style="1" customWidth="1"/>
-    <col min="5" max="10" width="18.83203125" customWidth="1"/>
+    <col min="1" max="3" width="18.875" customWidth="1"/>
+    <col min="4" max="4" width="18.875" style="1" customWidth="1"/>
+    <col min="5" max="10" width="18.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4841,7 +4642,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -4861,7 +4662,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -4881,7 +4682,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -4904,7 +4705,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -4924,7 +4725,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -4944,7 +4745,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -4964,7 +4765,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -4984,7 +4785,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -5004,7 +4805,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>34</v>
       </c>
@@ -5012,7 +4813,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>36</v>
       </c>
@@ -5020,12 +4821,12 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -5057,7 +4858,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1</v>
       </c>
@@ -5086,7 +4887,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2</v>
       </c>
@@ -5115,7 +4916,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>3</v>
       </c>
@@ -5144,7 +4945,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>4</v>
       </c>
@@ -5173,7 +4974,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>5</v>
       </c>
@@ -5202,7 +5003,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>6</v>
       </c>
@@ -5231,7 +5032,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>7</v>
       </c>
@@ -5260,7 +5061,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>8</v>
       </c>
@@ -5289,7 +5090,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D24"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Corrected errors in cards database for both excel file and events.csv
</commit_message>
<xml_diff>
--- a/data/TP Database.xlsx
+++ b/data/TP Database.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_My Files\_Uni\Year 3\Term 1\3 - Team Project\_TP Code\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sophiachung/Team Project/cs01-main/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41FD4BA5-A2DD-4BD3-81F9-144B5265B7FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A21ED4D-3171-0B4D-955E-77A80A2517FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-1290" windowWidth="29040" windowHeight="15840" xr2:uid="{F6F91125-3C8A-D047-93DD-1F3A6DE88698}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="18120" windowHeight="15860" activeTab="1" xr2:uid="{F6F91125-3C8A-D047-93DD-1F3A6DE88698}"/>
   </bookViews>
   <sheets>
     <sheet name="Activities" sheetId="2" r:id="rId1"/>
@@ -902,9 +902,6 @@
     <t>n0:1:3</t>
   </si>
   <si>
-    <t>n41:1, , n(42/45/46):2</t>
-  </si>
-  <si>
     <t>n(43/44):2</t>
   </si>
   <si>
@@ -923,9 +920,6 @@
     <t>n(17/18/19/20/21/22/23/24/25/26/27/28):1</t>
   </si>
   <si>
-    <t>n(33/34/35/36):1, n(45/46):1</t>
-  </si>
-  <si>
     <t>b0:2:4</t>
   </si>
   <si>
@@ -1029,6 +1023,12 @@
   </si>
   <si>
     <t>f5:1</t>
+  </si>
+  <si>
+    <t>n41:1&amp;n(42/45/46):2</t>
+  </si>
+  <si>
+    <t>n(33/34/35/36):1&amp;n(45/46):1</t>
   </si>
 </sst>
 </file>
@@ -1491,21 +1491,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18AE550B-A04F-B142-B067-7E2D879988FA}">
   <dimension ref="A1:H59"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="102" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScale="102" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.625" customWidth="1"/>
-    <col min="2" max="2" width="15.125" customWidth="1"/>
-    <col min="3" max="3" width="10.375" customWidth="1"/>
-    <col min="4" max="4" width="25.125" customWidth="1"/>
+    <col min="1" max="1" width="9.6640625" customWidth="1"/>
+    <col min="2" max="2" width="15.1640625" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" customWidth="1"/>
+    <col min="4" max="4" width="25.1640625" customWidth="1"/>
     <col min="5" max="6" width="17.5" customWidth="1"/>
     <col min="7" max="7" width="9.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1531,7 +1531,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2">
         <f t="shared" ref="A2:A33" si="0">ROW() - 1</f>
         <v>1</v>
@@ -1555,7 +1555,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -1579,7 +1579,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -1600,7 +1600,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1621,7 +1621,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1642,7 +1642,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1663,7 +1663,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1684,7 +1684,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1705,7 +1705,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1726,7 +1726,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1747,7 +1747,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1768,7 +1768,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1789,7 +1789,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1810,7 +1810,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1831,7 +1831,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1852,7 +1852,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1873,7 +1873,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1894,7 +1894,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -1915,7 +1915,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -1936,7 +1936,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -1957,7 +1957,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -1978,7 +1978,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -1999,7 +1999,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -2020,7 +2020,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -2041,7 +2041,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -2062,7 +2062,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -2083,7 +2083,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -2104,7 +2104,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -2125,7 +2125,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -2146,7 +2146,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -2167,7 +2167,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -2188,7 +2188,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -2209,7 +2209,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34">
         <f t="shared" ref="A34:A59" si="1">ROW() - 1</f>
         <v>33</v>
@@ -2230,7 +2230,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35">
         <f t="shared" si="1"/>
         <v>34</v>
@@ -2251,7 +2251,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36">
         <f t="shared" si="1"/>
         <v>35</v>
@@ -2272,7 +2272,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37">
         <f t="shared" si="1"/>
         <v>36</v>
@@ -2293,7 +2293,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38">
         <f t="shared" si="1"/>
         <v>37</v>
@@ -2314,7 +2314,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39">
         <f t="shared" si="1"/>
         <v>38</v>
@@ -2335,7 +2335,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40">
         <f t="shared" si="1"/>
         <v>39</v>
@@ -2356,7 +2356,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41">
         <f t="shared" si="1"/>
         <v>40</v>
@@ -2377,7 +2377,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42">
         <f t="shared" si="1"/>
         <v>41</v>
@@ -2398,7 +2398,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43">
         <f t="shared" si="1"/>
         <v>42</v>
@@ -2419,7 +2419,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44">
         <f t="shared" si="1"/>
         <v>43</v>
@@ -2440,7 +2440,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45">
         <f t="shared" si="1"/>
         <v>44</v>
@@ -2461,7 +2461,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46">
         <f t="shared" si="1"/>
         <v>45</v>
@@ -2482,7 +2482,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47">
         <f t="shared" si="1"/>
         <v>46</v>
@@ -2503,7 +2503,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48">
         <f t="shared" si="1"/>
         <v>47</v>
@@ -2524,7 +2524,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49">
         <f t="shared" si="1"/>
         <v>48</v>
@@ -2545,7 +2545,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50">
         <f t="shared" si="1"/>
         <v>49</v>
@@ -2566,7 +2566,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51">
         <f t="shared" si="1"/>
         <v>50</v>
@@ -2587,7 +2587,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52">
         <f t="shared" si="1"/>
         <v>51</v>
@@ -2608,7 +2608,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53">
         <f t="shared" si="1"/>
         <v>52</v>
@@ -2629,7 +2629,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54">
         <f t="shared" si="1"/>
         <v>53</v>
@@ -2650,7 +2650,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55">
         <f t="shared" si="1"/>
         <v>54</v>
@@ -2671,7 +2671,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56">
         <f t="shared" si="1"/>
         <v>55</v>
@@ -2692,7 +2692,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57">
         <f t="shared" si="1"/>
         <v>56</v>
@@ -2713,7 +2713,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58">
         <f t="shared" si="1"/>
         <v>57</v>
@@ -2734,7 +2734,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59">
         <f t="shared" si="1"/>
         <v>58</v>
@@ -2767,24 +2767,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84DC5E79-A11F-0148-B3A8-F5384824D987}">
   <dimension ref="A1:J66"/>
   <sheetViews>
-    <sheetView zoomScale="99" zoomScaleNormal="99" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="99" zoomScaleNormal="99" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.125" customWidth="1"/>
+    <col min="1" max="1" width="9.1640625" customWidth="1"/>
     <col min="2" max="2" width="9.5" customWidth="1"/>
-    <col min="3" max="3" width="10.625" customWidth="1"/>
-    <col min="4" max="4" width="25.875" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" customWidth="1"/>
+    <col min="4" max="4" width="25.83203125" customWidth="1"/>
     <col min="5" max="5" width="26" customWidth="1"/>
     <col min="6" max="6" width="14" customWidth="1"/>
     <col min="7" max="7" width="17" customWidth="1"/>
-    <col min="8" max="8" width="15.875" customWidth="1"/>
+    <col min="8" max="8" width="24.6640625" customWidth="1"/>
     <col min="9" max="9" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2810,10 +2810,10 @@
         <v>126</v>
       </c>
       <c r="I1" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2">
         <f t="shared" ref="A2:A33" si="0">ROW() + 57</f>
         <v>59</v>
@@ -2840,7 +2840,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3">
         <f t="shared" si="0"/>
         <v>60</v>
@@ -2867,7 +2867,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4">
         <f t="shared" si="0"/>
         <v>61</v>
@@ -2894,7 +2894,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>62</v>
@@ -2912,7 +2912,7 @@
         <v>129</v>
       </c>
       <c r="G5" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="H5" t="s">
         <v>261</v>
@@ -2921,7 +2921,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>63</v>
@@ -2939,7 +2939,7 @@
         <v>129</v>
       </c>
       <c r="G6" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="H6" t="s">
         <v>261</v>
@@ -2948,7 +2948,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>64</v>
@@ -2975,7 +2975,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>65</v>
@@ -3005,7 +3005,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>66</v>
@@ -3032,7 +3032,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>67</v>
@@ -3062,7 +3062,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>68</v>
@@ -3092,7 +3092,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>69</v>
@@ -3122,7 +3122,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>70</v>
@@ -3149,7 +3149,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>71</v>
@@ -3176,7 +3176,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>72</v>
@@ -3191,7 +3191,7 @@
         <v>156</v>
       </c>
       <c r="F15" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="G15" t="s">
         <v>129</v>
@@ -3206,7 +3206,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>73</v>
@@ -3224,16 +3224,16 @@
         <v>129</v>
       </c>
       <c r="G16" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="H16" t="s">
         <v>260</v>
       </c>
       <c r="I16" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>74</v>
@@ -3260,7 +3260,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>75</v>
@@ -3287,7 +3287,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>76</v>
@@ -3314,7 +3314,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>77</v>
@@ -3341,7 +3341,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>78</v>
@@ -3368,7 +3368,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22">
         <f t="shared" si="0"/>
         <v>79</v>
@@ -3395,7 +3395,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23">
         <f t="shared" si="0"/>
         <v>80</v>
@@ -3422,7 +3422,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24">
         <f t="shared" si="0"/>
         <v>81</v>
@@ -3449,7 +3449,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25">
         <f t="shared" si="0"/>
         <v>82</v>
@@ -3476,7 +3476,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26">
         <f t="shared" si="0"/>
         <v>83</v>
@@ -3497,7 +3497,7 @@
         <v>279</v>
       </c>
       <c r="H26" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="I26" t="s">
         <v>129</v>
@@ -3506,7 +3506,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27">
         <f t="shared" si="0"/>
         <v>84</v>
@@ -3533,7 +3533,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28">
         <f t="shared" si="0"/>
         <v>85</v>
@@ -3551,7 +3551,7 @@
         <v>129</v>
       </c>
       <c r="G28" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="H28" t="s">
         <v>283</v>
@@ -3560,7 +3560,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29">
         <f t="shared" si="0"/>
         <v>86</v>
@@ -3587,7 +3587,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30">
         <f t="shared" si="0"/>
         <v>87</v>
@@ -3614,7 +3614,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31">
         <f t="shared" si="0"/>
         <v>88</v>
@@ -3641,7 +3641,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32">
         <f t="shared" si="0"/>
         <v>89</v>
@@ -3662,13 +3662,13 @@
         <v>129</v>
       </c>
       <c r="H32" t="s">
-        <v>288</v>
+        <v>329</v>
       </c>
       <c r="I32" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33">
         <f t="shared" si="0"/>
         <v>90</v>
@@ -3695,7 +3695,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34">
         <f t="shared" ref="A34:A66" si="1">ROW() + 57</f>
         <v>91</v>
@@ -3716,13 +3716,13 @@
         <v>252</v>
       </c>
       <c r="H34" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="I34" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35">
         <f t="shared" si="1"/>
         <v>92</v>
@@ -3743,13 +3743,13 @@
         <v>279</v>
       </c>
       <c r="H35" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="I35" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36">
         <f t="shared" si="1"/>
         <v>93</v>
@@ -3767,16 +3767,16 @@
         <v>129</v>
       </c>
       <c r="G36" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="H36" t="s">
         <v>277</v>
       </c>
       <c r="I36" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37">
         <f t="shared" si="1"/>
         <v>94</v>
@@ -3794,16 +3794,16 @@
         <v>129</v>
       </c>
       <c r="G37" t="s">
+        <v>290</v>
+      </c>
+      <c r="H37" t="s">
         <v>291</v>
       </c>
-      <c r="H37" t="s">
-        <v>292</v>
-      </c>
       <c r="I37" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38">
         <f t="shared" si="1"/>
         <v>95</v>
@@ -3821,16 +3821,16 @@
         <v>129</v>
       </c>
       <c r="G38" t="s">
+        <v>292</v>
+      </c>
+      <c r="H38" t="s">
         <v>293</v>
       </c>
-      <c r="H38" t="s">
-        <v>294</v>
-      </c>
       <c r="I38" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39">
         <f t="shared" si="1"/>
         <v>96</v>
@@ -3857,7 +3857,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40">
         <f t="shared" si="1"/>
         <v>97</v>
@@ -3884,7 +3884,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41">
         <f t="shared" si="1"/>
         <v>98</v>
@@ -3905,13 +3905,13 @@
         <v>279</v>
       </c>
       <c r="H41" t="s">
-        <v>295</v>
+        <v>330</v>
       </c>
       <c r="I41" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42">
         <f t="shared" si="1"/>
         <v>99</v>
@@ -3929,16 +3929,16 @@
         <v>129</v>
       </c>
       <c r="G42" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="H42" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="I42" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -3956,16 +3956,16 @@
         <v>129</v>
       </c>
       <c r="G43" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="H43" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="I43" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44">
         <f t="shared" si="1"/>
         <v>101</v>
@@ -3983,7 +3983,7 @@
         <v>129</v>
       </c>
       <c r="G44" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="H44" t="s">
         <v>287</v>
@@ -3992,7 +3992,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45">
         <f t="shared" si="1"/>
         <v>102</v>
@@ -4010,16 +4010,16 @@
         <v>129</v>
       </c>
       <c r="G45" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="H45" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="I45" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46">
         <f t="shared" si="1"/>
         <v>103</v>
@@ -4040,16 +4040,16 @@
         <v>252</v>
       </c>
       <c r="H46" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="I46" t="s">
         <v>129</v>
       </c>
       <c r="J46" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47">
         <f t="shared" si="1"/>
         <v>104</v>
@@ -4070,13 +4070,13 @@
         <v>254</v>
       </c>
       <c r="H47" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="I47" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48">
         <f t="shared" si="1"/>
         <v>105</v>
@@ -4094,16 +4094,16 @@
         <v>129</v>
       </c>
       <c r="G48" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="H48" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="I48" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49">
         <f t="shared" si="1"/>
         <v>106</v>
@@ -4121,19 +4121,19 @@
         <v>129</v>
       </c>
       <c r="G49" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="H49" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="I49" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="J49" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A50">
         <f t="shared" si="1"/>
         <v>107</v>
@@ -4151,16 +4151,16 @@
         <v>129</v>
       </c>
       <c r="G50" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="H50" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="I50" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A51">
         <f t="shared" si="1"/>
         <v>108</v>
@@ -4178,16 +4178,16 @@
         <v>129</v>
       </c>
       <c r="G51" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="H51" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="I51" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A52">
         <f t="shared" si="1"/>
         <v>109</v>
@@ -4205,16 +4205,16 @@
         <v>129</v>
       </c>
       <c r="G52" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="H52" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="I52" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A53">
         <f t="shared" si="1"/>
         <v>110</v>
@@ -4235,13 +4235,13 @@
         <v>284</v>
       </c>
       <c r="H53" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="I53" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A54">
         <f t="shared" si="1"/>
         <v>111</v>
@@ -4259,16 +4259,16 @@
         <v>129</v>
       </c>
       <c r="G54" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="H54" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="I54" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A55">
         <f t="shared" si="1"/>
         <v>112</v>
@@ -4286,16 +4286,16 @@
         <v>129</v>
       </c>
       <c r="G55" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H55" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="I55" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A56">
         <f t="shared" si="1"/>
         <v>113</v>
@@ -4313,16 +4313,16 @@
         <v>129</v>
       </c>
       <c r="G56" t="s">
+        <v>310</v>
+      </c>
+      <c r="H56" t="s">
         <v>312</v>
       </c>
-      <c r="H56" t="s">
-        <v>314</v>
-      </c>
       <c r="I56" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A57">
         <f t="shared" si="1"/>
         <v>114</v>
@@ -4340,16 +4340,16 @@
         <v>129</v>
       </c>
       <c r="G57" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="H57" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="I57" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A58">
         <f t="shared" si="1"/>
         <v>115</v>
@@ -4367,16 +4367,16 @@
         <v>129</v>
       </c>
       <c r="G58" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="H58" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="I58" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A59">
         <f t="shared" si="1"/>
         <v>116</v>
@@ -4397,16 +4397,16 @@
         <v>129</v>
       </c>
       <c r="H59" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="I59" t="s">
         <v>129</v>
       </c>
       <c r="J59" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A60">
         <f t="shared" si="1"/>
         <v>117</v>
@@ -4424,16 +4424,16 @@
         <v>129</v>
       </c>
       <c r="G60" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="H60" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="I60" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A61">
         <f t="shared" si="1"/>
         <v>118</v>
@@ -4451,16 +4451,16 @@
         <v>129</v>
       </c>
       <c r="G61" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="H61" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="I61" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A62">
         <f t="shared" si="1"/>
         <v>119</v>
@@ -4481,13 +4481,13 @@
         <v>254</v>
       </c>
       <c r="H62" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="I62" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A63">
         <f t="shared" si="1"/>
         <v>120</v>
@@ -4505,16 +4505,16 @@
         <v>129</v>
       </c>
       <c r="G63" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="H63" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="I63" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A64">
         <f t="shared" si="1"/>
         <v>121</v>
@@ -4532,16 +4532,16 @@
         <v>129</v>
       </c>
       <c r="G64" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="H64" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="I64" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65">
         <f t="shared" si="1"/>
         <v>122</v>
@@ -4559,16 +4559,16 @@
         <v>129</v>
       </c>
       <c r="G65" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="H65" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="I65" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66">
         <f t="shared" si="1"/>
         <v>123</v>
@@ -4589,7 +4589,7 @@
         <v>129</v>
       </c>
       <c r="H66" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="I66" t="s">
         <v>129</v>
@@ -4612,14 +4612,14 @@
       <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="3" width="18.875" customWidth="1"/>
-    <col min="4" max="4" width="18.875" style="1" customWidth="1"/>
-    <col min="5" max="10" width="18.875" customWidth="1"/>
+    <col min="1" max="3" width="18.83203125" customWidth="1"/>
+    <col min="4" max="4" width="18.83203125" style="1" customWidth="1"/>
+    <col min="5" max="10" width="18.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4642,7 +4642,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -4662,7 +4662,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -4682,7 +4682,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -4705,7 +4705,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -4725,7 +4725,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -4745,7 +4745,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -4765,7 +4765,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -4785,7 +4785,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -4805,7 +4805,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>34</v>
       </c>
@@ -4813,7 +4813,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>36</v>
       </c>
@@ -4821,12 +4821,12 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -4858,7 +4858,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>1</v>
       </c>
@@ -4887,7 +4887,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>2</v>
       </c>
@@ -4916,7 +4916,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>3</v>
       </c>
@@ -4945,7 +4945,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>4</v>
       </c>
@@ -4974,7 +4974,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>5</v>
       </c>
@@ -5003,7 +5003,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>6</v>
       </c>
@@ -5032,7 +5032,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>7</v>
       </c>
@@ -5061,7 +5061,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>8</v>
       </c>
@@ -5090,7 +5090,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="D24"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Made changes to Database.xlsx: changed all block out commands from b to o in Effect column
</commit_message>
<xml_diff>
--- a/data/TP Database.xlsx
+++ b/data/TP Database.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sophiachung/Team Project/cs01-main/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A21ED4D-3171-0B4D-955E-77A80A2517FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F99C2DF1-CD4C-B442-9998-868386BE17BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="18120" windowHeight="15860" activeTab="1" xr2:uid="{F6F91125-3C8A-D047-93DD-1F3A6DE88698}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="23680" windowHeight="15860" activeTab="1" xr2:uid="{F6F91125-3C8A-D047-93DD-1F3A6DE88698}"/>
   </bookViews>
   <sheets>
     <sheet name="Activities" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="670" uniqueCount="331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="670" uniqueCount="330">
   <si>
     <t>CardID</t>
   </si>
@@ -830,9 +830,6 @@
     <t>i(79/101/121):1:(2/3/4)</t>
   </si>
   <si>
-    <t>b0:2:(3&amp;4)</t>
-  </si>
-  <si>
     <t xml:space="preserve">remove one relevant or very relevant article tile </t>
   </si>
   <si>
@@ -920,9 +917,6 @@
     <t>n(17/18/19/20/21/22/23/24/25/26/27/28):1</t>
   </si>
   <si>
-    <t>b0:2:4</t>
-  </si>
-  <si>
     <t>n(33/34/35/36/43/44):2</t>
   </si>
   <si>
@@ -1029,6 +1023,9 @@
   </si>
   <si>
     <t>n(33/34/35/36):1&amp;n(45/46):1</t>
+  </si>
+  <si>
+    <t>o0:2:4</t>
   </si>
 </sst>
 </file>
@@ -2767,8 +2764,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84DC5E79-A11F-0148-B3A8-F5384824D987}">
   <dimension ref="A1:J66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="99" zoomScaleNormal="99" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="99" zoomScaleNormal="99" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2810,7 +2807,7 @@
         <v>126</v>
       </c>
       <c r="I1" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
@@ -2834,7 +2831,7 @@
         <v>129</v>
       </c>
       <c r="H2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="I2" t="s">
         <v>129</v>
@@ -2861,7 +2858,7 @@
         <v>129</v>
       </c>
       <c r="H3" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="I3" t="s">
         <v>129</v>
@@ -2912,7 +2909,7 @@
         <v>129</v>
       </c>
       <c r="G5" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="H5" t="s">
         <v>261</v>
@@ -2939,7 +2936,7 @@
         <v>129</v>
       </c>
       <c r="G6" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="H6" t="s">
         <v>261</v>
@@ -2996,13 +2993,13 @@
         <v>129</v>
       </c>
       <c r="H8" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="I8" t="s">
         <v>129</v>
       </c>
       <c r="J8" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
@@ -3026,7 +3023,7 @@
         <v>129</v>
       </c>
       <c r="H9" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="I9" t="s">
         <v>129</v>
@@ -3053,13 +3050,13 @@
         <v>254</v>
       </c>
       <c r="H10" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="I10" t="s">
         <v>129</v>
       </c>
       <c r="J10" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
@@ -3083,7 +3080,7 @@
         <v>257</v>
       </c>
       <c r="H11" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="I11" t="s">
         <v>129</v>
@@ -3113,7 +3110,7 @@
         <v>254</v>
       </c>
       <c r="H12" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="I12" t="s">
         <v>129</v>
@@ -3143,7 +3140,7 @@
         <v>255</v>
       </c>
       <c r="H13" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="I13" t="s">
         <v>129</v>
@@ -3170,7 +3167,7 @@
         <v>129</v>
       </c>
       <c r="H14" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="I14" t="s">
         <v>129</v>
@@ -3191,7 +3188,7 @@
         <v>156</v>
       </c>
       <c r="F15" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="G15" t="s">
         <v>129</v>
@@ -3203,7 +3200,7 @@
         <v>129</v>
       </c>
       <c r="J15" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
@@ -3224,13 +3221,13 @@
         <v>129</v>
       </c>
       <c r="G16" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="H16" t="s">
         <v>260</v>
       </c>
       <c r="I16" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
@@ -3254,7 +3251,7 @@
         <v>254</v>
       </c>
       <c r="H17" t="s">
-        <v>264</v>
+        <v>275</v>
       </c>
       <c r="I17" t="s">
         <v>129</v>
@@ -3362,7 +3359,7 @@
         <v>129</v>
       </c>
       <c r="H21" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="I21" t="s">
         <v>129</v>
@@ -3416,7 +3413,7 @@
         <v>258</v>
       </c>
       <c r="H23" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="I23" t="s">
         <v>129</v>
@@ -3443,7 +3440,7 @@
         <v>252</v>
       </c>
       <c r="H24" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="I24" t="s">
         <v>129</v>
@@ -3470,7 +3467,7 @@
         <v>129</v>
       </c>
       <c r="H25" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="I25" t="s">
         <v>129</v>
@@ -3494,16 +3491,16 @@
         <v>129</v>
       </c>
       <c r="G26" t="s">
+        <v>278</v>
+      </c>
+      <c r="H26" t="s">
+        <v>316</v>
+      </c>
+      <c r="I26" t="s">
+        <v>129</v>
+      </c>
+      <c r="J26" t="s">
         <v>279</v>
-      </c>
-      <c r="H26" t="s">
-        <v>318</v>
-      </c>
-      <c r="I26" t="s">
-        <v>129</v>
-      </c>
-      <c r="J26" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.2">
@@ -3524,10 +3521,10 @@
         <v>129</v>
       </c>
       <c r="G27" t="s">
+        <v>280</v>
+      </c>
+      <c r="H27" t="s">
         <v>281</v>
-      </c>
-      <c r="H27" t="s">
-        <v>282</v>
       </c>
       <c r="I27" t="s">
         <v>129</v>
@@ -3551,13 +3548,13 @@
         <v>129</v>
       </c>
       <c r="G28" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="H28" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="I28" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.2">
@@ -3581,7 +3578,7 @@
         <v>253</v>
       </c>
       <c r="H29" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="I29" t="s">
         <v>129</v>
@@ -3605,10 +3602,10 @@
         <v>129</v>
       </c>
       <c r="G30" t="s">
+        <v>283</v>
+      </c>
+      <c r="H30" t="s">
         <v>284</v>
-      </c>
-      <c r="H30" t="s">
-        <v>285</v>
       </c>
       <c r="I30" t="s">
         <v>129</v>
@@ -3635,7 +3632,7 @@
         <v>129</v>
       </c>
       <c r="H31" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="I31" t="s">
         <v>129</v>
@@ -3662,7 +3659,7 @@
         <v>129</v>
       </c>
       <c r="H32" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="I32" t="s">
         <v>129</v>
@@ -3689,7 +3686,7 @@
         <v>255</v>
       </c>
       <c r="H33" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I33" t="s">
         <v>129</v>
@@ -3716,7 +3713,7 @@
         <v>252</v>
       </c>
       <c r="H34" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="I34" t="s">
         <v>129</v>
@@ -3740,10 +3737,10 @@
         <v>129</v>
       </c>
       <c r="G35" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="H35" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="I35" t="s">
         <v>129</v>
@@ -3767,13 +3764,13 @@
         <v>129</v>
       </c>
       <c r="G36" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="H36" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="I36" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.2">
@@ -3794,10 +3791,10 @@
         <v>129</v>
       </c>
       <c r="G37" t="s">
+        <v>289</v>
+      </c>
+      <c r="H37" t="s">
         <v>290</v>
-      </c>
-      <c r="H37" t="s">
-        <v>291</v>
       </c>
       <c r="I37" t="s">
         <v>129</v>
@@ -3821,10 +3818,10 @@
         <v>129</v>
       </c>
       <c r="G38" t="s">
+        <v>291</v>
+      </c>
+      <c r="H38" t="s">
         <v>292</v>
-      </c>
-      <c r="H38" t="s">
-        <v>293</v>
       </c>
       <c r="I38" t="s">
         <v>129</v>
@@ -3851,7 +3848,7 @@
         <v>254</v>
       </c>
       <c r="H39" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="I39" t="s">
         <v>129</v>
@@ -3878,7 +3875,7 @@
         <v>254</v>
       </c>
       <c r="H40" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I40" t="s">
         <v>129</v>
@@ -3902,10 +3899,10 @@
         <v>129</v>
       </c>
       <c r="G41" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="H41" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="I41" t="s">
         <v>129</v>
@@ -3929,10 +3926,10 @@
         <v>129</v>
       </c>
       <c r="G42" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="H42" t="s">
-        <v>294</v>
+        <v>329</v>
       </c>
       <c r="I42" t="s">
         <v>129</v>
@@ -3956,10 +3953,10 @@
         <v>129</v>
       </c>
       <c r="G43" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H43" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="I43" t="s">
         <v>129</v>
@@ -3983,10 +3980,10 @@
         <v>129</v>
       </c>
       <c r="G44" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="H44" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I44" t="s">
         <v>129</v>
@@ -4010,10 +4007,10 @@
         <v>129</v>
       </c>
       <c r="G45" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="H45" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="I45" t="s">
         <v>129</v>
@@ -4040,13 +4037,13 @@
         <v>252</v>
       </c>
       <c r="H46" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="I46" t="s">
         <v>129</v>
       </c>
       <c r="J46" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.2">
@@ -4070,7 +4067,7 @@
         <v>254</v>
       </c>
       <c r="H47" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="I47" t="s">
         <v>129</v>
@@ -4094,10 +4091,10 @@
         <v>129</v>
       </c>
       <c r="G48" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="H48" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="I48" t="s">
         <v>129</v>
@@ -4121,16 +4118,16 @@
         <v>129</v>
       </c>
       <c r="G49" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="H49" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="I49" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="J49" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.2">
@@ -4151,13 +4148,13 @@
         <v>129</v>
       </c>
       <c r="G50" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="H50" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="I50" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.2">
@@ -4178,10 +4175,10 @@
         <v>129</v>
       </c>
       <c r="G51" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="H51" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="I51" t="s">
         <v>129</v>
@@ -4205,10 +4202,10 @@
         <v>129</v>
       </c>
       <c r="G52" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="H52" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="I52" t="s">
         <v>129</v>
@@ -4232,10 +4229,10 @@
         <v>129</v>
       </c>
       <c r="G53" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="H53" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="I53" t="s">
         <v>129</v>
@@ -4259,10 +4256,10 @@
         <v>129</v>
       </c>
       <c r="G54" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="H54" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="I54" t="s">
         <v>129</v>
@@ -4286,10 +4283,10 @@
         <v>129</v>
       </c>
       <c r="G55" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="H55" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="I55" t="s">
         <v>129</v>
@@ -4313,10 +4310,10 @@
         <v>129</v>
       </c>
       <c r="G56" t="s">
+        <v>308</v>
+      </c>
+      <c r="H56" t="s">
         <v>310</v>
-      </c>
-      <c r="H56" t="s">
-        <v>312</v>
       </c>
       <c r="I56" t="s">
         <v>129</v>
@@ -4340,10 +4337,10 @@
         <v>129</v>
       </c>
       <c r="G57" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="H57" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="I57" t="s">
         <v>129</v>
@@ -4367,13 +4364,13 @@
         <v>129</v>
       </c>
       <c r="G58" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="H58" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="I58" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.2">
@@ -4397,13 +4394,13 @@
         <v>129</v>
       </c>
       <c r="H59" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="I59" t="s">
         <v>129</v>
       </c>
       <c r="J59" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.2">
@@ -4424,10 +4421,10 @@
         <v>129</v>
       </c>
       <c r="G60" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="H60" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="I60" t="s">
         <v>129</v>
@@ -4451,10 +4448,10 @@
         <v>129</v>
       </c>
       <c r="G61" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="H61" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="I61" t="s">
         <v>129</v>
@@ -4481,7 +4478,7 @@
         <v>254</v>
       </c>
       <c r="H62" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="I62" t="s">
         <v>129</v>
@@ -4505,10 +4502,10 @@
         <v>129</v>
       </c>
       <c r="G63" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="H63" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="I63" t="s">
         <v>129</v>
@@ -4532,10 +4529,10 @@
         <v>129</v>
       </c>
       <c r="G64" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="H64" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="I64" t="s">
         <v>129</v>
@@ -4559,10 +4556,10 @@
         <v>129</v>
       </c>
       <c r="G65" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H65" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="I65" t="s">
         <v>129</v>
@@ -4589,7 +4586,7 @@
         <v>129</v>
       </c>
       <c r="H66" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="I66" t="s">
         <v>129</v>

</xml_diff>

<commit_message>
Combined master branch and event card branch
</commit_message>
<xml_diff>
--- a/data/TP Database.xlsx
+++ b/data/TP Database.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sophiachung/Team Project/cs01-main/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F99C2DF1-CD4C-B442-9998-868386BE17BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{003C6E83-FE0E-C24A-ABF8-911206465A4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="23680" windowHeight="15860" activeTab="1" xr2:uid="{F6F91125-3C8A-D047-93DD-1F3A6DE88698}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15880" activeTab="1" xr2:uid="{F6F91125-3C8A-D047-93DD-1F3A6DE88698}"/>
   </bookViews>
   <sheets>
     <sheet name="Activities" sheetId="2" r:id="rId1"/>
@@ -2764,8 +2764,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84DC5E79-A11F-0148-B3A8-F5384824D987}">
   <dimension ref="A1:J66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="99" zoomScaleNormal="99" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="99" zoomScaleNormal="99" workbookViewId="0">
+      <selection activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2777,7 +2777,7 @@
     <col min="5" max="5" width="26" customWidth="1"/>
     <col min="6" max="6" width="14" customWidth="1"/>
     <col min="7" max="7" width="17" customWidth="1"/>
-    <col min="8" max="8" width="24.6640625" customWidth="1"/>
+    <col min="8" max="8" width="15.83203125" customWidth="1"/>
     <col min="9" max="9" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
#37 - added save_condition into useEffect
## Changes Made
- added save_condition into useEffect
- if chosen card cannot be stored, eventBarStore will not be visible
</commit_message>
<xml_diff>
--- a/data/TP Database.xlsx
+++ b/data/TP Database.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sophiachung/Team Project/cs01-main/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{003C6E83-FE0E-C24A-ABF8-911206465A4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E18D73E5-B560-E343-AC8E-7457738EA3B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15880" activeTab="1" xr2:uid="{F6F91125-3C8A-D047-93DD-1F3A6DE88698}"/>
   </bookViews>
@@ -920,9 +920,6 @@
     <t>n(33/34/35/36/43/44):2</t>
   </si>
   <si>
-    <t>(17+18+19+20+21+22+23+24+25+26+27+28):&gt;1</t>
-  </si>
-  <si>
     <t>!14</t>
   </si>
   <si>
@@ -1026,6 +1023,9 @@
   </si>
   <si>
     <t>o0:2:4</t>
+  </si>
+  <si>
+    <t>(17+18+19+20+21+22+23+24+25+26+27+28):&gt;=2</t>
   </si>
 </sst>
 </file>
@@ -2764,8 +2764,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84DC5E79-A11F-0148-B3A8-F5384824D987}">
   <dimension ref="A1:J66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="99" zoomScaleNormal="99" workbookViewId="0">
-      <selection activeCell="N20" sqref="N20"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="99" zoomScaleNormal="99" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2807,7 +2807,7 @@
         <v>126</v>
       </c>
       <c r="I1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
@@ -3188,7 +3188,7 @@
         <v>156</v>
       </c>
       <c r="F15" t="s">
-        <v>294</v>
+        <v>329</v>
       </c>
       <c r="G15" t="s">
         <v>129</v>
@@ -3227,7 +3227,7 @@
         <v>260</v>
       </c>
       <c r="I16" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
@@ -3494,7 +3494,7 @@
         <v>278</v>
       </c>
       <c r="H26" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="I26" t="s">
         <v>129</v>
@@ -3659,7 +3659,7 @@
         <v>129</v>
       </c>
       <c r="H32" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="I32" t="s">
         <v>129</v>
@@ -3740,7 +3740,7 @@
         <v>278</v>
       </c>
       <c r="H35" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="I35" t="s">
         <v>129</v>
@@ -3770,7 +3770,7 @@
         <v>276</v>
       </c>
       <c r="I36" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.2">
@@ -3902,7 +3902,7 @@
         <v>278</v>
       </c>
       <c r="H41" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="I41" t="s">
         <v>129</v>
@@ -3929,7 +3929,7 @@
         <v>288</v>
       </c>
       <c r="H42" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="I42" t="s">
         <v>129</v>
@@ -3953,7 +3953,7 @@
         <v>129</v>
       </c>
       <c r="G43" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="H43" t="s">
         <v>293</v>
@@ -3980,7 +3980,7 @@
         <v>129</v>
       </c>
       <c r="G44" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="H44" t="s">
         <v>286</v>
@@ -4007,10 +4007,10 @@
         <v>129</v>
       </c>
       <c r="G45" t="s">
+        <v>294</v>
+      </c>
+      <c r="H45" t="s">
         <v>295</v>
-      </c>
-      <c r="H45" t="s">
-        <v>296</v>
       </c>
       <c r="I45" t="s">
         <v>129</v>
@@ -4037,13 +4037,13 @@
         <v>252</v>
       </c>
       <c r="H46" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="I46" t="s">
         <v>129</v>
       </c>
       <c r="J46" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.2">
@@ -4067,7 +4067,7 @@
         <v>254</v>
       </c>
       <c r="H47" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I47" t="s">
         <v>129</v>
@@ -4091,10 +4091,10 @@
         <v>129</v>
       </c>
       <c r="G48" t="s">
+        <v>297</v>
+      </c>
+      <c r="H48" t="s">
         <v>298</v>
-      </c>
-      <c r="H48" t="s">
-        <v>299</v>
       </c>
       <c r="I48" t="s">
         <v>129</v>
@@ -4121,13 +4121,13 @@
         <v>288</v>
       </c>
       <c r="H49" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="I49" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="J49" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.2">
@@ -4151,10 +4151,10 @@
         <v>288</v>
       </c>
       <c r="H50" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="I50" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.2">
@@ -4175,10 +4175,10 @@
         <v>129</v>
       </c>
       <c r="G51" t="s">
+        <v>302</v>
+      </c>
+      <c r="H51" t="s">
         <v>303</v>
-      </c>
-      <c r="H51" t="s">
-        <v>304</v>
       </c>
       <c r="I51" t="s">
         <v>129</v>
@@ -4202,10 +4202,10 @@
         <v>129</v>
       </c>
       <c r="G52" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="H52" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="I52" t="s">
         <v>129</v>
@@ -4232,7 +4232,7 @@
         <v>283</v>
       </c>
       <c r="H53" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="I53" t="s">
         <v>129</v>
@@ -4256,10 +4256,10 @@
         <v>129</v>
       </c>
       <c r="G54" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="H54" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="I54" t="s">
         <v>129</v>
@@ -4283,10 +4283,10 @@
         <v>129</v>
       </c>
       <c r="G55" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="H55" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="I55" t="s">
         <v>129</v>
@@ -4310,10 +4310,10 @@
         <v>129</v>
       </c>
       <c r="G56" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="H56" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="I56" t="s">
         <v>129</v>
@@ -4337,10 +4337,10 @@
         <v>129</v>
       </c>
       <c r="G57" t="s">
+        <v>312</v>
+      </c>
+      <c r="H57" t="s">
         <v>313</v>
-      </c>
-      <c r="H57" t="s">
-        <v>314</v>
       </c>
       <c r="I57" t="s">
         <v>129</v>
@@ -4367,10 +4367,10 @@
         <v>288</v>
       </c>
       <c r="H58" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="I58" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.2">
@@ -4394,13 +4394,13 @@
         <v>129</v>
       </c>
       <c r="H59" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="I59" t="s">
         <v>129</v>
       </c>
       <c r="J59" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.2">
@@ -4421,10 +4421,10 @@
         <v>129</v>
       </c>
       <c r="G60" t="s">
+        <v>294</v>
+      </c>
+      <c r="H60" t="s">
         <v>295</v>
-      </c>
-      <c r="H60" t="s">
-        <v>296</v>
       </c>
       <c r="I60" t="s">
         <v>129</v>
@@ -4448,10 +4448,10 @@
         <v>129</v>
       </c>
       <c r="G61" t="s">
+        <v>319</v>
+      </c>
+      <c r="H61" t="s">
         <v>320</v>
-      </c>
-      <c r="H61" t="s">
-        <v>321</v>
       </c>
       <c r="I61" t="s">
         <v>129</v>
@@ -4478,7 +4478,7 @@
         <v>254</v>
       </c>
       <c r="H62" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="I62" t="s">
         <v>129</v>
@@ -4502,10 +4502,10 @@
         <v>129</v>
       </c>
       <c r="G63" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="H63" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="I63" t="s">
         <v>129</v>
@@ -4529,10 +4529,10 @@
         <v>129</v>
       </c>
       <c r="G64" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="H64" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I64" t="s">
         <v>129</v>
@@ -4556,10 +4556,10 @@
         <v>129</v>
       </c>
       <c r="G65" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="H65" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="I65" t="s">
         <v>129</v>
@@ -4586,7 +4586,7 @@
         <v>129</v>
       </c>
       <c r="H66" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="I66" t="s">
         <v>129</v>

</xml_diff>

<commit_message>
#37 - finished requirements
## Changes Made
- requirements now show as a boolean function
	- true: requirements fulfilled, can use card
	- false: requirements not fulfilled, cannot use card
</commit_message>
<xml_diff>
--- a/data/TP Database.xlsx
+++ b/data/TP Database.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sophiachung/Team Project/cs01-main/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E18D73E5-B560-E343-AC8E-7457738EA3B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D0978E7-FD6F-2C4E-B68F-A2833F74FA61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15880" activeTab="1" xr2:uid="{F6F91125-3C8A-D047-93DD-1F3A6DE88698}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15880" activeTab="1" xr2:uid="{F6F91125-3C8A-D047-93DD-1F3A6DE88698}"/>
   </bookViews>
   <sheets>
     <sheet name="Activities" sheetId="2" r:id="rId1"/>
@@ -2764,7 +2764,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84DC5E79-A11F-0148-B3A8-F5384824D987}">
   <dimension ref="A1:J66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="99" zoomScaleNormal="99" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="99" zoomScaleNormal="99" workbookViewId="0">
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
#78 - Added descriptions to cards
- Added the descriptions to cards
- Fixed the database setup script

Closed #78
</commit_message>
<xml_diff>
--- a/data/TP Database.xlsx
+++ b/data/TP Database.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sophiachung/Team Project/cs01-main/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_My Files\_Uni\Year 3\Term 2\3 - Team Project\_TP Code\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F99C2DF1-CD4C-B442-9998-868386BE17BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C377C57E-C168-417E-837F-EE1877D87188}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="23680" windowHeight="15860" activeTab="1" xr2:uid="{F6F91125-3C8A-D047-93DD-1F3A6DE88698}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F6F91125-3C8A-D047-93DD-1F3A6DE88698}"/>
   </bookViews>
   <sheets>
     <sheet name="Activities" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="670" uniqueCount="330">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="697" uniqueCount="350">
   <si>
     <t>CardID</t>
   </si>
@@ -920,9 +920,6 @@
     <t>n(33/34/35/36/43/44):2</t>
   </si>
   <si>
-    <t>(17+18+19+20+21+22+23+24+25+26+27+28):&gt;1</t>
-  </si>
-  <si>
     <t>!14</t>
   </si>
   <si>
@@ -1026,13 +1023,76 @@
   </si>
   <si>
     <t>o0:2:4</t>
+  </si>
+  <si>
+    <t>(17+18+19+20+21+22+23+24+25+26+27+28):&gt;=2</t>
+  </si>
+  <si>
+    <t>Thinking is great! But it doesn’t directly produce anything. (Watch out for no upwards arrow!) Too much thinking and not enough planning will hamper your progress.</t>
+  </si>
+  <si>
+    <t>This means looking after your data and metadata. As a minimum this could simply be ensuring that you backup your work regularly, or it could be much more complex digital curation techniques.</t>
+  </si>
+  <si>
+    <t>Milestones are internal deadlines that you plan to keep yourself on track throughout the project, for example, completing a chapter, releasing a survey, or finishing a product prototype.</t>
+  </si>
+  <si>
+    <t>This refers to recognizing where you will need additional training and taking steps to learn what you need to before your project starts.</t>
+  </si>
+  <si>
+    <t>Holidays and breaks are really important. But don’t take too many!</t>
+  </si>
+  <si>
+    <t>Do you know what the ethical clearance procedure is for your project? If not you need to find out – quickly!</t>
+  </si>
+  <si>
+    <t>Your supervisor is a precious resource, plan your time with them well!</t>
+  </si>
+  <si>
+    <t>Contingency time is time allocated during planning for unforeseen events or problems that may arise.</t>
+  </si>
+  <si>
+    <t>This could be a government or industrial policy that is relevant to your research.</t>
+  </si>
+  <si>
+    <t>These could be physical or digital objects that you are studying or using in your research, for example artworks or existing apps.</t>
+  </si>
+  <si>
+    <t>This could be an existing database you have accessed and will use directly in your research.</t>
+  </si>
+  <si>
+    <t>Other people are a great contextual resource!</t>
+  </si>
+  <si>
+    <t>You may want to tweak your research questions as you do your contextual research, this will help you focus your study.</t>
+  </si>
+  <si>
+    <t>A reference management system will quickly pay back the time you take to learn how to use it. If you don’t already know of one, ask your tutor.</t>
+  </si>
+  <si>
+    <t>A methodology is a system of methods of doing or studying something. It is part of your design process for carrying out research and investigating others’ methods and methodologies is part of contextual review.</t>
+  </si>
+  <si>
+    <t>Sometimes an article that’s not relevant to you can still lead you to other good sources of information. (Watch out for no upwards arrow!)</t>
+  </si>
+  <si>
+    <t>Evaluating your work helps you to evidence your conclusions. Make sure you critically analyse your findings rather than just describing them.</t>
+  </si>
+  <si>
+    <t>Descriptive writing is necessary but it needs to be followed up by some explanation and critical analysis so that readers understand your research in context.</t>
+  </si>
+  <si>
+    <t>Although not part of what you submit, having support from family and/or friends can be really important for your wellbeing as you progress your research!</t>
+  </si>
+  <si>
+    <t>When writing up your conclusions, revisit your research questions and check that you are actually answering them!</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1042,6 +1102,13 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1080,12 +1147,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1488,21 +1556,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18AE550B-A04F-B142-B067-7E2D879988FA}">
   <dimension ref="A1:H59"/>
   <sheetViews>
-    <sheetView zoomScale="102" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" zoomScale="102" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.6640625" customWidth="1"/>
-    <col min="2" max="2" width="15.1640625" customWidth="1"/>
-    <col min="3" max="3" width="10.33203125" customWidth="1"/>
-    <col min="4" max="4" width="25.1640625" customWidth="1"/>
-    <col min="5" max="6" width="17.5" customWidth="1"/>
+    <col min="1" max="1" width="9.625" customWidth="1"/>
+    <col min="2" max="2" width="15.125" customWidth="1"/>
+    <col min="3" max="3" width="10.375" customWidth="1"/>
+    <col min="4" max="4" width="25.125" customWidth="1"/>
+    <col min="5" max="5" width="49.5" customWidth="1"/>
+    <col min="6" max="6" width="47.375" customWidth="1"/>
     <col min="7" max="7" width="9.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1528,7 +1597,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <f t="shared" ref="A2:A33" si="0">ROW() - 1</f>
         <v>1</v>
@@ -1545,6 +1614,9 @@
       <c r="E2" t="s">
         <v>9</v>
       </c>
+      <c r="F2" t="s">
+        <v>337</v>
+      </c>
       <c r="G2" t="s">
         <v>242</v>
       </c>
@@ -1552,7 +1624,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -1569,6 +1641,9 @@
       <c r="E3" t="s">
         <v>44</v>
       </c>
+      <c r="F3" t="s">
+        <v>335</v>
+      </c>
       <c r="G3" t="s">
         <v>242</v>
       </c>
@@ -1576,7 +1651,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -1593,11 +1668,14 @@
       <c r="E4" t="s">
         <v>46</v>
       </c>
+      <c r="F4" t="s">
+        <v>333</v>
+      </c>
       <c r="G4" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1614,11 +1692,14 @@
       <c r="E5" t="s">
         <v>48</v>
       </c>
+      <c r="F5" t="s">
+        <v>334</v>
+      </c>
       <c r="G5" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1635,11 +1716,14 @@
       <c r="E6" t="s">
         <v>50</v>
       </c>
+      <c r="F6" t="s">
+        <v>332</v>
+      </c>
       <c r="G6" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1656,11 +1740,14 @@
       <c r="E7" t="s">
         <v>52</v>
       </c>
+      <c r="F7" t="s">
+        <v>331</v>
+      </c>
       <c r="G7" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1677,11 +1764,14 @@
       <c r="E8" t="s">
         <v>54</v>
       </c>
+      <c r="F8" t="s">
+        <v>336</v>
+      </c>
       <c r="G8" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1698,11 +1788,14 @@
       <c r="E9" t="s">
         <v>12</v>
       </c>
+      <c r="F9" t="s">
+        <v>330</v>
+      </c>
       <c r="G9" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1719,11 +1812,14 @@
       <c r="E10" t="s">
         <v>56</v>
       </c>
+      <c r="F10" t="s">
+        <v>341</v>
+      </c>
       <c r="G10" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1740,11 +1836,14 @@
       <c r="E11" t="s">
         <v>58</v>
       </c>
+      <c r="F11" t="s">
+        <v>345</v>
+      </c>
       <c r="G11" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1761,11 +1860,14 @@
       <c r="E12" t="s">
         <v>60</v>
       </c>
+      <c r="F12" t="s">
+        <v>344</v>
+      </c>
       <c r="G12" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1782,11 +1884,14 @@
       <c r="E13" t="s">
         <v>60</v>
       </c>
+      <c r="F13" t="s">
+        <v>344</v>
+      </c>
       <c r="G13" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1803,11 +1908,14 @@
       <c r="E14" t="s">
         <v>63</v>
       </c>
+      <c r="F14" t="s">
+        <v>342</v>
+      </c>
       <c r="G14" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1824,11 +1932,14 @@
       <c r="E15" t="s">
         <v>65</v>
       </c>
+      <c r="F15" s="3" t="s">
+        <v>343</v>
+      </c>
       <c r="G15" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1849,7 +1960,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1870,7 +1981,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1891,7 +2002,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -1912,7 +2023,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -1929,11 +2040,14 @@
       <c r="E20" t="s">
         <v>16</v>
       </c>
+      <c r="F20" t="s">
+        <v>340</v>
+      </c>
       <c r="G20" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -1950,11 +2064,14 @@
       <c r="E21" t="s">
         <v>16</v>
       </c>
+      <c r="F21" t="s">
+        <v>340</v>
+      </c>
       <c r="G21" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -1975,7 +2092,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -1996,7 +2113,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -2017,7 +2134,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -2038,7 +2155,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -2055,11 +2172,14 @@
       <c r="E26" t="s">
         <v>79</v>
       </c>
+      <c r="F26" t="s">
+        <v>339</v>
+      </c>
       <c r="G26" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -2076,11 +2196,14 @@
       <c r="E27" t="s">
         <v>79</v>
       </c>
+      <c r="F27" t="s">
+        <v>339</v>
+      </c>
       <c r="G27" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -2097,11 +2220,14 @@
       <c r="E28" t="s">
         <v>82</v>
       </c>
+      <c r="F28" t="s">
+        <v>338</v>
+      </c>
       <c r="G28" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -2118,11 +2244,14 @@
       <c r="E29" t="s">
         <v>82</v>
       </c>
+      <c r="F29" t="s">
+        <v>338</v>
+      </c>
       <c r="G29" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -2143,7 +2272,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -2164,7 +2293,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -2185,7 +2314,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -2202,11 +2331,14 @@
       <c r="E33" t="s">
         <v>91</v>
       </c>
+      <c r="F33" t="s">
+        <v>344</v>
+      </c>
       <c r="G33" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34">
         <f t="shared" ref="A34:A59" si="1">ROW() - 1</f>
         <v>33</v>
@@ -2227,7 +2359,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35">
         <f t="shared" si="1"/>
         <v>34</v>
@@ -2248,7 +2380,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36">
         <f t="shared" si="1"/>
         <v>35</v>
@@ -2269,7 +2401,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37">
         <f t="shared" si="1"/>
         <v>36</v>
@@ -2290,7 +2422,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38">
         <f t="shared" si="1"/>
         <v>37</v>
@@ -2311,7 +2443,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39">
         <f t="shared" si="1"/>
         <v>38</v>
@@ -2332,7 +2464,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40">
         <f t="shared" si="1"/>
         <v>39</v>
@@ -2353,7 +2485,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41">
         <f t="shared" si="1"/>
         <v>40</v>
@@ -2374,7 +2506,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42">
         <f t="shared" si="1"/>
         <v>41</v>
@@ -2395,7 +2527,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43">
         <f t="shared" si="1"/>
         <v>42</v>
@@ -2416,7 +2548,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44">
         <f t="shared" si="1"/>
         <v>43</v>
@@ -2437,7 +2569,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45">
         <f t="shared" si="1"/>
         <v>44</v>
@@ -2458,7 +2590,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46">
         <f t="shared" si="1"/>
         <v>45</v>
@@ -2479,7 +2611,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47">
         <f t="shared" si="1"/>
         <v>46</v>
@@ -2500,7 +2632,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48">
         <f t="shared" si="1"/>
         <v>47</v>
@@ -2521,7 +2653,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49">
         <f t="shared" si="1"/>
         <v>48</v>
@@ -2542,7 +2674,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50">
         <f t="shared" si="1"/>
         <v>49</v>
@@ -2563,7 +2695,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51">
         <f t="shared" si="1"/>
         <v>50</v>
@@ -2580,11 +2712,14 @@
       <c r="E51" t="s">
         <v>32</v>
       </c>
+      <c r="F51" t="s">
+        <v>347</v>
+      </c>
       <c r="G51" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52">
         <f t="shared" si="1"/>
         <v>51</v>
@@ -2601,11 +2736,14 @@
       <c r="E52" t="s">
         <v>32</v>
       </c>
+      <c r="F52" t="s">
+        <v>347</v>
+      </c>
       <c r="G52" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53">
         <f t="shared" si="1"/>
         <v>52</v>
@@ -2622,11 +2760,14 @@
       <c r="E53" t="s">
         <v>32</v>
       </c>
+      <c r="F53" t="s">
+        <v>347</v>
+      </c>
       <c r="G53" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54">
         <f t="shared" si="1"/>
         <v>53</v>
@@ -2643,11 +2784,14 @@
       <c r="E54" t="s">
         <v>116</v>
       </c>
+      <c r="F54" t="s">
+        <v>346</v>
+      </c>
       <c r="G54" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55">
         <f t="shared" si="1"/>
         <v>54</v>
@@ -2668,7 +2812,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56">
         <f t="shared" si="1"/>
         <v>55</v>
@@ -2689,7 +2833,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57">
         <f t="shared" si="1"/>
         <v>56</v>
@@ -2706,11 +2850,14 @@
       <c r="E57" t="s">
         <v>119</v>
       </c>
+      <c r="F57" t="s">
+        <v>349</v>
+      </c>
       <c r="G57" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58">
         <f t="shared" si="1"/>
         <v>57</v>
@@ -2731,7 +2878,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59">
         <f t="shared" si="1"/>
         <v>58</v>
@@ -2748,14 +2895,18 @@
       <c r="E59" t="s">
         <v>123</v>
       </c>
+      <c r="F59" t="s">
+        <v>348</v>
+      </c>
       <c r="G59" t="s">
         <v>245</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -2764,24 +2915,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84DC5E79-A11F-0148-B3A8-F5384824D987}">
   <dimension ref="A1:J66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="99" zoomScaleNormal="99" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView zoomScale="99" zoomScaleNormal="99" workbookViewId="0">
+      <selection activeCell="J59" sqref="J59"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.1640625" customWidth="1"/>
+    <col min="1" max="1" width="9.125" customWidth="1"/>
     <col min="2" max="2" width="9.5" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" customWidth="1"/>
-    <col min="4" max="4" width="25.83203125" customWidth="1"/>
+    <col min="3" max="3" width="47.125" customWidth="1"/>
+    <col min="4" max="4" width="25.875" customWidth="1"/>
     <col min="5" max="5" width="26" customWidth="1"/>
     <col min="6" max="6" width="14" customWidth="1"/>
     <col min="7" max="7" width="17" customWidth="1"/>
-    <col min="8" max="8" width="24.6640625" customWidth="1"/>
+    <col min="8" max="8" width="15.875" customWidth="1"/>
     <col min="9" max="9" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2807,10 +2958,10 @@
         <v>126</v>
       </c>
       <c r="I1" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <f t="shared" ref="A2:A33" si="0">ROW() + 57</f>
         <v>59</v>
@@ -2837,7 +2988,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <f t="shared" si="0"/>
         <v>60</v>
@@ -2864,7 +3015,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <f t="shared" si="0"/>
         <v>61</v>
@@ -2891,7 +3042,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>62</v>
@@ -2918,7 +3069,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>63</v>
@@ -2945,7 +3096,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>64</v>
@@ -2972,7 +3123,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>65</v>
@@ -3002,7 +3153,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>66</v>
@@ -3029,7 +3180,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>67</v>
@@ -3059,7 +3210,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>68</v>
@@ -3089,7 +3240,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>69</v>
@@ -3119,7 +3270,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>70</v>
@@ -3146,7 +3297,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>71</v>
@@ -3173,7 +3324,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>72</v>
@@ -3188,7 +3339,7 @@
         <v>156</v>
       </c>
       <c r="F15" t="s">
-        <v>294</v>
+        <v>329</v>
       </c>
       <c r="G15" t="s">
         <v>129</v>
@@ -3203,7 +3354,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>73</v>
@@ -3227,10 +3378,10 @@
         <v>260</v>
       </c>
       <c r="I16" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>74</v>
@@ -3257,7 +3408,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>75</v>
@@ -3284,7 +3435,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>76</v>
@@ -3311,7 +3462,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>77</v>
@@ -3338,7 +3489,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>78</v>
@@ -3365,7 +3516,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22">
         <f t="shared" si="0"/>
         <v>79</v>
@@ -3392,7 +3543,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23">
         <f t="shared" si="0"/>
         <v>80</v>
@@ -3419,7 +3570,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24">
         <f t="shared" si="0"/>
         <v>81</v>
@@ -3446,7 +3597,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25">
         <f t="shared" si="0"/>
         <v>82</v>
@@ -3473,7 +3624,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26">
         <f t="shared" si="0"/>
         <v>83</v>
@@ -3494,7 +3645,7 @@
         <v>278</v>
       </c>
       <c r="H26" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="I26" t="s">
         <v>129</v>
@@ -3503,7 +3654,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27">
         <f t="shared" si="0"/>
         <v>84</v>
@@ -3530,7 +3681,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28">
         <f t="shared" si="0"/>
         <v>85</v>
@@ -3557,7 +3708,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29">
         <f t="shared" si="0"/>
         <v>86</v>
@@ -3584,7 +3735,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30">
         <f t="shared" si="0"/>
         <v>87</v>
@@ -3611,7 +3762,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31">
         <f t="shared" si="0"/>
         <v>88</v>
@@ -3638,7 +3789,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32">
         <f t="shared" si="0"/>
         <v>89</v>
@@ -3659,13 +3810,13 @@
         <v>129</v>
       </c>
       <c r="H32" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="I32" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33">
         <f t="shared" si="0"/>
         <v>90</v>
@@ -3692,7 +3843,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34">
         <f t="shared" ref="A34:A66" si="1">ROW() + 57</f>
         <v>91</v>
@@ -3719,7 +3870,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35">
         <f t="shared" si="1"/>
         <v>92</v>
@@ -3740,13 +3891,13 @@
         <v>278</v>
       </c>
       <c r="H35" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="I35" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36">
         <f t="shared" si="1"/>
         <v>93</v>
@@ -3770,10 +3921,10 @@
         <v>276</v>
       </c>
       <c r="I36" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37">
         <f t="shared" si="1"/>
         <v>94</v>
@@ -3800,7 +3951,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38">
         <f t="shared" si="1"/>
         <v>95</v>
@@ -3827,7 +3978,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39">
         <f t="shared" si="1"/>
         <v>96</v>
@@ -3854,7 +4005,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40">
         <f t="shared" si="1"/>
         <v>97</v>
@@ -3881,7 +4032,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41">
         <f t="shared" si="1"/>
         <v>98</v>
@@ -3902,13 +4053,13 @@
         <v>278</v>
       </c>
       <c r="H41" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="I41" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42">
         <f t="shared" si="1"/>
         <v>99</v>
@@ -3929,13 +4080,13 @@
         <v>288</v>
       </c>
       <c r="H42" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="I42" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -3953,7 +4104,7 @@
         <v>129</v>
       </c>
       <c r="G43" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="H43" t="s">
         <v>293</v>
@@ -3962,7 +4113,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44">
         <f t="shared" si="1"/>
         <v>101</v>
@@ -3980,7 +4131,7 @@
         <v>129</v>
       </c>
       <c r="G44" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="H44" t="s">
         <v>286</v>
@@ -3989,7 +4140,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45">
         <f t="shared" si="1"/>
         <v>102</v>
@@ -4007,16 +4158,16 @@
         <v>129</v>
       </c>
       <c r="G45" t="s">
+        <v>294</v>
+      </c>
+      <c r="H45" t="s">
         <v>295</v>
       </c>
-      <c r="H45" t="s">
-        <v>296</v>
-      </c>
       <c r="I45" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46">
         <f t="shared" si="1"/>
         <v>103</v>
@@ -4037,16 +4188,16 @@
         <v>252</v>
       </c>
       <c r="H46" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="I46" t="s">
         <v>129</v>
       </c>
       <c r="J46" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47">
         <f t="shared" si="1"/>
         <v>104</v>
@@ -4067,13 +4218,13 @@
         <v>254</v>
       </c>
       <c r="H47" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I47" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48">
         <f t="shared" si="1"/>
         <v>105</v>
@@ -4091,16 +4242,16 @@
         <v>129</v>
       </c>
       <c r="G48" t="s">
+        <v>297</v>
+      </c>
+      <c r="H48" t="s">
         <v>298</v>
       </c>
-      <c r="H48" t="s">
-        <v>299</v>
-      </c>
       <c r="I48" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49">
         <f t="shared" si="1"/>
         <v>106</v>
@@ -4121,16 +4272,16 @@
         <v>288</v>
       </c>
       <c r="H49" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="I49" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="J49" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50">
         <f t="shared" si="1"/>
         <v>107</v>
@@ -4151,13 +4302,13 @@
         <v>288</v>
       </c>
       <c r="H50" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="I50" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51">
         <f t="shared" si="1"/>
         <v>108</v>
@@ -4175,16 +4326,16 @@
         <v>129</v>
       </c>
       <c r="G51" t="s">
+        <v>302</v>
+      </c>
+      <c r="H51" t="s">
         <v>303</v>
       </c>
-      <c r="H51" t="s">
-        <v>304</v>
-      </c>
       <c r="I51" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52">
         <f t="shared" si="1"/>
         <v>109</v>
@@ -4202,16 +4353,16 @@
         <v>129</v>
       </c>
       <c r="G52" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="H52" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="I52" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53">
         <f t="shared" si="1"/>
         <v>110</v>
@@ -4232,13 +4383,13 @@
         <v>283</v>
       </c>
       <c r="H53" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="I53" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54">
         <f t="shared" si="1"/>
         <v>111</v>
@@ -4256,16 +4407,16 @@
         <v>129</v>
       </c>
       <c r="G54" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="H54" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="I54" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55">
         <f t="shared" si="1"/>
         <v>112</v>
@@ -4283,16 +4434,16 @@
         <v>129</v>
       </c>
       <c r="G55" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="H55" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="I55" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56">
         <f t="shared" si="1"/>
         <v>113</v>
@@ -4310,16 +4461,16 @@
         <v>129</v>
       </c>
       <c r="G56" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="H56" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="I56" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57">
         <f t="shared" si="1"/>
         <v>114</v>
@@ -4337,16 +4488,16 @@
         <v>129</v>
       </c>
       <c r="G57" t="s">
+        <v>312</v>
+      </c>
+      <c r="H57" t="s">
         <v>313</v>
       </c>
-      <c r="H57" t="s">
-        <v>314</v>
-      </c>
       <c r="I57" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58">
         <f t="shared" si="1"/>
         <v>115</v>
@@ -4367,13 +4518,13 @@
         <v>288</v>
       </c>
       <c r="H58" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="I58" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59">
         <f t="shared" si="1"/>
         <v>116</v>
@@ -4394,16 +4545,16 @@
         <v>129</v>
       </c>
       <c r="H59" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="I59" t="s">
         <v>129</v>
       </c>
       <c r="J59" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60">
         <f t="shared" si="1"/>
         <v>117</v>
@@ -4421,16 +4572,16 @@
         <v>129</v>
       </c>
       <c r="G60" t="s">
+        <v>294</v>
+      </c>
+      <c r="H60" t="s">
         <v>295</v>
       </c>
-      <c r="H60" t="s">
-        <v>296</v>
-      </c>
       <c r="I60" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61">
         <f t="shared" si="1"/>
         <v>118</v>
@@ -4448,16 +4599,16 @@
         <v>129</v>
       </c>
       <c r="G61" t="s">
+        <v>319</v>
+      </c>
+      <c r="H61" t="s">
         <v>320</v>
       </c>
-      <c r="H61" t="s">
-        <v>321</v>
-      </c>
       <c r="I61" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62">
         <f t="shared" si="1"/>
         <v>119</v>
@@ -4478,13 +4629,13 @@
         <v>254</v>
       </c>
       <c r="H62" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="I62" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63">
         <f t="shared" si="1"/>
         <v>120</v>
@@ -4502,16 +4653,16 @@
         <v>129</v>
       </c>
       <c r="G63" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="H63" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="I63" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64">
         <f t="shared" si="1"/>
         <v>121</v>
@@ -4529,16 +4680,16 @@
         <v>129</v>
       </c>
       <c r="G64" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="H64" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I64" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65">
         <f t="shared" si="1"/>
         <v>122</v>
@@ -4556,16 +4707,16 @@
         <v>129</v>
       </c>
       <c r="G65" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="H65" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="I65" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66">
         <f t="shared" si="1"/>
         <v>123</v>
@@ -4586,7 +4737,7 @@
         <v>129</v>
       </c>
       <c r="H66" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="I66" t="s">
         <v>129</v>
@@ -4609,14 +4760,14 @@
       <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="18.83203125" customWidth="1"/>
-    <col min="4" max="4" width="18.83203125" style="1" customWidth="1"/>
-    <col min="5" max="10" width="18.83203125" customWidth="1"/>
+    <col min="1" max="3" width="18.875" customWidth="1"/>
+    <col min="4" max="4" width="18.875" style="1" customWidth="1"/>
+    <col min="5" max="10" width="18.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4639,7 +4790,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -4659,7 +4810,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -4679,7 +4830,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -4702,7 +4853,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -4722,7 +4873,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -4742,7 +4893,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -4762,7 +4913,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -4782,7 +4933,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -4802,7 +4953,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>34</v>
       </c>
@@ -4810,7 +4961,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>36</v>
       </c>
@@ -4818,12 +4969,12 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -4855,7 +5006,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1</v>
       </c>
@@ -4884,7 +5035,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2</v>
       </c>
@@ -4913,7 +5064,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>3</v>
       </c>
@@ -4942,7 +5093,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>4</v>
       </c>
@@ -4971,7 +5122,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>5</v>
       </c>
@@ -5000,7 +5151,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>6</v>
       </c>
@@ -5029,7 +5180,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>7</v>
       </c>
@@ -5058,7 +5209,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>8</v>
       </c>
@@ -5087,7 +5238,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D24"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#37 - added a count in FinishHandler of eventBoard
## Changes Made
- if count reaches 5, it could be seen as the effect not working properly and will force it to finish
</commit_message>
<xml_diff>
--- a/data/TP Database.xlsx
+++ b/data/TP Database.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sophiachung/Team Project/cs01-main/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D0978E7-FD6F-2C4E-B68F-A2833F74FA61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{866E563B-C161-F34F-8E4E-4D72ABDF40D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15880" activeTab="1" xr2:uid="{F6F91125-3C8A-D047-93DD-1F3A6DE88698}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15880" activeTab="1" xr2:uid="{F6F91125-3C8A-D047-93DD-1F3A6DE88698}"/>
   </bookViews>
   <sheets>
     <sheet name="Activities" sheetId="2" r:id="rId1"/>
@@ -842,24 +842,6 @@
     <t>s3:1:(2/3/4)</t>
   </si>
   <si>
-    <t>p2:1</t>
-  </si>
-  <si>
-    <t>n30:1</t>
-  </si>
-  <si>
-    <t>p41:1</t>
-  </si>
-  <si>
-    <t>n(15/16/31):1</t>
-  </si>
-  <si>
-    <t>n0:1</t>
-  </si>
-  <si>
-    <t>n7:&lt;=9</t>
-  </si>
-  <si>
     <t>p31:1</t>
   </si>
   <si>
@@ -869,9 +851,6 @@
     <t>n0:3:3</t>
   </si>
   <si>
-    <t>n(37/38/39/40/42/45/46):3</t>
-  </si>
-  <si>
     <t>!3</t>
   </si>
   <si>
@@ -881,9 +860,6 @@
     <t>!41</t>
   </si>
   <si>
-    <t>n(42/45/46):1</t>
-  </si>
-  <si>
     <t>n0:2:3</t>
   </si>
   <si>
@@ -899,51 +875,30 @@
     <t>n0:1:3</t>
   </si>
   <si>
-    <t>n(43/44):2</t>
-  </si>
-  <si>
     <t>!5</t>
   </si>
   <si>
     <t>27/28</t>
   </si>
   <si>
-    <t>p(43/44):1</t>
-  </si>
-  <si>
     <t>!9</t>
   </si>
   <si>
-    <t>n(17/18/19/20/21/22/23/24/25/26/27/28):1</t>
-  </si>
-  <si>
-    <t>n(33/34/35/36/43/44):2</t>
-  </si>
-  <si>
     <t>!14</t>
   </si>
   <si>
-    <t>n(47/48/49/54/55/57):1</t>
-  </si>
-  <si>
     <t>remove any 3 non-adjacent tiles from current section</t>
   </si>
   <si>
     <t>!(31&amp;32)</t>
   </si>
   <si>
-    <t>n(47/48/57):2</t>
-  </si>
-  <si>
     <t>remove 2 non-adjacent thesis tiles from current section</t>
   </si>
   <si>
     <t>n-0:3:4</t>
   </si>
   <si>
-    <t>n-(47/48/49/54/55/57):2</t>
-  </si>
-  <si>
     <t>!53</t>
   </si>
   <si>
@@ -983,49 +938,94 @@
     <t>!(11/12/32):&gt;1</t>
   </si>
   <si>
-    <t>n41:1&amp;n(17/18/19/20/21/22/23/24/25/26/27/28):1</t>
-  </si>
-  <si>
-    <t>n(45/46):1&amp;n(43/44):1</t>
-  </si>
-  <si>
     <t>keep this card to protect against any future Jargon events</t>
   </si>
   <si>
-    <t>p(54/55):1&amp;i112:1</t>
-  </si>
-  <si>
     <t>!(33/34/35/36):&gt;2</t>
   </si>
   <si>
-    <t>n-(47/48/49/54/55/57):3</t>
-  </si>
-  <si>
     <t>!31:&gt;1</t>
   </si>
   <si>
     <t>!56</t>
   </si>
   <si>
-    <t>n49:2</t>
-  </si>
-  <si>
     <t>Else</t>
   </si>
   <si>
-    <t>f5:1</t>
-  </si>
-  <si>
-    <t>n41:1&amp;n(42/45/46):2</t>
-  </si>
-  <si>
-    <t>n(33/34/35/36):1&amp;n(45/46):1</t>
-  </si>
-  <si>
     <t>o0:2:4</t>
   </si>
   <si>
     <t>(17+18+19+20+21+22+23+24+25+26+27+28):&gt;=2</t>
+  </si>
+  <si>
+    <t>p2:1:1</t>
+  </si>
+  <si>
+    <t>n30:1:2</t>
+  </si>
+  <si>
+    <t>p41:1:3</t>
+  </si>
+  <si>
+    <t>n(15/16/31):1:2</t>
+  </si>
+  <si>
+    <t>n7:&lt;=9:1</t>
+  </si>
+  <si>
+    <t>n(37/38/39/40/42/45/46):3:3</t>
+  </si>
+  <si>
+    <t>n41:1:3&amp;n(17/18/19/20/21/22/23/24/25/26/27/28):1:3</t>
+  </si>
+  <si>
+    <t>n(42/45/46):1:3</t>
+  </si>
+  <si>
+    <t>n41:1:3&amp;n(42/45/46):2:3</t>
+  </si>
+  <si>
+    <t>n(43/44):2:3</t>
+  </si>
+  <si>
+    <t>n(45/46):1:3&amp;n(43/44):1:3</t>
+  </si>
+  <si>
+    <t>p(43/44):1:3</t>
+  </si>
+  <si>
+    <t>n(17/18/19/20/21/22/23/24/25/26/27/28):1:2</t>
+  </si>
+  <si>
+    <t>n(33/34/35/36):1:3&amp;n(45/46):1:3</t>
+  </si>
+  <si>
+    <t>n(33/34/35/36/43/44):2:3</t>
+  </si>
+  <si>
+    <t>n(47/48/49/54/55/57):1:4</t>
+  </si>
+  <si>
+    <t>n(47/48/57):2:4</t>
+  </si>
+  <si>
+    <t>n-(47/48/49/54/55/57):2:4</t>
+  </si>
+  <si>
+    <t>n-(47/48/49/54/55/57):3:4</t>
+  </si>
+  <si>
+    <t>n49:2:4</t>
+  </si>
+  <si>
+    <t>p(54/55):1:4&amp;i112:1:(2/3/4)</t>
+  </si>
+  <si>
+    <t>f5:1:1</t>
+  </si>
+  <si>
+    <t>f1:1:1</t>
   </si>
 </sst>
 </file>
@@ -2764,8 +2764,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84DC5E79-A11F-0148-B3A8-F5384824D987}">
   <dimension ref="A1:J66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="99" zoomScaleNormal="99" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" zoomScale="99" zoomScaleNormal="99" workbookViewId="0">
+      <selection activeCell="I40" sqref="I40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2777,8 +2777,8 @@
     <col min="5" max="5" width="26" customWidth="1"/>
     <col min="6" max="6" width="14" customWidth="1"/>
     <col min="7" max="7" width="17" customWidth="1"/>
-    <col min="8" max="8" width="15.83203125" customWidth="1"/>
-    <col min="9" max="9" width="13.5" customWidth="1"/>
+    <col min="8" max="8" width="35.6640625" customWidth="1"/>
+    <col min="9" max="9" width="22.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
@@ -2807,7 +2807,7 @@
         <v>126</v>
       </c>
       <c r="I1" t="s">
-        <v>324</v>
+        <v>304</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
@@ -2831,7 +2831,7 @@
         <v>129</v>
       </c>
       <c r="H2" t="s">
-        <v>268</v>
+        <v>307</v>
       </c>
       <c r="I2" t="s">
         <v>129</v>
@@ -2858,7 +2858,7 @@
         <v>129</v>
       </c>
       <c r="H3" t="s">
-        <v>269</v>
+        <v>308</v>
       </c>
       <c r="I3" t="s">
         <v>129</v>
@@ -2909,7 +2909,7 @@
         <v>129</v>
       </c>
       <c r="G5" t="s">
-        <v>288</v>
+        <v>279</v>
       </c>
       <c r="H5" t="s">
         <v>261</v>
@@ -2936,7 +2936,7 @@
         <v>129</v>
       </c>
       <c r="G6" t="s">
-        <v>288</v>
+        <v>279</v>
       </c>
       <c r="H6" t="s">
         <v>261</v>
@@ -3023,7 +3023,7 @@
         <v>129</v>
       </c>
       <c r="H9" t="s">
-        <v>270</v>
+        <v>309</v>
       </c>
       <c r="I9" t="s">
         <v>129</v>
@@ -3050,10 +3050,10 @@
         <v>254</v>
       </c>
       <c r="H10" t="s">
-        <v>271</v>
+        <v>310</v>
       </c>
       <c r="I10" t="s">
-        <v>129</v>
+        <v>329</v>
       </c>
       <c r="J10" t="s">
         <v>264</v>
@@ -3080,7 +3080,7 @@
         <v>257</v>
       </c>
       <c r="H11" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="I11" t="s">
         <v>129</v>
@@ -3110,10 +3110,10 @@
         <v>254</v>
       </c>
       <c r="H12" t="s">
-        <v>271</v>
+        <v>310</v>
       </c>
       <c r="I12" t="s">
-        <v>129</v>
+        <v>329</v>
       </c>
       <c r="J12" t="s">
         <v>150</v>
@@ -3140,7 +3140,7 @@
         <v>255</v>
       </c>
       <c r="H13" t="s">
-        <v>272</v>
+        <v>262</v>
       </c>
       <c r="I13" t="s">
         <v>129</v>
@@ -3167,7 +3167,7 @@
         <v>129</v>
       </c>
       <c r="H14" t="s">
-        <v>273</v>
+        <v>311</v>
       </c>
       <c r="I14" t="s">
         <v>129</v>
@@ -3188,7 +3188,7 @@
         <v>156</v>
       </c>
       <c r="F15" t="s">
-        <v>329</v>
+        <v>306</v>
       </c>
       <c r="G15" t="s">
         <v>129</v>
@@ -3221,13 +3221,13 @@
         <v>129</v>
       </c>
       <c r="G16" t="s">
-        <v>288</v>
+        <v>279</v>
       </c>
       <c r="H16" t="s">
         <v>260</v>
       </c>
       <c r="I16" t="s">
-        <v>325</v>
+        <v>328</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
@@ -3251,10 +3251,10 @@
         <v>254</v>
       </c>
       <c r="H17" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="I17" t="s">
-        <v>129</v>
+        <v>329</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
@@ -3281,7 +3281,7 @@
         <v>261</v>
       </c>
       <c r="I18" t="s">
-        <v>129</v>
+        <v>329</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
@@ -3308,7 +3308,7 @@
         <v>262</v>
       </c>
       <c r="I19" t="s">
-        <v>129</v>
+        <v>329</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
@@ -3359,7 +3359,7 @@
         <v>129</v>
       </c>
       <c r="H21" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="I21" t="s">
         <v>129</v>
@@ -3413,7 +3413,7 @@
         <v>258</v>
       </c>
       <c r="H23" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="I23" t="s">
         <v>129</v>
@@ -3440,7 +3440,7 @@
         <v>252</v>
       </c>
       <c r="H24" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="I24" t="s">
         <v>129</v>
@@ -3467,7 +3467,7 @@
         <v>129</v>
       </c>
       <c r="H25" t="s">
-        <v>277</v>
+        <v>312</v>
       </c>
       <c r="I25" t="s">
         <v>129</v>
@@ -3491,16 +3491,16 @@
         <v>129</v>
       </c>
       <c r="G26" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
       <c r="H26" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="I26" t="s">
         <v>129</v>
       </c>
       <c r="J26" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.2">
@@ -3521,10 +3521,10 @@
         <v>129</v>
       </c>
       <c r="G27" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="H27" t="s">
-        <v>281</v>
+        <v>314</v>
       </c>
       <c r="I27" t="s">
         <v>129</v>
@@ -3548,13 +3548,13 @@
         <v>129</v>
       </c>
       <c r="G28" t="s">
-        <v>288</v>
+        <v>279</v>
       </c>
       <c r="H28" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="I28" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.2">
@@ -3578,7 +3578,7 @@
         <v>253</v>
       </c>
       <c r="H29" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="I29" t="s">
         <v>129</v>
@@ -3602,10 +3602,10 @@
         <v>129</v>
       </c>
       <c r="G30" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
       <c r="H30" t="s">
-        <v>284</v>
+        <v>276</v>
       </c>
       <c r="I30" t="s">
         <v>129</v>
@@ -3632,7 +3632,7 @@
         <v>129</v>
       </c>
       <c r="H31" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
       <c r="I31" t="s">
         <v>129</v>
@@ -3659,7 +3659,7 @@
         <v>129</v>
       </c>
       <c r="H32" t="s">
-        <v>326</v>
+        <v>315</v>
       </c>
       <c r="I32" t="s">
         <v>129</v>
@@ -3686,7 +3686,7 @@
         <v>255</v>
       </c>
       <c r="H33" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
       <c r="I33" t="s">
         <v>129</v>
@@ -3713,7 +3713,7 @@
         <v>252</v>
       </c>
       <c r="H34" t="s">
-        <v>287</v>
+        <v>316</v>
       </c>
       <c r="I34" t="s">
         <v>129</v>
@@ -3737,10 +3737,10 @@
         <v>129</v>
       </c>
       <c r="G35" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
       <c r="H35" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="I35" t="s">
         <v>129</v>
@@ -3764,13 +3764,13 @@
         <v>129</v>
       </c>
       <c r="G36" t="s">
-        <v>288</v>
+        <v>279</v>
       </c>
       <c r="H36" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="I36" t="s">
-        <v>325</v>
+        <v>328</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.2">
@@ -3791,10 +3791,10 @@
         <v>129</v>
       </c>
       <c r="G37" t="s">
-        <v>289</v>
+        <v>280</v>
       </c>
       <c r="H37" t="s">
-        <v>290</v>
+        <v>318</v>
       </c>
       <c r="I37" t="s">
         <v>129</v>
@@ -3818,10 +3818,10 @@
         <v>129</v>
       </c>
       <c r="G38" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="H38" t="s">
-        <v>292</v>
+        <v>319</v>
       </c>
       <c r="I38" t="s">
         <v>129</v>
@@ -3848,10 +3848,10 @@
         <v>254</v>
       </c>
       <c r="H39" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="I39" t="s">
-        <v>129</v>
+        <v>329</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.2">
@@ -3875,10 +3875,10 @@
         <v>254</v>
       </c>
       <c r="H40" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
       <c r="I40" t="s">
-        <v>129</v>
+        <v>329</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.2">
@@ -3899,10 +3899,10 @@
         <v>129</v>
       </c>
       <c r="G41" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
       <c r="H41" t="s">
-        <v>327</v>
+        <v>320</v>
       </c>
       <c r="I41" t="s">
         <v>129</v>
@@ -3926,10 +3926,10 @@
         <v>129</v>
       </c>
       <c r="G42" t="s">
-        <v>288</v>
+        <v>279</v>
       </c>
       <c r="H42" t="s">
-        <v>328</v>
+        <v>305</v>
       </c>
       <c r="I42" t="s">
         <v>129</v>
@@ -3953,10 +3953,10 @@
         <v>129</v>
       </c>
       <c r="G43" t="s">
-        <v>310</v>
+        <v>295</v>
       </c>
       <c r="H43" t="s">
-        <v>293</v>
+        <v>321</v>
       </c>
       <c r="I43" t="s">
         <v>129</v>
@@ -3980,10 +3980,10 @@
         <v>129</v>
       </c>
       <c r="G44" t="s">
-        <v>311</v>
+        <v>296</v>
       </c>
       <c r="H44" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
       <c r="I44" t="s">
         <v>129</v>
@@ -4007,10 +4007,10 @@
         <v>129</v>
       </c>
       <c r="G45" t="s">
-        <v>294</v>
+        <v>282</v>
       </c>
       <c r="H45" t="s">
-        <v>295</v>
+        <v>322</v>
       </c>
       <c r="I45" t="s">
         <v>129</v>
@@ -4037,13 +4037,13 @@
         <v>252</v>
       </c>
       <c r="H46" t="s">
-        <v>300</v>
+        <v>286</v>
       </c>
       <c r="I46" t="s">
         <v>129</v>
       </c>
       <c r="J46" t="s">
-        <v>296</v>
+        <v>283</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.2">
@@ -4067,10 +4067,10 @@
         <v>254</v>
       </c>
       <c r="H47" t="s">
-        <v>295</v>
+        <v>322</v>
       </c>
       <c r="I47" t="s">
-        <v>129</v>
+        <v>329</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.2">
@@ -4091,10 +4091,10 @@
         <v>129</v>
       </c>
       <c r="G48" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="H48" t="s">
-        <v>298</v>
+        <v>323</v>
       </c>
       <c r="I48" t="s">
         <v>129</v>
@@ -4118,16 +4118,16 @@
         <v>129</v>
       </c>
       <c r="G49" t="s">
-        <v>288</v>
+        <v>279</v>
       </c>
       <c r="H49" t="s">
-        <v>301</v>
+        <v>324</v>
       </c>
       <c r="I49" t="s">
-        <v>295</v>
+        <v>322</v>
       </c>
       <c r="J49" t="s">
-        <v>299</v>
+        <v>285</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.2">
@@ -4148,13 +4148,13 @@
         <v>129</v>
       </c>
       <c r="G50" t="s">
-        <v>288</v>
+        <v>279</v>
       </c>
       <c r="H50" t="s">
-        <v>301</v>
+        <v>324</v>
       </c>
       <c r="I50" t="s">
-        <v>295</v>
+        <v>322</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.2">
@@ -4175,10 +4175,10 @@
         <v>129</v>
       </c>
       <c r="G51" t="s">
-        <v>302</v>
+        <v>287</v>
       </c>
       <c r="H51" t="s">
-        <v>303</v>
+        <v>288</v>
       </c>
       <c r="I51" t="s">
         <v>129</v>
@@ -4202,10 +4202,10 @@
         <v>129</v>
       </c>
       <c r="G52" t="s">
-        <v>304</v>
+        <v>289</v>
       </c>
       <c r="H52" t="s">
-        <v>301</v>
+        <v>324</v>
       </c>
       <c r="I52" t="s">
         <v>129</v>
@@ -4229,10 +4229,10 @@
         <v>129</v>
       </c>
       <c r="G53" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
       <c r="H53" t="s">
-        <v>305</v>
+        <v>290</v>
       </c>
       <c r="I53" t="s">
         <v>129</v>
@@ -4256,10 +4256,10 @@
         <v>129</v>
       </c>
       <c r="G54" t="s">
-        <v>314</v>
+        <v>299</v>
       </c>
       <c r="H54" t="s">
-        <v>301</v>
+        <v>324</v>
       </c>
       <c r="I54" t="s">
         <v>129</v>
@@ -4283,10 +4283,10 @@
         <v>129</v>
       </c>
       <c r="G55" t="s">
-        <v>308</v>
+        <v>293</v>
       </c>
       <c r="H55" t="s">
-        <v>306</v>
+        <v>291</v>
       </c>
       <c r="I55" t="s">
         <v>129</v>
@@ -4310,10 +4310,10 @@
         <v>129</v>
       </c>
       <c r="G56" t="s">
-        <v>307</v>
+        <v>292</v>
       </c>
       <c r="H56" t="s">
-        <v>309</v>
+        <v>294</v>
       </c>
       <c r="I56" t="s">
         <v>129</v>
@@ -4337,10 +4337,10 @@
         <v>129</v>
       </c>
       <c r="G57" t="s">
-        <v>312</v>
+        <v>297</v>
       </c>
       <c r="H57" t="s">
-        <v>313</v>
+        <v>298</v>
       </c>
       <c r="I57" t="s">
         <v>129</v>
@@ -4364,13 +4364,13 @@
         <v>129</v>
       </c>
       <c r="G58" t="s">
-        <v>288</v>
+        <v>279</v>
       </c>
       <c r="H58" t="s">
-        <v>301</v>
+        <v>324</v>
       </c>
       <c r="I58" t="s">
-        <v>325</v>
+        <v>328</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.2">
@@ -4394,13 +4394,13 @@
         <v>129</v>
       </c>
       <c r="H59" t="s">
-        <v>318</v>
+        <v>327</v>
       </c>
       <c r="I59" t="s">
         <v>129</v>
       </c>
       <c r="J59" t="s">
-        <v>317</v>
+        <v>300</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.2">
@@ -4421,10 +4421,10 @@
         <v>129</v>
       </c>
       <c r="G60" t="s">
-        <v>294</v>
+        <v>282</v>
       </c>
       <c r="H60" t="s">
-        <v>295</v>
+        <v>322</v>
       </c>
       <c r="I60" t="s">
         <v>129</v>
@@ -4448,10 +4448,10 @@
         <v>129</v>
       </c>
       <c r="G61" t="s">
-        <v>319</v>
+        <v>301</v>
       </c>
       <c r="H61" t="s">
-        <v>320</v>
+        <v>325</v>
       </c>
       <c r="I61" t="s">
         <v>129</v>
@@ -4478,10 +4478,10 @@
         <v>254</v>
       </c>
       <c r="H62" t="s">
-        <v>309</v>
+        <v>294</v>
       </c>
       <c r="I62" t="s">
-        <v>129</v>
+        <v>329</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.2">
@@ -4502,10 +4502,10 @@
         <v>129</v>
       </c>
       <c r="G63" t="s">
-        <v>321</v>
+        <v>302</v>
       </c>
       <c r="H63" t="s">
-        <v>301</v>
+        <v>324</v>
       </c>
       <c r="I63" t="s">
         <v>129</v>
@@ -4529,10 +4529,10 @@
         <v>129</v>
       </c>
       <c r="G64" t="s">
+        <v>303</v>
+      </c>
+      <c r="H64" t="s">
         <v>322</v>
-      </c>
-      <c r="H64" t="s">
-        <v>295</v>
       </c>
       <c r="I64" t="s">
         <v>129</v>
@@ -4556,10 +4556,10 @@
         <v>129</v>
       </c>
       <c r="G65" t="s">
-        <v>310</v>
+        <v>295</v>
       </c>
       <c r="H65" t="s">
-        <v>301</v>
+        <v>324</v>
       </c>
       <c r="I65" t="s">
         <v>129</v>
@@ -4586,7 +4586,7 @@
         <v>129</v>
       </c>
       <c r="H66" t="s">
-        <v>323</v>
+        <v>326</v>
       </c>
       <c r="I66" t="s">
         <v>129</v>

</xml_diff>

<commit_message>
updated event card columns (effect and else)
</commit_message>
<xml_diff>
--- a/data/TP Database.xlsx
+++ b/data/TP Database.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_My Files\_Uni\Year 3\Term 2\3 - Team Project\_TP Code\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sophiachung/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C377C57E-C168-417E-837F-EE1877D87188}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{599726AD-275B-6049-9F37-E56AC2656D56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F6F91125-3C8A-D047-93DD-1F3A6DE88698}"/>
+    <workbookView xWindow="1700" yWindow="760" windowWidth="23680" windowHeight="15860" xr2:uid="{F6F91125-3C8A-D047-93DD-1F3A6DE88698}"/>
   </bookViews>
   <sheets>
     <sheet name="Activities" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="697" uniqueCount="350">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="698" uniqueCount="350">
   <si>
     <t>CardID</t>
   </si>
@@ -842,24 +842,6 @@
     <t>s3:1:(2/3/4)</t>
   </si>
   <si>
-    <t>p2:1</t>
-  </si>
-  <si>
-    <t>n30:1</t>
-  </si>
-  <si>
-    <t>p41:1</t>
-  </si>
-  <si>
-    <t>n(15/16/31):1</t>
-  </si>
-  <si>
-    <t>n0:1</t>
-  </si>
-  <si>
-    <t>n7:&lt;=9</t>
-  </si>
-  <si>
     <t>p31:1</t>
   </si>
   <si>
@@ -869,9 +851,6 @@
     <t>n0:3:3</t>
   </si>
   <si>
-    <t>n(37/38/39/40/42/45/46):3</t>
-  </si>
-  <si>
     <t>!3</t>
   </si>
   <si>
@@ -881,9 +860,6 @@
     <t>!41</t>
   </si>
   <si>
-    <t>n(42/45/46):1</t>
-  </si>
-  <si>
     <t>n0:2:3</t>
   </si>
   <si>
@@ -899,51 +875,33 @@
     <t>n0:1:3</t>
   </si>
   <si>
-    <t>n(43/44):2</t>
-  </si>
-  <si>
     <t>!5</t>
   </si>
   <si>
     <t>27/28</t>
   </si>
   <si>
-    <t>p(43/44):1</t>
-  </si>
-  <si>
     <t>!9</t>
   </si>
   <si>
-    <t>n(17/18/19/20/21/22/23/24/25/26/27/28):1</t>
-  </si>
-  <si>
-    <t>n(33/34/35/36/43/44):2</t>
+    <t>(17+18+19+20+21+22+23+24+25+26+27+28):&gt;1</t>
   </si>
   <si>
     <t>!14</t>
   </si>
   <si>
-    <t>n(47/48/49/54/55/57):1</t>
-  </si>
-  <si>
     <t>remove any 3 non-adjacent tiles from current section</t>
   </si>
   <si>
     <t>!(31&amp;32)</t>
   </si>
   <si>
-    <t>n(47/48/57):2</t>
-  </si>
-  <si>
     <t>remove 2 non-adjacent thesis tiles from current section</t>
   </si>
   <si>
     <t>n-0:3:4</t>
   </si>
   <si>
-    <t>n-(47/48/49/54/55/57):2</t>
-  </si>
-  <si>
     <t>!53</t>
   </si>
   <si>
@@ -983,109 +941,151 @@
     <t>!(11/12/32):&gt;1</t>
   </si>
   <si>
-    <t>n41:1&amp;n(17/18/19/20/21/22/23/24/25/26/27/28):1</t>
-  </si>
-  <si>
-    <t>n(45/46):1&amp;n(43/44):1</t>
-  </si>
-  <si>
     <t>keep this card to protect against any future Jargon events</t>
   </si>
   <si>
-    <t>p(54/55):1&amp;i112:1</t>
-  </si>
-  <si>
     <t>!(33/34/35/36):&gt;2</t>
   </si>
   <si>
-    <t>n-(47/48/49/54/55/57):3</t>
-  </si>
-  <si>
     <t>!31:&gt;1</t>
   </si>
   <si>
     <t>!56</t>
   </si>
   <si>
-    <t>n49:2</t>
-  </si>
-  <si>
     <t>Else</t>
   </si>
   <si>
-    <t>f5:1</t>
-  </si>
-  <si>
-    <t>n41:1&amp;n(42/45/46):2</t>
-  </si>
-  <si>
-    <t>n(33/34/35/36):1&amp;n(45/46):1</t>
-  </si>
-  <si>
     <t>o0:2:4</t>
   </si>
   <si>
-    <t>(17+18+19+20+21+22+23+24+25+26+27+28):&gt;=2</t>
+    <t>p2:1:1</t>
+  </si>
+  <si>
+    <t>n30:1:2</t>
+  </si>
+  <si>
+    <t>p41:1:3</t>
+  </si>
+  <si>
+    <t>n(15/16/31):1:2</t>
+  </si>
+  <si>
+    <t>f1:1:1</t>
+  </si>
+  <si>
+    <t>n7:&lt;=9:1</t>
+  </si>
+  <si>
+    <t>f5:1:1</t>
+  </si>
+  <si>
+    <t>n(37/38/39/40/42/45/46):3:3</t>
+  </si>
+  <si>
+    <t>n41:1:3&amp;n(17/18/19/20/21/22/23/24/25/26/27/28):1:3</t>
+  </si>
+  <si>
+    <t>n(42/45/46):1:3</t>
+  </si>
+  <si>
+    <t>n41:1:3&amp;n(42/45/46):2:3</t>
+  </si>
+  <si>
+    <t>n(43/44):2:3</t>
+  </si>
+  <si>
+    <t>n(45/46):1:3&amp;n(43/44):1:3</t>
+  </si>
+  <si>
+    <t>p(43/44):1:3</t>
+  </si>
+  <si>
+    <t>n(17/18/19/20/21/22/23/24/25/26/27/28):1:2</t>
+  </si>
+  <si>
+    <t>n(33/34/35/36):1:3&amp;n(45/46):1:3</t>
+  </si>
+  <si>
+    <t>n(33/34/35/36/43/44):2:3</t>
+  </si>
+  <si>
+    <t>n(47/48/49/54/55/57):1:4</t>
+  </si>
+  <si>
+    <t>n(47/48/57):2:4</t>
+  </si>
+  <si>
+    <t>n-(47/48/49/54/55/57):2:4</t>
+  </si>
+  <si>
+    <t>p(54/55):1:4&amp;i112:1:(2/3/4)</t>
+  </si>
+  <si>
+    <t>n-(47/48/49/54/55/57):3:4</t>
+  </si>
+  <si>
+    <t>n49:2:4</t>
+  </si>
+  <si>
+    <t>Contingency time is time allocated during planning for unforeseen events or problems that may arise.</t>
+  </si>
+  <si>
+    <t>Do you know what the ethical clearance procedure is for your project? If not you need to find out – quickly!</t>
+  </si>
+  <si>
+    <t>This refers to recognizing where you will need additional training and taking steps to learn what you need to before your project starts.</t>
+  </si>
+  <si>
+    <t>Holidays and breaks are really important. But don’t take too many!</t>
+  </si>
+  <si>
+    <t>Milestones are internal deadlines that you plan to keep yourself on track throughout the project, for example, completing a chapter, releasing a survey, or finishing a product prototype.</t>
+  </si>
+  <si>
+    <t>This means looking after your data and metadata. As a minimum this could simply be ensuring that you backup your work regularly, or it could be much more complex digital curation techniques.</t>
+  </si>
+  <si>
+    <t>Your supervisor is a precious resource, plan your time with them well!</t>
   </si>
   <si>
     <t>Thinking is great! But it doesn’t directly produce anything. (Watch out for no upwards arrow!) Too much thinking and not enough planning will hamper your progress.</t>
   </si>
   <si>
-    <t>This means looking after your data and metadata. As a minimum this could simply be ensuring that you backup your work regularly, or it could be much more complex digital curation techniques.</t>
-  </si>
-  <si>
-    <t>Milestones are internal deadlines that you plan to keep yourself on track throughout the project, for example, completing a chapter, releasing a survey, or finishing a product prototype.</t>
-  </si>
-  <si>
-    <t>This refers to recognizing where you will need additional training and taking steps to learn what you need to before your project starts.</t>
-  </si>
-  <si>
-    <t>Holidays and breaks are really important. But don’t take too many!</t>
-  </si>
-  <si>
-    <t>Do you know what the ethical clearance procedure is for your project? If not you need to find out – quickly!</t>
-  </si>
-  <si>
-    <t>Your supervisor is a precious resource, plan your time with them well!</t>
-  </si>
-  <si>
-    <t>Contingency time is time allocated during planning for unforeseen events or problems that may arise.</t>
+    <t>Other people are a great contextual resource!</t>
+  </si>
+  <si>
+    <t>Sometimes an article that’s not relevant to you can still lead you to other good sources of information. (Watch out for no upwards arrow!)</t>
+  </si>
+  <si>
+    <t>A methodology is a system of methods of doing or studying something. It is part of your design process for carrying out research and investigating others’ methods and methodologies is part of contextual review.</t>
+  </si>
+  <si>
+    <t>You may want to tweak your research questions as you do your contextual research, this will help you focus your study.</t>
+  </si>
+  <si>
+    <t>A reference management system will quickly pay back the time you take to learn how to use it. If you don’t already know of one, ask your tutor.</t>
+  </si>
+  <si>
+    <t>This could be an existing database you have accessed and will use directly in your research.</t>
+  </si>
+  <si>
+    <t>These could be physical or digital objects that you are studying or using in your research, for example artworks or existing apps.</t>
   </si>
   <si>
     <t>This could be a government or industrial policy that is relevant to your research.</t>
   </si>
   <si>
-    <t>These could be physical or digital objects that you are studying or using in your research, for example artworks or existing apps.</t>
-  </si>
-  <si>
-    <t>This could be an existing database you have accessed and will use directly in your research.</t>
-  </si>
-  <si>
-    <t>Other people are a great contextual resource!</t>
-  </si>
-  <si>
-    <t>You may want to tweak your research questions as you do your contextual research, this will help you focus your study.</t>
-  </si>
-  <si>
-    <t>A reference management system will quickly pay back the time you take to learn how to use it. If you don’t already know of one, ask your tutor.</t>
-  </si>
-  <si>
-    <t>A methodology is a system of methods of doing or studying something. It is part of your design process for carrying out research and investigating others’ methods and methodologies is part of contextual review.</t>
-  </si>
-  <si>
-    <t>Sometimes an article that’s not relevant to you can still lead you to other good sources of information. (Watch out for no upwards arrow!)</t>
+    <t>Descriptive writing is necessary but it needs to be followed up by some explanation and critical analysis so that readers understand your research in context.</t>
   </si>
   <si>
     <t>Evaluating your work helps you to evidence your conclusions. Make sure you critically analyse your findings rather than just describing them.</t>
   </si>
   <si>
-    <t>Descriptive writing is necessary but it needs to be followed up by some explanation and critical analysis so that readers understand your research in context.</t>
+    <t>When writing up your conclusions, revisit your research questions and check that you are actually answering them!</t>
   </si>
   <si>
     <t>Although not part of what you submit, having support from family and/or friends can be really important for your wellbeing as you progress your research!</t>
-  </si>
-  <si>
-    <t>When writing up your conclusions, revisit your research questions and check that you are actually answering them!</t>
   </si>
 </sst>
 </file>
@@ -1147,13 +1147,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1185,8 +1186,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4A58CFC2-94C3-1B4C-9FA9-2EDE6B381A1D}" name="Table13" displayName="Table13" ref="A1:G59" totalsRowShown="0">
-  <autoFilter ref="A1:G59" xr:uid="{4A58CFC2-94C3-1B4C-9FA9-2EDE6B381A1D}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4A58CFC2-94C3-1B4C-9FA9-2EDE6B381A1D}" name="Table13" displayName="Table13" ref="A1:G60" totalsRowShown="0">
+  <autoFilter ref="A1:G60" xr:uid="{4A58CFC2-94C3-1B4C-9FA9-2EDE6B381A1D}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{93B3FC9C-96B8-F541-B39A-A82E1D56BCAA}" name="CardID" dataDxfId="3">
       <calculatedColumnFormula>ROW() - 1</calculatedColumnFormula>
@@ -1554,24 +1555,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18AE550B-A04F-B142-B067-7E2D879988FA}">
-  <dimension ref="A1:H59"/>
+  <dimension ref="A1:H60"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="102" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.625" customWidth="1"/>
-    <col min="2" max="2" width="15.125" customWidth="1"/>
-    <col min="3" max="3" width="10.375" customWidth="1"/>
-    <col min="4" max="4" width="25.125" customWidth="1"/>
-    <col min="5" max="5" width="49.5" customWidth="1"/>
-    <col min="6" max="6" width="47.375" customWidth="1"/>
+    <col min="1" max="1" width="9.6640625" customWidth="1"/>
+    <col min="2" max="2" width="15.1640625" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" customWidth="1"/>
+    <col min="4" max="4" width="25.1640625" customWidth="1"/>
+    <col min="5" max="5" width="17.5" customWidth="1"/>
+    <col min="6" max="6" width="53" customWidth="1"/>
     <col min="7" max="7" width="9.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1597,7 +1598,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2">
         <f t="shared" ref="A2:A33" si="0">ROW() - 1</f>
         <v>1</v>
@@ -1615,7 +1616,7 @@
         <v>9</v>
       </c>
       <c r="F2" t="s">
-        <v>337</v>
+        <v>5</v>
       </c>
       <c r="G2" t="s">
         <v>242</v>
@@ -1624,7 +1625,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -1642,7 +1643,7 @@
         <v>44</v>
       </c>
       <c r="F3" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="G3" t="s">
         <v>242</v>
@@ -1651,7 +1652,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -1669,13 +1670,13 @@
         <v>46</v>
       </c>
       <c r="F4" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="G4" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1693,13 +1694,13 @@
         <v>48</v>
       </c>
       <c r="F5" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="G5" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1717,13 +1718,13 @@
         <v>50</v>
       </c>
       <c r="F6" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="G6" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1741,13 +1742,13 @@
         <v>52</v>
       </c>
       <c r="F7" t="s">
-        <v>331</v>
+        <v>334</v>
       </c>
       <c r="G7" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1765,13 +1766,13 @@
         <v>54</v>
       </c>
       <c r="F8" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="G8" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1789,13 +1790,13 @@
         <v>12</v>
       </c>
       <c r="F9" t="s">
-        <v>330</v>
+        <v>336</v>
       </c>
       <c r="G9" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1813,13 +1814,13 @@
         <v>56</v>
       </c>
       <c r="F10" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="G10" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1837,13 +1838,13 @@
         <v>58</v>
       </c>
       <c r="F11" t="s">
-        <v>345</v>
+        <v>338</v>
       </c>
       <c r="G11" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1861,13 +1862,13 @@
         <v>60</v>
       </c>
       <c r="F12" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="G12" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1885,13 +1886,13 @@
         <v>60</v>
       </c>
       <c r="F13" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="G13" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1909,13 +1910,13 @@
         <v>63</v>
       </c>
       <c r="F14" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="G14" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1932,14 +1933,14 @@
       <c r="E15" t="s">
         <v>65</v>
       </c>
-      <c r="F15" s="3" t="s">
-        <v>343</v>
+      <c r="F15" t="s">
+        <v>341</v>
       </c>
       <c r="G15" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1956,11 +1957,14 @@
       <c r="E16" t="s">
         <v>67</v>
       </c>
+      <c r="F16" s="3" t="s">
+        <v>342</v>
+      </c>
       <c r="G16" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1981,7 +1985,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -2002,7 +2006,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -2023,7 +2027,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -2040,14 +2044,11 @@
       <c r="E20" t="s">
         <v>16</v>
       </c>
-      <c r="F20" t="s">
-        <v>340</v>
-      </c>
       <c r="G20" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -2065,13 +2066,13 @@
         <v>16</v>
       </c>
       <c r="F21" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="G21" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -2088,11 +2089,14 @@
       <c r="E22" t="s">
         <v>73</v>
       </c>
+      <c r="F22" t="s">
+        <v>343</v>
+      </c>
       <c r="G22" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -2113,7 +2117,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -2134,7 +2138,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -2155,7 +2159,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -2172,14 +2176,11 @@
       <c r="E26" t="s">
         <v>79</v>
       </c>
-      <c r="F26" t="s">
-        <v>339</v>
-      </c>
       <c r="G26" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -2197,13 +2198,13 @@
         <v>79</v>
       </c>
       <c r="F27" t="s">
-        <v>339</v>
+        <v>344</v>
       </c>
       <c r="G27" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -2221,13 +2222,13 @@
         <v>82</v>
       </c>
       <c r="F28" t="s">
-        <v>338</v>
+        <v>344</v>
       </c>
       <c r="G28" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -2245,13 +2246,13 @@
         <v>82</v>
       </c>
       <c r="F29" t="s">
-        <v>338</v>
+        <v>345</v>
       </c>
       <c r="G29" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -2268,11 +2269,14 @@
       <c r="E30" t="s">
         <v>85</v>
       </c>
+      <c r="F30" t="s">
+        <v>345</v>
+      </c>
       <c r="G30" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -2293,7 +2297,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -2314,7 +2318,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -2331,14 +2335,11 @@
       <c r="E33" t="s">
         <v>91</v>
       </c>
-      <c r="F33" t="s">
-        <v>344</v>
-      </c>
       <c r="G33" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34">
         <f t="shared" ref="A34:A59" si="1">ROW() - 1</f>
         <v>33</v>
@@ -2355,11 +2356,14 @@
       <c r="E34" t="s">
         <v>23</v>
       </c>
+      <c r="F34" t="s">
+        <v>340</v>
+      </c>
       <c r="G34" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35">
         <f t="shared" si="1"/>
         <v>34</v>
@@ -2380,7 +2384,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36">
         <f t="shared" si="1"/>
         <v>35</v>
@@ -2401,7 +2405,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37">
         <f t="shared" si="1"/>
         <v>36</v>
@@ -2422,7 +2426,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38">
         <f t="shared" si="1"/>
         <v>37</v>
@@ -2443,7 +2447,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39">
         <f t="shared" si="1"/>
         <v>38</v>
@@ -2464,7 +2468,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40">
         <f t="shared" si="1"/>
         <v>39</v>
@@ -2485,7 +2489,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41">
         <f t="shared" si="1"/>
         <v>40</v>
@@ -2506,7 +2510,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42">
         <f t="shared" si="1"/>
         <v>41</v>
@@ -2527,7 +2531,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43">
         <f t="shared" si="1"/>
         <v>42</v>
@@ -2548,7 +2552,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44">
         <f t="shared" si="1"/>
         <v>43</v>
@@ -2569,7 +2573,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45">
         <f t="shared" si="1"/>
         <v>44</v>
@@ -2590,7 +2594,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46">
         <f t="shared" si="1"/>
         <v>45</v>
@@ -2611,7 +2615,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47">
         <f t="shared" si="1"/>
         <v>46</v>
@@ -2632,7 +2636,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48">
         <f t="shared" si="1"/>
         <v>47</v>
@@ -2653,7 +2657,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49">
         <f t="shared" si="1"/>
         <v>48</v>
@@ -2674,7 +2678,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50">
         <f t="shared" si="1"/>
         <v>49</v>
@@ -2695,7 +2699,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51">
         <f t="shared" si="1"/>
         <v>50</v>
@@ -2712,14 +2716,11 @@
       <c r="E51" t="s">
         <v>32</v>
       </c>
-      <c r="F51" t="s">
-        <v>347</v>
-      </c>
       <c r="G51" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52">
         <f t="shared" si="1"/>
         <v>51</v>
@@ -2737,13 +2738,13 @@
         <v>32</v>
       </c>
       <c r="F52" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="G52" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53">
         <f t="shared" si="1"/>
         <v>52</v>
@@ -2761,13 +2762,13 @@
         <v>32</v>
       </c>
       <c r="F53" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="G53" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54">
         <f t="shared" si="1"/>
         <v>53</v>
@@ -2791,7 +2792,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55">
         <f t="shared" si="1"/>
         <v>54</v>
@@ -2808,11 +2809,14 @@
       <c r="E55" t="s">
         <v>29</v>
       </c>
+      <c r="F55" t="s">
+        <v>347</v>
+      </c>
       <c r="G55" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56">
         <f t="shared" si="1"/>
         <v>55</v>
@@ -2833,7 +2837,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57">
         <f t="shared" si="1"/>
         <v>56</v>
@@ -2850,14 +2854,11 @@
       <c r="E57" t="s">
         <v>119</v>
       </c>
-      <c r="F57" t="s">
-        <v>349</v>
-      </c>
       <c r="G57" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58">
         <f t="shared" si="1"/>
         <v>57</v>
@@ -2874,11 +2875,14 @@
       <c r="E58" t="s">
         <v>121</v>
       </c>
+      <c r="F58" t="s">
+        <v>348</v>
+      </c>
       <c r="G58" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59">
         <f t="shared" si="1"/>
         <v>58</v>
@@ -2895,18 +2899,23 @@
       <c r="E59" t="s">
         <v>123</v>
       </c>
-      <c r="F59" t="s">
-        <v>348</v>
-      </c>
       <c r="G59" t="s">
         <v>245</v>
       </c>
     </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A60" s="4">
+        <f>ROW() - 1</f>
+        <v>59</v>
+      </c>
+      <c r="F60" t="s">
+        <v>349</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
 </file>
@@ -2916,23 +2925,23 @@
   <dimension ref="A1:J66"/>
   <sheetViews>
     <sheetView zoomScale="99" zoomScaleNormal="99" workbookViewId="0">
-      <selection activeCell="J59" sqref="J59"/>
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.125" customWidth="1"/>
+    <col min="1" max="1" width="9.1640625" customWidth="1"/>
     <col min="2" max="2" width="9.5" customWidth="1"/>
-    <col min="3" max="3" width="47.125" customWidth="1"/>
-    <col min="4" max="4" width="25.875" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" customWidth="1"/>
+    <col min="4" max="4" width="25.83203125" customWidth="1"/>
     <col min="5" max="5" width="26" customWidth="1"/>
     <col min="6" max="6" width="14" customWidth="1"/>
     <col min="7" max="7" width="17" customWidth="1"/>
-    <col min="8" max="8" width="15.875" customWidth="1"/>
+    <col min="8" max="8" width="24.6640625" customWidth="1"/>
     <col min="9" max="9" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2958,10 +2967,10 @@
         <v>126</v>
       </c>
       <c r="I1" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2">
         <f t="shared" ref="A2:A33" si="0">ROW() + 57</f>
         <v>59</v>
@@ -2982,13 +2991,13 @@
         <v>129</v>
       </c>
       <c r="H2" t="s">
-        <v>268</v>
+        <v>307</v>
       </c>
       <c r="I2" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3">
         <f t="shared" si="0"/>
         <v>60</v>
@@ -3009,13 +3018,13 @@
         <v>129</v>
       </c>
       <c r="H3" t="s">
-        <v>269</v>
+        <v>308</v>
       </c>
       <c r="I3" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4">
         <f t="shared" si="0"/>
         <v>61</v>
@@ -3042,7 +3051,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>62</v>
@@ -3060,7 +3069,7 @@
         <v>129</v>
       </c>
       <c r="G5" t="s">
-        <v>288</v>
+        <v>279</v>
       </c>
       <c r="H5" t="s">
         <v>261</v>
@@ -3069,7 +3078,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>63</v>
@@ -3087,7 +3096,7 @@
         <v>129</v>
       </c>
       <c r="G6" t="s">
-        <v>288</v>
+        <v>279</v>
       </c>
       <c r="H6" t="s">
         <v>261</v>
@@ -3096,7 +3105,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>64</v>
@@ -3123,7 +3132,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>65</v>
@@ -3153,7 +3162,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>66</v>
@@ -3174,13 +3183,13 @@
         <v>129</v>
       </c>
       <c r="H9" t="s">
-        <v>270</v>
+        <v>309</v>
       </c>
       <c r="I9" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>67</v>
@@ -3201,16 +3210,16 @@
         <v>254</v>
       </c>
       <c r="H10" t="s">
-        <v>271</v>
+        <v>310</v>
       </c>
       <c r="I10" t="s">
-        <v>129</v>
+        <v>311</v>
       </c>
       <c r="J10" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>68</v>
@@ -3231,7 +3240,7 @@
         <v>257</v>
       </c>
       <c r="H11" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="I11" t="s">
         <v>129</v>
@@ -3240,7 +3249,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>69</v>
@@ -3261,16 +3270,16 @@
         <v>254</v>
       </c>
       <c r="H12" t="s">
-        <v>271</v>
+        <v>310</v>
       </c>
       <c r="I12" t="s">
-        <v>129</v>
+        <v>311</v>
       </c>
       <c r="J12" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>70</v>
@@ -3291,13 +3300,13 @@
         <v>255</v>
       </c>
       <c r="H13" t="s">
-        <v>272</v>
+        <v>262</v>
       </c>
       <c r="I13" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>71</v>
@@ -3318,13 +3327,13 @@
         <v>129</v>
       </c>
       <c r="H14" t="s">
-        <v>273</v>
+        <v>312</v>
       </c>
       <c r="I14" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>72</v>
@@ -3339,7 +3348,7 @@
         <v>156</v>
       </c>
       <c r="F15" t="s">
-        <v>329</v>
+        <v>282</v>
       </c>
       <c r="G15" t="s">
         <v>129</v>
@@ -3354,7 +3363,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>73</v>
@@ -3372,16 +3381,16 @@
         <v>129</v>
       </c>
       <c r="G16" t="s">
-        <v>288</v>
+        <v>279</v>
       </c>
       <c r="H16" t="s">
         <v>260</v>
       </c>
       <c r="I16" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>74</v>
@@ -3402,13 +3411,13 @@
         <v>254</v>
       </c>
       <c r="H17" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="I17" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>75</v>
@@ -3432,10 +3441,10 @@
         <v>261</v>
       </c>
       <c r="I18" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>76</v>
@@ -3459,10 +3468,10 @@
         <v>262</v>
       </c>
       <c r="I19" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>77</v>
@@ -3489,7 +3498,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>78</v>
@@ -3510,13 +3519,13 @@
         <v>129</v>
       </c>
       <c r="H21" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="I21" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22">
         <f t="shared" si="0"/>
         <v>79</v>
@@ -3543,7 +3552,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23">
         <f t="shared" si="0"/>
         <v>80</v>
@@ -3564,13 +3573,13 @@
         <v>258</v>
       </c>
       <c r="H23" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="I23" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24">
         <f t="shared" si="0"/>
         <v>81</v>
@@ -3591,13 +3600,13 @@
         <v>252</v>
       </c>
       <c r="H24" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="I24" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25">
         <f t="shared" si="0"/>
         <v>82</v>
@@ -3618,13 +3627,13 @@
         <v>129</v>
       </c>
       <c r="H25" t="s">
-        <v>277</v>
+        <v>314</v>
       </c>
       <c r="I25" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26">
         <f t="shared" si="0"/>
         <v>83</v>
@@ -3642,7 +3651,7 @@
         <v>129</v>
       </c>
       <c r="G26" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
       <c r="H26" t="s">
         <v>315</v>
@@ -3651,10 +3660,10 @@
         <v>129</v>
       </c>
       <c r="J26" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27">
         <f t="shared" si="0"/>
         <v>84</v>
@@ -3672,16 +3681,16 @@
         <v>129</v>
       </c>
       <c r="G27" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="H27" t="s">
-        <v>281</v>
+        <v>316</v>
       </c>
       <c r="I27" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28">
         <f t="shared" si="0"/>
         <v>85</v>
@@ -3699,16 +3708,16 @@
         <v>129</v>
       </c>
       <c r="G28" t="s">
-        <v>288</v>
+        <v>279</v>
       </c>
       <c r="H28" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="I28" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29">
         <f t="shared" si="0"/>
         <v>86</v>
@@ -3729,13 +3738,13 @@
         <v>253</v>
       </c>
       <c r="H29" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="I29" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30">
         <f t="shared" si="0"/>
         <v>87</v>
@@ -3753,16 +3762,16 @@
         <v>129</v>
       </c>
       <c r="G30" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
       <c r="H30" t="s">
-        <v>284</v>
+        <v>276</v>
       </c>
       <c r="I30" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31">
         <f t="shared" si="0"/>
         <v>88</v>
@@ -3783,13 +3792,13 @@
         <v>129</v>
       </c>
       <c r="H31" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
       <c r="I31" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32">
         <f t="shared" si="0"/>
         <v>89</v>
@@ -3810,13 +3819,13 @@
         <v>129</v>
       </c>
       <c r="H32" t="s">
-        <v>326</v>
+        <v>317</v>
       </c>
       <c r="I32" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33">
         <f t="shared" si="0"/>
         <v>90</v>
@@ -3837,13 +3846,13 @@
         <v>255</v>
       </c>
       <c r="H33" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
       <c r="I33" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34">
         <f t="shared" ref="A34:A66" si="1">ROW() + 57</f>
         <v>91</v>
@@ -3864,13 +3873,13 @@
         <v>252</v>
       </c>
       <c r="H34" t="s">
-        <v>287</v>
+        <v>318</v>
       </c>
       <c r="I34" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35">
         <f t="shared" si="1"/>
         <v>92</v>
@@ -3888,16 +3897,16 @@
         <v>129</v>
       </c>
       <c r="G35" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
       <c r="H35" t="s">
-        <v>316</v>
+        <v>319</v>
       </c>
       <c r="I35" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36">
         <f t="shared" si="1"/>
         <v>93</v>
@@ -3915,16 +3924,16 @@
         <v>129</v>
       </c>
       <c r="G36" t="s">
-        <v>288</v>
+        <v>279</v>
       </c>
       <c r="H36" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="I36" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37">
         <f t="shared" si="1"/>
         <v>94</v>
@@ -3942,16 +3951,16 @@
         <v>129</v>
       </c>
       <c r="G37" t="s">
-        <v>289</v>
+        <v>280</v>
       </c>
       <c r="H37" t="s">
-        <v>290</v>
+        <v>320</v>
       </c>
       <c r="I37" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38">
         <f t="shared" si="1"/>
         <v>95</v>
@@ -3969,16 +3978,16 @@
         <v>129</v>
       </c>
       <c r="G38" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="H38" t="s">
-        <v>292</v>
+        <v>321</v>
       </c>
       <c r="I38" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39">
         <f t="shared" si="1"/>
         <v>96</v>
@@ -3999,13 +4008,13 @@
         <v>254</v>
       </c>
       <c r="H39" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="I39" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40">
         <f t="shared" si="1"/>
         <v>97</v>
@@ -4026,13 +4035,13 @@
         <v>254</v>
       </c>
       <c r="H40" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
       <c r="I40" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41">
         <f t="shared" si="1"/>
         <v>98</v>
@@ -4050,16 +4059,16 @@
         <v>129</v>
       </c>
       <c r="G41" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
       <c r="H41" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="I41" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42">
         <f t="shared" si="1"/>
         <v>99</v>
@@ -4077,16 +4086,16 @@
         <v>129</v>
       </c>
       <c r="G42" t="s">
-        <v>288</v>
+        <v>279</v>
       </c>
       <c r="H42" t="s">
-        <v>328</v>
+        <v>306</v>
       </c>
       <c r="I42" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4104,16 +4113,16 @@
         <v>129</v>
       </c>
       <c r="G43" t="s">
-        <v>310</v>
+        <v>296</v>
       </c>
       <c r="H43" t="s">
-        <v>293</v>
+        <v>323</v>
       </c>
       <c r="I43" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44">
         <f t="shared" si="1"/>
         <v>101</v>
@@ -4131,16 +4140,16 @@
         <v>129</v>
       </c>
       <c r="G44" t="s">
-        <v>311</v>
+        <v>297</v>
       </c>
       <c r="H44" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
       <c r="I44" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45">
         <f t="shared" si="1"/>
         <v>102</v>
@@ -4158,16 +4167,16 @@
         <v>129</v>
       </c>
       <c r="G45" t="s">
-        <v>294</v>
+        <v>283</v>
       </c>
       <c r="H45" t="s">
-        <v>295</v>
+        <v>324</v>
       </c>
       <c r="I45" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46">
         <f t="shared" si="1"/>
         <v>103</v>
@@ -4188,16 +4197,16 @@
         <v>252</v>
       </c>
       <c r="H46" t="s">
-        <v>300</v>
+        <v>287</v>
       </c>
       <c r="I46" t="s">
         <v>129</v>
       </c>
       <c r="J46" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47">
         <f t="shared" si="1"/>
         <v>104</v>
@@ -4218,13 +4227,13 @@
         <v>254</v>
       </c>
       <c r="H47" t="s">
-        <v>295</v>
+        <v>324</v>
       </c>
       <c r="I47" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48">
         <f t="shared" si="1"/>
         <v>105</v>
@@ -4242,16 +4251,16 @@
         <v>129</v>
       </c>
       <c r="G48" t="s">
-        <v>297</v>
+        <v>285</v>
       </c>
       <c r="H48" t="s">
-        <v>298</v>
+        <v>325</v>
       </c>
       <c r="I48" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49">
         <f t="shared" si="1"/>
         <v>106</v>
@@ -4269,19 +4278,19 @@
         <v>129</v>
       </c>
       <c r="G49" t="s">
-        <v>288</v>
+        <v>279</v>
       </c>
       <c r="H49" t="s">
-        <v>301</v>
+        <v>326</v>
       </c>
       <c r="I49" t="s">
-        <v>295</v>
+        <v>324</v>
       </c>
       <c r="J49" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A50">
         <f t="shared" si="1"/>
         <v>107</v>
@@ -4299,16 +4308,16 @@
         <v>129</v>
       </c>
       <c r="G50" t="s">
-        <v>288</v>
+        <v>279</v>
       </c>
       <c r="H50" t="s">
-        <v>301</v>
+        <v>326</v>
       </c>
       <c r="I50" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A51">
         <f t="shared" si="1"/>
         <v>108</v>
@@ -4326,16 +4335,16 @@
         <v>129</v>
       </c>
       <c r="G51" t="s">
-        <v>302</v>
+        <v>288</v>
       </c>
       <c r="H51" t="s">
-        <v>303</v>
+        <v>289</v>
       </c>
       <c r="I51" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A52">
         <f t="shared" si="1"/>
         <v>109</v>
@@ -4353,16 +4362,16 @@
         <v>129</v>
       </c>
       <c r="G52" t="s">
-        <v>304</v>
+        <v>290</v>
       </c>
       <c r="H52" t="s">
-        <v>301</v>
+        <v>326</v>
       </c>
       <c r="I52" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A53">
         <f t="shared" si="1"/>
         <v>110</v>
@@ -4380,16 +4389,16 @@
         <v>129</v>
       </c>
       <c r="G53" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
       <c r="H53" t="s">
-        <v>305</v>
+        <v>291</v>
       </c>
       <c r="I53" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A54">
         <f t="shared" si="1"/>
         <v>111</v>
@@ -4407,16 +4416,16 @@
         <v>129</v>
       </c>
       <c r="G54" t="s">
-        <v>314</v>
+        <v>300</v>
       </c>
       <c r="H54" t="s">
-        <v>301</v>
+        <v>326</v>
       </c>
       <c r="I54" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A55">
         <f t="shared" si="1"/>
         <v>112</v>
@@ -4434,16 +4443,16 @@
         <v>129</v>
       </c>
       <c r="G55" t="s">
-        <v>308</v>
+        <v>294</v>
       </c>
       <c r="H55" t="s">
-        <v>306</v>
+        <v>292</v>
       </c>
       <c r="I55" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A56">
         <f t="shared" si="1"/>
         <v>113</v>
@@ -4461,16 +4470,16 @@
         <v>129</v>
       </c>
       <c r="G56" t="s">
-        <v>307</v>
+        <v>293</v>
       </c>
       <c r="H56" t="s">
-        <v>309</v>
+        <v>295</v>
       </c>
       <c r="I56" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A57">
         <f t="shared" si="1"/>
         <v>114</v>
@@ -4488,16 +4497,16 @@
         <v>129</v>
       </c>
       <c r="G57" t="s">
-        <v>312</v>
+        <v>298</v>
       </c>
       <c r="H57" t="s">
-        <v>313</v>
+        <v>299</v>
       </c>
       <c r="I57" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A58">
         <f t="shared" si="1"/>
         <v>115</v>
@@ -4515,16 +4524,16 @@
         <v>129</v>
       </c>
       <c r="G58" t="s">
-        <v>288</v>
+        <v>279</v>
       </c>
       <c r="H58" t="s">
-        <v>301</v>
+        <v>326</v>
       </c>
       <c r="I58" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A59">
         <f t="shared" si="1"/>
         <v>116</v>
@@ -4545,16 +4554,16 @@
         <v>129</v>
       </c>
       <c r="H59" t="s">
-        <v>318</v>
+        <v>327</v>
       </c>
       <c r="I59" t="s">
         <v>129</v>
       </c>
       <c r="J59" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A60">
         <f t="shared" si="1"/>
         <v>117</v>
@@ -4572,16 +4581,16 @@
         <v>129</v>
       </c>
       <c r="G60" t="s">
-        <v>294</v>
+        <v>283</v>
       </c>
       <c r="H60" t="s">
-        <v>295</v>
+        <v>324</v>
       </c>
       <c r="I60" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A61">
         <f t="shared" si="1"/>
         <v>118</v>
@@ -4599,16 +4608,16 @@
         <v>129</v>
       </c>
       <c r="G61" t="s">
-        <v>319</v>
+        <v>302</v>
       </c>
       <c r="H61" t="s">
-        <v>320</v>
+        <v>328</v>
       </c>
       <c r="I61" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A62">
         <f t="shared" si="1"/>
         <v>119</v>
@@ -4629,13 +4638,13 @@
         <v>254</v>
       </c>
       <c r="H62" t="s">
-        <v>309</v>
+        <v>295</v>
       </c>
       <c r="I62" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A63">
         <f t="shared" si="1"/>
         <v>120</v>
@@ -4653,16 +4662,16 @@
         <v>129</v>
       </c>
       <c r="G63" t="s">
-        <v>321</v>
+        <v>303</v>
       </c>
       <c r="H63" t="s">
-        <v>301</v>
+        <v>326</v>
       </c>
       <c r="I63" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A64">
         <f t="shared" si="1"/>
         <v>121</v>
@@ -4680,16 +4689,16 @@
         <v>129</v>
       </c>
       <c r="G64" t="s">
-        <v>322</v>
+        <v>304</v>
       </c>
       <c r="H64" t="s">
-        <v>295</v>
+        <v>324</v>
       </c>
       <c r="I64" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65">
         <f t="shared" si="1"/>
         <v>122</v>
@@ -4707,16 +4716,16 @@
         <v>129</v>
       </c>
       <c r="G65" t="s">
-        <v>310</v>
+        <v>296</v>
       </c>
       <c r="H65" t="s">
-        <v>301</v>
+        <v>326</v>
       </c>
       <c r="I65" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66">
         <f t="shared" si="1"/>
         <v>123</v>
@@ -4737,7 +4746,7 @@
         <v>129</v>
       </c>
       <c r="H66" t="s">
-        <v>323</v>
+        <v>329</v>
       </c>
       <c r="I66" t="s">
         <v>129</v>
@@ -4760,14 +4769,14 @@
       <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="3" width="18.875" customWidth="1"/>
-    <col min="4" max="4" width="18.875" style="1" customWidth="1"/>
-    <col min="5" max="10" width="18.875" customWidth="1"/>
+    <col min="1" max="3" width="18.83203125" customWidth="1"/>
+    <col min="4" max="4" width="18.83203125" style="1" customWidth="1"/>
+    <col min="5" max="10" width="18.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4790,7 +4799,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -4810,7 +4819,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -4830,7 +4839,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -4853,7 +4862,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -4873,7 +4882,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -4893,7 +4902,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -4913,7 +4922,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -4933,7 +4942,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -4953,7 +4962,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>34</v>
       </c>
@@ -4961,7 +4970,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>36</v>
       </c>
@@ -4969,12 +4978,12 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -5006,7 +5015,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>1</v>
       </c>
@@ -5035,7 +5044,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>2</v>
       </c>
@@ -5064,7 +5073,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>3</v>
       </c>
@@ -5093,7 +5102,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>4</v>
       </c>
@@ -5122,7 +5131,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>5</v>
       </c>
@@ -5151,7 +5160,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>6</v>
       </c>
@@ -5180,7 +5189,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>7</v>
       </c>
@@ -5209,7 +5218,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>8</v>
       </c>
@@ -5238,7 +5247,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="D24"/>
     </row>
   </sheetData>

</xml_diff>